<commit_message>
updated todo list with additional items
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="10035"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="86">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -270,6 +265,15 @@
   </si>
   <si>
     <t>Steve/Aron</t>
+  </si>
+  <si>
+    <t>Ty/Mike</t>
+  </si>
+  <si>
+    <t>CSP model bug fixes per AOP</t>
+  </si>
+  <si>
+    <t>Loss diagrams renderer updates and update for tech</t>
   </si>
 </sst>
 </file>
@@ -300,7 +304,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -348,7 +353,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -367,9 +372,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,7 +436,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,7 +471,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -674,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,23 +716,23 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="10" t="s">
         <v>82</v>
       </c>
       <c r="D2" s="11">
         <v>3</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="10"/>
+      <c r="F2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
@@ -1510,6 +1516,34 @@
         <v>66</v>
       </c>
       <c r="E53" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" s="9" t="s">
         <v>67</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated todo with 'orange' testing label for report generator.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="87">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -274,6 +274,9 @@
   </si>
   <si>
     <t>Loss diagrams renderer updates and update for tech</t>
+  </si>
+  <si>
+    <t>Testing</t>
   </si>
 </sst>
 </file>
@@ -312,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +331,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -353,7 +362,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -376,6 +385,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -683,7 +695,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,8 +788,8 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>61</v>
+      <c r="A5" s="14" t="s">
+        <v>86</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
basic saving of graphs in project files, and results viewer perspective too. saves also excel exchange summary does NOT save graph order or sizes yet...
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -48,9 +48,6 @@
     <t>finish up send-to-excel with equations</t>
   </si>
   <si>
-    <t>Excel exchange for base case (+parametrics?)</t>
-  </si>
-  <si>
     <t>Help system UI and content</t>
   </si>
   <si>
@@ -108,9 +105,6 @@
     <t>building load estimator impl in C++ and integration</t>
   </si>
   <si>
-    <t>General polishing and usability (i.e saving views in outputs, graphs etc)</t>
-  </si>
-  <si>
     <t>Web update system</t>
   </si>
   <si>
@@ -276,7 +270,13 @@
     <t>Loss diagrams renderer updates and update for tech</t>
   </si>
   <si>
+    <t>Excel exchange for base case</t>
+  </si>
+  <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>General usability, including saving views in outputs, graphs</t>
   </si>
 </sst>
 </file>
@@ -315,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -331,6 +331,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -362,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -378,14 +396,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -695,7 +719,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,863 +727,896 @@
     <col min="1" max="1" width="12.28515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="89.42578125" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="9" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="8" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" customWidth="1"/>
     <col min="6" max="6" width="47.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="D2" s="11">
+        <v>59</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="12">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" s="12"/>
+      <c r="E2" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="9">
+      <c r="C3" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" s="15">
         <v>2</v>
       </c>
-      <c r="E3" t="s">
-        <v>68</v>
+      <c r="E3" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="H3">
         <f>SUM(D2:D15)</f>
         <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B4" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="15">
+        <v>8</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="9">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" s="9">
+      <c r="C5" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="15">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
-        <v>68</v>
+      <c r="E5" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D6" s="9">
+        <v>59</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="15">
         <v>4</v>
       </c>
-      <c r="E6" t="s">
-        <v>68</v>
+      <c r="E6" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="9">
+        <v>59</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="15">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
-        <v>68</v>
+      <c r="E7" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="9">
+        <v>59</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="15">
         <v>0.5</v>
       </c>
-      <c r="E8" t="s">
-        <v>68</v>
+      <c r="E8" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D9" s="9">
+      <c r="A9" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="15">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
-        <v>68</v>
+      <c r="E9" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="9">
+        <v>59</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="15">
         <v>5</v>
       </c>
-      <c r="E10" t="s">
-        <v>68</v>
+      <c r="E10" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="9">
+        <v>59</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="15">
         <v>3</v>
       </c>
-      <c r="E11" t="s">
-        <v>68</v>
+      <c r="E11" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="B12" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="15">
         <v>0</v>
       </c>
-      <c r="E12" t="s">
-        <v>68</v>
+      <c r="E12" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>49</v>
-      </c>
-      <c r="D13" s="9">
+        <v>59</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="15">
         <v>0.5</v>
       </c>
-      <c r="E13" t="s">
-        <v>68</v>
+      <c r="E13" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="9">
+        <v>59</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D14" s="15">
         <v>1</v>
       </c>
-      <c r="E14" t="s">
-        <v>68</v>
+      <c r="E14" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="9">
+      <c r="C15" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="15">
         <v>0</v>
       </c>
-      <c r="E15" t="s">
-        <v>68</v>
+      <c r="E15" s="14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C16" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="9">
+      <c r="C16" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="17">
         <v>8</v>
       </c>
-      <c r="E16" t="s">
-        <v>69</v>
+      <c r="E16" s="16" t="s">
+        <v>67</v>
       </c>
       <c r="H16">
         <f>SUM(D16:D37)</f>
         <v>77</v>
       </c>
       <c r="I16" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B17" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
-        <v>74</v>
-      </c>
-      <c r="D17" s="9">
+      <c r="C17" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="17">
         <v>4</v>
       </c>
-      <c r="E17" t="s">
-        <v>69</v>
+      <c r="E17" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C18" t="s">
-        <v>51</v>
-      </c>
-      <c r="D18" s="9">
+      <c r="C18" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="17">
         <v>4</v>
       </c>
-      <c r="E18" t="s">
-        <v>69</v>
+      <c r="E18" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B19" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
-        <v>51</v>
-      </c>
-      <c r="D19" s="9">
+      <c r="C19" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="17">
         <v>2</v>
       </c>
-      <c r="E19" t="s">
-        <v>69</v>
+      <c r="E19" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="9">
+      <c r="C20" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="17">
         <v>2</v>
       </c>
-      <c r="E20" t="s">
-        <v>69</v>
+      <c r="E20" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" t="s">
-        <v>55</v>
-      </c>
-      <c r="D21" s="9">
+        <v>59</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="17">
         <v>3</v>
       </c>
-      <c r="E21" t="s">
-        <v>69</v>
+      <c r="E21" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="C22" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="9">
+      <c r="C22" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D22" s="17">
         <v>2</v>
       </c>
-      <c r="E22" t="s">
-        <v>69</v>
+      <c r="E22" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="9">
+      <c r="A23" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="17">
         <v>1.5</v>
       </c>
-      <c r="E23" t="s">
-        <v>69</v>
+      <c r="E23" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="9">
+        <v>59</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D24" s="17">
         <v>5</v>
       </c>
-      <c r="E24" t="s">
-        <v>69</v>
+      <c r="E24" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="9">
+        <v>59</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="17">
         <v>5</v>
       </c>
-      <c r="E25" t="s">
-        <v>69</v>
+      <c r="E25" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="9">
+        <v>59</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="17">
         <v>2</v>
       </c>
-      <c r="E26" t="s">
-        <v>69</v>
+      <c r="E26" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" t="s">
-        <v>71</v>
-      </c>
-      <c r="D27" s="9">
+        <v>59</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="17">
         <v>3</v>
       </c>
-      <c r="E27" t="s">
-        <v>69</v>
+      <c r="E27" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C28" t="s">
-        <v>50</v>
-      </c>
-      <c r="D28" s="9">
+        <v>59</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="17">
         <v>1</v>
       </c>
-      <c r="E28" t="s">
-        <v>69</v>
+      <c r="E28" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="C29" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="9">
+        <v>59</v>
+      </c>
+      <c r="B29" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="17">
         <v>2</v>
       </c>
-      <c r="E29" t="s">
-        <v>69</v>
+      <c r="E29" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="9">
+        <v>59</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" s="17">
         <v>1</v>
       </c>
-      <c r="E30" t="s">
-        <v>69</v>
+      <c r="E30" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C31" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="9">
+        <v>59</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D31" s="17">
         <v>10</v>
       </c>
-      <c r="E31" t="s">
-        <v>69</v>
+      <c r="E31" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D32" s="9">
+        <v>59</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="17">
         <v>3</v>
       </c>
-      <c r="E32" t="s">
-        <v>69</v>
+      <c r="E32" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D33" s="9">
+        <v>59</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="17">
         <v>1</v>
       </c>
-      <c r="E33" t="s">
-        <v>69</v>
+      <c r="E33" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C34" t="s">
-        <v>52</v>
-      </c>
-      <c r="D34" s="9">
+        <v>59</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="17">
         <v>10</v>
       </c>
-      <c r="E34" t="s">
-        <v>69</v>
+      <c r="E34" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C35" t="s">
-        <v>53</v>
-      </c>
-      <c r="D35" s="9">
+        <v>59</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="17">
         <v>5</v>
       </c>
-      <c r="E35" t="s">
-        <v>69</v>
+      <c r="E35" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" s="9">
+        <v>59</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D36" s="17">
         <v>0.5</v>
       </c>
-      <c r="E36" t="s">
-        <v>69</v>
+      <c r="E36" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="9">
+        <v>59</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="17">
         <v>2</v>
       </c>
-      <c r="E37" t="s">
-        <v>69</v>
+      <c r="E37" s="16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B38" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C38" t="s">
-        <v>75</v>
-      </c>
-      <c r="E38" t="s">
-        <v>67</v>
+      <c r="C38" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38" s="19"/>
+      <c r="E38" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B39" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E39" t="s">
-        <v>67</v>
+      <c r="C39" s="18"/>
+      <c r="D39" s="19"/>
+      <c r="E39" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B40" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E40" t="s">
-        <v>67</v>
+      <c r="C40" s="18"/>
+      <c r="D40" s="19"/>
+      <c r="E40" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B41" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="18"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" s="18"/>
+      <c r="D42" s="19"/>
+      <c r="E42" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="E43" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C43" s="18"/>
+      <c r="D43" s="19"/>
+      <c r="E43" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B44" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="E44" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C44" s="18"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B45" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C45" s="18"/>
+      <c r="D45" s="19"/>
+      <c r="E45" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B46" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="E46" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B46" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="18"/>
+      <c r="D46" s="19"/>
+      <c r="E46" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B47" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E47" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B47" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B48" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E48" t="s">
-        <v>67</v>
+      <c r="C48" s="18"/>
+      <c r="D48" s="19"/>
+      <c r="E48" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B49" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="E49" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B49" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C49" s="18"/>
+      <c r="D49" s="19"/>
+      <c r="E49" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E50" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B50" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="18"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E51" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B51" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="C51" s="18"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="E52" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C52" s="18"/>
+      <c r="D52" s="19"/>
+      <c r="E52" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B53" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="E53" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C53" s="18"/>
+      <c r="D53" s="19"/>
+      <c r="E53" s="18" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B54" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="C54" t="s">
-        <v>83</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="19"/>
+      <c r="E54" s="19" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="B55" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="C55" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" s="9" t="s">
-        <v>67</v>
+        <v>59</v>
+      </c>
+      <c r="B55" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to scripting capability: additional invoke functions and input/output variable browser added
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aron\Documents\Projects\SAMnt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -724,7 +724,7 @@
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,8 +834,8 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>59</v>
+      <c r="A6" s="5" t="s">
+        <v>58</v>
       </c>
       <c r="B6" s="14" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
installer scripts for Windows.  Updated SAM TODO.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -399,7 +399,14 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -424,6 +431,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -431,7 +445,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -452,7 +466,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -766,7 +787,7 @@
   <dimension ref="A1:I56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -819,7 +840,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
@@ -843,7 +864,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>10</v>
@@ -996,7 +1017,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>38</v>
@@ -1688,13 +1709,13 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="2" operator="beginsWith" text="Done">
+    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="Done">
       <formula>LEFT(A1,LEN("Done"))="Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updates for solar prospector
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -755,7 +755,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -883,7 +883,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Fixed a bug on the capital costs page causing an error to display when you selected the Sandia PV module model.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="97">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>Update defaults for all cases</t>
+  </si>
+  <si>
+    <t>Re-arrange self-shading inputs in UI with system design? Check inputs for usability in SDK</t>
   </si>
 </sst>
 </file>
@@ -752,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1067,7 @@
         <v>67</v>
       </c>
       <c r="H17">
-        <f>SUM(D17:D39)</f>
+        <f>SUM(D17:D40)</f>
         <v>77</v>
       </c>
       <c r="I17" t="s">
@@ -1348,7 +1351,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B34" s="12" t="s">
         <v>26</v>
@@ -1368,30 +1371,26 @@
         <v>59</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>27</v>
+        <v>96</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="13">
-        <v>10</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>67</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D35" s="13"/>
+      <c r="E35" s="12"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D36" s="13">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>67</v>
@@ -1402,13 +1401,13 @@
         <v>59</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D37" s="13">
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>67</v>
@@ -1419,13 +1418,13 @@
         <v>59</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>93</v>
+        <v>33</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>94</v>
+        <v>48</v>
+      </c>
+      <c r="D38" s="13">
+        <v>0.5</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>67</v>
@@ -1436,13 +1435,13 @@
         <v>59</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D39" s="13">
-        <v>2</v>
+        <v>47</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>67</v>
@@ -1450,25 +1449,27 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="14" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D40" s="13">
+        <v>2</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>73</v>
@@ -1483,9 +1484,11 @@
         <v>59</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C42" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D42" s="15"/>
       <c r="E42" s="14" t="s">
         <v>65</v>
@@ -1496,7 +1499,7 @@
         <v>59</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C43" s="14"/>
       <c r="D43" s="15"/>
@@ -1509,7 +1512,7 @@
         <v>59</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C44" s="14"/>
       <c r="D44" s="15"/>
@@ -1522,7 +1525,7 @@
         <v>59</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C45" s="14"/>
       <c r="D45" s="15"/>
@@ -1535,7 +1538,7 @@
         <v>59</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="15"/>
@@ -1548,7 +1551,7 @@
         <v>59</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="15"/>
@@ -1561,7 +1564,7 @@
         <v>59</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="15"/>
@@ -1574,7 +1577,7 @@
         <v>59</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="15"/>
@@ -1587,7 +1590,7 @@
         <v>59</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="15"/>
@@ -1600,7 +1603,7 @@
         <v>59</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="15"/>
@@ -1613,7 +1616,7 @@
         <v>59</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="15"/>
@@ -1626,7 +1629,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="15"/>
@@ -1639,7 +1642,7 @@
         <v>59</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="15"/>
@@ -1652,7 +1655,7 @@
         <v>59</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="15"/>
@@ -1665,13 +1668,11 @@
         <v>59</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>81</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C56" s="14"/>
       <c r="D56" s="15"/>
-      <c r="E56" s="15" t="s">
+      <c r="E56" s="14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1680,10 +1681,10 @@
         <v>59</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="15" t="s">
@@ -1695,12 +1696,12 @@
         <v>59</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D58" s="14"/>
+        <v>49</v>
+      </c>
+      <c r="D58" s="15"/>
       <c r="E58" s="15" t="s">
         <v>65</v>
       </c>
@@ -1710,18 +1711,22 @@
         <v>59</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C59" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="D59" s="14"/>
-      <c r="E59" s="15"/>
+      <c r="E59" s="15" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
@@ -1732,15 +1737,26 @@
         <v>59</v>
       </c>
       <c r="B61" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="15"/>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B62" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C62" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D61" s="14" t="s">
+      <c r="D62" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E61" s="15" t="s">
+      <c r="E62" s="15" t="s">
         <v>91</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added shading tool specific TODOs to list just for future reference
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="105">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -310,6 +310,27 @@
   </si>
   <si>
     <t>Re-arrange self-shading inputs in UI with system design? Sizing check? Check inputs for usability in SDK</t>
+  </si>
+  <si>
+    <t>hidden objects should not be included in shade analysis?</t>
+  </si>
+  <si>
+    <t>remove checkboxes to show/hide objects</t>
+  </si>
+  <si>
+    <t>zoom to fit, 'F' key</t>
+  </si>
+  <si>
+    <t>clear properties on de-select object</t>
+  </si>
+  <si>
+    <t>object list sorted by group</t>
+  </si>
+  <si>
+    <t>active area polygon rotation</t>
+  </si>
+  <si>
+    <t>composite objects: regular fixed array</t>
   </si>
 </sst>
 </file>
@@ -355,7 +376,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +407,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -408,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -432,11 +459,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -758,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="F79" sqref="F79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1774,18 +1844,74 @@
         <v>91</v>
       </c>
     </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B67" s="19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B68" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>104</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:G52">
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="Done">
+    <cfRule type="beginsWith" dxfId="7" priority="2" operator="beginsWith" text="Done">
       <formula>LEFT(A1,LEN("Done"))="Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated/fixed shading file imports- PVsyst and SunEye hourly have been tested and are correct, SunEye obstructions and both Solar Pathfinder functions compile but have not been tested with real files
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="107">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -334,6 +334,9 @@
   </si>
   <si>
     <t>Make summary page prettier? Put example graphs/tables on graphs/data pages?</t>
+  </si>
+  <si>
+    <t>Check SunEye Obstructions and both Solar Pathfinder file imports</t>
   </si>
 </sst>
 </file>
@@ -789,10 +792,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I74"/>
+  <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1101,7 +1104,7 @@
         <v>67</v>
       </c>
       <c r="H17">
-        <f>SUM(D17:D42)</f>
+        <f>SUM(D17:D43)</f>
         <v>77</v>
       </c>
       <c r="I17" t="s">
@@ -1508,39 +1511,37 @@
         <v>59</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>40</v>
+        <v>106</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D42" s="13">
-        <v>2</v>
-      </c>
-      <c r="E42" s="12" t="s">
-        <v>67</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D42" s="13"/>
+      <c r="E42" s="12"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="15"/>
-      <c r="E43" s="14" t="s">
-        <v>65</v>
+        <v>59</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D43" s="13">
+        <v>2</v>
+      </c>
+      <c r="E43" s="12" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>73</v>
@@ -1555,9 +1556,11 @@
         <v>59</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="C45" s="14"/>
+        <v>5</v>
+      </c>
+      <c r="C45" s="14" t="s">
+        <v>73</v>
+      </c>
       <c r="D45" s="15"/>
       <c r="E45" s="14" t="s">
         <v>65</v>
@@ -1568,7 +1571,7 @@
         <v>59</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="15"/>
@@ -1581,7 +1584,7 @@
         <v>59</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C47" s="14"/>
       <c r="D47" s="15"/>
@@ -1594,7 +1597,7 @@
         <v>59</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>55</v>
+        <v>21</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="15"/>
@@ -1607,7 +1610,7 @@
         <v>59</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="15"/>
@@ -1620,7 +1623,7 @@
         <v>59</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="15"/>
@@ -1633,7 +1636,7 @@
         <v>59</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="15"/>
@@ -1646,7 +1649,7 @@
         <v>59</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="15"/>
@@ -1659,7 +1662,7 @@
         <v>59</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="15"/>
@@ -1672,7 +1675,7 @@
         <v>59</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="15"/>
@@ -1685,7 +1688,7 @@
         <v>59</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>36</v>
+        <v>62</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="15"/>
@@ -1698,7 +1701,7 @@
         <v>59</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C56" s="14"/>
       <c r="D56" s="15"/>
@@ -1711,7 +1714,7 @@
         <v>59</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="15"/>
@@ -1724,7 +1727,7 @@
         <v>59</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="15"/>
@@ -1737,13 +1740,11 @@
         <v>59</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="C59" s="14" t="s">
-        <v>81</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C59" s="14"/>
       <c r="D59" s="15"/>
-      <c r="E59" s="15" t="s">
+      <c r="E59" s="14" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1752,10 +1753,10 @@
         <v>59</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>49</v>
+        <v>81</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15" t="s">
@@ -1767,12 +1768,12 @@
         <v>59</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D61" s="14"/>
+        <v>49</v>
+      </c>
+      <c r="D61" s="15"/>
       <c r="E61" s="15" t="s">
         <v>65</v>
       </c>
@@ -1782,18 +1783,22 @@
         <v>59</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="C62" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="C62" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="D62" s="14"/>
-      <c r="E62" s="15"/>
+      <c r="E62" s="15" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
@@ -1804,71 +1809,82 @@
         <v>59</v>
       </c>
       <c r="B64" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="15"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C64" s="14" t="s">
+      <c r="C65" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D64" s="14" t="s">
+      <c r="D65" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="E64" s="15" t="s">
+      <c r="E65" s="15" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B68" s="19" t="s">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B69" s="19" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B69" s="19" t="s">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B70" s="19" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B70" s="19" t="s">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71" s="19" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B71" s="19" t="s">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72" s="19" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B72" s="19" t="s">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73" s="19" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B73" s="19" t="s">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B74" s="19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B74" s="19" t="s">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B75" s="19" t="s">
         <v>104</v>
       </c>
     </row>

</xml_diff>

<commit_message>
changes to wxSimpleCurl API, improvements throughout. works with OpenEI API
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="106">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -271,9 +271,6 @@
   </si>
   <si>
     <t>Excel exchange for base case</t>
-  </si>
-  <si>
-    <t>Testing</t>
   </si>
   <si>
     <t>General usability, including saving views in outputs, graphs</t>
@@ -794,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,7 +827,7 @@
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>79</v>
@@ -957,10 +954,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>85</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>86</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>52</v>
@@ -974,7 +971,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>30</v>
@@ -1059,13 +1056,13 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="10"/>
@@ -1247,7 +1244,7 @@
         <v>67</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1286,7 +1283,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>18</v>
@@ -1408,7 +1405,7 @@
         <v>59</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>47</v>
@@ -1472,13 +1469,13 @@
         <v>58</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C39" s="12" t="s">
         <v>47</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>67</v>
@@ -1489,7 +1486,7 @@
         <v>59</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
@@ -1500,7 +1497,7 @@
         <v>59</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
@@ -1511,7 +1508,7 @@
         <v>59</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>47</v>
@@ -1783,7 +1780,7 @@
         <v>59</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>47</v>
@@ -1798,7 +1795,7 @@
         <v>59</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
@@ -1809,7 +1806,7 @@
         <v>59</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
@@ -1820,16 +1817,16 @@
         <v>59</v>
       </c>
       <c r="B65" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C65" s="14" t="s">
         <v>90</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>91</v>
-      </c>
       <c r="D65" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1837,7 +1834,7 @@
         <v>59</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1845,7 +1842,7 @@
         <v>59</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -1853,7 +1850,7 @@
         <v>59</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -1861,7 +1858,7 @@
         <v>59</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1869,7 +1866,7 @@
         <v>59</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1877,7 +1874,7 @@
         <v>59</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1885,7 +1882,7 @@
         <v>59</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bug fixes to 3D shading integration for photovoltaics with multiple sub arrays.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -78,9 +78,6 @@
     <t>P50/P90 UI</t>
   </si>
   <si>
-    <t>Sensitivity (tornado) UI</t>
-  </si>
-  <si>
     <t>Parallelized simulation engine</t>
   </si>
   <si>
@@ -334,6 +331,9 @@
   </si>
   <si>
     <t>Check SunEye Obstructions and both Solar Pathfinder file imports</t>
+  </si>
+  <si>
+    <t>Macro system UI</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,70 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -792,7 +855,7 @@
   <dimension ref="A1:I75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,686 +870,686 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>79</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>80</v>
       </c>
       <c r="D2" s="8">
         <v>3</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D3" s="11">
         <v>2</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3">
         <f>SUM(D2:D16)</f>
         <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D4" s="11">
         <v>8</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="11">
         <v>3</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D6" s="11">
         <v>4</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" s="11">
         <v>4</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D8" s="11">
         <v>0.5</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D9" s="11">
         <v>5</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D10" s="11">
         <v>5</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="11">
         <v>3</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D12" s="11">
         <v>0</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D13" s="11">
         <v>0.5</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D14" s="11">
         <v>1</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D16" s="11">
         <v>0</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>1</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="13">
         <v>8</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17">
         <f>SUM(D17:D43)</f>
         <v>77</v>
       </c>
       <c r="I17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D18" s="13">
         <v>4</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>3</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="13">
         <v>4</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B20" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="13">
         <v>2</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B21" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="13">
         <v>2</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="13">
         <v>3</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B23" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D23" s="13">
         <v>2</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="13">
         <v>1.5</v>
       </c>
       <c r="E24" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>12</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D25" s="13">
         <v>5</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F25" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D26" s="13">
         <v>5</v>
       </c>
       <c r="E26" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="12" t="s">
         <v>15</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" s="13">
         <v>2</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B28" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D28" s="13">
         <v>3</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B29" s="12" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="13">
         <v>1</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="13">
         <v>2</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D31" s="13">
         <v>1</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D32" s="13">
         <v>10</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" s="13">
         <v>3</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D34" s="13">
         <v>1</v>
       </c>
       <c r="E34" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D35" s="13"/>
       <c r="E35" s="12"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D36" s="13">
         <v>10</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D37" s="13">
         <v>5</v>
       </c>
       <c r="E37" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D38" s="13">
         <v>0.5</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D39" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="C39" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>93</v>
-      </c>
       <c r="E39" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C40" s="12"/>
       <c r="D40" s="13"/>
@@ -1494,10 +1557,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="12" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
@@ -1505,67 +1568,67 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B42" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D42" s="13"/>
       <c r="E42" s="12"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D43" s="13">
         <v>2</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>7</v>
@@ -1573,12 +1636,12 @@
       <c r="C46" s="14"/>
       <c r="D46" s="15"/>
       <c r="E46" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>16</v>
@@ -1586,216 +1649,216 @@
       <c r="C47" s="14"/>
       <c r="D47" s="15"/>
       <c r="E47" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="15"/>
       <c r="E48" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="15"/>
       <c r="E49" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="15"/>
       <c r="E50" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="15"/>
       <c r="E51" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C52" s="14"/>
       <c r="D52" s="15"/>
       <c r="E52" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="15"/>
       <c r="E53" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="15"/>
       <c r="E54" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="15"/>
       <c r="E55" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C56" s="14"/>
       <c r="D56" s="15"/>
       <c r="E56" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="15"/>
       <c r="E57" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="15"/>
       <c r="E58" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="15"/>
       <c r="E59" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D60" s="15"/>
       <c r="E60" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D61" s="15"/>
       <c r="E61" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
@@ -1803,10 +1866,10 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C64" s="14"/>
       <c r="D64" s="14"/>
@@ -1814,75 +1877,75 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B65" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C65" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="C65" s="14" t="s">
-        <v>90</v>
-      </c>
       <c r="D65" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E65" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DView tabs now save and restore view between simulations, eg for time series, monthly profiles, dmap, etc...
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Aron\Documents\Projects\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="10035"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -473,28 +478,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -572,7 +556,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -607,7 +591,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -819,7 +803,7 @@
   <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,12 +1503,14 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B41" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="D41" s="13"/>
       <c r="E41" s="12"/>
     </row>
@@ -1962,13 +1948,13 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="2" operator="beginsWith" text="Done">
+    <cfRule type="beginsWith" dxfId="1" priority="2" operator="beginsWith" text="Done">
       <formula>LEFT(A1,LEN("Done"))="Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
mark dish-Stirling as 'done' - some testing still needed.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -802,8 +802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1574,7 +1574,7 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
Update TODO list and update defaults.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="10035"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="111">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -482,14 +487,24 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="43">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
+  <dxfs count="28">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -509,6 +524,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFCAF14"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -519,6 +554,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCAF14"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -529,6 +584,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFCAF14"/>
         </patternFill>
       </fill>
@@ -539,6 +614,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="1"/>
         </patternFill>
       </fill>
@@ -549,6 +644,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFCAF14"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
@@ -559,6 +674,26 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCAF14"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
@@ -569,11 +704,44 @@
       </font>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
           <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCAF14"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -581,62 +749,6 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -647,170 +759,12 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCAF14"/>
         </patternFill>
       </fill>
     </dxf>
@@ -875,7 +829,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -910,7 +864,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1121,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I77"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,8 +1385,8 @@
         <v>66</v>
       </c>
       <c r="H17">
-        <f>SUM(D17:D44)</f>
-        <v>77</v>
+        <f>SUM(D17:D39)</f>
+        <v>57</v>
       </c>
       <c r="I17" t="s">
         <v>75</v>
@@ -1440,16 +1394,16 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="13">
         <v>2</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" s="13">
-        <v>4</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>66</v>
@@ -1460,13 +1414,13 @@
         <v>58</v>
       </c>
       <c r="B19" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="13">
         <v>3</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" s="13">
-        <v>4</v>
       </c>
       <c r="E19" s="12" t="s">
         <v>66</v>
@@ -1477,10 +1431,10 @@
         <v>58</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D20" s="13">
         <v>2</v>
@@ -1494,13 +1448,13 @@
         <v>57</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>6</v>
+        <v>81</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="D21" s="13">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>66</v>
@@ -1508,33 +1462,36 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B22" s="12" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="D22" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>66</v>
       </c>
+      <c r="F22" s="18" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D23" s="13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E23" s="12" t="s">
         <v>66</v>
@@ -1542,16 +1499,16 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="B24" s="12" t="s">
-        <v>81</v>
+        <v>15</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="D24" s="13">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>66</v>
@@ -1562,33 +1519,30 @@
         <v>57</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D25" s="13">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E25" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="F25" s="18" t="s">
-        <v>87</v>
-      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D26" s="13">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>66</v>
@@ -1596,13 +1550,13 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="B27" s="12" t="s">
-        <v>15</v>
+        <v>53</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="D27" s="13">
         <v>2</v>
@@ -1616,13 +1570,13 @@
         <v>57</v>
       </c>
       <c r="B28" s="12" t="s">
-        <v>18</v>
+        <v>101</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D28" s="13">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>66</v>
@@ -1630,16 +1584,16 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D29" s="13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>66</v>
@@ -1650,13 +1604,13 @@
         <v>57</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="D30" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>66</v>
@@ -1667,7 +1621,7 @@
         <v>57</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>46</v>
@@ -1681,33 +1635,29 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="D32" s="13">
-        <v>10</v>
-      </c>
-      <c r="E32" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D32" s="13"/>
+      <c r="E32" s="12"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="17" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="D33" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>66</v>
@@ -1718,13 +1668,13 @@
         <v>57</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D34" s="13">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="E34" s="12" t="s">
         <v>66</v>
@@ -1732,159 +1682,157 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="C35" s="12" t="s">
         <v>46</v>
       </c>
       <c r="D35" s="13"/>
-      <c r="E35" s="12"/>
+      <c r="E35" s="12" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
         <v>58</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C36" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="13">
-        <v>10</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="12"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="17" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="B37" s="12" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="13">
-        <v>5</v>
-      </c>
-      <c r="E37" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="D37" s="13"/>
+      <c r="E37" s="12"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>32</v>
+        <v>100</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D38" s="13">
-        <v>0.5</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>66</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D38" s="13"/>
+      <c r="E38" s="12"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>88</v>
+        <v>39</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="13"/>
+        <v>47</v>
+      </c>
+      <c r="D39" s="13">
+        <v>2</v>
+      </c>
       <c r="E39" s="12" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B40" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="12"/>
+        <v>57</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D40" s="15"/>
+      <c r="E40" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="12" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="13"/>
-      <c r="E41" s="12"/>
+      <c r="B41" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D41" s="15"/>
+      <c r="E41" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C42" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="13"/>
-      <c r="E42" s="12"/>
+      <c r="B42" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D42" s="15"/>
+      <c r="E42" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" s="12" t="s">
+      <c r="B43" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="13"/>
-      <c r="E43" s="12"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B44" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C44" s="12" t="s">
+      <c r="B44" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C44" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D44" s="13">
-        <v>2</v>
-      </c>
-      <c r="E44" s="12" t="s">
-        <v>66</v>
+      <c r="D44" s="15"/>
+      <c r="E44" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="14" t="s">
@@ -1896,10 +1844,10 @@
         <v>57</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="14" t="s">
@@ -1908,13 +1856,13 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="D47" s="15"/>
       <c r="E47" s="14" t="s">
@@ -1923,14 +1871,12 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="14" t="s">
-        <v>46</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C48" s="14"/>
       <c r="D48" s="15"/>
       <c r="E48" s="14" t="s">
         <v>64</v>
@@ -1938,14 +1884,12 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>47</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C49" s="14"/>
       <c r="D49" s="15"/>
       <c r="E49" s="14" t="s">
         <v>64</v>
@@ -1956,11 +1900,9 @@
         <v>58</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="C50" s="14" t="s">
-        <v>48</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C50" s="14"/>
       <c r="D50" s="15"/>
       <c r="E50" s="14" t="s">
         <v>64</v>
@@ -1968,14 +1910,12 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C51" s="14" t="s">
-        <v>47</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C51" s="14"/>
       <c r="D51" s="15"/>
       <c r="E51" s="14" t="s">
         <v>64</v>
@@ -1983,10 +1923,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C52" s="14" t="s">
         <v>47</v>
@@ -2001,7 +1941,7 @@
         <v>58</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="15"/>
@@ -2014,7 +1954,7 @@
         <v>58</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="15"/>
@@ -2024,10 +1964,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="15"/>
@@ -2040,39 +1980,43 @@
         <v>58</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C56" s="14"/>
+        <v>79</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>78</v>
+      </c>
       <c r="D56" s="15"/>
-      <c r="E56" s="14" t="s">
+      <c r="E56" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D57" s="15"/>
-      <c r="E57" s="14" t="s">
+      <c r="E57" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C58" s="14"/>
-      <c r="D58" s="15"/>
-      <c r="E58" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C58" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="14"/>
+      <c r="E58" s="15" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2081,55 +2025,55 @@
         <v>58</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C59" s="14"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="D59" s="14"/>
+      <c r="E59" s="15"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="C60" s="14"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="D60" s="14"/>
+      <c r="E60" s="15"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>79</v>
+        <v>102</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D61" s="15"/>
+        <v>86</v>
+      </c>
+      <c r="D61" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="E61" s="15" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>80</v>
+        <v>103</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D62" s="15"/>
+        <v>86</v>
+      </c>
+      <c r="D62" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="E62" s="15" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2137,14 +2081,16 @@
         <v>57</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D63" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="D63" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="E63" s="15" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2152,38 +2098,50 @@
         <v>58</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C64" s="14"/>
-      <c r="D64" s="14"/>
-      <c r="E64" s="15"/>
+        <v>2</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D64" s="14">
+        <v>4</v>
+      </c>
+      <c r="E64" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>58</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="C65" s="14"/>
-      <c r="D65" s="14"/>
-      <c r="E65" s="15"/>
+        <v>3</v>
+      </c>
+      <c r="C65" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D65" s="14">
+        <v>4</v>
+      </c>
+      <c r="E65" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>102</v>
+        <v>4</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D66" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E66" s="15" t="s">
-        <v>86</v>
+        <v>72</v>
+      </c>
+      <c r="D66" s="14">
+        <v>2</v>
+      </c>
+      <c r="E66" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2191,33 +2149,31 @@
         <v>58</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D67" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E67" s="15" t="s">
-        <v>86</v>
+        <v>46</v>
+      </c>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E68" s="15" t="s">
-        <v>86</v>
+        <v>49</v>
+      </c>
+      <c r="D68" s="14">
+        <v>10</v>
+      </c>
+      <c r="E68" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2291,18 +2247,60 @@
   <sortState ref="A2:G52">
     <sortCondition ref="E2:E52"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="Done">
+  <conditionalFormatting sqref="A69:A1048576 A1:A63">
+    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A64:A66">
+    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
+    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
+    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A64)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A64)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A67">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",A67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A67)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A67)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A68">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",A68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A68)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A68)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated TODO list. added scripting reference manual to the help window, and included the latest version of the manual
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="112">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Weather file settings dialog to set search path and download folder, rescan library, updates to UI</t>
   </si>
 </sst>
 </file>
@@ -482,7 +485,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="20">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFCAF14"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -948,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I77"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1628,23 +1671,21 @@
       <c r="A40" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D40" s="15"/>
-      <c r="E40" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="B40" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" s="13"/>
+      <c r="E40" s="12"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>72</v>
@@ -1659,7 +1700,7 @@
         <v>57</v>
       </c>
       <c r="B42" s="14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>72</v>
@@ -1671,13 +1712,13 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="D43" s="15"/>
       <c r="E43" s="14" t="s">
@@ -1686,13 +1727,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D44" s="15"/>
       <c r="E44" s="14" t="s">
@@ -1701,13 +1742,13 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>54</v>
+        <v>20</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D45" s="15"/>
       <c r="E45" s="14" t="s">
@@ -1716,13 +1757,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D46" s="15"/>
       <c r="E46" s="14" t="s">
@@ -1731,10 +1772,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C47" s="14" t="s">
         <v>47</v>
@@ -1746,12 +1787,14 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="17" t="s">
-        <v>107</v>
+        <v>58</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="C48" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="D48" s="15"/>
       <c r="E48" s="14" t="s">
         <v>64</v>
@@ -1759,10 +1802,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="15"/>
@@ -1775,7 +1818,7 @@
         <v>58</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>60</v>
+        <v>34</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="15"/>
@@ -1788,7 +1831,7 @@
         <v>58</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C51" s="14"/>
       <c r="D51" s="15"/>
@@ -1798,14 +1841,12 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C52" s="14" t="s">
-        <v>47</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C52" s="14"/>
       <c r="D52" s="15"/>
       <c r="E52" s="14" t="s">
         <v>64</v>
@@ -1813,12 +1854,14 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C53" s="14"/>
+        <v>35</v>
+      </c>
+      <c r="C53" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="D53" s="15"/>
       <c r="E53" s="14" t="s">
         <v>64</v>
@@ -1829,7 +1872,7 @@
         <v>58</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="15"/>
@@ -1839,10 +1882,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="15"/>
@@ -1852,16 +1895,14 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>78</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C56" s="14"/>
       <c r="D56" s="15"/>
-      <c r="E56" s="15" t="s">
+      <c r="E56" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1870,10 +1911,10 @@
         <v>58</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>48</v>
+        <v>78</v>
       </c>
       <c r="D57" s="15"/>
       <c r="E57" s="15" t="s">
@@ -1882,36 +1923,40 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D58" s="14"/>
+        <v>48</v>
+      </c>
+      <c r="D58" s="15"/>
       <c r="E58" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="C59" s="14"/>
+        <v>83</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="D59" s="14"/>
-      <c r="E59" s="15"/>
+      <c r="E59" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>58</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14"/>
@@ -1919,27 +1964,21 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="C61" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D61" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E61" s="15" t="s">
-        <v>86</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="15"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>86</v>
@@ -1953,13 +1992,13 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C63" s="14" t="s">
-        <v>47</v>
+        <v>86</v>
       </c>
       <c r="D63" s="14" t="s">
         <v>86</v>
@@ -1970,19 +2009,19 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D64" s="14">
-        <v>4</v>
-      </c>
-      <c r="E64" s="14" t="s">
-        <v>64</v>
+        <v>47</v>
+      </c>
+      <c r="D64" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1990,10 +2029,10 @@
         <v>58</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="D65" s="14">
         <v>4</v>
@@ -2007,13 +2046,13 @@
         <v>58</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C66" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D66" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E66" s="14" t="s">
         <v>64</v>
@@ -2021,42 +2060,51 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D67" s="14"/>
+        <v>72</v>
+      </c>
+      <c r="D67" s="14">
+        <v>2</v>
+      </c>
       <c r="E67" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B68" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B69" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C68" s="14" t="s">
+      <c r="C69" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="D68" s="14">
+      <c r="D69" s="14">
         <v>10</v>
       </c>
-      <c r="E68" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A70" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B70" s="19" t="s">
-        <v>93</v>
+      <c r="E69" s="14" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2064,7 +2112,7 @@
         <v>58</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
@@ -2072,7 +2120,7 @@
         <v>58</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -2080,7 +2128,7 @@
         <v>58</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2088,7 +2136,7 @@
         <v>58</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2096,7 +2144,7 @@
         <v>58</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2104,7 +2152,7 @@
         <v>58</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2112,9 +2160,17 @@
         <v>58</v>
       </c>
       <c r="B77" s="19" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B78" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C78" t="s">
         <v>109</v>
       </c>
     </row>
@@ -2122,60 +2178,60 @@
   <sortState ref="A2:G52">
     <sortCondition ref="E2:E52"/>
   </sortState>
-  <conditionalFormatting sqref="A69:A1048576 A1:A63">
-    <cfRule type="containsText" dxfId="15" priority="13" operator="containsText" text="Testing">
+  <conditionalFormatting sqref="A70:A1048576 A1:A64">
+    <cfRule type="containsText" dxfId="19" priority="13" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="14" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="18" priority="14" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="15" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="17" priority="15" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A64:A66">
-    <cfRule type="containsText" dxfId="11" priority="9" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",A64)))</formula>
+  <conditionalFormatting sqref="A65:A67">
+    <cfRule type="containsText" dxfId="15" priority="9" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",A65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="10" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A64)))</formula>
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="11" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A64)))</formula>
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A65)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="12" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A64)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A67">
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Testing">
-      <formula>NOT(ISERROR(SEARCH("Testing",A67)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A67)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A67)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A67)))</formula>
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A68">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",A68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A68)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A68)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A69">
+    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",A69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A69)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A69)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated SAM to do from last meeting - needs some sprucing up
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="10035"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="15600" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="142">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -370,6 +370,78 @@
   </si>
   <si>
     <t>Fix output variable group names in SSC: Flat Plate, PVWatts, Wind, CSP Trough &amp; Towers, Res, Comm</t>
+  </si>
+  <si>
+    <t>Janine has to fix what Aron broke in the Macros</t>
+  </si>
+  <si>
+    <t>Janine can sort TODO list</t>
+  </si>
+  <si>
+    <t>Tower fixes  - Steve &amp; Mike</t>
+  </si>
+  <si>
+    <t>Molten salt linear fresnel</t>
+  </si>
+  <si>
+    <t>Reorganize dispatch widget to UI</t>
+  </si>
+  <si>
+    <t>Sample files - esp Novatec - Mike</t>
+  </si>
+  <si>
+    <t>Wind - cost and scaling model - Janine</t>
+  </si>
+  <si>
+    <t>Check the reports</t>
+  </si>
+  <si>
+    <t>Check the macros</t>
+  </si>
+  <si>
+    <t>Documentation updates from Paul</t>
+  </si>
+  <si>
+    <t>Progress updates for solarpilot - Aron</t>
+  </si>
+  <si>
+    <t>Steve/Mike</t>
+  </si>
+  <si>
+    <t>Ty/Steve</t>
+  </si>
+  <si>
+    <t>Mike</t>
+  </si>
+  <si>
+    <t>Steam tower</t>
+  </si>
+  <si>
+    <t>Cavity receiver</t>
+  </si>
+  <si>
+    <t>Ty/Mike/Steve</t>
+  </si>
+  <si>
+    <t>Review default values, financial, cost #s for PV res/com/util</t>
+  </si>
+  <si>
+    <t>Subhourly simulation for physical trough</t>
+  </si>
+  <si>
+    <t>Aron/Mike</t>
+  </si>
+  <si>
+    <t>Check all results, and summarize for release notes</t>
+  </si>
+  <si>
+    <t>Add performance adjustment factors to wind model</t>
+  </si>
+  <si>
+    <t>Curtailment month by hour factors in popup widget thingy</t>
+  </si>
+  <si>
+    <t>Possible registration issues</t>
   </si>
 </sst>
 </file>
@@ -859,10 +931,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="C103" sqref="C103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1603,7 +1675,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B44" s="14" t="s">
         <v>54</v>
@@ -1648,7 +1720,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B47" s="14" t="s">
         <v>34</v>
@@ -1674,7 +1746,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>61</v>
@@ -1730,7 +1802,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>80</v>
@@ -1773,7 +1845,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B56" s="14" t="s">
         <v>85</v>
@@ -1854,7 +1926,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B61" s="14" t="s">
         <v>3</v>
@@ -1903,7 +1975,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B64" s="14" t="s">
         <v>26</v>
@@ -2138,6 +2210,158 @@
         <v>10</v>
       </c>
       <c r="E83" s="19"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="C84" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B86" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="C86" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B87" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="C87" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B88" s="19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C88" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B89" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="C89" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B90" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C90" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B91" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="C91" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B92" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="C92" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B93" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="C93" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B94" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="C94" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B95" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="C95" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B96" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="C96" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B97" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="C97" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B98" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="C98" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B99" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="C99" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B100" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="C100" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B101" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C101" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B102" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C102" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B103" s="19" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:G52">

</xml_diff>

<commit_message>
Direct Steam power tower updates for latest solar pilot integration - not running yet
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="15600" windowHeight="10035"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="145">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -448,6 +453,9 @@
   </si>
   <si>
     <t>Check all default values</t>
+  </si>
+  <si>
+    <t>Fix issue with InnoSetup uninstall win32 and x64 - windows 7 and window 8</t>
   </si>
 </sst>
 </file>
@@ -581,7 +589,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="11">
     <dxf>
       <font>
         <color theme="0"/>
@@ -639,66 +647,6 @@
       <fill>
         <patternFill>
           <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF33CC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -814,7 +762,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -849,7 +797,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1058,10 +1006,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2595,6 +2543,14 @@
         <v>10</v>
       </c>
       <c r="E103" s="19"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B105" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C105" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:G52">

</xml_diff>

<commit_message>
add project ideas and registration codes to todo list spreadsheet
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,27 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="15600" windowHeight="10035"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="To Do" sheetId="1" r:id="rId1"/>
+    <sheet name="Project Ideas" sheetId="2" r:id="rId2"/>
+    <sheet name="Registration Codes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="157">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -456,13 +451,49 @@
   </si>
   <si>
     <t>Fix issue with InnoSetup uninstall win32 and x64 - windows 7 and window 8</t>
+  </si>
+  <si>
+    <t>Customizable reports</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>CB18B612-F85E-47C9-AB54-AFBCD468BB4B</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>2014.9.30</t>
+  </si>
+  <si>
+    <t>Christina Schall</t>
+  </si>
+  <si>
+    <t>christina.schall@schottsolar.com</t>
+  </si>
+  <si>
+    <t>Germany</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -496,6 +527,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -557,10 +596,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -585,8 +625,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
@@ -762,7 +805,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,7 +840,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1008,7 +1051,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A105" sqref="A105"/>
     </sheetView>
   </sheetViews>
@@ -2607,19 +2650,83 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="45.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="45" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="17.7109375" customWidth="1"/>
+    <col min="5" max="5" width="43.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="20">
+        <v>41921</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>155</v>
+      </c>
+      <c r="F2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update to do and beta feedback spreadsheets
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="175">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1106,8 +1106,8 @@
   <dimension ref="A1:I120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2643,19 +2643,24 @@
       <c r="E103" s="19"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A105" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="B105" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C105" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="F105" t="s">
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+      <c r="F105" s="19" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B106" s="19" t="s">
         <v>156</v>
@@ -2663,7 +2668,9 @@
       <c r="C106" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F106" t="s">
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+      <c r="F106" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2677,7 +2684,9 @@
       <c r="C107" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F107" t="s">
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+      <c r="F107" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2691,7 +2700,9 @@
       <c r="C108" s="19" t="s">
         <v>159</v>
       </c>
-      <c r="F108" t="s">
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
+      <c r="F108" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2705,7 +2716,9 @@
       <c r="C109" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F109" t="s">
+      <c r="D109" s="19"/>
+      <c r="E109" s="19"/>
+      <c r="F109" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2719,6 +2732,9 @@
       <c r="C110" s="19" t="s">
         <v>47</v>
       </c>
+      <c r="D110" s="19"/>
+      <c r="E110" s="19"/>
+      <c r="F110" s="19"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="17" t="s">
@@ -2730,6 +2746,9 @@
       <c r="C111" s="19" t="s">
         <v>47</v>
       </c>
+      <c r="D111" s="19"/>
+      <c r="E111" s="19"/>
+      <c r="F111" s="19"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="17" t="s">
@@ -2741,7 +2760,9 @@
       <c r="C112" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F112" t="s">
+      <c r="D112" s="19"/>
+      <c r="E112" s="19"/>
+      <c r="F112" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2755,7 +2776,9 @@
       <c r="C113" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F113" t="s">
+      <c r="D113" s="19"/>
+      <c r="E113" s="19"/>
+      <c r="F113" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2766,23 +2789,38 @@
       <c r="B114" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="F114" t="s">
+      <c r="C114" s="19"/>
+      <c r="D114" s="19"/>
+      <c r="E114" s="19"/>
+      <c r="F114" s="19" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A115" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="B115" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="F115" t="s">
+      <c r="C115" s="19"/>
+      <c r="D115" s="19"/>
+      <c r="E115" s="19"/>
+      <c r="F115" s="19" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A116" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="B116" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="F116" t="s">
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2793,10 +2831,12 @@
       <c r="B117" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="C117" t="s">
+      <c r="C117" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="F117" t="s">
+      <c r="D117" s="19"/>
+      <c r="E117" s="19"/>
+      <c r="F117" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2807,10 +2847,12 @@
       <c r="B118" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="C118" t="s">
+      <c r="C118" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F118" t="s">
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
+      <c r="F118" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2821,10 +2863,12 @@
       <c r="B119" s="19" t="s">
         <v>169</v>
       </c>
-      <c r="C119" t="s">
+      <c r="C119" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F119" t="s">
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
+      <c r="F119" s="19" t="s">
         <v>162</v>
       </c>
     </row>
@@ -2835,10 +2879,12 @@
       <c r="B120" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="C120" t="s">
+      <c r="C120" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="F120" t="s">
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update todo and beta feedback spreadsheets
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="179">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -541,6 +541,18 @@
   </si>
   <si>
     <t>Wind - cost and scaling model</t>
+  </si>
+  <si>
+    <t>direct steam tower: receiver height calculated value is zero</t>
+  </si>
+  <si>
+    <t>biopower: feedstock download buttons do not work</t>
+  </si>
+  <si>
+    <t>H_rec and rec_height variables in UI, H_rec in ssc</t>
+  </si>
+  <si>
+    <t>geothermal: Lookup temp and depth button does not work</t>
   </si>
 </sst>
 </file>
@@ -1103,11 +1115,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I120"/>
+  <dimension ref="A1:I125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121"/>
+      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2887,6 +2899,27 @@
       <c r="F120" s="19" t="s">
         <v>171</v>
       </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B122" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="F122" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B123" s="19" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B124" s="19" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B125" s="19"/>
     </row>
   </sheetData>
   <sortState ref="A2:G52">

</xml_diff>

<commit_message>
added idea for stepped trackers
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="12990"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="181">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -556,6 +556,9 @@
   </si>
   <si>
     <t>Average multiple images when importing Solar Pathfinder files</t>
+  </si>
+  <si>
+    <t>Trackers for PV should step at discrete angle increments rather than continuously.  Not a big issue for 1 hour TS, but at 1 min TS might be a bigger issue</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1123,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A103" sqref="A103"/>
     </sheetView>
@@ -2987,9 +2990,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2999,6 +3004,11 @@
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more future improvement ideas
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="185">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -559,6 +559,18 @@
   </si>
   <si>
     <t>Trackers for PV should step at discrete angle increments rather than continuously.  Not a big issue for 1 hour TS, but at 1 min TS might be a bigger issue</t>
+  </si>
+  <si>
+    <t>Searchable help system table of contents</t>
+  </si>
+  <si>
+    <t>Plots for stochastic and p50/p90 simulation outputs</t>
+  </si>
+  <si>
+    <t>"pinnable" results widgets on summary page - customization of summary page, perhaps with a script widget too</t>
+  </si>
+  <si>
+    <t>step-by-step interactive debugger for LK language integrated in SAM</t>
   </si>
 </sst>
 </file>
@@ -2990,10 +3002,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3009,6 +3021,26 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add idea for future
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="186">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>step-by-step interactive debugger for LK language integrated in SAM</t>
+  </si>
+  <si>
+    <t>import case from another .sam file</t>
   </si>
 </sst>
 </file>
@@ -3002,10 +3005,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3041,6 +3044,11 @@
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add export sam to sdk to future items in ToDo list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="187">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -574,6 +574,9 @@
   </si>
   <si>
     <t>import case from another .sam file</t>
+  </si>
+  <si>
+    <t>Tool to export .sam inputs to SDK</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1142,8 @@
   <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A103" sqref="A103"/>
+      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B108" sqref="B108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3005,10 +3008,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3049,6 +3052,11 @@
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some more future ideas.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="189">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -577,6 +577,12 @@
   </si>
   <si>
     <t>Tool to export .sam inputs to SDK</t>
+  </si>
+  <si>
+    <t>Support for multiple inverter types</t>
+  </si>
+  <si>
+    <t>Multiple MPPT inputs to an inverter</t>
   </si>
 </sst>
 </file>
@@ -3008,10 +3014,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,6 +3063,16 @@
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
other: TODO list update from 10/23/14 meeting
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
     <sheet name="Project Ideas" sheetId="2" r:id="rId2"/>
     <sheet name="Registration Codes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="191">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -583,6 +588,12 @@
   </si>
   <si>
     <t>Multiple MPPT inputs to an inverter</t>
+  </si>
+  <si>
+    <t>ITC over multiple years</t>
+  </si>
+  <si>
+    <t>POUT</t>
   </si>
 </sst>
 </file>
@@ -901,7 +912,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -936,7 +947,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1147,9 +1158,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I126"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A93" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B108" sqref="B108"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1770,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B36" s="14" t="s">
         <v>1</v>
@@ -1798,7 +1809,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>21</v>
@@ -1815,7 +1826,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="14" t="s">
         <v>9</v>
@@ -1905,7 +1916,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="B45" s="14" t="s">
         <v>28</v>
@@ -1920,7 +1931,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="B46" s="14" t="s">
         <v>60</v>
@@ -1961,7 +1972,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B49" s="14" t="s">
         <v>79</v>
@@ -2011,7 +2022,9 @@
       <c r="B52" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="C52" s="14"/>
+      <c r="C52" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="D52" s="14"/>
       <c r="E52" s="15" t="s">
         <v>64</v>
@@ -2104,7 +2117,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B58" s="14" t="s">
         <v>4</v>
@@ -2141,7 +2154,9 @@
       <c r="B60" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="14"/>
+      <c r="C60" s="14" t="s">
+        <v>46</v>
+      </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
     </row>
@@ -2173,7 +2188,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B63" s="14" t="s">
         <v>120</v>
@@ -2186,7 +2201,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B64" s="14" t="s">
         <v>131</v>
@@ -2199,7 +2214,7 @@
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B65" s="14" t="s">
         <v>132</v>
@@ -2212,7 +2227,7 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B66" s="14" t="s">
         <v>121</v>
@@ -2225,7 +2240,7 @@
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B67" s="14" t="s">
         <v>122</v>
@@ -2238,7 +2253,7 @@
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B68" s="14" t="s">
         <v>123</v>
@@ -2316,7 +2331,7 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B74" s="14" t="s">
         <v>135</v>
@@ -2779,7 +2794,7 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B111" s="19" t="s">
         <v>172</v>
@@ -2793,7 +2808,7 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B112" s="19" t="s">
         <v>173</v>
@@ -2944,6 +2959,9 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A123" s="17" t="s">
+        <v>57</v>
+      </c>
       <c r="B123" s="19" t="s">
         <v>175</v>
       </c>
@@ -2952,11 +2970,17 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A124" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="B124" s="19" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A125" s="17" t="s">
+        <v>58</v>
+      </c>
       <c r="B125" s="19" t="s">
         <v>178</v>
       </c>
@@ -3014,10 +3038,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3073,6 +3097,11 @@
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>188</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
other: none: updated to-do list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
@@ -16,12 +11,12 @@
     <sheet name="Project Ideas" sheetId="2" r:id="rId2"/>
     <sheet name="Registration Codes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="194">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -594,6 +589,15 @@
   </si>
   <si>
     <t>POUT</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Improve the schedule versus single value button</t>
+  </si>
+  <si>
+    <t>SNL module page: get rid of temp coeffs and make the a, b, dT more useable</t>
   </si>
 </sst>
 </file>
@@ -707,7 +711,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -734,12 +738,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
       <font>
         <color theme="0"/>
@@ -747,6 +752,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF33CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -912,7 +927,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -947,7 +962,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1156,11 +1171,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I126"/>
+  <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A125" sqref="A125"/>
+      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1916,10 +1931,10 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
-        <v>190</v>
+        <v>57</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>47</v>
@@ -1931,10 +1946,10 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>190</v>
+        <v>57</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="15"/>
@@ -1947,13 +1962,13 @@
         <v>57</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="C47" s="14" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D47" s="15"/>
-      <c r="E47" s="14" t="s">
+      <c r="E47" s="15" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1962,25 +1977,27 @@
         <v>57</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="14"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="14"/>
+      <c r="E48" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="17" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C49" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D49" s="15"/>
+        <v>48</v>
+      </c>
+      <c r="D49" s="14"/>
       <c r="E49" s="15" t="s">
         <v>64</v>
       </c>
@@ -1990,12 +2007,14 @@
         <v>57</v>
       </c>
       <c r="B50" s="14" t="s">
-        <v>80</v>
+        <v>102</v>
       </c>
       <c r="C50" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D50" s="15"/>
+        <v>86</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="E50" s="15" t="s">
         <v>64</v>
       </c>
@@ -2005,45 +2024,49 @@
         <v>57</v>
       </c>
       <c r="B51" s="14" t="s">
-        <v>83</v>
+        <v>103</v>
       </c>
       <c r="C51" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D51" s="14"/>
+        <v>86</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="E51" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
       <c r="C52" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="14"/>
+        <v>47</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>86</v>
+      </c>
       <c r="E52" s="15" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>102</v>
+        <v>2</v>
       </c>
       <c r="C53" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D53" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E53" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D53" s="14">
+        <v>4</v>
+      </c>
+      <c r="E53" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2052,15 +2075,15 @@
         <v>57</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>103</v>
+        <v>3</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D54" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E54" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D54" s="14">
+        <v>4</v>
+      </c>
+      <c r="E54" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2069,93 +2092,81 @@
         <v>57</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>105</v>
+        <v>4</v>
       </c>
       <c r="C55" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="E55" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="14">
+        <v>2</v>
+      </c>
+      <c r="E55" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>2</v>
+        <v>104</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D56" s="14">
-        <v>4</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D56" s="14"/>
       <c r="E56" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>3</v>
+        <v>117</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="14">
-        <v>4</v>
-      </c>
-      <c r="E57" s="14" t="s">
-        <v>64</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>4</v>
+        <v>118</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D58" s="14">
-        <v>2</v>
-      </c>
-      <c r="E58" s="14" t="s">
-        <v>64</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>57</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="C59" s="14" t="s">
         <v>46</v>
       </c>
       <c r="D59" s="14"/>
-      <c r="E59" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="E59" s="14"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" s="14" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>46</v>
+        <v>128</v>
       </c>
       <c r="D60" s="14"/>
       <c r="E60" s="14"/>
@@ -2165,10 +2176,10 @@
         <v>57</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C61" s="14" t="s">
-        <v>46</v>
+        <v>129</v>
       </c>
       <c r="D61" s="14"/>
       <c r="E61" s="14"/>
@@ -2178,10 +2189,10 @@
         <v>57</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C62" s="14" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D62" s="14"/>
       <c r="E62" s="14"/>
@@ -2191,687 +2202,712 @@
         <v>57</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="C63" s="14" t="s">
-        <v>128</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="C63" s="14"/>
       <c r="D63" s="14"/>
-      <c r="E63" s="14"/>
+      <c r="E63" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
-        <v>57</v>
+        <v>191</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>131</v>
+        <v>174</v>
       </c>
       <c r="C64" s="14" t="s">
-        <v>129</v>
+        <v>72</v>
       </c>
       <c r="D64" s="14"/>
       <c r="E64" s="14"/>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C65" s="14" t="s">
-        <v>133</v>
+        <v>51</v>
       </c>
       <c r="D65" s="14"/>
       <c r="E65" s="14"/>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C66" s="14" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D66" s="14"/>
       <c r="E66" s="14"/>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D67" s="14"/>
       <c r="E67" s="14"/>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>130</v>
+        <v>73</v>
       </c>
       <c r="D68" s="14"/>
       <c r="E68" s="14"/>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>114</v>
+        <v>140</v>
       </c>
       <c r="C69" s="14"/>
       <c r="D69" s="14"/>
-      <c r="E69" s="14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="14"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B70" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="D70" s="14"/>
-      <c r="E70" s="14"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B70" s="19" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B71" s="14" t="s">
-        <v>134</v>
-      </c>
-      <c r="C71" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D71" s="14"/>
-      <c r="E71" s="14"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="D71" s="19"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B72" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="C72" s="14" t="s">
+      <c r="B72" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="D73" s="19"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A74" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D74" s="19"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A75" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>172</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" s="19"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="19"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>173</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" s="19"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="19"/>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" s="19"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" s="19"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A79" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B79" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C79" s="19"/>
+      <c r="D79" s="19"/>
+      <c r="E79" s="19"/>
+      <c r="F79" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="19"/>
+      <c r="D80" s="19"/>
+      <c r="E80" s="19"/>
+      <c r="F80" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C81" s="19" t="s">
         <v>71</v>
       </c>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A73" s="17" t="s">
+      <c r="D81" s="19"/>
+      <c r="E81" s="19"/>
+      <c r="F81" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" s="19"/>
+      <c r="E82" s="19"/>
+      <c r="F82" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>175</v>
+      </c>
+      <c r="C85" s="19"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="B73" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="C73" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D73" s="14"/>
-      <c r="E73" s="14"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B74" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="C74" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="D74" s="14"/>
-      <c r="E74" s="14"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B75" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D75" s="14"/>
-      <c r="E75" s="14"/>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B76" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="C76" s="14"/>
-      <c r="D76" s="14"/>
-      <c r="E76" s="14"/>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B77" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C77" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="14"/>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B78" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C78" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D78" s="14"/>
-      <c r="E78" s="14"/>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B79" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="C79" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D79" s="14"/>
-      <c r="E79" s="14"/>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B80" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="C80" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D80" s="14"/>
-      <c r="E80" s="14"/>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B81" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C81" s="19"/>
-      <c r="D81" s="19"/>
-      <c r="E81" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B82" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C82" s="19"/>
-      <c r="D82" s="19"/>
-      <c r="E82" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B83" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C83" s="19"/>
-      <c r="D83" s="19"/>
-      <c r="E83" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B84" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D84" s="19"/>
-      <c r="E84" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B85" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C85" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D85" s="19">
-        <v>10</v>
-      </c>
-      <c r="E85" s="19" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="17" t="s">
-        <v>113</v>
-      </c>
       <c r="B86" s="19" t="s">
-        <v>93</v>
+        <v>176</v>
       </c>
       <c r="C86" s="19"/>
       <c r="D86" s="19"/>
       <c r="E86" s="19"/>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F86" s="19"/>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>94</v>
+        <v>178</v>
       </c>
       <c r="C87" s="19"/>
       <c r="D87" s="19"/>
       <c r="E87" s="19"/>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F87" s="19"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B88" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C88" s="19"/>
-      <c r="D88" s="19"/>
-      <c r="E88" s="19"/>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="B88" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="C88" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B89" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="C89" s="19"/>
-      <c r="D89" s="19"/>
-      <c r="E89" s="19"/>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="B89" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="C89" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B90" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="C90" s="19"/>
-      <c r="D90" s="19"/>
-      <c r="E90" s="19"/>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="B90" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C90" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B91" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C91" s="19"/>
-      <c r="D91" s="19"/>
-      <c r="E91" s="19"/>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="B91" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="C91" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B92" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="19"/>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="B92" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" s="15"/>
+      <c r="E92" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B93" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C93" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="D93" s="19"/>
-      <c r="E93" s="19"/>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="B93" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C93" s="14"/>
+      <c r="D93" s="15"/>
+      <c r="E93" s="14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
       <c r="C94" s="19"/>
       <c r="D94" s="19"/>
-      <c r="E94" s="19"/>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E94" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>112</v>
+        <v>61</v>
       </c>
       <c r="C95" s="19"/>
       <c r="D95" s="19"/>
-      <c r="E95" s="19"/>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E95" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C96" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D96" s="19">
-        <v>2</v>
-      </c>
-      <c r="E96" s="19"/>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="C96" s="19"/>
+      <c r="D96" s="19"/>
+      <c r="E96" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C97" s="19"/>
+        <v>54</v>
+      </c>
+      <c r="C97" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="D97" s="19"/>
-      <c r="E97" s="19"/>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E97" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19"/>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C98" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D98" s="19">
+        <v>10</v>
+      </c>
+      <c r="E98" s="19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="C99" s="19"/>
       <c r="D99" s="19"/>
       <c r="E99" s="19"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C100" s="19"/>
       <c r="D100" s="19"/>
       <c r="E100" s="19"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>115</v>
+        <v>95</v>
       </c>
       <c r="C101" s="19"/>
       <c r="D101" s="19"/>
       <c r="E101" s="19"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="C102" s="19" t="s">
-        <v>46</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C102" s="19"/>
       <c r="D102" s="19"/>
       <c r="E102" s="19"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C103" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C103" s="19"/>
       <c r="D103" s="19"/>
       <c r="E103" s="19"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="17" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="C104" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D104" s="19">
-        <v>10</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C104" s="19"/>
+      <c r="D104" s="19"/>
       <c r="E104" s="19"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A105" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B105" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="C105" s="19"/>
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="C106" s="19" t="s">
-        <v>48</v>
+        <v>109</v>
       </c>
       <c r="D106" s="19"/>
       <c r="E106" s="19"/>
-      <c r="F106" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="17" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>156</v>
-      </c>
-      <c r="C107" s="19" t="s">
-        <v>71</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C107" s="19"/>
       <c r="D107" s="19"/>
       <c r="E107" s="19"/>
-      <c r="F107" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="C108" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C108" s="19"/>
       <c r="D108" s="19"/>
       <c r="E108" s="19"/>
-      <c r="F108" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="17" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>158</v>
+        <v>15</v>
       </c>
       <c r="C109" s="19" t="s">
-        <v>159</v>
-      </c>
-      <c r="D109" s="19"/>
+        <v>73</v>
+      </c>
+      <c r="D109" s="19">
+        <v>2</v>
+      </c>
       <c r="E109" s="19"/>
-      <c r="F109" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>160</v>
-      </c>
-      <c r="C110" s="19" t="s">
-        <v>68</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="C110" s="19"/>
       <c r="D110" s="19"/>
       <c r="E110" s="19"/>
-      <c r="F110" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="17" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>172</v>
-      </c>
-      <c r="C111" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="C111" s="19"/>
       <c r="D111" s="19"/>
       <c r="E111" s="19"/>
-      <c r="F111" s="19"/>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="17" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>173</v>
-      </c>
-      <c r="C112" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C112" s="19"/>
       <c r="D112" s="19"/>
       <c r="E112" s="19"/>
-      <c r="F112" s="19"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C113" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C113" s="19"/>
       <c r="D113" s="19"/>
       <c r="E113" s="19"/>
-      <c r="F113" s="19" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" s="17" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="C114" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C114" s="19"/>
       <c r="D114" s="19"/>
       <c r="E114" s="19"/>
-      <c r="F114" s="19" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="C115" s="19"/>
+        <v>179</v>
+      </c>
+      <c r="C115" s="19" t="s">
+        <v>46</v>
+      </c>
       <c r="D115" s="19"/>
       <c r="E115" s="19"/>
-      <c r="F115" s="19" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C116" s="19"/>
       <c r="D116" s="19"/>
@@ -2882,152 +2918,167 @@
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>166</v>
-      </c>
-      <c r="C117" s="19"/>
+        <v>139</v>
+      </c>
+      <c r="C117" s="19" t="s">
+        <v>47</v>
+      </c>
       <c r="D117" s="19"/>
       <c r="E117" s="19"/>
-      <c r="F117" s="19" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B118" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="C118" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D118" s="19"/>
-      <c r="E118" s="19"/>
-      <c r="F118" s="19" t="s">
-        <v>162</v>
+        <v>113</v>
+      </c>
+      <c r="B118" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D118" s="15"/>
+      <c r="E118" s="15" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B119" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="C119" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D119" s="19"/>
-      <c r="E119" s="19"/>
-      <c r="F119" s="19" t="s">
-        <v>162</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B119" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="C119" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D119" s="14"/>
+      <c r="E119" s="14"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B120" s="19" t="s">
-        <v>169</v>
-      </c>
-      <c r="C120" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D120" s="19"/>
-      <c r="E120" s="19"/>
-      <c r="F120" s="19" t="s">
-        <v>162</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B120" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="C120" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D120" s="14"/>
+      <c r="E120" s="14"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B121" s="19" t="s">
-        <v>170</v>
-      </c>
-      <c r="C121" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="D121" s="19"/>
-      <c r="E121" s="19"/>
-      <c r="F121" s="19" t="s">
-        <v>171</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B121" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="C121" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D121" s="14"/>
+      <c r="E121" s="14"/>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A122" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B122" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D122" s="14"/>
+      <c r="E122" s="14"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B123" s="19" t="s">
-        <v>175</v>
-      </c>
-      <c r="F123" s="19" t="s">
-        <v>177</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B123" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C123" s="14"/>
+      <c r="D123" s="14"/>
+      <c r="E123" s="14"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B124" s="19" t="s">
-        <v>176</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B124" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C124" s="14"/>
+      <c r="D124" s="14"/>
+      <c r="E124" s="14"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B125" s="19" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B126" s="19"/>
+        <v>23</v>
+      </c>
+      <c r="C125" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="D125" s="19">
+        <v>10</v>
+      </c>
+      <c r="E125" s="19"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B127" s="22"/>
     </row>
   </sheetData>
   <sortState ref="A2:G52">
     <sortCondition ref="E2:E52"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A60 A69:A79 A81:A1048576">
-    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="NGTD">
+  <conditionalFormatting sqref="A1:A90 A92:A1048576">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="10" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="8" priority="11" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A61:A68 A80">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A61)))</formula>
+  <conditionalFormatting sqref="A91">
+    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A61)))</formula>
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Test">
+      <formula>NOT(ISERROR(SEARCH("Test",A91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A61)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",A91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A61)))</formula>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A91)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A61)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="POUT">
+      <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
update TODO list #other #none
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1174,8 +1174,8 @@
   <dimension ref="A1:I127"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B114" sqref="B114"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B67" s="14" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
none: none: to-do list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="195">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -598,6 +598,9 @@
   </si>
   <si>
     <t>SNL module page: get rid of temp coeffs and make the a, b, dT more useable</t>
+  </si>
+  <si>
+    <t>Vote against that horrible marigold color :)</t>
   </si>
 </sst>
 </file>
@@ -1171,11 +1174,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I127"/>
+  <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A77" sqref="A77"/>
+      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2610,27 +2613,25 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D92" s="15"/>
-      <c r="E92" s="14" t="s">
-        <v>64</v>
-      </c>
+        <v>194</v>
+      </c>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>190</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C93" s="14"/>
+        <v>28</v>
+      </c>
+      <c r="C93" s="14" t="s">
+        <v>47</v>
+      </c>
       <c r="D93" s="15"/>
       <c r="E93" s="14" t="s">
         <v>64</v>
@@ -2638,14 +2639,14 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B94" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C94" s="19"/>
-      <c r="D94" s="19"/>
-      <c r="E94" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B94" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C94" s="14"/>
+      <c r="D94" s="15"/>
+      <c r="E94" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2654,7 +2655,7 @@
         <v>113</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="C95" s="19"/>
       <c r="D95" s="19"/>
@@ -2667,7 +2668,7 @@
         <v>113</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C96" s="19"/>
       <c r="D96" s="19"/>
@@ -2680,11 +2681,9 @@
         <v>113</v>
       </c>
       <c r="B97" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C97" s="19" t="s">
-        <v>48</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C97" s="19"/>
       <c r="D97" s="19"/>
       <c r="E97" s="19" t="s">
         <v>64</v>
@@ -2695,14 +2694,12 @@
         <v>113</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C98" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D98" s="19">
-        <v>10</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="D98" s="19"/>
       <c r="E98" s="19" t="s">
         <v>64</v>
       </c>
@@ -2712,18 +2709,24 @@
         <v>113</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C99" s="19"/>
-      <c r="D99" s="19"/>
-      <c r="E99" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="C99" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D99" s="19">
+        <v>10</v>
+      </c>
+      <c r="E99" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C100" s="19"/>
       <c r="D100" s="19"/>
@@ -2734,7 +2737,7 @@
         <v>113</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C101" s="19"/>
       <c r="D101" s="19"/>
@@ -2745,7 +2748,7 @@
         <v>113</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C102" s="19"/>
       <c r="D102" s="19"/>
@@ -2756,7 +2759,7 @@
         <v>113</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C103" s="19"/>
       <c r="D103" s="19"/>
@@ -2767,7 +2770,7 @@
         <v>113</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C104" s="19"/>
       <c r="D104" s="19"/>
@@ -2778,7 +2781,7 @@
         <v>113</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C105" s="19"/>
       <c r="D105" s="19"/>
@@ -2789,11 +2792,9 @@
         <v>113</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C106" s="19" t="s">
-        <v>109</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C106" s="19"/>
       <c r="D106" s="19"/>
       <c r="E106" s="19"/>
     </row>
@@ -2802,9 +2803,11 @@
         <v>113</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="C107" s="19"/>
+        <v>108</v>
+      </c>
+      <c r="C107" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="D107" s="19"/>
       <c r="E107" s="19"/>
     </row>
@@ -2813,7 +2816,7 @@
         <v>113</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C108" s="19"/>
       <c r="D108" s="19"/>
@@ -2824,14 +2827,10 @@
         <v>113</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C109" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D109" s="19">
-        <v>2</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="C109" s="19"/>
+      <c r="D109" s="19"/>
       <c r="E109" s="19"/>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
@@ -2839,10 +2838,14 @@
         <v>113</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C110" s="19"/>
-      <c r="D110" s="19"/>
+        <v>15</v>
+      </c>
+      <c r="C110" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D110" s="19">
+        <v>2</v>
+      </c>
       <c r="E110" s="19"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2850,7 +2853,7 @@
         <v>113</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="C111" s="19"/>
       <c r="D111" s="19"/>
@@ -2861,7 +2864,7 @@
         <v>113</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C112" s="19"/>
       <c r="D112" s="19"/>
@@ -2872,7 +2875,7 @@
         <v>113</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>116</v>
+        <v>62</v>
       </c>
       <c r="C113" s="19"/>
       <c r="D113" s="19"/>
@@ -2883,7 +2886,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C114" s="19"/>
       <c r="D114" s="19"/>
@@ -2894,11 +2897,9 @@
         <v>113</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="C115" s="19" t="s">
-        <v>46</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C115" s="19"/>
       <c r="D115" s="19"/>
       <c r="E115" s="19"/>
     </row>
@@ -2907,65 +2908,65 @@
         <v>113</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>164</v>
-      </c>
-      <c r="C116" s="19"/>
+        <v>179</v>
+      </c>
+      <c r="C116" s="19" t="s">
+        <v>46</v>
+      </c>
       <c r="D116" s="19"/>
       <c r="E116" s="19"/>
-      <c r="F116" s="19" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C117" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="C117" s="19"/>
       <c r="D117" s="19"/>
       <c r="E117" s="19"/>
+      <c r="F117" s="19" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B118" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C118" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D118" s="15"/>
-      <c r="E118" s="15" t="s">
-        <v>64</v>
-      </c>
+      <c r="B118" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C118" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D118" s="19"/>
+      <c r="E118" s="19"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A119" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>132</v>
+        <v>79</v>
       </c>
       <c r="C119" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D119" s="14"/>
-      <c r="E119" s="14"/>
+        <v>78</v>
+      </c>
+      <c r="D119" s="15"/>
+      <c r="E119" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="C120" s="14" t="s">
-        <v>48</v>
+        <v>133</v>
       </c>
       <c r="D120" s="14"/>
       <c r="E120" s="14"/>
@@ -2975,10 +2976,10 @@
         <v>113</v>
       </c>
       <c r="B121" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>130</v>
+        <v>48</v>
       </c>
       <c r="D121" s="14"/>
       <c r="E121" s="14"/>
@@ -2988,10 +2989,10 @@
         <v>113</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D122" s="14"/>
       <c r="E122" s="14"/>
@@ -3001,9 +3002,11 @@
         <v>113</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="C123" s="14"/>
+        <v>135</v>
+      </c>
+      <c r="C123" s="14" t="s">
+        <v>136</v>
+      </c>
       <c r="D123" s="14"/>
       <c r="E123" s="14"/>
     </row>
@@ -3012,7 +3015,7 @@
         <v>113</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C124" s="14"/>
       <c r="D124" s="14"/>
@@ -3020,27 +3023,38 @@
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B125" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C125" s="14"/>
+      <c r="D125" s="14"/>
+      <c r="E125" s="14"/>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A126" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B125" s="19" t="s">
+      <c r="B126" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C125" s="19" t="s">
+      <c r="C126" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D125" s="19">
+      <c r="D126" s="19">
         <v>10</v>
       </c>
-      <c r="E125" s="19"/>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B127" s="22"/>
+      <c r="E126" s="19"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B128" s="22"/>
     </row>
   </sheetData>
   <sortState ref="A2:G52">
     <sortCondition ref="E2:E52"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A90 A92:A1048576">
+  <conditionalFormatting sqref="A1:A90 A93:A1048576">
     <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -3057,7 +3071,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A91">
+  <conditionalFormatting sqref="A91:A92">
     <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A91)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
updated TO DO spreadsheet #other #all
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1177,8 +1177,8 @@
   <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2323,7 +2323,7 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B72" s="19" t="s">
         <v>157</v>

</xml_diff>

<commit_message>
minor updates in TODO list #other
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="198">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -601,6 +601,15 @@
   </si>
   <si>
     <t>Vote against that horrible marigold color :)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simultaneous triple-view in 3D shading tool to help reduce error in scene generation. </t>
+  </si>
+  <si>
+    <t>3D Shading scene editor: Grouping and duplication of multiple objects simultaneously, with appropriate handling for XYZ coords</t>
+  </si>
+  <si>
+    <t>Transient thermal models for PV module/array in support of subhourly simulations (realign thermal/mounting structure inputs and standardize across module models)</t>
   </si>
 </sst>
 </file>
@@ -1177,8 +1186,8 @@
   <dimension ref="A1:I128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A63" sqref="A63"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3103,10 +3112,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A11"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3167,6 +3176,21 @@
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODO list update - completed items and added a few more items
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
@@ -11,12 +16,12 @@
     <sheet name="Project Ideas" sheetId="2" r:id="rId2"/>
     <sheet name="Registration Codes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="201">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -610,6 +615,15 @@
   </si>
   <si>
     <t>Transient thermal models for PV module/array in support of subhourly simulations (realign thermal/mounting structure inputs and standardize across module models)</t>
+  </si>
+  <si>
+    <t>SDK build</t>
+  </si>
+  <si>
+    <t>CEC Inverter updates</t>
+  </si>
+  <si>
+    <t>PBNS update for dispatch factors</t>
   </si>
 </sst>
 </file>
@@ -939,7 +953,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -974,7 +988,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1183,11 +1197,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I128"/>
+  <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B42" sqref="B42"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C90" sqref="C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2067,7 +2081,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B53" s="14" t="s">
         <v>2</v>
@@ -2570,49 +2584,52 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B88" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C88" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D88" s="14"/>
-      <c r="E88" s="14"/>
+        <v>58</v>
+      </c>
+      <c r="B88" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C88" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D88" s="19"/>
+      <c r="E88" s="19"/>
+      <c r="F88" s="19"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B89" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="C89" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D89" s="14"/>
-      <c r="E89" s="14"/>
+        <v>58</v>
+      </c>
+      <c r="B89" s="19" t="s">
+        <v>199</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D89" s="19"/>
+      <c r="E89" s="19"/>
+      <c r="F89" s="19"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
-        <v>141</v>
-      </c>
-      <c r="B90" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="C90" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D90" s="14"/>
-      <c r="E90" s="14"/>
+        <v>58</v>
+      </c>
+      <c r="B90" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D90" s="19"/>
+      <c r="E90" s="19"/>
+      <c r="F90" s="19"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
         <v>141</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>51</v>
@@ -2625,76 +2642,76 @@
         <v>141</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="C92" s="14"/>
+        <v>125</v>
+      </c>
+      <c r="C92" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="D92" s="14"/>
       <c r="E92" s="14"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>28</v>
+        <v>137</v>
       </c>
       <c r="C93" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D93" s="15"/>
-      <c r="E93" s="14" t="s">
-        <v>64</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" s="17" t="s">
-        <v>190</v>
+        <v>141</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="C94" s="14"/>
-      <c r="D94" s="15"/>
-      <c r="E94" s="14" t="s">
-        <v>64</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="C94" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B95" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C95" s="19"/>
-      <c r="D95" s="19"/>
-      <c r="E95" s="19" t="s">
-        <v>64</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="B95" s="14" t="s">
+        <v>194</v>
+      </c>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B96" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C96" s="19"/>
-      <c r="D96" s="19"/>
-      <c r="E96" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B96" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C96" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D96" s="15"/>
+      <c r="E96" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B97" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B97" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C97" s="14"/>
+      <c r="D97" s="15"/>
+      <c r="E97" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2703,11 +2720,9 @@
         <v>113</v>
       </c>
       <c r="B98" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C98" s="19" t="s">
-        <v>48</v>
-      </c>
+        <v>85</v>
+      </c>
+      <c r="C98" s="19"/>
       <c r="D98" s="19"/>
       <c r="E98" s="19" t="s">
         <v>64</v>
@@ -2718,14 +2733,10 @@
         <v>113</v>
       </c>
       <c r="B99" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C99" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D99" s="19">
-        <v>10</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C99" s="19"/>
+      <c r="D99" s="19"/>
       <c r="E99" s="19" t="s">
         <v>64</v>
       </c>
@@ -2735,40 +2746,52 @@
         <v>113</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="C100" s="19"/>
       <c r="D100" s="19"/>
-      <c r="E100" s="19"/>
+      <c r="E100" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C101" s="19"/>
+        <v>54</v>
+      </c>
+      <c r="C101" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="D101" s="19"/>
-      <c r="E101" s="19"/>
+      <c r="E101" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="C102" s="19"/>
-      <c r="D102" s="19"/>
-      <c r="E102" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="C102" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D102" s="19">
+        <v>10</v>
+      </c>
+      <c r="E102" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C103" s="19"/>
       <c r="D103" s="19"/>
@@ -2779,7 +2802,7 @@
         <v>113</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C104" s="19"/>
       <c r="D104" s="19"/>
@@ -2790,7 +2813,7 @@
         <v>113</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C105" s="19"/>
       <c r="D105" s="19"/>
@@ -2801,7 +2824,7 @@
         <v>113</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C106" s="19"/>
       <c r="D106" s="19"/>
@@ -2812,11 +2835,9 @@
         <v>113</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C107" s="19" t="s">
-        <v>109</v>
-      </c>
+        <v>97</v>
+      </c>
+      <c r="C107" s="19"/>
       <c r="D107" s="19"/>
       <c r="E107" s="19"/>
     </row>
@@ -2825,7 +2846,7 @@
         <v>113</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="C108" s="19"/>
       <c r="D108" s="19"/>
@@ -2836,7 +2857,7 @@
         <v>113</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="C109" s="19"/>
       <c r="D109" s="19"/>
@@ -2847,14 +2868,12 @@
         <v>113</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
       <c r="C110" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D110" s="19">
-        <v>2</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="D110" s="19"/>
       <c r="E110" s="19"/>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -2862,7 +2881,7 @@
         <v>113</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>31</v>
+        <v>111</v>
       </c>
       <c r="C111" s="19"/>
       <c r="D111" s="19"/>
@@ -2873,7 +2892,7 @@
         <v>113</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="C112" s="19"/>
       <c r="D112" s="19"/>
@@ -2884,10 +2903,14 @@
         <v>113</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="C113" s="19"/>
-      <c r="D113" s="19"/>
+        <v>15</v>
+      </c>
+      <c r="C113" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D113" s="19">
+        <v>2</v>
+      </c>
       <c r="E113" s="19"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2895,7 +2918,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>116</v>
+        <v>31</v>
       </c>
       <c r="C114" s="19"/>
       <c r="D114" s="19"/>
@@ -2906,7 +2929,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>115</v>
+        <v>36</v>
       </c>
       <c r="C115" s="19"/>
       <c r="D115" s="19"/>
@@ -2917,11 +2940,9 @@
         <v>113</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="C116" s="19" t="s">
-        <v>46</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="C116" s="19"/>
       <c r="D116" s="19"/>
       <c r="E116" s="19"/>
     </row>
@@ -2930,25 +2951,20 @@
         <v>113</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>164</v>
+        <v>116</v>
       </c>
       <c r="C117" s="19"/>
       <c r="D117" s="19"/>
       <c r="E117" s="19"/>
-      <c r="F117" s="19" t="s">
-        <v>162</v>
-      </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="C118" s="19" t="s">
-        <v>47</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="C118" s="19"/>
       <c r="D118" s="19"/>
       <c r="E118" s="19"/>
     </row>
@@ -2956,65 +2972,66 @@
       <c r="A119" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B119" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D119" s="15"/>
-      <c r="E119" s="15" t="s">
-        <v>64</v>
-      </c>
+      <c r="B119" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="C119" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D119" s="19"/>
+      <c r="E119" s="19"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B120" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D120" s="14"/>
-      <c r="E120" s="14"/>
+      <c r="B120" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="C120" s="19"/>
+      <c r="D120" s="19"/>
+      <c r="E120" s="19"/>
+      <c r="F120" s="19" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B121" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="C121" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D121" s="14"/>
-      <c r="E121" s="14"/>
+      <c r="B121" s="19" t="s">
+        <v>139</v>
+      </c>
+      <c r="C121" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D121" s="19"/>
+      <c r="E121" s="19"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D122" s="14"/>
-      <c r="E122" s="14"/>
+        <v>78</v>
+      </c>
+      <c r="D122" s="15"/>
+      <c r="E122" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C123" s="14" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D123" s="14"/>
       <c r="E123" s="14"/>
@@ -3024,9 +3041,11 @@
         <v>113</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="C124" s="14"/>
+        <v>122</v>
+      </c>
+      <c r="C124" s="14" t="s">
+        <v>48</v>
+      </c>
       <c r="D124" s="14"/>
       <c r="E124" s="14"/>
     </row>
@@ -3035,35 +3054,72 @@
         <v>113</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="C125" s="14"/>
+        <v>123</v>
+      </c>
+      <c r="C125" s="14" t="s">
+        <v>130</v>
+      </c>
       <c r="D125" s="14"/>
       <c r="E125" s="14"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A126" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B126" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C126" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D126" s="14"/>
+      <c r="E126" s="14"/>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A127" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B127" s="14" t="s">
+        <v>192</v>
+      </c>
+      <c r="C127" s="14"/>
+      <c r="D127" s="14"/>
+      <c r="E127" s="14"/>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A128" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B128" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="C128" s="14"/>
+      <c r="D128" s="14"/>
+      <c r="E128" s="14"/>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A129" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B126" s="19" t="s">
+      <c r="B129" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C126" s="19" t="s">
+      <c r="C129" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D126" s="19">
+      <c r="D129" s="19">
         <v>10</v>
       </c>
-      <c r="E126" s="19"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B128" s="22"/>
+      <c r="E129" s="19"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B131" s="22"/>
     </row>
   </sheetData>
   <sortState ref="A2:G52">
     <sortCondition ref="E2:E52"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A90 A93:A1048576">
+  <conditionalFormatting sqref="A1:A93 A96:A1048576">
     <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -3080,21 +3136,21 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A91:A92">
+  <conditionalFormatting sqref="A94:A95">
     <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A91)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A94)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A91)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A94)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A91)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A94)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A91)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A94)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A91)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A94)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
TO DO list updates (check off biopower feedstock service call and geothermal temp/depth link)
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
@@ -16,7 +11,7 @@
     <sheet name="Project Ideas" sheetId="2" r:id="rId2"/>
     <sheet name="Registration Codes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -950,7 +945,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -985,7 +980,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1197,8 +1192,8 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,7 +2414,7 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="B77" s="19" t="s">
         <v>161</v>
@@ -2465,7 +2460,7 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
-        <v>58</v>
+        <v>190</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>166</v>
@@ -2557,7 +2552,7 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>176</v>
@@ -2571,7 +2566,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B87" s="19" t="s">
         <v>178</v>

</xml_diff>

<commit_message>
#bugfix - Dish Stirling_Commercial defaults update TODO item update
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Project Ideas" sheetId="2" r:id="rId2"/>
     <sheet name="Registration Codes" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -945,7 +950,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -980,7 +985,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1192,8 +1197,8 @@
   <dimension ref="A1:I131"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A111" sqref="A111"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2674,7 +2679,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
-        <v>141</v>
+        <v>57</v>
       </c>
       <c r="B95" s="14" t="s">
         <v>193</v>

</xml_diff>

<commit_message>
#new - Update PBNS Power Block.ui and add CSP PBNS Dispatch Control.ui for CSP steam technologies #bugfix - update defaults for all CSP steam technologies
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="202">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -621,6 +621,12 @@
   </si>
   <si>
     <t>Molten salt linear fresnel - match with script from Ty</t>
+  </si>
+  <si>
+    <t>Move all CSP constants from ui to respective compute modules</t>
+  </si>
+  <si>
+    <t>Fix issue with parametric grid editor read only display of monthly and hourly outputs.</t>
   </si>
 </sst>
 </file>
@@ -767,7 +773,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="19">
     <dxf>
       <font>
         <color theme="0"/>
@@ -835,6 +841,76 @@
       <fill>
         <patternFill>
           <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF33CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1194,11 +1270,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I131"/>
+  <dimension ref="A1:I133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2209,7 +2285,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B62" s="14" t="s">
         <v>199</v>
@@ -2599,7 +2675,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
-        <v>58</v>
+        <v>113</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>197</v>
@@ -2613,7 +2689,7 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B90" s="19" t="s">
         <v>198</v>
@@ -2627,36 +2703,36 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B91" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C91" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D91" s="14"/>
-      <c r="E91" s="14"/>
+        <v>58</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="19"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
-        <v>140</v>
-      </c>
-      <c r="B92" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="C92" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="D92" s="14"/>
-      <c r="E92" s="14"/>
+        <v>58</v>
+      </c>
+      <c r="B92" s="19" t="s">
+        <v>201</v>
+      </c>
+      <c r="C92" s="19"/>
+      <c r="D92" s="19"/>
+      <c r="E92" s="19"/>
+      <c r="F92" s="19"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
         <v>140</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="C93" s="14" t="s">
         <v>51</v>
@@ -2669,7 +2745,7 @@
         <v>140</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="C94" s="14" t="s">
         <v>51</v>
@@ -2679,66 +2755,66 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" s="17" t="s">
-        <v>57</v>
+        <v>140</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="C95" s="14"/>
+        <v>136</v>
+      </c>
+      <c r="C95" s="14" t="s">
+        <v>51</v>
+      </c>
       <c r="D95" s="14"/>
       <c r="E95" s="14"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" s="17" t="s">
-        <v>189</v>
+        <v>140</v>
       </c>
       <c r="B96" s="14" t="s">
-        <v>28</v>
+        <v>141</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="D96" s="15"/>
-      <c r="E96" s="14" t="s">
-        <v>64</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D96" s="14"/>
+      <c r="E96" s="14"/>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="17" t="s">
-        <v>189</v>
+        <v>57</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>60</v>
+        <v>192</v>
       </c>
       <c r="C97" s="14"/>
-      <c r="D97" s="15"/>
-      <c r="E97" s="14" t="s">
-        <v>64</v>
-      </c>
+      <c r="D97" s="14"/>
+      <c r="E97" s="14"/>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B98" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="C98" s="19"/>
-      <c r="D98" s="19"/>
-      <c r="E98" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="B98" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C98" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D98" s="15"/>
+      <c r="E98" s="14" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B99" s="19" t="s">
-        <v>61</v>
-      </c>
-      <c r="C99" s="19"/>
-      <c r="D99" s="19"/>
-      <c r="E99" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="B99" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C99" s="14"/>
+      <c r="D99" s="15"/>
+      <c r="E99" s="14" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2747,7 +2823,7 @@
         <v>113</v>
       </c>
       <c r="B100" s="19" t="s">
-        <v>34</v>
+        <v>85</v>
       </c>
       <c r="C100" s="19"/>
       <c r="D100" s="19"/>
@@ -2760,11 +2836,9 @@
         <v>113</v>
       </c>
       <c r="B101" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="C101" s="19" t="s">
-        <v>48</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C101" s="19"/>
       <c r="D101" s="19"/>
       <c r="E101" s="19" t="s">
         <v>64</v>
@@ -2775,14 +2849,10 @@
         <v>113</v>
       </c>
       <c r="B102" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="C102" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D102" s="19">
-        <v>10</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
       <c r="E102" s="19" t="s">
         <v>64</v>
       </c>
@@ -2792,29 +2862,39 @@
         <v>113</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>93</v>
-      </c>
-      <c r="C103" s="19"/>
+        <v>54</v>
+      </c>
+      <c r="C103" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
+      <c r="E103" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B104" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="C104" s="19"/>
-      <c r="D104" s="19"/>
-      <c r="E104" s="19"/>
+        <v>26</v>
+      </c>
+      <c r="C104" s="19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D104" s="19">
+        <v>10</v>
+      </c>
+      <c r="E104" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B105" s="19" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C105" s="19"/>
       <c r="D105" s="19"/>
@@ -2825,7 +2905,7 @@
         <v>113</v>
       </c>
       <c r="B106" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C106" s="19"/>
       <c r="D106" s="19"/>
@@ -2836,7 +2916,7 @@
         <v>113</v>
       </c>
       <c r="B107" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C107" s="19"/>
       <c r="D107" s="19"/>
@@ -2847,7 +2927,7 @@
         <v>113</v>
       </c>
       <c r="B108" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C108" s="19"/>
       <c r="D108" s="19"/>
@@ -2858,7 +2938,7 @@
         <v>113</v>
       </c>
       <c r="B109" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C109" s="19"/>
       <c r="D109" s="19"/>
@@ -2869,11 +2949,9 @@
         <v>113</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="C110" s="19" t="s">
-        <v>109</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="C110" s="19"/>
       <c r="D110" s="19"/>
       <c r="E110" s="19"/>
     </row>
@@ -2882,7 +2960,7 @@
         <v>113</v>
       </c>
       <c r="B111" s="19" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C111" s="19"/>
       <c r="D111" s="19"/>
@@ -2893,9 +2971,11 @@
         <v>113</v>
       </c>
       <c r="B112" s="19" t="s">
-        <v>112</v>
-      </c>
-      <c r="C112" s="19"/>
+        <v>108</v>
+      </c>
+      <c r="C112" s="19" t="s">
+        <v>109</v>
+      </c>
       <c r="D112" s="19"/>
       <c r="E112" s="19"/>
     </row>
@@ -2904,14 +2984,10 @@
         <v>113</v>
       </c>
       <c r="B113" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C113" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D113" s="19">
-        <v>2</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="C113" s="19"/>
+      <c r="D113" s="19"/>
       <c r="E113" s="19"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2919,7 +2995,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="19" t="s">
-        <v>31</v>
+        <v>112</v>
       </c>
       <c r="C114" s="19"/>
       <c r="D114" s="19"/>
@@ -2930,10 +3006,14 @@
         <v>113</v>
       </c>
       <c r="B115" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="C115" s="19"/>
-      <c r="D115" s="19"/>
+        <v>15</v>
+      </c>
+      <c r="C115" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D115" s="19">
+        <v>2</v>
+      </c>
       <c r="E115" s="19"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -2941,7 +3021,7 @@
         <v>113</v>
       </c>
       <c r="B116" s="19" t="s">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="C116" s="19"/>
       <c r="D116" s="19"/>
@@ -2952,7 +3032,7 @@
         <v>113</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>116</v>
+        <v>36</v>
       </c>
       <c r="C117" s="19"/>
       <c r="D117" s="19"/>
@@ -2963,7 +3043,7 @@
         <v>113</v>
       </c>
       <c r="B118" s="19" t="s">
-        <v>115</v>
+        <v>62</v>
       </c>
       <c r="C118" s="19"/>
       <c r="D118" s="19"/>
@@ -2974,11 +3054,9 @@
         <v>113</v>
       </c>
       <c r="B119" s="19" t="s">
-        <v>178</v>
-      </c>
-      <c r="C119" s="19" t="s">
-        <v>46</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C119" s="19"/>
       <c r="D119" s="19"/>
       <c r="E119" s="19"/>
     </row>
@@ -2987,24 +3065,21 @@
         <v>113</v>
       </c>
       <c r="B120" s="19" t="s">
-        <v>163</v>
+        <v>115</v>
       </c>
       <c r="C120" s="19"/>
       <c r="D120" s="19"/>
       <c r="E120" s="19"/>
-      <c r="F120" s="19" t="s">
-        <v>161</v>
-      </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A121" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
       <c r="C121" s="19" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D121" s="19"/>
       <c r="E121" s="19"/>
@@ -3013,52 +3088,53 @@
       <c r="A122" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B122" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="C122" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="D122" s="15"/>
-      <c r="E122" s="15" t="s">
-        <v>64</v>
+      <c r="B122" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C122" s="19"/>
+      <c r="D122" s="19"/>
+      <c r="E122" s="19"/>
+      <c r="F122" s="19" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A123" s="17" t="s">
         <v>113</v>
       </c>
-      <c r="B123" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="C123" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D123" s="14"/>
-      <c r="E123" s="14"/>
+      <c r="B123" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="C123" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="D123" s="19"/>
+      <c r="E123" s="19"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A124" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>121</v>
+        <v>79</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D124" s="14"/>
-      <c r="E124" s="14"/>
+        <v>78</v>
+      </c>
+      <c r="D124" s="15"/>
+      <c r="E124" s="15" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A125" s="17" t="s">
         <v>113</v>
       </c>
       <c r="B125" s="14" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C125" s="14" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="D125" s="14"/>
       <c r="E125" s="14"/>
@@ -3068,10 +3144,10 @@
         <v>113</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="C126" s="14" t="s">
-        <v>135</v>
+        <v>48</v>
       </c>
       <c r="D126" s="14"/>
       <c r="E126" s="14"/>
@@ -3081,9 +3157,11 @@
         <v>113</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="C127" s="14"/>
+        <v>122</v>
+      </c>
+      <c r="C127" s="14" t="s">
+        <v>129</v>
+      </c>
       <c r="D127" s="14"/>
       <c r="E127" s="14"/>
     </row>
@@ -3092,35 +3170,59 @@
         <v>113</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="C128" s="14"/>
+        <v>134</v>
+      </c>
+      <c r="C128" s="14" t="s">
+        <v>135</v>
+      </c>
       <c r="D128" s="14"/>
       <c r="E128" s="14"/>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B129" s="14" t="s">
+        <v>190</v>
+      </c>
+      <c r="C129" s="14"/>
+      <c r="D129" s="14"/>
+      <c r="E129" s="14"/>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A130" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="B130" s="14" t="s">
+        <v>191</v>
+      </c>
+      <c r="C130" s="14"/>
+      <c r="D130" s="14"/>
+      <c r="E130" s="14"/>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A131" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="B129" s="19" t="s">
+      <c r="B131" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C129" s="19" t="s">
+      <c r="C131" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="D129" s="19">
+      <c r="D131" s="19">
         <v>10</v>
       </c>
-      <c r="E129" s="19"/>
-    </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B131" s="22"/>
+      <c r="E131" s="19"/>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B133" s="22"/>
     </row>
   </sheetData>
   <sortState ref="A2:G52">
     <sortCondition ref="E2:E52"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A93 A96:A1048576">
+  <conditionalFormatting sqref="A98:A1048576 A1:A95">
     <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -3137,21 +3239,21 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A94:A95">
+  <conditionalFormatting sqref="A96:A97">
     <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A94)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">

</xml_diff>

<commit_message>
Remove registration key list from TODO spreadsheet, and add new CSV file to track registration keys requested by email
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
     <sheet name="Project Ideas" sheetId="2" r:id="rId2"/>
-    <sheet name="Registration Codes" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="191">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -448,39 +447,6 @@
   </si>
   <si>
     <t>Customizable reports</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Email address</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>CB18B612-F85E-47C9-AB54-AFBCD468BB4B</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>2014.9.30</t>
-  </si>
-  <si>
-    <t>Christina Schall</t>
-  </si>
-  <si>
-    <t>christina.schall@schottsolar.com</t>
-  </si>
-  <si>
-    <t>Germany</t>
   </si>
   <si>
     <t>UI text to explain URDB utility name aliasing issue (e.g., PG&amp;E appears in list but without rates)</t>
@@ -628,7 +594,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -662,14 +628,6 @@
     <font>
       <b/>
       <sz val="14"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -731,11 +689,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -760,12 +717,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="12">
@@ -1197,7 +1151,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
     </sheetView>
@@ -2213,7 +2167,7 @@
         <v>57</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C62" s="14" t="s">
         <v>48</v>
@@ -2239,7 +2193,7 @@
         <v>57</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C64" s="14" t="s">
         <v>72</v>
@@ -2323,7 +2277,7 @@
       <c r="D70" s="19"/>
       <c r="E70" s="19"/>
       <c r="F70" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -2331,7 +2285,7 @@
         <v>57</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="C71" s="19" t="s">
         <v>71</v>
@@ -2339,7 +2293,7 @@
       <c r="D71" s="19"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,7 +2301,7 @@
         <v>57</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="C72" s="19" t="s">
         <v>47</v>
@@ -2355,7 +2309,7 @@
       <c r="D72" s="19"/>
       <c r="E72" s="19"/>
       <c r="F72" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -2363,15 +2317,15 @@
         <v>57</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D73" s="19"/>
       <c r="E73" s="19"/>
       <c r="F73" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -2379,7 +2333,7 @@
         <v>57</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="C74" s="19" t="s">
         <v>68</v>
@@ -2387,7 +2341,7 @@
       <c r="D74" s="19"/>
       <c r="E74" s="19"/>
       <c r="F74" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2395,7 +2349,7 @@
         <v>57</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C75" s="19" t="s">
         <v>47</v>
@@ -2409,7 +2363,7 @@
         <v>57</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="C76" s="19" t="s">
         <v>47</v>
@@ -2420,10 +2374,10 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="C77" s="19" t="s">
         <v>47</v>
@@ -2431,7 +2385,7 @@
       <c r="D77" s="19"/>
       <c r="E77" s="19"/>
       <c r="F77" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2439,7 +2393,7 @@
         <v>57</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="C78" s="19" t="s">
         <v>47</v>
@@ -2447,7 +2401,7 @@
       <c r="D78" s="19"/>
       <c r="E78" s="19"/>
       <c r="F78" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2455,27 +2409,27 @@
         <v>57</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C79" s="19"/>
       <c r="D79" s="19"/>
       <c r="E79" s="19"/>
       <c r="F79" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" s="17" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C80" s="19"/>
       <c r="D80" s="19"/>
       <c r="E80" s="19"/>
       <c r="F80" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2483,7 +2437,7 @@
         <v>57</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="C81" s="19" t="s">
         <v>71</v>
@@ -2491,7 +2445,7 @@
       <c r="D81" s="19"/>
       <c r="E81" s="19"/>
       <c r="F81" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2499,7 +2453,7 @@
         <v>57</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C82" s="19" t="s">
         <v>47</v>
@@ -2507,7 +2461,7 @@
       <c r="D82" s="19"/>
       <c r="E82" s="19"/>
       <c r="F82" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2515,7 +2469,7 @@
         <v>57</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C83" s="19" t="s">
         <v>47</v>
@@ -2523,7 +2477,7 @@
       <c r="D83" s="19"/>
       <c r="E83" s="19"/>
       <c r="F83" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2531,7 +2485,7 @@
         <v>57</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C84" s="19" t="s">
         <v>47</v>
@@ -2539,7 +2493,7 @@
       <c r="D84" s="19"/>
       <c r="E84" s="19"/>
       <c r="F84" s="19" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2547,13 +2501,13 @@
         <v>57</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="C85" s="19"/>
       <c r="D85" s="19"/>
       <c r="E85" s="19"/>
       <c r="F85" s="19" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2561,7 +2515,7 @@
         <v>57</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C86" s="19" t="s">
         <v>47</v>
@@ -2575,7 +2529,7 @@
         <v>57</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C87" s="19" t="s">
         <v>47</v>
@@ -2589,7 +2543,7 @@
         <v>58</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C88" s="19" t="s">
         <v>48</v>
@@ -2603,7 +2557,7 @@
         <v>113</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C89" s="19" t="s">
         <v>48</v>
@@ -2617,7 +2571,7 @@
         <v>57</v>
       </c>
       <c r="B90" s="19" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C90" s="19" t="s">
         <v>48</v>
@@ -2631,7 +2585,7 @@
         <v>113</v>
       </c>
       <c r="B91" s="19" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C91" s="19" t="s">
         <v>48</v>
@@ -2645,7 +2599,7 @@
         <v>58</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="C92" s="19"/>
       <c r="D92" s="19"/>
@@ -2709,7 +2663,7 @@
         <v>57</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C97" s="14"/>
       <c r="D97" s="14"/>
@@ -2717,7 +2671,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>28</v>
@@ -2732,7 +2686,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B99" s="14" t="s">
         <v>60</v>
@@ -3001,7 +2955,7 @@
         <v>113</v>
       </c>
       <c r="B121" s="19" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C121" s="19" t="s">
         <v>46</v>
@@ -3014,13 +2968,13 @@
         <v>113</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C122" s="19"/>
       <c r="D122" s="19"/>
       <c r="E122" s="19"/>
       <c r="F122" s="19" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -3108,7 +3062,7 @@
         <v>113</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="C129" s="14"/>
       <c r="D129" s="14"/>
@@ -3119,7 +3073,7 @@
         <v>113</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C130" s="14"/>
       <c r="D130" s="14"/>
@@ -3141,7 +3095,7 @@
       <c r="E131" s="19"/>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="22"/>
+      <c r="B133" s="20"/>
     </row>
   </sheetData>
   <sortState ref="A2:G52">
@@ -3198,7 +3152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -3214,137 +3168,70 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="45" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" customWidth="1"/>
-    <col min="5" max="5" width="43.5703125" customWidth="1"/>
-    <col min="6" max="6" width="21.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>149</v>
-      </c>
-      <c r="B2" s="20">
-        <v>41921</v>
-      </c>
-      <c r="C2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>153</v>
-      </c>
-      <c r="F2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add post-release bugs and issues to TODO list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="201">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -588,13 +588,43 @@
   </si>
   <si>
     <t>Fix issue with parametric grid editor read only display of monthly and hourly outputs.</t>
+  </si>
+  <si>
+    <t>Display issues on very high resolution screens (see screenshots from Ted James)</t>
+  </si>
+  <si>
+    <t>Mystery sam.exe crash on some Windows computers</t>
+  </si>
+  <si>
+    <t>Remove lk autosave to avoid junk temporary files</t>
+  </si>
+  <si>
+    <t>Add monthly scaling to input hourly load page (monthly scaling available for residential belpe but not commercial)</t>
+  </si>
+  <si>
+    <t>Physical trough default T_startup (lowered from 300 to 250 to avoid simulation warnings, but causes 3% annual output reduction)</t>
+  </si>
+  <si>
+    <t>Steve/Ty</t>
+  </si>
+  <si>
+    <t>Add LHS and stepwise script functions to LK</t>
+  </si>
+  <si>
+    <t>Not Done</t>
+  </si>
+  <si>
+    <t>Post SAM 2014.11.24 Release</t>
+  </si>
+  <si>
+    <t>Change curtailment and availability factors to percentages to be consistent with other losses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -632,8 +662,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -670,6 +714,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -692,7 +742,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -717,7 +767,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1149,17 +1209,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I133"/>
+  <dimension ref="A1:I140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A92" sqref="A92"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="17" customWidth="1"/>
-    <col min="2" max="2" width="102.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="102.85546875" style="24" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" style="4" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" customWidth="1"/>
@@ -3094,8 +3154,95 @@
       </c>
       <c r="E131" s="19"/>
     </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A132" s="17"/>
+      <c r="B132"/>
+    </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B133" s="20"/>
+      <c r="A133" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="B133" s="22"/>
+      <c r="C133" s="22"/>
+      <c r="D133" s="23"/>
+      <c r="E133" s="22"/>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A134" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B134" s="24" t="s">
+        <v>191</v>
+      </c>
+      <c r="C134" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A135" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B135" s="24" t="s">
+        <v>200</v>
+      </c>
+      <c r="C135" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A136" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B136" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="C136" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A137" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B137" s="24" t="s">
+        <v>193</v>
+      </c>
+      <c r="C137" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A138" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B138" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="C138" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B139" s="24" t="s">
+        <v>195</v>
+      </c>
+      <c r="C139" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A140" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="B140" s="24" t="s">
+        <v>197</v>
+      </c>
+      <c r="C140" t="s">
+        <v>47</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:G52">
@@ -3152,7 +3299,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update TODO list with CSP items from Craig Turchi
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="228">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -691,6 +691,18 @@
   </si>
   <si>
     <t>Update the model to use MPPT information in the inverter model when using the CEC model</t>
+  </si>
+  <si>
+    <t>Review CSP time series outpu variables, e.g., cycle power output appears twice without gross and net designation</t>
+  </si>
+  <si>
+    <t>Make sure all monthly and annual data variables have units</t>
+  </si>
+  <si>
+    <t>Fix cash flow spreadsheet so it works with TOD factors, also total installed cost UI labels for all technologies, test for all technologies</t>
+  </si>
+  <si>
+    <t>Fix replacement reserve defaults for CSP models</t>
   </si>
 </sst>
 </file>
@@ -1356,11 +1368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I143"/>
+  <dimension ref="A1:I147"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B150" sqref="B150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,7 +3160,7 @@
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="B120" s="19" t="s">
         <v>115</v>
@@ -3422,6 +3434,41 @@
       </c>
       <c r="C143" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B144" s="24" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B145" s="24" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A146" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B146" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="C146" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B147" s="24" t="s">
+        <v>227</v>
       </c>
     </row>
   </sheetData>
@@ -3592,8 +3639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated to do spreadsheet.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="231">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -709,6 +709,9 @@
   </si>
   <si>
     <t>Add parallelized simulation support in script via parsim() and parout()</t>
+  </si>
+  <si>
+    <t>Fix installer script so that .zsam files open with old SAM and .sam files open with new SAM</t>
   </si>
 </sst>
 </file>
@@ -1377,8 +1380,8 @@
   <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B137" sqref="B137"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3486,6 +3489,17 @@
       </c>
       <c r="B148" s="24" t="s">
         <v>227</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="20" t="s">
+        <v>228</v>
+      </c>
+      <c r="B149" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C149" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
@@ -3660,7 +3674,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added phys trough subhourly issue to post release TO DO.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="232">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -705,13 +705,16 @@
     <t>Fix replacement reserve defaults for CSP models</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>Add parallelized simulation support in script via parsim() and parout()</t>
   </si>
   <si>
     <t>Fix installer script so that .zsam files open with old SAM and .sam files open with new SAM</t>
+  </si>
+  <si>
+    <t>Steve/Ty/Aron</t>
+  </si>
+  <si>
+    <t>Fix physical trough model to enable subhourly simulations, as in previous versions of SAM</t>
   </si>
 </sst>
 </file>
@@ -1380,8 +1383,8 @@
   <dimension ref="A1:I151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B124" sqref="B124"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A142" sqref="A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3337,7 +3340,7 @@
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="17" t="s">
-        <v>228</v>
+        <v>57</v>
       </c>
       <c r="B134" s="24" t="s">
         <v>191</v>
@@ -3370,7 +3373,7 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="17" t="s">
-        <v>228</v>
+        <v>57</v>
       </c>
       <c r="B137" s="24" t="s">
         <v>193</v>
@@ -3392,7 +3395,7 @@
     </row>
     <row r="139" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A139" s="17" t="s">
-        <v>228</v>
+        <v>57</v>
       </c>
       <c r="B139" s="24" t="s">
         <v>195</v>
@@ -3403,7 +3406,7 @@
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="17" t="s">
-        <v>228</v>
+        <v>57</v>
       </c>
       <c r="B140" s="24" t="s">
         <v>197</v>
@@ -3414,10 +3417,10 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B141" s="24" t="s">
         <v>228</v>
-      </c>
-      <c r="B141" s="24" t="s">
-        <v>229</v>
       </c>
       <c r="C141" t="s">
         <v>47</v>
@@ -3493,13 +3496,24 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" s="20" t="s">
-        <v>228</v>
+        <v>57</v>
       </c>
       <c r="B149" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C149" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B150" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="C150" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#defaults update equipment reserve account defaults for all CSP technologies
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1412,8 +1412,8 @@
   <dimension ref="A1:I156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B156" sqref="B156"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B152" sqref="B152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3523,7 +3523,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B148" s="24" t="s">
         <v>236</v>

</xml_diff>

<commit_message>
Fixed units on GCR variables #pv
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
@@ -19,7 +14,7 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$T$1:$T$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -1165,7 +1160,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1200,7 +1195,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1411,9 +1406,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B152" sqref="B152"/>
+      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3559,7 +3554,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B151" s="24" t="s">
         <v>230</v>
@@ -3795,7 +3790,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update TODO list, fix empirical trough parasitics bug, add csp generic thermal storage/tod factor library UI bug
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="247">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -738,7 +738,28 @@
     <t>Potential weather file download or unzip issue ("Failed to decompress downloaded weather data" error reported by Chris Richards in support mailbox). Related to internet connectivity issue/proxy settings.</t>
   </si>
   <si>
-    <t>Add UI check on depreciation for sums greater than 100%</t>
+    <t>Update LK script examples in SDK</t>
+  </si>
+  <si>
+    <t>Paul/Steve</t>
+  </si>
+  <si>
+    <t>Empirical trough parasitics page user entry bug (values not saved when you leave page) -- also check receivers and other libraries</t>
+  </si>
+  <si>
+    <t>Solar resource page global horizontal shows 1.#R for international weather files that do not have GHI data</t>
+  </si>
+  <si>
+    <t>Test CEC module with user specs (see 2 emails from sam support email)</t>
+  </si>
+  <si>
+    <t>Paul/Janine</t>
+  </si>
+  <si>
+    <t>Fix units issue in UI for equipment reserve accounts (dollar amount in UI is off by a factor of 1000)</t>
+  </si>
+  <si>
+    <t>Update CSP Generic Thermal storage page to work correctly with TOD factors libarary</t>
   </si>
 </sst>
 </file>
@@ -1404,11 +1425,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I156"/>
+  <dimension ref="A1:I161"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A152" sqref="A152"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A157" sqref="A157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3518,7 +3539,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="B148" s="24" t="s">
         <v>236</v>
@@ -3554,7 +3575,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="20" t="s">
-        <v>57</v>
+        <v>198</v>
       </c>
       <c r="B151" s="24" t="s">
         <v>230</v>
@@ -3610,15 +3631,67 @@
         <v>47</v>
       </c>
     </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A156" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B156" s="24" t="s">
+        <v>241</v>
+      </c>
+      <c r="C156" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" s="20" t="s">
         <v>198</v>
       </c>
-      <c r="B156" s="24" t="s">
+      <c r="B157" s="24" t="s">
         <v>239</v>
       </c>
-      <c r="C156" t="s">
-        <v>48</v>
+      <c r="C157" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B158" s="24" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B159" s="24" t="s">
+        <v>243</v>
+      </c>
+      <c r="C159" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B160" s="24" t="s">
+        <v>245</v>
+      </c>
+      <c r="C160" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B161" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="C161" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -3790,7 +3863,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add CSP UI bugs to TODO list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="249">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -760,6 +760,14 @@
   </si>
   <si>
     <t>Update CSP Generic Thermal storage page to work correctly with TOD factors libarary</t>
+  </si>
+  <si>
+    <t>Fix linear fresnel direct UI bug: Could not evaluate callback function:Linear Fresnel Boiler Geometry-&gt;on_load
+[24]: error in call to 'value()': variable 'csp.lf.sf.azimuth' does not exist in this context[8]: error inside function</t>
+  </si>
+  <si>
+    <t>Fix dis stirling UI bug: Could not evaluate callback function:Dish Capital Costs-&gt;on_load
+[3]: error in call to 'value()': variable 'case.financing' does not exist in this context</t>
   </si>
 </sst>
 </file>
@@ -1425,11 +1433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I161"/>
+  <dimension ref="A1:I163"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A150" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A157" sqref="A157"/>
+      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A164" sqref="A164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3692,6 +3700,22 @@
       </c>
       <c r="C161" t="s">
         <v>240</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A162" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B162" s="24" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A163" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B163" s="24" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TODO list add physical trough Royal CSP receiver to library and fix physical trough UI callback bug
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="250">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -766,8 +766,11 @@
 [24]: error in call to 'value()': variable 'csp.lf.sf.azimuth' does not exist in this context[8]: error inside function</t>
   </si>
   <si>
-    <t>Fix dis stirling UI bug: Could not evaluate callback function:Dish Capital Costs-&gt;on_load
+    <t>Fix dish stirling UI bug: Could not evaluate callback function:Dish Capital Costs-&gt;on_load
 [3]: error in call to 'value()': variable 'case.financing' does not exist in this context</t>
+  </si>
+  <si>
+    <t>Fix physical trough UI bug: callback function refers to wrong variable name for average focal length</t>
   </si>
 </sst>
 </file>
@@ -1433,11 +1436,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I163"/>
+  <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A164" sqref="A164"/>
+      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3503,7 +3506,7 @@
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B144" s="24" t="s">
         <v>206</v>
@@ -3716,6 +3719,17 @@
       </c>
       <c r="B163" s="24" t="s">
         <v>248</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B164" s="24" t="s">
+        <v>249</v>
+      </c>
+      <c r="C164" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#new - Generic CSP update thermal storage to work with dispatch factors.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$T$1:$T$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1192,7 +1197,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1227,7 +1232,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1439,8 +1444,8 @@
   <dimension ref="A1:I164"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
+      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A149" sqref="A149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3550,7 +3555,7 @@
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B148" s="24" t="s">
         <v>236</v>
@@ -3655,7 +3660,7 @@
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B157" s="24" t="s">
         <v>239</v>
@@ -3696,7 +3701,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B161" s="24" t="s">
         <v>246</v>

</xml_diff>

<commit_message>
#bugfix - direct steam linear Fresnel update for collector and receiver page and callback to solar field page.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="251">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -776,6 +776,9 @@
   </si>
   <si>
     <t>Fix physical trough UI bug: callback function refers to wrong variable name for average focal length</t>
+  </si>
+  <si>
+    <t>Fix recapitalization for all technologies and test for geothermal</t>
   </si>
 </sst>
 </file>
@@ -1441,11 +1444,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I164"/>
+  <dimension ref="A1:I165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A149" sqref="A149"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A163" sqref="A163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3712,7 +3715,7 @@
     </row>
     <row r="162" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A162" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B162" s="24" t="s">
         <v>247</v>
@@ -3735,6 +3738,17 @@
       </c>
       <c r="C164" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B165" s="24" t="s">
+        <v>250</v>
+      </c>
+      <c r="C165" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#bugfix dish Stirling cost page label for all financial markets.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1447,8 +1447,8 @@
   <dimension ref="A1:I165"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A163" sqref="A163"/>
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B153" sqref="B153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3723,7 +3723,7 @@
     </row>
     <row r="163" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A163" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B163" s="24" t="s">
         <v>248</v>

</xml_diff>

<commit_message>
#bugfix - biopower items from Paul 12/18/14
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="254">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -782,6 +782,12 @@
   </si>
   <si>
     <t>Fix swh aux gas macro: convert units from W to kW</t>
+  </si>
+  <si>
+    <t>Biopower issues per email from Paul 12/18/14</t>
+  </si>
+  <si>
+    <t>Debt fraction as input to DHF Single Owner and Leveraged Partnership flip</t>
   </si>
 </sst>
 </file>
@@ -1447,11 +1453,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I166"/>
+  <dimension ref="A1:I168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B165" sqref="B165"/>
+      <selection pane="bottomLeft" activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3763,6 +3769,28 @@
       </c>
       <c r="C166" t="s">
         <v>71</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B167" s="24" t="s">
+        <v>252</v>
+      </c>
+      <c r="C167" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B168" s="24" t="s">
+        <v>253</v>
+      </c>
+      <c r="C168" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODO items updates based on meetings and emails and user support issues
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="256">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -788,6 +788,12 @@
   </si>
   <si>
     <t>Debt fraction as input to DHF Single Owner and Leveraged Partnership flip</t>
+  </si>
+  <si>
+    <t>Issue with multiple processor simulaitons - see scripts from Mark stops around 2700 runs</t>
+  </si>
+  <si>
+    <t>Financial Model warning and error messages for non-convergence</t>
   </si>
 </sst>
 </file>
@@ -1453,11 +1459,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I168"/>
+  <dimension ref="A1:I170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A168" sqref="A168"/>
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A171" sqref="A171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2900,7 +2906,7 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B92" s="19" t="s">
         <v>190</v>
@@ -3614,7 +3620,7 @@
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A152" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B152" s="24" t="s">
         <v>231</v>
@@ -3784,12 +3790,31 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B168" s="24" t="s">
         <v>253</v>
       </c>
       <c r="C168" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B169" s="24" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B170" s="24" t="s">
+        <v>255</v>
+      </c>
+      <c r="C170" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#bugfix - recapitalization for all technologies and update defaults
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="257">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -794,6 +794,9 @@
   </si>
   <si>
     <t>Financial Model warning and error messages for non-convergence</t>
+  </si>
+  <si>
+    <t>Recheck all defaults</t>
   </si>
 </sst>
 </file>
@@ -1459,11 +1462,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I170"/>
+  <dimension ref="A1:I171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A171" sqref="A171"/>
+      <selection pane="bottomLeft" activeCell="A172" sqref="A172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3757,7 +3760,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B165" s="24" t="s">
         <v>250</v>
@@ -3816,6 +3819,14 @@
       </c>
       <c r="C170" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B171" s="24" t="s">
+        <v>256</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#bugfix - ui display of NaN - change from 1.#R or 1.#J or 1.#QNAN to "NaN" per TODO list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="257">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1465,8 +1465,8 @@
   <dimension ref="A1:I171"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A172" sqref="A172"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A159" sqref="A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="17" t="s">
-        <v>178</v>
+        <v>57</v>
       </c>
       <c r="B98" s="14" t="s">
         <v>28</v>
@@ -3692,10 +3692,13 @@
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B158" s="24" t="s">
         <v>242</v>
+      </c>
+      <c r="C158" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added monthly utility bill scaling to hourly electric load input. Tested and working. Removed two unused defaults from electric load page. Updated defaults accordingly. Updated commercial monthly scaling defaults to appropriate magnitude. #new #electricload
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -17,14 +12,14 @@
     <sheet name="SAM Variable Changes" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Types">'SAM Variable Changes'!$T$1:$T$3</definedName>
+    <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="270">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -657,9 +652,6 @@
   </si>
   <si>
     <t>Input Page</t>
-  </si>
-  <si>
-    <t>Default Value (if new)</t>
   </si>
   <si>
     <t>New variable</t>
@@ -797,6 +789,48 @@
   </si>
   <si>
     <t>Recheck all defaults</t>
+  </si>
+  <si>
+    <t>Electric Load Other</t>
+  </si>
+  <si>
+    <t>Variable Type</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>normalize_to_utility_bill</t>
+  </si>
+  <si>
+    <t>**** this already existed as a variable on the input page but it wasn't being used- so I don't think it affects the defaults files?</t>
+  </si>
+  <si>
+    <t>utility_bill_data</t>
+  </si>
+  <si>
+    <t>****same as above</t>
+  </si>
+  <si>
+    <t>depends on residential vs commercial</t>
+  </si>
+  <si>
+    <t>p_scale_f</t>
+  </si>
+  <si>
+    <t>p_offset_value</t>
+  </si>
+  <si>
+    <t>Default Value (if new) or reason deleted</t>
+  </si>
+  <si>
+    <t>not used on form</t>
   </si>
 </sst>
 </file>
@@ -856,7 +890,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -905,6 +939,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -927,7 +967,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -963,7 +1003,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,15 +1155,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1130,7 +1172,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8020050" y="752475"/>
+          <a:off x="10782300" y="1724025"/>
           <a:ext cx="3990975" cy="1581150"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -1218,7 +1260,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1253,7 +1295,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1464,9 +1506,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A159" sqref="A159"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3466,7 +3508,7 @@
     </row>
     <row r="138" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A138" s="17" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B138" s="24" t="s">
         <v>194</v>
@@ -3502,7 +3544,7 @@
         <v>57</v>
       </c>
       <c r="B141" s="24" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C141" t="s">
         <v>47</v>
@@ -3546,7 +3588,7 @@
         <v>198</v>
       </c>
       <c r="B145" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C145" t="s">
         <v>127</v>
@@ -3557,7 +3599,7 @@
         <v>198</v>
       </c>
       <c r="B146" s="24" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C146" t="s">
         <v>71</v>
@@ -3568,7 +3610,7 @@
         <v>198</v>
       </c>
       <c r="B147" s="24" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C147" t="s">
         <v>71</v>
@@ -3579,7 +3621,7 @@
         <v>57</v>
       </c>
       <c r="B148" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C148" t="s">
         <v>48</v>
@@ -3590,7 +3632,7 @@
         <v>57</v>
       </c>
       <c r="B149" s="24" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C149" t="s">
         <v>47</v>
@@ -3601,13 +3643,13 @@
         <v>198</v>
       </c>
       <c r="B150" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C150" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D150" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -3615,7 +3657,7 @@
         <v>198</v>
       </c>
       <c r="B151" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C151" t="s">
         <v>46</v>
@@ -3626,10 +3668,10 @@
         <v>57</v>
       </c>
       <c r="B152" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="C152" t="s">
         <v>231</v>
-      </c>
-      <c r="C152" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -3637,13 +3679,13 @@
         <v>198</v>
       </c>
       <c r="B153" s="24" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C153" t="s">
         <v>77</v>
       </c>
       <c r="D153" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
@@ -3651,7 +3693,7 @@
         <v>57</v>
       </c>
       <c r="B154" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C154" t="s">
         <v>48</v>
@@ -3662,7 +3704,7 @@
         <v>57</v>
       </c>
       <c r="B155" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C155" t="s">
         <v>47</v>
@@ -3673,7 +3715,7 @@
         <v>57</v>
       </c>
       <c r="B156" s="24" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C156" t="s">
         <v>71</v>
@@ -3684,10 +3726,10 @@
         <v>57</v>
       </c>
       <c r="B157" s="24" t="s">
+        <v>238</v>
+      </c>
+      <c r="C157" t="s">
         <v>239</v>
-      </c>
-      <c r="C157" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -3695,7 +3737,7 @@
         <v>57</v>
       </c>
       <c r="B158" s="24" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C158" t="s">
         <v>48</v>
@@ -3706,10 +3748,10 @@
         <v>198</v>
       </c>
       <c r="B159" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="C159" t="s">
         <v>243</v>
-      </c>
-      <c r="C159" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
@@ -3717,7 +3759,7 @@
         <v>57</v>
       </c>
       <c r="B160" s="24" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C160" t="s">
         <v>71</v>
@@ -3728,10 +3770,10 @@
         <v>57</v>
       </c>
       <c r="B161" s="24" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C161" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="162" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3739,7 +3781,7 @@
         <v>57</v>
       </c>
       <c r="B162" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="163" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3747,7 +3789,7 @@
         <v>57</v>
       </c>
       <c r="B163" s="24" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
@@ -3755,7 +3797,7 @@
         <v>57</v>
       </c>
       <c r="B164" s="24" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C164" t="s">
         <v>71</v>
@@ -3766,7 +3808,7 @@
         <v>57</v>
       </c>
       <c r="B165" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C165" t="s">
         <v>48</v>
@@ -3777,7 +3819,7 @@
         <v>57</v>
       </c>
       <c r="B166" s="24" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C166" t="s">
         <v>71</v>
@@ -3788,7 +3830,7 @@
         <v>57</v>
       </c>
       <c r="B167" s="24" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C167" t="s">
         <v>48</v>
@@ -3799,7 +3841,7 @@
         <v>57</v>
       </c>
       <c r="B168" s="24" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C168" t="s">
         <v>48</v>
@@ -3810,7 +3852,7 @@
         <v>198</v>
       </c>
       <c r="B169" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -3818,7 +3860,7 @@
         <v>198</v>
       </c>
       <c r="B170" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C170" t="s">
         <v>48</v>
@@ -3829,7 +3871,7 @@
         <v>198</v>
       </c>
       <c r="B171" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -3983,12 +4025,12 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -3998,85 +4040,169 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T4"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" style="25" customWidth="1"/>
+    <col min="2" max="3" width="21.140625" style="25" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="37.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="26" t="s">
+        <v>257</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="E1" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="F1" s="26" t="s">
+        <v>268</v>
+      </c>
+      <c r="U1" t="s">
         <v>211</v>
       </c>
-      <c r="T1" t="s">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" s="27">
+        <v>10</v>
+      </c>
+      <c r="U2" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="C2" t="s">
-        <v>215</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B3" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="T2" t="s">
+      <c r="D3" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="F3" s="27"/>
+      <c r="U3" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="B3" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" t="s">
-        <v>218</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="B4" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>219</v>
       </c>
-      <c r="T3" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>214</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D4" s="27"/>
+      <c r="E4" s="27" t="s">
         <v>220</v>
       </c>
-      <c r="D4" t="s">
-        <v>221</v>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="F5" s="25">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>263</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>265</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>266</v>
+      </c>
+      <c r="E7" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="E8" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="F8" s="25" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allow total_installed_cost on generic system costs page to be a parametric input.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -1506,9 +1506,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I171"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A139" sqref="A139"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A140" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3552,7 +3552,7 @@
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B142" s="24" t="s">
         <v>201</v>
@@ -3654,7 +3654,7 @@
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A151" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B151" s="24" t="s">
         <v>229</v>
@@ -4042,8 +4042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changed availability and curtailment to loss factors instead of derates and updated all default values accordingly #new
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="276">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -840,6 +840,15 @@
   </si>
   <si>
     <t>Fix WxWidgets date and time bug that causes DView to crash one computers with location set to time zones greater than GMT+7</t>
+  </si>
+  <si>
+    <t>multiple</t>
+  </si>
+  <si>
+    <t>adjust</t>
+  </si>
+  <si>
+    <t>**CONVENTION CHANGED from derate to loss factor. Values from old files will work, but will be wrong!</t>
   </si>
 </sst>
 </file>
@@ -1516,8 +1525,8 @@
   <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A148" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A173" sqref="A173"/>
+      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A136" sqref="A136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3484,7 +3493,7 @@
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="17" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B135" s="24" t="s">
         <v>200</v>
@@ -4068,10 +4077,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4233,6 +4242,26 @@
         <v>269</v>
       </c>
     </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>274</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="F9" s="25" t="s">
+        <v>275</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A50">

</xml_diff>

<commit_message>
#bugfix CEC Performance Model with User Entered Specifications did not convert %/C units on bvoc or aisc. Fixed, new display variable added, and defaults updated accordingly.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="279">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -849,6 +849,15 @@
   </si>
   <si>
     <t>**CONVENTION CHANGED from derate to loss factor. Values from old files will work, but will be wrong!</t>
+  </si>
+  <si>
+    <t>6par_aisc_display</t>
+  </si>
+  <si>
+    <t>CEC Perf model with user entered…</t>
+  </si>
+  <si>
+    <t>6par_bvoc_display</t>
   </si>
 </sst>
 </file>
@@ -1525,8 +1534,8 @@
   <dimension ref="A1:I172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A136" sqref="A136"/>
+      <pane ySplit="1" topLeftCell="A133" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3763,7 +3772,7 @@
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A159" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B159" s="24" t="s">
         <v>242</v>
@@ -4077,10 +4086,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4262,6 +4271,40 @@
         <v>275</v>
       </c>
     </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>276</v>
+      </c>
+      <c r="E10" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="F10" s="25">
+        <v>-0.11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>259</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>278</v>
+      </c>
+      <c r="E11" s="25" t="s">
+        <v>277</v>
+      </c>
+      <c r="F11" s="25">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A50">

</xml_diff>

<commit_message>
#bugfix - single owner spreadsheet to match with SAM - debt closing cost and annual cost and LCOE calculation.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="11760"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,7 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -1293,7 +1298,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1328,7 +1333,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1539,7 +1544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
     </sheetView>
@@ -3984,7 +3989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated TODO - CSP hourly output variables reviewed.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -19,12 +14,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="282">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -869,6 +864,22 @@
   </si>
   <si>
     <t>Ty/Paul</t>
+  </si>
+  <si>
+    <r>
+      <t>Steve/</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mike</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1298,7 +1309,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1333,7 +1344,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1544,9 +1555,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I173"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A134" sqref="A134"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B127" sqref="B127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3623,13 +3634,13 @@
     </row>
     <row r="145" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A145" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B145" s="24" t="s">
         <v>234</v>
       </c>
       <c r="C145" t="s">
-        <v>127</v>
+        <v>281</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3989,7 +4000,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add user requests to ToDo spreadsheet
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="650" uniqueCount="286">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -881,12 +881,24 @@
       <t>Mike</t>
     </r>
   </si>
+  <si>
+    <t>Cavity receiver for tower models</t>
+  </si>
+  <si>
+    <t>Make source code available</t>
+  </si>
+  <si>
+    <t>User Requests (search forum for details)</t>
+  </si>
+  <si>
+    <t>Display input summary data on navigation menu buttons. Steve's alternative: Display summary from inputs browser in notes window.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -934,6 +946,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="0.79998168889431442"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1016,7 +1035,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1055,6 +1074,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1555,9 +1575,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I173"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B127" sqref="B127"/>
+      <selection pane="bottomLeft" activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3998,10 +4018,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4110,6 +4130,26 @@
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>271</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#bugfix single_owner.xlsx annual cost for LCOE calculation - match with SAM for all defaults and for PTC. Update SAM TODO.xlsx
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -14,12 +19,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="651" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="288">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -780,9 +785,6 @@
   </si>
   <si>
     <t>Debt fraction as input to DHF Single Owner and Leveraged Partnership flip</t>
-  </si>
-  <si>
-    <t>Issue with multiple processor simulaitons - see scripts from Mark stops around 2700 runs</t>
   </si>
   <si>
     <t>Financial Model warning and error messages for non-convergence</t>
@@ -895,6 +897,12 @@
   </si>
   <si>
     <t>Update the LPPA and LCOE metrics to make more sense to end users. Somehow.</t>
+  </si>
+  <si>
+    <t>Allow ui equations and callbacks to be exported to lk scripts for use with SDK (from Ty).</t>
+  </si>
+  <si>
+    <t>Issue with multiple processor simulations - see scripts from Mark stops around 2700 runs</t>
   </si>
 </sst>
 </file>
@@ -1332,7 +1340,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1367,7 +1375,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1578,9 +1586,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I173"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B132" sqref="B132"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B170" sqref="B170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2981,7 +2989,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="B89" s="19" t="s">
         <v>186</v>
@@ -3663,7 +3671,7 @@
         <v>234</v>
       </c>
       <c r="C145" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -3924,7 +3932,7 @@
         <v>198</v>
       </c>
       <c r="B169" s="24" t="s">
-        <v>253</v>
+        <v>287</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
@@ -3932,7 +3940,7 @@
         <v>198</v>
       </c>
       <c r="B170" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C170" t="s">
         <v>48</v>
@@ -3943,7 +3951,7 @@
         <v>198</v>
       </c>
       <c r="B171" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="172" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -3951,7 +3959,7 @@
         <v>57</v>
       </c>
       <c r="B172" s="24" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C172" t="s">
         <v>48</v>
@@ -3962,10 +3970,10 @@
         <v>57</v>
       </c>
       <c r="B173" s="24" t="s">
+        <v>278</v>
+      </c>
+      <c r="C173" t="s">
         <v>279</v>
-      </c>
-      <c r="C173" t="s">
-        <v>280</v>
       </c>
     </row>
   </sheetData>
@@ -4023,8 +4031,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4122,7 +4130,7 @@
         <v>221</v>
       </c>
       <c r="B18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -4132,32 +4140,37 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -4188,7 +4201,7 @@
         <v>207</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C1" s="26" t="s">
         <v>208</v>
@@ -4200,7 +4213,7 @@
         <v>210</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="U1" t="s">
         <v>211</v>
@@ -4211,7 +4224,7 @@
         <v>211</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
@@ -4232,7 +4245,7 @@
         <v>212</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C3" s="27" t="s">
         <v>216</v>
@@ -4253,7 +4266,7 @@
         <v>213</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C4" s="27" t="s">
         <v>219</v>
@@ -4269,19 +4282,19 @@
         <v>211</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E5" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F5" s="25">
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -4289,19 +4302,19 @@
         <v>211</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D6" s="25" t="s">
+        <v>262</v>
+      </c>
+      <c r="E6" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="F6" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="G6" s="25" t="s">
         <v>263</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>256</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -4309,13 +4322,13 @@
         <v>213</v>
       </c>
       <c r="C7" s="25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E7" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F7" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -4323,13 +4336,13 @@
         <v>213</v>
       </c>
       <c r="C8" s="25" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E8" s="25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F8" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -4337,19 +4350,19 @@
         <v>212</v>
       </c>
       <c r="B9" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="C9" s="25" t="s">
         <v>273</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="D9" s="25" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="F9" s="25" t="s">
         <v>274</v>
-      </c>
-      <c r="D9" s="25" t="s">
-        <v>274</v>
-      </c>
-      <c r="E9" s="25" t="s">
-        <v>273</v>
-      </c>
-      <c r="F9" s="25" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -4357,13 +4370,13 @@
         <v>211</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D10" s="25" t="s">
+        <v>275</v>
+      </c>
+      <c r="E10" s="25" t="s">
         <v>276</v>
-      </c>
-      <c r="E10" s="25" t="s">
-        <v>277</v>
       </c>
       <c r="F10" s="25">
         <v>-0.11</v>
@@ -4374,13 +4387,13 @@
         <v>211</v>
       </c>
       <c r="B11" s="25" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D11" s="25" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F11" s="25">
         <v>4.0000000000000001E-3</v>

</xml_diff>

<commit_message>
2015.1.26 internal release for testing
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="289">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -903,6 +903,9 @@
   </si>
   <si>
     <t>Issue with multiple processor simulations - see scripts from Mark stops around 2700 runs</t>
+  </si>
+  <si>
+    <t>Test mac updater for ssc.dylib and framework</t>
   </si>
 </sst>
 </file>
@@ -1584,11 +1587,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I173"/>
+  <dimension ref="A1:I174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B170" sqref="B170"/>
+      <selection pane="bottomLeft" activeCell="B180" sqref="B180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3974,6 +3977,17 @@
       </c>
       <c r="C173" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="B174" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="C174" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#bugfix - Save rate to file... dialog update per email from Paul and sam support 2/2/15
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="1"/>
   </bookViews>
@@ -14,12 +19,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="667" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="297">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -922,6 +927,9 @@
   </si>
   <si>
     <t>Improve weather file checker macro to handle Solar Prospector issues: https://sam.nrel.gov/node/69274#comment-2095</t>
+  </si>
+  <si>
+    <t>Open lk scripts from command line https://sam.nrel.gov/node/69289</t>
   </si>
 </sst>
 </file>
@@ -1359,7 +1367,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1394,7 +1402,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4092,10 +4100,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4249,6 +4257,11 @@
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shift+F5 does not appear to add variable-length data arrays to the lk script
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="318">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -982,6 +982,12 @@
   </si>
   <si>
     <t>Ty/Paul/Steve</t>
+  </si>
+  <si>
+    <t>Shift+F5 does not appear to save variable-length arrays to the .lk script</t>
+  </si>
+  <si>
+    <t>Nick</t>
   </si>
 </sst>
 </file>
@@ -1733,11 +1739,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I189"/>
+  <dimension ref="A1:I190"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A180" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A190" sqref="A190"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D197" sqref="D197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4290,6 +4296,17 @@
       </c>
       <c r="C189" t="s">
         <v>315</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A190" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B190" s="24" t="s">
+        <v>316</v>
+      </c>
+      <c r="C190" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added an "unsolved mysteries" tab to the To-Do list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
     <sheet name="Project Ideas" sheetId="2" r:id="rId2"/>
     <sheet name="SAM Variable Changes" sheetId="3" r:id="rId3"/>
+    <sheet name="Unsolved mysteries" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="319">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -988,6 +989,9 @@
   </si>
   <si>
     <t>Nick</t>
+  </si>
+  <si>
+    <t>Equations/UI mystery bug: total module area calculation doesn't update in the UI in 2014.11.24 release, but works fine in 2015.1.30 release</t>
   </si>
 </sst>
 </file>
@@ -1741,7 +1745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I190"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D197" sqref="D197"/>
     </sheetView>
@@ -4812,4 +4816,24 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
#update for Physical Trough ui variable names
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="327">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -992,6 +992,30 @@
   </si>
   <si>
     <t>Equations/UI mystery bug: total module area calculation doesn't update in the UI in 2014.11.24 release, but works fine in 2015.1.30 release</t>
+  </si>
+  <si>
+    <t>matrix</t>
+  </si>
+  <si>
+    <t>field_fl_props</t>
+  </si>
+  <si>
+    <t>user_defined_htf_array</t>
+  </si>
+  <si>
+    <t>Physical Trough Solar Field</t>
+  </si>
+  <si>
+    <t>Match cmods and tcs names</t>
+  </si>
+  <si>
+    <t>csp.dtr.tes.user_htf</t>
+  </si>
+  <si>
+    <t>store_fl_props</t>
+  </si>
+  <si>
+    <t>Physical Trough Thermal Storage</t>
   </si>
 </sst>
 </file>
@@ -4587,18 +4611,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U11"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="25" customWidth="1"/>
-    <col min="2" max="3" width="21.140625" style="25" customWidth="1"/>
+    <col min="2" max="2" width="21.140625" style="25" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="25" customWidth="1"/>
+    <col min="5" max="5" width="33" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="37.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -4804,6 +4829,52 @@
       </c>
       <c r="F11" s="25">
         <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>321</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>320</v>
+      </c>
+      <c r="E12" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>326</v>
+      </c>
+      <c r="F13" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>312</v>
       </c>
     </row>
   </sheetData>
@@ -4822,7 +4893,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
#update for MSLF ui variable names
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="723" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="329">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1016,6 +1016,12 @@
   </si>
   <si>
     <t>Physical Trough Thermal Storage</t>
+  </si>
+  <si>
+    <t>user_fluid</t>
+  </si>
+  <si>
+    <t>Molten Salt Linear Fresnel Storage</t>
   </si>
 </sst>
 </file>
@@ -4611,10 +4617,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4874,6 +4880,29 @@
         <v>323</v>
       </c>
       <c r="G13" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>319</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>327</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>325</v>
+      </c>
+      <c r="E14" s="25" t="s">
+        <v>328</v>
+      </c>
+      <c r="F14" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="G14" s="25" t="s">
         <v>312</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated ui variable mapping for IAM arrays in Physical trough model
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="365">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1022,6 +1022,114 @@
   </si>
   <si>
     <t>Molten Salt Linear Fresnel Storage</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam0_1</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam1_1</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam0_2</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam2_1</t>
+  </si>
+  <si>
+    <t>IAMs_1[0]</t>
+  </si>
+  <si>
+    <t>IAMs_1[1]</t>
+  </si>
+  <si>
+    <t>IAMs_1[2]</t>
+  </si>
+  <si>
+    <t>Physical Trough Collector Type 1</t>
+  </si>
+  <si>
+    <t>Physical Trough Collector Type 2</t>
+  </si>
+  <si>
+    <t>Physical Trough Collector Type 3</t>
+  </si>
+  <si>
+    <t>Allowing table/array of IAM coefficients as inputs</t>
+  </si>
+  <si>
+    <t>Ty      If IAM beceoms available in User Library, may want to make values array instead of set at 3 variables</t>
+  </si>
+  <si>
+    <t>IamF0</t>
+  </si>
+  <si>
+    <t>Physical Trough Collector Header</t>
+  </si>
+  <si>
+    <t>IAM_matrix</t>
+  </si>
+  <si>
+    <t>combining collector IAM coef. Arrays into 1 output matrix</t>
+  </si>
+  <si>
+    <t>IamF1</t>
+  </si>
+  <si>
+    <t>IamF2</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam1_2</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam2_2</t>
+  </si>
+  <si>
+    <t>IAMs_2[0]</t>
+  </si>
+  <si>
+    <t>IAMs_2[1]</t>
+  </si>
+  <si>
+    <t>IAMs_2[2]</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam0_3</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam1_3</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam2_3</t>
+  </si>
+  <si>
+    <t>IAMs_3[0]</t>
+  </si>
+  <si>
+    <t>IAMs_3[1]</t>
+  </si>
+  <si>
+    <t>IAMs_3[2]</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam0_4</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam1_4</t>
+  </si>
+  <si>
+    <t>csp_dtr_sca_iam2_4</t>
+  </si>
+  <si>
+    <t>IAMs_4[0]</t>
+  </si>
+  <si>
+    <t>IAMs_4[1]</t>
+  </si>
+  <si>
+    <t>IAMs_4[2]</t>
+  </si>
+  <si>
+    <t>Physical Trough Collector Type 4</t>
   </si>
 </sst>
 </file>
@@ -1424,14 +1532,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:colOff>200025</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1441,7 +1549,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10782300" y="1724025"/>
+          <a:off x="11953875" y="4010025"/>
           <a:ext cx="3990975" cy="1581150"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -4617,10 +4725,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U14"/>
+  <dimension ref="A1:U29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4630,7 +4738,7 @@
     <col min="3" max="3" width="22.28515625" style="25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="37.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51" style="25" customWidth="1"/>
     <col min="21" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4906,9 +5014,354 @@
         <v>312</v>
       </c>
     </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>329</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>333</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="F15" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B16" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>334</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="F16" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>332</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>335</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>336</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B18" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>331</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="F18" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C20" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="F20" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C21" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="F21" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B22" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>356</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B23" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C23" s="25" t="s">
+        <v>354</v>
+      </c>
+      <c r="D23" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B26" s="25" t="s">
+        <v>258</v>
+      </c>
+      <c r="C26" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="E26" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B27" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="C27" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="D27" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="E27" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B28" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="C28" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="D28" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="E28" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="F28" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="B29" s="25" t="s">
+        <v>257</v>
+      </c>
+      <c r="C29" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A50">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A58">
       <formula1>Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
update TODO list to show all changes to SAMnt and SSC since 2015.1.30 release
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="451">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1142,6 +1142,254 @@
   </si>
   <si>
     <t>PPA price by year, e.g., 10 PPA agreement at one price, followed by 25 years at another price. Could be implemented as schedule for ppa escalation?</t>
+  </si>
+  <si>
+    <t>SVN</t>
+  </si>
+  <si>
+    <t>1600</t>
+  </si>
+  <si>
+    <t>1595</t>
+  </si>
+  <si>
+    <t>1594</t>
+  </si>
+  <si>
+    <t>1592,</t>
+  </si>
+  <si>
+    <t>1597</t>
+  </si>
+  <si>
+    <t>1596</t>
+  </si>
+  <si>
+    <t>Update CSP (physical trough only?) tank volume equation to include dt_hot and dt_cold (SAMnt)</t>
+  </si>
+  <si>
+    <t>Fix physical trough collector library so IAM coefficients appear in table (SAMnt)</t>
+  </si>
+  <si>
+    <t>Convert physical trough IAM inputs from individual varaibles to array (SAMnt)</t>
+  </si>
+  <si>
+    <t>Fix physical trough receiver library entry for Royal Tech receiver (SAMnt)</t>
+  </si>
+  <si>
+    <t>HCPV costs available for parametrics, make HCPV cost group names consistent (SAMnt)</t>
+  </si>
+  <si>
+    <t>Change CSP Storage UI HX derate to HX exergetic efficiency and update equations (SAMnt)</t>
+  </si>
+  <si>
+    <t>#defaults updated for user defined HTFs, storage calculations changes, and array-based IAMs (SAMnt)</t>
+  </si>
+  <si>
+    <t>1589,1591,1590,1589</t>
+  </si>
+  <si>
+    <t>Excel exchange fixes to work with .xlsm, update SAM inputs with values from Excel (SAMnt)</t>
+  </si>
+  <si>
+    <t>added SSC callback function and then on_change() functions that reference the callback in both Solar Field and TES pages to test HTF equivalence. Now setting 'is_hx' in that function, and "hx_derate" is dependent on "is_hx"</t>
+  </si>
+  <si>
+    <t>1585</t>
+  </si>
+  <si>
+    <t>1586</t>
+  </si>
+  <si>
+    <t>changed ui names to match ssc and tcs names. documented in SAM TODO</t>
+  </si>
+  <si>
+    <t>1582</t>
+  </si>
+  <si>
+    <t>#bugfix correct mslf storage tank diameter UI equation</t>
+  </si>
+  <si>
+    <t>Fixed typo for Santa Fe NM weather file (was Sata Fe and therefore didn't show up when searching)</t>
+  </si>
+  <si>
+    <t>1575</t>
+  </si>
+  <si>
+    <t>1576</t>
+  </si>
+  <si>
+    <t>#bugfix rescom send to excel workbook fix error in property tax assessed value equation (forgot to divide percentage by 100). does not affect cash flow results in workbook.</t>
+  </si>
+  <si>
+    <t>Added red message warning that inverter had no voltage limits, and hence only one module would be used</t>
+  </si>
+  <si>
+    <t>1567,1614</t>
+  </si>
+  <si>
+    <t>1569</t>
+  </si>
+  <si>
+    <t>#bugfix UI changes for custom HTF in physical trough, empirical trough, salt fresnel, and salt tower: Disable edit button for library htf, disable min/max operating temp calculated values for custom htf, update Help topics accordingly.</t>
+  </si>
+  <si>
+    <t>1566</t>
+  </si>
+  <si>
+    <t>#bugfix - project update to fix runtime error on Vista. Tested on Vista and Windows 8.</t>
+  </si>
+  <si>
+    <t>I think this is already in the trunk</t>
+  </si>
+  <si>
+    <t>1564</t>
+  </si>
+  <si>
+    <t>#bugfix shorten registration text so registration information window is less than 600px high -- was preventing people with small screens from registering</t>
+  </si>
+  <si>
+    <t>1559,1554</t>
+  </si>
+  <si>
+    <t>rename CSP user HTF matrix</t>
+  </si>
+  <si>
+    <t>1557,1556,1555</t>
+  </si>
+  <si>
+    <t>#bugfix pv report vmp value (change old variable name to new one)</t>
+  </si>
+  <si>
+    <t>1550</t>
+  </si>
+  <si>
+    <t>#new - subarray shading applied based on group number for mxh and diffuse shading.
+remove beta expiration messages.
+testing Vista fix for debug processing.</t>
+  </si>
+  <si>
+    <t>1549</t>
+  </si>
+  <si>
+    <t>Mac build updates</t>
+  </si>
+  <si>
+    <t>1536</t>
+  </si>
+  <si>
+    <t>Stochastic update to check folder location on Mac</t>
+  </si>
+  <si>
+    <t>1535</t>
+  </si>
+  <si>
+    <t>#ui - update hourly edit dialog to show time step before other buttons for improved work flow as requested by Paul 2/10/15</t>
+  </si>
+  <si>
+    <t>1529</t>
+  </si>
+  <si>
+    <t>#bugfix fix issue with pv report template with cec user specified module and for weather files with no ghi data</t>
+  </si>
+  <si>
+    <t>1525</t>
+  </si>
+  <si>
+    <t>#ui update dview labels for load time series variables to be consistent with new ssc output variable labels</t>
+  </si>
+  <si>
+    <t>1524</t>
+  </si>
+  <si>
+    <t>#bugfix generic system cost inputs, fix issues with parametric and group variable properties</t>
+  </si>
+  <si>
+    <t>1518</t>
+  </si>
+  <si>
+    <t>#bugfix - Save rate to file... dialog update per email from Paul and sam support 2/2/15</t>
+  </si>
+  <si>
+    <t>1517</t>
+  </si>
+  <si>
+    <t>2595,2594,2593,2592</t>
+  </si>
+  <si>
+    <t>deleted old IAM array TCS_INPUTS and code, updated to accept IAMs reported from UI as a variably-sized matrix instead of fixed, syntax update</t>
+  </si>
+  <si>
+    <t>Custom HTF, HX fixes</t>
+  </si>
+  <si>
+    <t>2567-2588</t>
+  </si>
+  <si>
+    <t>Fixed a bug in Equation 21 from the 2014 wind technical manual. #bugfix</t>
+  </si>
+  <si>
+    <t>2563</t>
+  </si>
+  <si>
+    <t>fixed serious bug: sf_type not defined in compute module. this resulted in the solver using the incorrect solution mode and setting the field inlet to the design temperature rather than a recirculated temperature during startup. This resulted in the system "losing" internal energy between timesteps and an artificially low annual energy output. Also, freeze protection energy was not reported in the previous version and is here.</t>
+  </si>
+  <si>
+    <t>2558,2559,2560</t>
+  </si>
+  <si>
+    <t>#bugfix - weather file reader divide by zero if number of records is zero - reported by Paul 2/20/15</t>
+  </si>
+  <si>
+    <t>2557</t>
+  </si>
+  <si>
+    <t>Update tckernel - add set_unit_value_ssc_... functions to translate from tcs to ssc names per Ty</t>
+  </si>
+  <si>
+    <t>2556</t>
+  </si>
+  <si>
+    <t>improved error checking on user-defined HTF, corrected to pass UI user defined field fluid property matrix to correct TCS types</t>
+  </si>
+  <si>
+    <t>2543-2553</t>
+  </si>
+  <si>
+    <t>#new - overloaded set_unit_value_ssc_matrix that take an ssc input matrix of and sets to a tcs matrix with a different name as requested by Ty 2/18/15. Example in cmod_tcsmolten_salt.cpp line 969</t>
+  </si>
+  <si>
+    <t>2554</t>
+  </si>
+  <si>
+    <t>deleted old store_fl_props code</t>
+  </si>
+  <si>
+    <t>2555</t>
+  </si>
+  <si>
+    <t>#ui update load/utility rate output variable names</t>
+  </si>
+  <si>
+    <t>2532</t>
+  </si>
+  <si>
+    <t>#ui update labels for electric load-related output variables</t>
+  </si>
+  <si>
+    <t>2517</t>
+  </si>
+  <si>
+    <t>#new - add utility rate output to show peak demand in hour occurs on a TOU period per month basis as requested by Paul 2/6/15</t>
+  </si>
+  <si>
+    <t>2516</t>
+  </si>
+  <si>
+    <t>#bugfix - year one sales purchases include TOU demand charges per email from Paul 2/6/15</t>
+  </si>
+  <si>
+    <t>2515</t>
   </si>
 </sst>
 </file>
@@ -1285,7 +1533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1325,6 +1573,8 @@
     <xf numFmtId="0" fontId="3" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1893,11 +2143,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I192"/>
+  <dimension ref="A1:I232"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A171" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A193" sqref="A193"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B233" sqref="B233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1905,7 +2155,7 @@
     <col min="1" max="1" width="12.28515625" style="20" customWidth="1"/>
     <col min="2" max="2" width="102.85546875" style="24" customWidth="1"/>
     <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" style="4" customWidth="1"/>
     <col min="5" max="5" width="27.5703125" customWidth="1"/>
     <col min="6" max="6" width="47.85546875" customWidth="1"/>
   </cols>
@@ -4335,7 +4585,9 @@
       </c>
       <c r="B179" s="21"/>
       <c r="C179" s="21"/>
-      <c r="D179" s="21"/>
+      <c r="D179" s="21" t="s">
+        <v>369</v>
+      </c>
       <c r="E179" s="21"/>
       <c r="F179" s="21"/>
     </row>
@@ -4483,6 +4735,569 @@
       </c>
       <c r="C192" t="s">
         <v>367</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A193" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B193" s="24" t="s">
+        <v>377</v>
+      </c>
+      <c r="C193" t="s">
+        <v>71</v>
+      </c>
+      <c r="D193" s="29" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A194" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B194" s="24" t="s">
+        <v>378</v>
+      </c>
+      <c r="C194" t="s">
+        <v>312</v>
+      </c>
+      <c r="D194" s="30" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A195" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B195" s="24" t="s">
+        <v>379</v>
+      </c>
+      <c r="C195" t="s">
+        <v>71</v>
+      </c>
+      <c r="D195" s="29" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A196" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B196" s="24" t="s">
+        <v>380</v>
+      </c>
+      <c r="C196" t="s">
+        <v>71</v>
+      </c>
+      <c r="D196" s="29" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A197" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B197" s="24" t="s">
+        <v>376</v>
+      </c>
+      <c r="C197" t="s">
+        <v>312</v>
+      </c>
+      <c r="D197" s="29" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A198" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B198" s="24" t="s">
+        <v>381</v>
+      </c>
+      <c r="C198" t="s">
+        <v>312</v>
+      </c>
+      <c r="D198" s="29" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A199" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B199" s="24" t="s">
+        <v>382</v>
+      </c>
+      <c r="C199" t="s">
+        <v>312</v>
+      </c>
+      <c r="D199" s="29" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A200" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B200" s="24" t="s">
+        <v>384</v>
+      </c>
+      <c r="C200" t="s">
+        <v>48</v>
+      </c>
+      <c r="D200" s="29" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A201" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B201" s="24" t="s">
+        <v>385</v>
+      </c>
+      <c r="C201" t="s">
+        <v>312</v>
+      </c>
+      <c r="D201" s="29" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A202" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B202" s="24" t="s">
+        <v>388</v>
+      </c>
+      <c r="C202" t="s">
+        <v>312</v>
+      </c>
+      <c r="D202" s="29" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A203" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B203" s="24" t="s">
+        <v>390</v>
+      </c>
+      <c r="C203" t="s">
+        <v>71</v>
+      </c>
+      <c r="D203" s="29" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A204" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B204" s="24" t="s">
+        <v>391</v>
+      </c>
+      <c r="C204" t="s">
+        <v>46</v>
+      </c>
+      <c r="D204" s="29" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A205" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B205" s="24" t="s">
+        <v>394</v>
+      </c>
+      <c r="C205" t="s">
+        <v>71</v>
+      </c>
+      <c r="D205" s="29" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A206" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B206" s="24" t="s">
+        <v>395</v>
+      </c>
+      <c r="C206" t="s">
+        <v>317</v>
+      </c>
+      <c r="D206" s="29" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A207" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B207" s="24" t="s">
+        <v>398</v>
+      </c>
+      <c r="C207" t="s">
+        <v>71</v>
+      </c>
+      <c r="D207" s="29" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A208" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B208" s="24" t="s">
+        <v>400</v>
+      </c>
+      <c r="C208" t="s">
+        <v>48</v>
+      </c>
+      <c r="D208" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="E208" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A209" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B209" s="24" t="s">
+        <v>403</v>
+      </c>
+      <c r="C209" t="s">
+        <v>231</v>
+      </c>
+      <c r="D209" s="29" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B210" s="24" t="s">
+        <v>405</v>
+      </c>
+      <c r="C210" t="s">
+        <v>312</v>
+      </c>
+      <c r="D210" s="29" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B211" s="24" t="s">
+        <v>407</v>
+      </c>
+      <c r="C211" t="s">
+        <v>71</v>
+      </c>
+      <c r="D211" s="29" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="212" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A212" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B212" s="24" t="s">
+        <v>409</v>
+      </c>
+      <c r="C212" t="s">
+        <v>48</v>
+      </c>
+      <c r="D212" s="29" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B213" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="C213" t="s">
+        <v>48</v>
+      </c>
+      <c r="D213" s="29" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B214" s="24" t="s">
+        <v>413</v>
+      </c>
+      <c r="C214" t="s">
+        <v>48</v>
+      </c>
+      <c r="D214" s="29" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B215" s="24" t="s">
+        <v>415</v>
+      </c>
+      <c r="C215" t="s">
+        <v>48</v>
+      </c>
+      <c r="D215" s="29" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B216" s="24" t="s">
+        <v>417</v>
+      </c>
+      <c r="C216" t="s">
+        <v>71</v>
+      </c>
+      <c r="D216" s="29" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A217" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B217" s="24" t="s">
+        <v>419</v>
+      </c>
+      <c r="C217" t="s">
+        <v>71</v>
+      </c>
+      <c r="D217" s="29" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B218" s="24" t="s">
+        <v>421</v>
+      </c>
+      <c r="C218" t="s">
+        <v>71</v>
+      </c>
+      <c r="D218" s="29" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B219" s="24" t="s">
+        <v>423</v>
+      </c>
+      <c r="C219" t="s">
+        <v>48</v>
+      </c>
+      <c r="D219" s="29" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A220" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B220" s="24" t="s">
+        <v>426</v>
+      </c>
+      <c r="C220" t="s">
+        <v>312</v>
+      </c>
+      <c r="D220" s="29" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B221" s="24" t="s">
+        <v>427</v>
+      </c>
+      <c r="C221" t="s">
+        <v>312</v>
+      </c>
+      <c r="D221" s="29" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B222" s="24" t="s">
+        <v>429</v>
+      </c>
+      <c r="C222" t="s">
+        <v>46</v>
+      </c>
+      <c r="D222" s="29" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B223" s="24" t="s">
+        <v>431</v>
+      </c>
+      <c r="C223" t="s">
+        <v>312</v>
+      </c>
+      <c r="D223" s="29" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B224" s="24" t="s">
+        <v>433</v>
+      </c>
+      <c r="C224" t="s">
+        <v>48</v>
+      </c>
+      <c r="D224" s="29" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A225" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B225" s="24" t="s">
+        <v>435</v>
+      </c>
+      <c r="C225" t="s">
+        <v>48</v>
+      </c>
+      <c r="D225" s="29" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="226" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A226" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B226" s="24" t="s">
+        <v>437</v>
+      </c>
+      <c r="C226" t="s">
+        <v>312</v>
+      </c>
+      <c r="D226" s="29" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B227" s="24" t="s">
+        <v>439</v>
+      </c>
+      <c r="C227" t="s">
+        <v>48</v>
+      </c>
+      <c r="D227" s="29" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B228" s="24" t="s">
+        <v>441</v>
+      </c>
+      <c r="C228" t="s">
+        <v>312</v>
+      </c>
+      <c r="D228" s="29" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B229" s="24" t="s">
+        <v>443</v>
+      </c>
+      <c r="C229" t="s">
+        <v>71</v>
+      </c>
+      <c r="D229" s="29" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B230" s="24" t="s">
+        <v>445</v>
+      </c>
+      <c r="C230" t="s">
+        <v>71</v>
+      </c>
+      <c r="D230" s="29" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B231" s="24" t="s">
+        <v>447</v>
+      </c>
+      <c r="C231" t="s">
+        <v>48</v>
+      </c>
+      <c r="D231" s="29" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B232" s="24" t="s">
+        <v>449</v>
+      </c>
+      <c r="C232" t="s">
+        <v>48</v>
+      </c>
+      <c r="D232" s="29" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -4565,7 +5380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update TODO List Start on calculated value display in input browser.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
   </bookViews>
@@ -15,12 +20,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1005" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1008" uniqueCount="453">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1144,9 +1149,6 @@
     <t>PPA price by year, e.g., 10 PPA agreement at one price, followed by 25 years at another price. Could be implemented as schedule for ppa escalation?</t>
   </si>
   <si>
-    <t>SVN</t>
-  </si>
-  <si>
     <t>1600</t>
   </si>
   <si>
@@ -1393,6 +1395,12 @@
   </si>
   <si>
     <t>Move to trunk for update (yes/no)</t>
+  </si>
+  <si>
+    <t>SVN (SAMnt 1000, ssc 2000)</t>
+  </si>
+  <si>
+    <t>#bugfix - dispatch_calculations class in common_financial.cpp - update to properly handle ppa and degradation inputs and check sizes. Fixes bug reported by Paul 3/12/15</t>
   </si>
 </sst>
 </file>
@@ -1902,7 +1910,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1937,7 +1945,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2146,11 +2154,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I232"/>
+  <dimension ref="A1:I233"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A177" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E179" sqref="E179"/>
+      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D224" sqref="D224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4589,10 +4597,10 @@
       <c r="B179" s="21"/>
       <c r="C179" s="21"/>
       <c r="D179" s="21" t="s">
-        <v>369</v>
+        <v>451</v>
       </c>
       <c r="E179" s="21" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="F179" s="21"/>
     </row>
@@ -4747,13 +4755,13 @@
         <v>57</v>
       </c>
       <c r="B193" s="24" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C193" t="s">
         <v>71</v>
       </c>
       <c r="D193" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -4761,13 +4769,13 @@
         <v>57</v>
       </c>
       <c r="B194" s="24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C194" t="s">
         <v>312</v>
       </c>
       <c r="D194" s="30" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -4775,13 +4783,13 @@
         <v>57</v>
       </c>
       <c r="B195" s="24" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C195" t="s">
         <v>71</v>
       </c>
       <c r="D195" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -4789,13 +4797,13 @@
         <v>57</v>
       </c>
       <c r="B196" s="24" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C196" t="s">
         <v>71</v>
       </c>
       <c r="D196" s="29" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -4803,13 +4811,13 @@
         <v>57</v>
       </c>
       <c r="B197" s="24" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C197" t="s">
         <v>312</v>
       </c>
       <c r="D197" s="29" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -4817,13 +4825,13 @@
         <v>57</v>
       </c>
       <c r="B198" s="24" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C198" t="s">
         <v>312</v>
       </c>
       <c r="D198" s="29" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -4831,13 +4839,13 @@
         <v>57</v>
       </c>
       <c r="B199" s="24" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C199" t="s">
         <v>312</v>
       </c>
       <c r="D199" s="29" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -4845,13 +4853,13 @@
         <v>57</v>
       </c>
       <c r="B200" s="24" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C200" t="s">
         <v>48</v>
       </c>
       <c r="D200" s="29" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -4859,13 +4867,13 @@
         <v>57</v>
       </c>
       <c r="B201" s="24" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C201" t="s">
         <v>312</v>
       </c>
       <c r="D201" s="29" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -4873,13 +4881,13 @@
         <v>57</v>
       </c>
       <c r="B202" s="24" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C202" t="s">
         <v>312</v>
       </c>
       <c r="D202" s="29" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -4887,13 +4895,13 @@
         <v>57</v>
       </c>
       <c r="B203" s="24" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="C203" t="s">
         <v>71</v>
       </c>
       <c r="D203" s="29" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -4901,13 +4909,13 @@
         <v>57</v>
       </c>
       <c r="B204" s="24" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C204" t="s">
         <v>46</v>
       </c>
       <c r="D204" s="29" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -4915,13 +4923,13 @@
         <v>57</v>
       </c>
       <c r="B205" s="24" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C205" t="s">
         <v>71</v>
       </c>
       <c r="D205" s="29" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -4929,13 +4937,13 @@
         <v>57</v>
       </c>
       <c r="B206" s="24" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C206" t="s">
         <v>317</v>
       </c>
       <c r="D206" s="29" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -4943,13 +4951,13 @@
         <v>57</v>
       </c>
       <c r="B207" s="24" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C207" t="s">
         <v>71</v>
       </c>
       <c r="D207" s="29" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -4957,16 +4965,16 @@
         <v>57</v>
       </c>
       <c r="B208" s="24" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C208" t="s">
         <v>48</v>
       </c>
       <c r="D208" s="29" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E208" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="209" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -4974,13 +4982,13 @@
         <v>57</v>
       </c>
       <c r="B209" s="24" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C209" t="s">
         <v>231</v>
       </c>
       <c r="D209" s="29" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
@@ -4988,13 +4996,13 @@
         <v>57</v>
       </c>
       <c r="B210" s="24" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C210" t="s">
         <v>312</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
@@ -5002,13 +5010,13 @@
         <v>57</v>
       </c>
       <c r="B211" s="24" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C211" t="s">
         <v>71</v>
       </c>
       <c r="D211" s="29" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="212" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -5016,13 +5024,13 @@
         <v>57</v>
       </c>
       <c r="B212" s="24" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C212" t="s">
         <v>48</v>
       </c>
       <c r="D212" s="29" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
@@ -5030,13 +5038,13 @@
         <v>57</v>
       </c>
       <c r="B213" s="24" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C213" t="s">
         <v>48</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
@@ -5044,13 +5052,13 @@
         <v>57</v>
       </c>
       <c r="B214" s="24" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C214" t="s">
         <v>48</v>
       </c>
       <c r="D214" s="29" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
@@ -5058,13 +5066,13 @@
         <v>57</v>
       </c>
       <c r="B215" s="24" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C215" t="s">
         <v>48</v>
       </c>
       <c r="D215" s="29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
@@ -5072,13 +5080,13 @@
         <v>57</v>
       </c>
       <c r="B216" s="24" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C216" t="s">
         <v>71</v>
       </c>
       <c r="D216" s="29" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="217" spans="1:4" x14ac:dyDescent="0.25">
@@ -5086,13 +5094,13 @@
         <v>57</v>
       </c>
       <c r="B217" s="24" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C217" t="s">
         <v>71</v>
       </c>
       <c r="D217" s="29" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
@@ -5100,13 +5108,13 @@
         <v>57</v>
       </c>
       <c r="B218" s="24" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C218" t="s">
         <v>71</v>
       </c>
       <c r="D218" s="29" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
@@ -5114,13 +5122,13 @@
         <v>57</v>
       </c>
       <c r="B219" s="24" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C219" t="s">
         <v>48</v>
       </c>
       <c r="D219" s="29" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5128,13 +5136,13 @@
         <v>57</v>
       </c>
       <c r="B220" s="24" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C220" t="s">
         <v>312</v>
       </c>
       <c r="D220" s="29" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
@@ -5142,13 +5150,13 @@
         <v>57</v>
       </c>
       <c r="B221" s="24" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C221" t="s">
         <v>312</v>
       </c>
       <c r="D221" s="29" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
@@ -5156,27 +5164,27 @@
         <v>57</v>
       </c>
       <c r="B222" s="24" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="C222" t="s">
         <v>46</v>
       </c>
       <c r="D222" s="29" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="223" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A223" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B223" s="24" t="s">
         <v>430</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B223" s="24" t="s">
-        <v>431</v>
       </c>
       <c r="C223" t="s">
         <v>312</v>
       </c>
       <c r="D223" s="29" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
@@ -5184,13 +5192,13 @@
         <v>57</v>
       </c>
       <c r="B224" s="24" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="C224" t="s">
         <v>48</v>
       </c>
       <c r="D224" s="29" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="225" spans="1:4" x14ac:dyDescent="0.25">
@@ -5198,13 +5206,13 @@
         <v>57</v>
       </c>
       <c r="B225" s="24" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C225" t="s">
         <v>48</v>
       </c>
       <c r="D225" s="29" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="226" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -5212,27 +5220,27 @@
         <v>57</v>
       </c>
       <c r="B226" s="24" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C226" t="s">
         <v>312</v>
       </c>
       <c r="D226" s="29" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="227" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A227" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B227" s="24" t="s">
         <v>438</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B227" s="24" t="s">
-        <v>439</v>
       </c>
       <c r="C227" t="s">
         <v>48</v>
       </c>
       <c r="D227" s="29" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
@@ -5240,13 +5248,13 @@
         <v>57</v>
       </c>
       <c r="B228" s="24" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C228" t="s">
         <v>312</v>
       </c>
       <c r="D228" s="29" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
@@ -5254,13 +5262,13 @@
         <v>57</v>
       </c>
       <c r="B229" s="24" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C229" t="s">
         <v>71</v>
       </c>
       <c r="D229" s="29" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
@@ -5268,27 +5276,27 @@
         <v>57</v>
       </c>
       <c r="B230" s="24" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C230" t="s">
         <v>71</v>
       </c>
       <c r="D230" s="29" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="231" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A231" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B231" s="24" t="s">
         <v>446</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B231" s="24" t="s">
-        <v>447</v>
       </c>
       <c r="C231" t="s">
         <v>48</v>
       </c>
       <c r="D231" s="29" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
@@ -5296,13 +5304,27 @@
         <v>57</v>
       </c>
       <c r="B232" s="24" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C232" t="s">
         <v>48</v>
       </c>
       <c r="D232" s="29" t="s">
-        <v>450</v>
+        <v>449</v>
+      </c>
+    </row>
+    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A233" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B233" s="24" t="s">
+        <v>452</v>
+      </c>
+      <c r="C233" t="s">
+        <v>48</v>
+      </c>
+      <c r="D233" s="4">
+        <v>2606</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to-do list with Yes/No list of what should go in patch
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1025" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="464">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1237,9 +1237,6 @@
     <t>#bugfix - project update to fix runtime error on Vista. Tested on Vista and Windows 8.</t>
   </si>
   <si>
-    <t>I think this is already in the trunk</t>
-  </si>
-  <si>
     <t>1564</t>
   </si>
   <si>
@@ -1416,7 +1413,22 @@
     <t>#ui add empirical trough custom storage HTF option to make it possible to model direct storage with a custom field HTF</t>
   </si>
   <si>
-    <t>No longer appears to be an issue</t>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>(below)</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>This may already be in the trunk.</t>
+  </si>
+  <si>
+    <t>Fix remaining bug with Wind CSM</t>
+  </si>
+  <si>
+    <t>maybe</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1618,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="22">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -2170,11 +2203,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I238"/>
+  <dimension ref="A1:I239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A173" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E185" sqref="E185"/>
+      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A191" sqref="A191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4613,10 +4646,10 @@
       <c r="B179" s="21"/>
       <c r="C179" s="21"/>
       <c r="D179" s="21" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E179" s="21" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F179" s="21"/>
     </row>
@@ -4629,6 +4662,9 @@
       </c>
       <c r="C180" t="s">
         <v>279</v>
+      </c>
+      <c r="E180" s="4" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
@@ -4641,6 +4677,9 @@
       <c r="C181" t="s">
         <v>77</v>
       </c>
+      <c r="E181" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A182" s="20" t="s">
@@ -4652,6 +4691,9 @@
       <c r="C182" t="s">
         <v>231</v>
       </c>
+      <c r="E182" t="s">
+        <v>463</v>
+      </c>
       <c r="F182" t="s">
         <v>304</v>
       </c>
@@ -4666,6 +4708,9 @@
       <c r="C183" t="s">
         <v>48</v>
       </c>
+      <c r="E183" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A184" s="20" t="s">
@@ -4677,6 +4722,9 @@
       <c r="C184" t="s">
         <v>71</v>
       </c>
+      <c r="E184" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A185" s="20" t="s">
@@ -4688,6 +4736,9 @@
       <c r="C185" t="s">
         <v>71</v>
       </c>
+      <c r="E185" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A186" s="20" t="s">
@@ -4699,6 +4750,9 @@
       <c r="C186" t="s">
         <v>71</v>
       </c>
+      <c r="E186" t="s">
+        <v>459</v>
+      </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A187" s="20" t="s">
@@ -4710,6 +4764,9 @@
       <c r="C187" t="s">
         <v>71</v>
       </c>
+      <c r="E187" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="20" t="s">
@@ -4721,6 +4778,9 @@
       <c r="C188" t="s">
         <v>312</v>
       </c>
+      <c r="E188" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="s">
@@ -4732,6 +4792,9 @@
       <c r="C189" t="s">
         <v>315</v>
       </c>
+      <c r="E189" t="s">
+        <v>458</v>
+      </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A190" s="20" t="s">
@@ -4743,8 +4806,8 @@
       <c r="C190" t="s">
         <v>317</v>
       </c>
-      <c r="F190" t="s">
-        <v>459</v>
+      <c r="E190" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4757,6 +4820,9 @@
       <c r="C191" t="s">
         <v>48</v>
       </c>
+      <c r="E191" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="20" t="s">
@@ -4768,8 +4834,11 @@
       <c r="C192" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E192" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A193" s="20" t="s">
         <v>57</v>
       </c>
@@ -4782,8 +4851,11 @@
       <c r="D193" s="29" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E193" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A194" s="20" t="s">
         <v>57</v>
       </c>
@@ -4796,8 +4868,11 @@
       <c r="D194" s="30" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E194" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A195" s="20" t="s">
         <v>57</v>
       </c>
@@ -4810,8 +4885,11 @@
       <c r="D195" s="29" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E195" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A196" s="20" t="s">
         <v>57</v>
       </c>
@@ -4824,8 +4902,11 @@
       <c r="D196" s="29" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E196" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A197" s="20" t="s">
         <v>57</v>
       </c>
@@ -4838,8 +4919,11 @@
       <c r="D197" s="29" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E197" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="20" t="s">
         <v>57</v>
       </c>
@@ -4852,8 +4936,11 @@
       <c r="D198" s="29" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E198" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A199" s="20" t="s">
         <v>57</v>
       </c>
@@ -4866,8 +4953,11 @@
       <c r="D199" s="29" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E199" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A200" s="20" t="s">
         <v>57</v>
       </c>
@@ -4880,8 +4970,11 @@
       <c r="D200" s="29" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="201" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E200" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A201" s="20" t="s">
         <v>57</v>
       </c>
@@ -4894,8 +4987,11 @@
       <c r="D201" s="29" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E201" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A202" s="20" t="s">
         <v>57</v>
       </c>
@@ -4908,8 +5004,11 @@
       <c r="D202" s="29" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E202" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A203" s="20" t="s">
         <v>57</v>
       </c>
@@ -4922,8 +5021,11 @@
       <c r="D203" s="29" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E203" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="20" t="s">
         <v>57</v>
       </c>
@@ -4936,8 +5038,11 @@
       <c r="D204" s="29" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="205" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="E204" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A205" s="20" t="s">
         <v>57</v>
       </c>
@@ -4950,8 +5055,11 @@
       <c r="D205" s="29" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E205" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A206" s="20" t="s">
         <v>57</v>
       </c>
@@ -4964,8 +5072,11 @@
       <c r="D206" s="29" t="s">
         <v>395</v>
       </c>
-    </row>
-    <row r="207" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E206" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="20" t="s">
         <v>57</v>
       </c>
@@ -4978,8 +5089,11 @@
       <c r="D207" s="29" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E207" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A208" s="20" t="s">
         <v>57</v>
       </c>
@@ -4990,354 +5104,429 @@
         <v>48</v>
       </c>
       <c r="D208" s="29" t="s">
+        <v>400</v>
+      </c>
+      <c r="E208" t="s">
+        <v>57</v>
+      </c>
+      <c r="F208" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A209" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B209" s="24" t="s">
         <v>401</v>
-      </c>
-      <c r="E208" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A209" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B209" s="24" t="s">
-        <v>402</v>
       </c>
       <c r="C209" t="s">
         <v>231</v>
       </c>
       <c r="D209" s="29" t="s">
+        <v>402</v>
+      </c>
+      <c r="E209" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A210" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B210" s="24" t="s">
         <v>403</v>
-      </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B210" s="24" t="s">
-        <v>404</v>
       </c>
       <c r="C210" t="s">
         <v>312</v>
       </c>
       <c r="D210" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="E210" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A211" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B211" s="24" t="s">
         <v>405</v>
-      </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B211" s="24" t="s">
-        <v>406</v>
       </c>
       <c r="C211" t="s">
         <v>71</v>
       </c>
       <c r="D211" s="29" t="s">
+        <v>406</v>
+      </c>
+      <c r="E211" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A212" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B212" s="24" t="s">
         <v>407</v>
-      </c>
-    </row>
-    <row r="212" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A212" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B212" s="24" t="s">
-        <v>408</v>
       </c>
       <c r="C212" t="s">
         <v>48</v>
       </c>
       <c r="D212" s="29" t="s">
+        <v>408</v>
+      </c>
+      <c r="E212" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A213" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B213" s="24" t="s">
         <v>409</v>
-      </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B213" s="24" t="s">
-        <v>410</v>
       </c>
       <c r="C213" t="s">
         <v>48</v>
       </c>
       <c r="D213" s="29" t="s">
+        <v>410</v>
+      </c>
+      <c r="E213" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A214" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B214" s="24" t="s">
         <v>411</v>
-      </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B214" s="24" t="s">
-        <v>412</v>
       </c>
       <c r="C214" t="s">
         <v>48</v>
       </c>
       <c r="D214" s="29" t="s">
+        <v>412</v>
+      </c>
+      <c r="E214" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A215" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B215" s="24" t="s">
         <v>413</v>
-      </c>
-    </row>
-    <row r="215" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A215" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B215" s="24" t="s">
-        <v>414</v>
       </c>
       <c r="C215" t="s">
         <v>48</v>
       </c>
       <c r="D215" s="29" t="s">
+        <v>414</v>
+      </c>
+      <c r="E215" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B216" s="24" t="s">
         <v>415</v>
-      </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B216" s="24" t="s">
-        <v>416</v>
       </c>
       <c r="C216" t="s">
         <v>71</v>
       </c>
       <c r="D216" s="29" t="s">
+        <v>416</v>
+      </c>
+      <c r="E216" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B217" s="24" t="s">
         <v>417</v>
-      </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A217" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B217" s="24" t="s">
-        <v>418</v>
       </c>
       <c r="C217" t="s">
         <v>71</v>
       </c>
       <c r="D217" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="E217" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B218" s="24" t="s">
         <v>419</v>
-      </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B218" s="24" t="s">
-        <v>420</v>
       </c>
       <c r="C218" t="s">
         <v>71</v>
       </c>
       <c r="D218" s="29" t="s">
+        <v>420</v>
+      </c>
+      <c r="E218" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B219" s="24" t="s">
         <v>421</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B219" s="24" t="s">
-        <v>422</v>
       </c>
       <c r="C219" t="s">
         <v>48</v>
       </c>
       <c r="D219" s="29" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="220" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>422</v>
+      </c>
+      <c r="E219" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B220" s="24" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C220" t="s">
         <v>312</v>
       </c>
       <c r="D220" s="29" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+        <v>423</v>
+      </c>
+      <c r="E220" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B221" s="24" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C221" t="s">
         <v>312</v>
       </c>
       <c r="D221" s="29" t="s">
+        <v>426</v>
+      </c>
+      <c r="E221" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B222" s="24" t="s">
         <v>427</v>
-      </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B222" s="24" t="s">
-        <v>428</v>
       </c>
       <c r="C222" t="s">
         <v>46</v>
       </c>
       <c r="D222" s="29" t="s">
+        <v>428</v>
+      </c>
+      <c r="E222" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A223" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B223" s="24" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="223" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A223" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B223" s="24" t="s">
-        <v>430</v>
       </c>
       <c r="C223" t="s">
         <v>312</v>
       </c>
       <c r="D223" s="29" t="s">
+        <v>430</v>
+      </c>
+      <c r="E223" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B224" s="24" t="s">
         <v>431</v>
-      </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B224" s="24" t="s">
-        <v>432</v>
       </c>
       <c r="C224" t="s">
         <v>48</v>
       </c>
       <c r="D224" s="29" t="s">
+        <v>432</v>
+      </c>
+      <c r="E224" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A225" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B225" s="24" t="s">
         <v>433</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A225" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B225" s="24" t="s">
-        <v>434</v>
       </c>
       <c r="C225" t="s">
         <v>48</v>
       </c>
       <c r="D225" s="29" t="s">
+        <v>434</v>
+      </c>
+      <c r="E225" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A226" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B226" s="24" t="s">
         <v>435</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A226" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B226" s="24" t="s">
-        <v>436</v>
       </c>
       <c r="C226" t="s">
         <v>312</v>
       </c>
       <c r="D226" s="29" t="s">
+        <v>436</v>
+      </c>
+      <c r="E226" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A227" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B227" s="24" t="s">
         <v>437</v>
-      </c>
-    </row>
-    <row r="227" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A227" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B227" s="24" t="s">
-        <v>438</v>
       </c>
       <c r="C227" t="s">
         <v>48</v>
       </c>
       <c r="D227" s="29" t="s">
+        <v>438</v>
+      </c>
+      <c r="E227" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A228" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B228" s="24" t="s">
         <v>439</v>
-      </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B228" s="24" t="s">
-        <v>440</v>
       </c>
       <c r="C228" t="s">
         <v>312</v>
       </c>
       <c r="D228" s="29" t="s">
+        <v>440</v>
+      </c>
+      <c r="E228" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A229" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B229" s="24" t="s">
         <v>441</v>
-      </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B229" s="24" t="s">
-        <v>442</v>
       </c>
       <c r="C229" t="s">
         <v>71</v>
       </c>
       <c r="D229" s="29" t="s">
+        <v>442</v>
+      </c>
+      <c r="E229" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A230" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B230" s="24" t="s">
         <v>443</v>
-      </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B230" s="24" t="s">
-        <v>444</v>
       </c>
       <c r="C230" t="s">
         <v>71</v>
       </c>
       <c r="D230" s="29" t="s">
+        <v>444</v>
+      </c>
+      <c r="E230" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A231" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B231" s="24" t="s">
         <v>445</v>
-      </c>
-    </row>
-    <row r="231" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A231" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B231" s="24" t="s">
-        <v>446</v>
       </c>
       <c r="C231" t="s">
         <v>48</v>
       </c>
       <c r="D231" s="29" t="s">
+        <v>446</v>
+      </c>
+      <c r="E231" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A232" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B232" s="24" t="s">
         <v>447</v>
-      </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B232" s="24" t="s">
-        <v>448</v>
       </c>
       <c r="C232" t="s">
         <v>48</v>
       </c>
       <c r="D232" s="29" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="233" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>448</v>
+      </c>
+      <c r="E232" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B233" s="24" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C233" t="s">
         <v>48</v>
@@ -5345,27 +5534,33 @@
       <c r="D233" s="4">
         <v>2606</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E233" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A234" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B234" s="24" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C234" t="s">
         <v>71</v>
       </c>
       <c r="D234" s="29" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="235" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+      <c r="E234" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B235" s="24" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C235" t="s">
         <v>71</v>
@@ -5373,13 +5568,16 @@
       <c r="D235" s="4">
         <v>1624</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="E235" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B236" s="24" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C236" t="s">
         <v>71</v>
@@ -5387,13 +5585,16 @@
       <c r="D236" s="4">
         <v>1620</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E236" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B237" s="24" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C237" t="s">
         <v>71</v>
@@ -5401,19 +5602,39 @@
       <c r="D237" s="4">
         <v>1619</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="E237" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B238" s="24" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C238" t="s">
         <v>71</v>
       </c>
       <c r="D238" s="4">
         <v>1640</v>
+      </c>
+      <c r="E238" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A239" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B239" s="24" t="s">
+        <v>462</v>
+      </c>
+      <c r="C239" t="s">
+        <v>46</v>
+      </c>
+      <c r="E239" t="s">
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -5421,70 +5642,81 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A95 A98:A1048576">
-    <cfRule type="containsText" dxfId="18" priority="15" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="19" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="13" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="14" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E180:E239">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",E180)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="maybe">
+      <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated to-do list for patch
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1095" uniqueCount="466">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1429,6 +1429,12 @@
   </si>
   <si>
     <t>maybe</t>
+  </si>
+  <si>
+    <t>CEC module library update</t>
+  </si>
+  <si>
+    <t>Inverter update</t>
   </si>
 </sst>
 </file>
@@ -1618,7 +1624,49 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="28">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2203,11 +2251,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I239"/>
+  <dimension ref="A1:I241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A191" sqref="A191"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5637,85 +5685,113 @@
         <v>458</v>
       </c>
     </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A240" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B240" s="24" t="s">
+        <v>464</v>
+      </c>
+      <c r="C240" t="s">
+        <v>48</v>
+      </c>
+      <c r="E240" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A241" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B241" s="24" t="s">
+        <v>465</v>
+      </c>
+      <c r="C241" t="s">
+        <v>48</v>
+      </c>
+      <c r="E241" t="s">
+        <v>458</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:G52">
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A95 A98:A1048576">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="27" priority="18" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="26" priority="19" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="25" priority="20" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="22" priority="13" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="21" priority="14" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="20" priority="15" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="12" priority="9" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E180:E239">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="E180:E241">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update several patch items and update SAM TODO.xlsx
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
   </bookViews>
@@ -15,12 +20,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="473">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1422,9 +1427,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>This may already be in the trunk.</t>
-  </si>
-  <si>
     <t>Fix remaining bug with Wind CSM</t>
   </si>
   <si>
@@ -1438,6 +1440,27 @@
   </si>
   <si>
     <t>Inverter sizing macro bug fixes</t>
+  </si>
+  <si>
+    <t>Binary builds for mac only  - checked in 2015.1.30 branch SAMnt rev 1656</t>
+  </si>
+  <si>
+    <t>Already in 2015.1.30 branch and in trunk</t>
+  </si>
+  <si>
+    <t>In 2015.1.30 branch, Subject to review by Paul, see email from Steve 3/21/15</t>
+  </si>
+  <si>
+    <t>Checked in 2015.1.30 branch SAMnt svn rev 1656</t>
+  </si>
+  <si>
+    <t>Checked in 2015.1.30 branch ssc svn rev 2620</t>
+  </si>
+  <si>
+    <t>Checked in 2015.1.30 branch SAMnt svn rev 1657</t>
+  </si>
+  <si>
+    <t>Checked in 2015.1.30 branch SAMnt svn rev 1653</t>
   </si>
 </sst>
 </file>
@@ -1627,7 +1650,280 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="61">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1968,7 +2264,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2003,7 +2299,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2215,8 +2511,8 @@
   <dimension ref="A1:I242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E243" sqref="E243"/>
+      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F233" sqref="F233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4675,6 +4971,9 @@
       <c r="E180" s="4" t="s">
         <v>458</v>
       </c>
+      <c r="F180" s="4" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="20" t="s">
@@ -4687,7 +4986,10 @@
         <v>77</v>
       </c>
       <c r="E181" t="s">
-        <v>463</v>
+        <v>57</v>
+      </c>
+      <c r="F181" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -4701,7 +5003,7 @@
         <v>231</v>
       </c>
       <c r="E182" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F182" t="s">
         <v>304</v>
@@ -4776,6 +5078,9 @@
       <c r="E187" t="s">
         <v>458</v>
       </c>
+      <c r="F187" s="4" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A188" s="20" t="s">
@@ -4788,7 +5093,7 @@
         <v>312</v>
       </c>
       <c r="E188" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -4803,6 +5108,9 @@
       </c>
       <c r="E189" t="s">
         <v>458</v>
+      </c>
+      <c r="F189" s="4" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -4980,7 +5288,10 @@
         <v>386</v>
       </c>
       <c r="E200" t="s">
-        <v>458</v>
+        <v>57</v>
+      </c>
+      <c r="F200" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="201" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5099,7 +5410,7 @@
         <v>398</v>
       </c>
       <c r="E207" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -5119,10 +5430,10 @@
         <v>57</v>
       </c>
       <c r="F208" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="209" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A209" s="20" t="s">
         <v>57</v>
       </c>
@@ -5136,10 +5447,13 @@
         <v>402</v>
       </c>
       <c r="E209" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F209" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="20" t="s">
         <v>57</v>
       </c>
@@ -5156,7 +5470,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A211" s="20" t="s">
         <v>57</v>
       </c>
@@ -5173,7 +5487,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="212" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A212" s="20" t="s">
         <v>57</v>
       </c>
@@ -5190,7 +5504,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="20" t="s">
         <v>57</v>
       </c>
@@ -5207,7 +5521,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A214" s="20" t="s">
         <v>57</v>
       </c>
@@ -5221,10 +5535,10 @@
         <v>412</v>
       </c>
       <c r="E214" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="215" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="20" t="s">
         <v>57</v>
       </c>
@@ -5238,10 +5552,10 @@
         <v>414</v>
       </c>
       <c r="E215" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A216" s="20" t="s">
         <v>57</v>
       </c>
@@ -5258,7 +5572,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A217" s="20" t="s">
         <v>57</v>
       </c>
@@ -5272,10 +5586,10 @@
         <v>418</v>
       </c>
       <c r="E217" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="20" t="s">
         <v>57</v>
       </c>
@@ -5292,7 +5606,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A219" s="20" t="s">
         <v>57</v>
       </c>
@@ -5309,7 +5623,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="220" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A220" s="20" t="s">
         <v>57</v>
       </c>
@@ -5326,7 +5640,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="20" t="s">
         <v>57</v>
       </c>
@@ -5340,10 +5654,10 @@
         <v>426</v>
       </c>
       <c r="E221" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A222" s="20" t="s">
         <v>57</v>
       </c>
@@ -5360,7 +5674,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="223" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A223" s="20" t="s">
         <v>57</v>
       </c>
@@ -5376,8 +5690,11 @@
       <c r="E223" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F223" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A224" s="20" t="s">
         <v>57</v>
       </c>
@@ -5391,10 +5708,13 @@
         <v>432</v>
       </c>
       <c r="E224" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="F224" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A225" s="20" t="s">
         <v>57</v>
       </c>
@@ -5411,7 +5731,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="226" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="20" t="s">
         <v>57</v>
       </c>
@@ -5428,7 +5748,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="227" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="20" t="s">
         <v>57</v>
       </c>
@@ -5445,7 +5765,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A228" s="20" t="s">
         <v>57</v>
       </c>
@@ -5462,7 +5782,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A229" s="20" t="s">
         <v>57</v>
       </c>
@@ -5476,10 +5796,10 @@
         <v>442</v>
       </c>
       <c r="E229" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A230" s="20" t="s">
         <v>57</v>
       </c>
@@ -5493,10 +5813,10 @@
         <v>444</v>
       </c>
       <c r="E230" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="231" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A231" s="20" t="s">
         <v>57</v>
       </c>
@@ -5513,7 +5833,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="20" t="s">
         <v>57</v>
       </c>
@@ -5530,7 +5850,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="233" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A233" s="20" t="s">
         <v>57</v>
       </c>
@@ -5547,7 +5867,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="234" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A234" s="20" t="s">
         <v>57</v>
       </c>
@@ -5564,7 +5884,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="235" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="20" t="s">
         <v>57</v>
       </c>
@@ -5581,7 +5901,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="236" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="20" t="s">
         <v>57</v>
       </c>
@@ -5595,10 +5915,10 @@
         <v>1620</v>
       </c>
       <c r="E236" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A237" s="20" t="s">
         <v>57</v>
       </c>
@@ -5612,10 +5932,10 @@
         <v>1619</v>
       </c>
       <c r="E237" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="238" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="20" t="s">
         <v>57</v>
       </c>
@@ -5629,15 +5949,15 @@
         <v>1640</v>
       </c>
       <c r="E238" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B239" s="24" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C239" t="s">
         <v>46</v>
@@ -5646,18 +5966,21 @@
         <v>57</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A240" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B240" s="24" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C240" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E240" t="s">
-        <v>458</v>
+        <v>57</v>
+      </c>
+      <c r="F240" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -5665,7 +5988,7 @@
         <v>198</v>
       </c>
       <c r="B241" s="24" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C241" t="s">
         <v>48</v>
@@ -5679,7 +6002,7 @@
         <v>57</v>
       </c>
       <c r="B242" s="24" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C242" t="s">
         <v>46</v>
@@ -5693,81 +6016,114 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A95 A98:A1048576">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="60" priority="33" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="19" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="59" priority="34" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="58" priority="35" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="21" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="57" priority="36" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="55" priority="28" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="14" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="54" priority="29" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="53" priority="30" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="16" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="52" priority="31" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="17" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="50" priority="26" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="12" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="49" priority="27" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="48" priority="21" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="47" priority="22" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="46" priority="23" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="45" priority="24" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="43" priority="19" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="5" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E180:E242">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Yes">
+  <conditionalFormatting sqref="E180:E242 F180:F181 F240">
+    <cfRule type="containsText" dxfId="41" priority="18" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="40" priority="17" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="39" priority="16" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F187">
+    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="maybe">
+      <formula>NOT(ISERROR(SEARCH("maybe",F187)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",F187)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",F187)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F189">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="maybe">
+      <formula>NOT(ISERROR(SEARCH("maybe",F189)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",F189)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",F189)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F223">
+    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="maybe">
+      <formula>NOT(ISERROR(SEARCH("maybe",F223)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",F223)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",F223)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#new - Third party ownership configurations and defaults running. Needs updated metrics, autographs, and cash flow.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="476">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1461,6 +1461,15 @@
   </si>
   <si>
     <t>Checked in 2015.1.30 branch SAMnt svn rev 1653</t>
+  </si>
+  <si>
+    <t>Checked in 2015.1.30 branch ssc svn rev 2621</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Checked in 2015.1.30 branch SAMnt svn rev 1659</t>
   </si>
 </sst>
 </file>
@@ -1650,112 +1659,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="61">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill>
@@ -1858,69 +1762,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2511,8 +2352,8 @@
   <dimension ref="A1:I242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F233" sqref="F233"/>
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F216" sqref="F216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4977,7 +4818,7 @@
     </row>
     <row r="181" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A181" s="20" t="s">
-        <v>113</v>
+        <v>57</v>
       </c>
       <c r="B181" s="24" t="s">
         <v>301</v>
@@ -5552,7 +5393,10 @@
         <v>414</v>
       </c>
       <c r="E215" t="s">
-        <v>462</v>
+        <v>57</v>
+      </c>
+      <c r="F215" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -5847,7 +5691,10 @@
         <v>448</v>
       </c>
       <c r="E232" t="s">
-        <v>458</v>
+        <v>474</v>
+      </c>
+      <c r="F232" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -6016,114 +5863,125 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A95 A98:A1048576">
-    <cfRule type="containsText" dxfId="60" priority="33" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="34" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="35" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="36" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="37" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="55" priority="28" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="29" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="30" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="31" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="32" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="50" priority="26" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="27" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="48" priority="21" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="22" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="23" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="24" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="25" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="43" priority="19" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="20" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E180:E242 F180:F181 F240">
-    <cfRule type="containsText" dxfId="41" priority="18" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="17" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="16" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F187">
-    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F187)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F189">
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F189)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F223">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F223)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F215">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="maybe">
+      <formula>NOT(ISERROR(SEARCH("maybe",F215)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",F215)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",F215)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
2015.1.30 patch item updates to TODO list.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="479">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1470,6 +1470,15 @@
   </si>
   <si>
     <t>Checked in 2015.1.30 branch SAMnt svn rev 1659</t>
+  </si>
+  <si>
+    <t>Checked in trunk and 2015.1.30 branch SAMnt rev 1665</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Done </t>
+  </si>
+  <si>
+    <t>Checked in 2015.1.30 branch ssc svn rev 2627</t>
   </si>
 </sst>
 </file>
@@ -1659,7 +1668,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="40">
     <dxf>
       <fill>
         <patternFill>
@@ -1684,7 +1693,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1698,7 +1707,28 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2352,8 +2382,8 @@
   <dimension ref="A1:I242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F216" sqref="F216"/>
+      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F231" sqref="F231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4861,7 +4891,10 @@
         <v>48</v>
       </c>
       <c r="E183" t="s">
-        <v>459</v>
+        <v>477</v>
+      </c>
+      <c r="F183" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -5185,6 +5218,9 @@
       <c r="E203" t="s">
         <v>458</v>
       </c>
+      <c r="F203" s="4" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="204" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A204" s="20" t="s">
@@ -5376,7 +5412,10 @@
         <v>412</v>
       </c>
       <c r="E214" t="s">
-        <v>462</v>
+        <v>57</v>
+      </c>
+      <c r="F214" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="215" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5464,7 +5503,10 @@
         <v>422</v>
       </c>
       <c r="E219" t="s">
-        <v>458</v>
+        <v>57</v>
+      </c>
+      <c r="F219" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="220" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5711,7 +5753,10 @@
         <v>2606</v>
       </c>
       <c r="E233" t="s">
-        <v>458</v>
+        <v>57</v>
+      </c>
+      <c r="F233" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -5863,125 +5908,136 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A95 A98:A1048576">
-    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="30" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="24" priority="24" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="19" priority="22" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="23" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E180:E242 F180:F181 F240">
-    <cfRule type="containsText" dxfId="17" priority="21" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="20" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="19" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F187">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F187)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F189">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F189)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F223">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F223)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F215">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F215)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F203">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="maybe">
+      <formula>NOT(ISERROR(SEARCH("maybe",F203)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",F203)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Yes">
+      <formula>NOT(ISERROR(SEARCH("Yes",F203)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated status of patch To-Do list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
   </bookViews>
@@ -20,12 +15,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="480">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1479,6 +1474,9 @@
   </si>
   <si>
     <t>Checked in 2015.1.30 branch ssc svn rev 2627</t>
+  </si>
+  <si>
+    <t>In 2015.1.30 branch</t>
   </si>
 </sst>
 </file>
@@ -1672,7 +1670,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1686,7 +1684,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2135,7 +2133,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2170,7 +2168,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2382,8 +2380,8 @@
   <dimension ref="A1:I242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F231" sqref="F231"/>
+      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4967,7 +4965,10 @@
         <v>312</v>
       </c>
       <c r="E188" t="s">
-        <v>462</v>
+        <v>57</v>
+      </c>
+      <c r="F188" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -5974,7 +5975,7 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E180:E242 F180:F181 F240">
+  <conditionalFormatting sqref="E180:E242 F180:F181 F240 F188">
     <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Updated SAM TODO with 2015.1.30 patch status
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="481">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1477,6 +1477,9 @@
   </si>
   <si>
     <t>In 2015.1.30 branch</t>
+  </si>
+  <si>
+    <t>In 2015.1.30 branch, verified works</t>
   </si>
 </sst>
 </file>
@@ -1666,28 +1669,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="37">
     <dxf>
       <fill>
         <patternFill>
@@ -2380,8 +2362,8 @@
   <dimension ref="A1:I242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A169" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F190" sqref="F190"/>
+      <pane ySplit="1" topLeftCell="A181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F200" sqref="F200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5273,6 +5255,9 @@
       <c r="E206" t="s">
         <v>458</v>
       </c>
+      <c r="F206" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="207" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A207" s="20" t="s">
@@ -5909,135 +5894,135 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A95 A98:A1048576">
-    <cfRule type="containsText" dxfId="39" priority="39" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="40" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="35" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="41" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="34" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="42" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="33" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="43" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="34" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="27" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="29" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="18" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E180:E242 F180:F181 F240 F188">
-    <cfRule type="containsText" dxfId="20" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="17" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="22" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="15" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F187">
-    <cfRule type="containsText" dxfId="17" priority="13" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="14" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="15" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F187)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F189">
-    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F189)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F189)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F223">
-    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F223)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F215">
-    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F215)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F203">
-    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F203)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F203)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F203)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
SAM TODO.xlsx updates for 2015.1.30 patch 1 full install and updated lhs and stepwise executables built with gfortran.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
   </bookViews>
@@ -15,12 +20,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1115" uniqueCount="483">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1483,6 +1488,9 @@
   </si>
   <si>
     <t>Done except for disabling min/max operating temps when they are set to zero.</t>
+  </si>
+  <si>
+    <t>In process - should be done by 3/30/15</t>
   </si>
 </sst>
 </file>
@@ -1549,7 +1557,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1604,6 +1612,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1626,7 +1640,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1668,11 +1682,75 @@
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="43">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2097,7 +2175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2132,7 +2210,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2344,8 +2422,8 @@
   <dimension ref="A1:I241"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E243" sqref="E243"/>
+      <pane ySplit="1" topLeftCell="A226" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E192" sqref="E192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4991,7 +5069,7 @@
         <v>368</v>
       </c>
       <c r="E192" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="F192" t="s">
         <v>480</v>
@@ -5844,6 +5922,9 @@
       </c>
       <c r="E240" t="s">
         <v>457</v>
+      </c>
+      <c r="F240" s="31" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.25">
@@ -5865,124 +5946,124 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A95 A98:A1048576">
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="42" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="39" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="38" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="37" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="34" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="33" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="32" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="31" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="29" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="27" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="16" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="25" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="24" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F180:F181 F239 F187 E180:E241">
-    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="maybe">
+  <conditionalFormatting sqref="F180:F181 F187 E180:E241 F239:F240">
+    <cfRule type="containsText" dxfId="5" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="4" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F188">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="23" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F188)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="22" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F188)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F188)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F222">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="20" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F222)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="19" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F222)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F222)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F214">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F214)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="16" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F214)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F214)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F202">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="14" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F202)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="13" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F202)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F202)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Update SAM TODO.xlsx for 2015.1.30 patch
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="12135" windowHeight="10845"/>
   </bookViews>
@@ -15,12 +20,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1109" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="482">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1249,11 +1254,6 @@
     <t>1550</t>
   </si>
   <si>
-    <t>#new - subarray shading applied based on group number for mxh and diffuse shading.
-remove beta expiration messages.
-testing Vista fix for debug processing.</t>
-  </si>
-  <si>
     <t>1549</t>
   </si>
   <si>
@@ -1401,9 +1401,6 @@
     <t>#ui add empirical trough custom storage HTF option to make it possible to model direct storage with a custom field HTF</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
     <t>(below)</t>
   </si>
   <si>
@@ -1473,13 +1470,22 @@
     <t>Done except for disabling min/max operating temps when they are set to zero.</t>
   </si>
   <si>
-    <t>In process - should be done by 3/30/15</t>
-  </si>
-  <si>
     <t>CSP with custom HTF: disable min/max operating temperatures to minimize user confusion. For library HTFs, these are hard-coded in the UI so they are not available for custom HTFs. (email with Paul, Ty, and Craig 1/7/2015)</t>
   </si>
   <si>
     <t>MSLF: fixed serious bug: sf_type not defined in compute module. this resulted in the solver using the incorrect solution mode and setting the field inlet to the design temperature rather than a recirculated temperature during startup. This resulted in the system "losing" internal energy between timesteps and an artificially low annual energy output. Also, freeze protection energy was not reported in the previous version and is here.</t>
+  </si>
+  <si>
+    <t>Updated through March 2015 in trunk SAMnt rev 1698 and 2015.1.30 branch SAMnt rev 1699</t>
+  </si>
+  <si>
+    <t>remove beta expiration messages.</t>
+  </si>
+  <si>
+    <t>#new - subarray shading applied based on group number for mxh and diffuse shading.</t>
+  </si>
+  <si>
+    <t>testing Vista fix for debug processing.</t>
   </si>
 </sst>
 </file>
@@ -2101,7 +2107,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2136,7 +2142,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2345,11 +2351,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I240"/>
+  <dimension ref="A1:I242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A221" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E240" sqref="E240"/>
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4788,10 +4794,10 @@
       <c r="B179" s="21"/>
       <c r="C179" s="21"/>
       <c r="D179" s="21" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="E179" s="21" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F179" s="21"/>
     </row>
@@ -4800,13 +4806,13 @@
         <v>57</v>
       </c>
       <c r="B180" s="24" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C180" t="s">
         <v>279</v>
       </c>
       <c r="E180" s="4" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F180" s="4"/>
     </row>
@@ -4824,7 +4830,7 @@
         <v>57</v>
       </c>
       <c r="F181" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.25">
@@ -4838,7 +4844,7 @@
         <v>231</v>
       </c>
       <c r="E182" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F182" t="s">
         <v>303</v>
@@ -4855,10 +4861,10 @@
         <v>48</v>
       </c>
       <c r="E183" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F183" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="184" spans="1:6" x14ac:dyDescent="0.25">
@@ -4872,7 +4878,7 @@
         <v>71</v>
       </c>
       <c r="E184" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="185" spans="1:6" x14ac:dyDescent="0.25">
@@ -4886,7 +4892,7 @@
         <v>71</v>
       </c>
       <c r="E185" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="186" spans="1:6" x14ac:dyDescent="0.25">
@@ -4900,7 +4906,7 @@
         <v>71</v>
       </c>
       <c r="E186" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="187" spans="1:6" x14ac:dyDescent="0.25">
@@ -4917,7 +4923,7 @@
         <v>57</v>
       </c>
       <c r="F187" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="188" spans="1:6" x14ac:dyDescent="0.25">
@@ -4931,7 +4937,7 @@
         <v>314</v>
       </c>
       <c r="E188" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
@@ -4945,7 +4951,7 @@
         <v>48</v>
       </c>
       <c r="E189" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -4959,7 +4965,7 @@
         <v>364</v>
       </c>
       <c r="E190" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="191" spans="1:6" x14ac:dyDescent="0.25">
@@ -4976,10 +4982,10 @@
         <v>366</v>
       </c>
       <c r="E191" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="F191" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
@@ -4996,7 +5002,7 @@
         <v>371</v>
       </c>
       <c r="E192" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="193" spans="1:6" x14ac:dyDescent="0.25">
@@ -5030,7 +5036,7 @@
         <v>368</v>
       </c>
       <c r="E194" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="195" spans="1:6" x14ac:dyDescent="0.25">
@@ -5047,7 +5053,7 @@
         <v>369</v>
       </c>
       <c r="E195" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
@@ -5064,7 +5070,7 @@
         <v>379</v>
       </c>
       <c r="E196" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
@@ -5081,7 +5087,7 @@
         <v>370</v>
       </c>
       <c r="E197" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
@@ -5101,7 +5107,7 @@
         <v>57</v>
       </c>
       <c r="F198" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="199" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5118,7 +5124,7 @@
         <v>382</v>
       </c>
       <c r="E199" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="200" spans="1:6" x14ac:dyDescent="0.25">
@@ -5135,7 +5141,7 @@
         <v>385</v>
       </c>
       <c r="E200" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="201" spans="1:6" x14ac:dyDescent="0.25">
@@ -5155,7 +5161,7 @@
         <v>57</v>
       </c>
       <c r="F201" s="4" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
     </row>
     <row r="202" spans="1:6" x14ac:dyDescent="0.25">
@@ -5209,7 +5215,7 @@
         <v>57</v>
       </c>
       <c r="F204" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="205" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -5226,10 +5232,10 @@
         <v>395</v>
       </c>
       <c r="E205" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F205" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.25">
@@ -5249,7 +5255,7 @@
         <v>57</v>
       </c>
       <c r="F206" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="207" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5269,7 +5275,7 @@
         <v>57</v>
       </c>
       <c r="F207" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="208" spans="1:6" x14ac:dyDescent="0.25">
@@ -5286,7 +5292,7 @@
         <v>401</v>
       </c>
       <c r="E208" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.25">
@@ -5306,21 +5312,21 @@
         <v>57</v>
       </c>
     </row>
-    <row r="210" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A210" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B210" s="24" t="s">
-        <v>404</v>
+        <v>480</v>
       </c>
       <c r="C210" t="s">
         <v>48</v>
       </c>
       <c r="D210" s="29" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="E210" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.25">
@@ -5328,16 +5334,16 @@
         <v>57</v>
       </c>
       <c r="B211" s="24" t="s">
-        <v>406</v>
+        <v>481</v>
       </c>
       <c r="C211" t="s">
         <v>48</v>
       </c>
-      <c r="D211" s="29" t="s">
-        <v>407</v>
+      <c r="D211" s="29">
+        <v>1549</v>
       </c>
       <c r="E211" t="s">
-        <v>456</v>
+        <v>57</v>
       </c>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.25">
@@ -5345,39 +5351,33 @@
         <v>57</v>
       </c>
       <c r="B212" s="24" t="s">
-        <v>408</v>
+        <v>479</v>
       </c>
       <c r="C212" t="s">
         <v>48</v>
       </c>
-      <c r="D212" s="29" t="s">
-        <v>409</v>
+      <c r="D212" s="29">
+        <v>1549</v>
       </c>
       <c r="E212" t="s">
         <v>57</v>
       </c>
-      <c r="F212" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A213" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B213" s="24" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="C213" t="s">
         <v>48</v>
       </c>
       <c r="D213" s="29" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E213" t="s">
         <v>57</v>
-      </c>
-      <c r="F213" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
@@ -5385,33 +5385,39 @@
         <v>57</v>
       </c>
       <c r="B214" s="24" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C214" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D214" s="29" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="E214" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F214" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A215" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B215" s="24" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C215" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D215" s="29" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="E215" t="s">
-        <v>458</v>
+        <v>57</v>
+      </c>
+      <c r="F215" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.25">
@@ -5419,13 +5425,13 @@
         <v>57</v>
       </c>
       <c r="B216" s="24" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C216" t="s">
         <v>71</v>
       </c>
       <c r="D216" s="29" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="E216" t="s">
         <v>57</v>
@@ -5436,36 +5442,33 @@
         <v>57</v>
       </c>
       <c r="B217" s="24" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C217" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D217" s="29" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="E217" t="s">
-        <v>57</v>
-      </c>
-      <c r="F217" t="s">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A218" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B218" s="24" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C218" t="s">
-        <v>309</v>
+        <v>71</v>
       </c>
       <c r="D218" s="29" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E218" t="s">
-        <v>456</v>
+        <v>57</v>
       </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.25">
@@ -5473,53 +5476,53 @@
         <v>57</v>
       </c>
       <c r="B219" s="24" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="C219" t="s">
+        <v>48</v>
+      </c>
+      <c r="D219" s="29" t="s">
+        <v>418</v>
+      </c>
+      <c r="E219" t="s">
+        <v>57</v>
+      </c>
+      <c r="F219" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A220" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B220" s="24" t="s">
+        <v>420</v>
+      </c>
+      <c r="C220" t="s">
         <v>309</v>
       </c>
-      <c r="D219" s="29" t="s">
-        <v>423</v>
-      </c>
-      <c r="E219" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A220" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B220" s="24" t="s">
-        <v>424</v>
-      </c>
-      <c r="C220" t="s">
-        <v>46</v>
-      </c>
       <c r="D220" s="29" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="E220" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A221" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B221" s="24" t="s">
-        <v>480</v>
+        <v>421</v>
       </c>
       <c r="C221" t="s">
         <v>309</v>
       </c>
       <c r="D221" s="29" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E221" t="s">
-        <v>57</v>
-      </c>
-      <c r="F221" s="4" t="s">
-        <v>464</v>
+        <v>456</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.25">
@@ -5527,104 +5530,107 @@
         <v>57</v>
       </c>
       <c r="B222" s="24" t="s">
+        <v>423</v>
+      </c>
+      <c r="C222" t="s">
+        <v>46</v>
+      </c>
+      <c r="D222" s="29" t="s">
+        <v>424</v>
+      </c>
+      <c r="E222" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A223" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B223" s="24" t="s">
+        <v>477</v>
+      </c>
+      <c r="C223" t="s">
+        <v>309</v>
+      </c>
+      <c r="D223" s="29" t="s">
+        <v>425</v>
+      </c>
+      <c r="E223" t="s">
+        <v>57</v>
+      </c>
+      <c r="F223" s="4" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A224" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B224" s="24" t="s">
+        <v>426</v>
+      </c>
+      <c r="C224" t="s">
+        <v>48</v>
+      </c>
+      <c r="D224" s="29" t="s">
         <v>427</v>
       </c>
-      <c r="C222" t="s">
-        <v>48</v>
-      </c>
-      <c r="D222" s="29" t="s">
+      <c r="E224" t="s">
+        <v>57</v>
+      </c>
+      <c r="F224" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A225" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B225" s="24" t="s">
         <v>428</v>
-      </c>
-      <c r="E222" t="s">
-        <v>57</v>
-      </c>
-      <c r="F222" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B223" s="24" t="s">
-        <v>429</v>
-      </c>
-      <c r="C223" t="s">
-        <v>48</v>
-      </c>
-      <c r="D223" s="29" t="s">
-        <v>430</v>
-      </c>
-      <c r="E223" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A224" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B224" s="24" t="s">
-        <v>431</v>
-      </c>
-      <c r="C224" t="s">
-        <v>309</v>
-      </c>
-      <c r="D224" s="29" t="s">
-        <v>432</v>
-      </c>
-      <c r="E224" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A225" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B225" s="24" t="s">
-        <v>433</v>
       </c>
       <c r="C225" t="s">
         <v>48</v>
       </c>
       <c r="D225" s="29" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="E225" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A226" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B226" s="24" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="C226" t="s">
         <v>309</v>
       </c>
       <c r="D226" s="29" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="E226" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A227" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B227" s="24" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C227" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D227" s="29" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="E227" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.25">
@@ -5632,30 +5638,30 @@
         <v>57</v>
       </c>
       <c r="B228" s="24" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="C228" t="s">
+        <v>309</v>
+      </c>
+      <c r="D228" s="29" t="s">
+        <v>435</v>
+      </c>
+      <c r="E228" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A229" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B229" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="C229" t="s">
         <v>71</v>
       </c>
-      <c r="D228" s="29" t="s">
-        <v>440</v>
-      </c>
-      <c r="E228" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A229" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="B229" s="24" t="s">
-        <v>441</v>
-      </c>
-      <c r="C229" t="s">
-        <v>48</v>
-      </c>
       <c r="D229" s="29" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E229" t="s">
         <v>456</v>
@@ -5666,19 +5672,16 @@
         <v>57</v>
       </c>
       <c r="B230" s="24" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="C230" t="s">
-        <v>48</v>
+        <v>71</v>
       </c>
       <c r="D230" s="29" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="E230" t="s">
-        <v>470</v>
-      </c>
-      <c r="F230" t="s">
-        <v>469</v>
+        <v>456</v>
       </c>
     </row>
     <row r="231" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5686,36 +5689,36 @@
         <v>57</v>
       </c>
       <c r="B231" s="24" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="C231" t="s">
         <v>48</v>
       </c>
-      <c r="D231" s="4">
-        <v>2606</v>
+      <c r="D231" s="29" t="s">
+        <v>441</v>
       </c>
       <c r="E231" t="s">
-        <v>57</v>
-      </c>
-      <c r="F231" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A232" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B232" s="24" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
       <c r="C232" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D232" s="29" t="s">
-        <v>452</v>
+        <v>443</v>
       </c>
       <c r="E232" t="s">
-        <v>57</v>
+        <v>468</v>
+      </c>
+      <c r="F232" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="233" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -5723,16 +5726,19 @@
         <v>57</v>
       </c>
       <c r="B233" s="24" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C233" t="s">
-        <v>71</v>
+        <v>48</v>
       </c>
       <c r="D233" s="4">
-        <v>1624</v>
+        <v>2606</v>
       </c>
       <c r="E233" t="s">
         <v>57</v>
+      </c>
+      <c r="F233" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="234" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -5740,50 +5746,50 @@
         <v>57</v>
       </c>
       <c r="B234" s="24" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C234" t="s">
         <v>71</v>
       </c>
-      <c r="D234" s="4">
-        <v>1620</v>
+      <c r="D234" s="29" t="s">
+        <v>451</v>
       </c>
       <c r="E234" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A235" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B235" s="24" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C235" t="s">
         <v>71</v>
       </c>
       <c r="D235" s="4">
-        <v>1619</v>
+        <v>1624</v>
       </c>
       <c r="E235" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B236" s="24" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C236" t="s">
         <v>71</v>
       </c>
       <c r="D236" s="4">
-        <v>1640</v>
+        <v>1620</v>
       </c>
       <c r="E236" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.25">
@@ -5791,47 +5797,47 @@
         <v>57</v>
       </c>
       <c r="B237" s="24" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C237" t="s">
-        <v>46</v>
+        <v>71</v>
+      </c>
+      <c r="D237" s="4">
+        <v>1619</v>
       </c>
       <c r="E237" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" x14ac:dyDescent="0.25">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A238" s="20" t="s">
         <v>57</v>
       </c>
       <c r="B238" s="24" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="C238" t="s">
-        <v>47</v>
+        <v>71</v>
+      </c>
+      <c r="D238" s="4">
+        <v>1640</v>
       </c>
       <c r="E238" t="s">
-        <v>57</v>
-      </c>
-      <c r="F238" t="s">
-        <v>468</v>
+        <v>456</v>
       </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A239" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B239" s="24" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="C239" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E239" t="s">
-        <v>454</v>
-      </c>
-      <c r="F239" s="31" t="s">
-        <v>478</v>
+        <v>57</v>
       </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.25">
@@ -5839,12 +5845,46 @@
         <v>57</v>
       </c>
       <c r="B240" s="24" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C240" t="s">
+        <v>47</v>
+      </c>
+      <c r="E240" t="s">
+        <v>57</v>
+      </c>
+      <c r="F240" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A241" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B241" s="24" t="s">
+        <v>458</v>
+      </c>
+      <c r="C241" t="s">
+        <v>48</v>
+      </c>
+      <c r="E241" t="s">
+        <v>57</v>
+      </c>
+      <c r="F241" s="31" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A242" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B242" s="24" t="s">
+        <v>459</v>
+      </c>
+      <c r="C242" t="s">
         <v>46</v>
       </c>
-      <c r="E240" t="s">
+      <c r="E242" t="s">
         <v>57</v>
       </c>
     </row>
@@ -5919,7 +5959,7 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F180:F181 F238:F239 E180:E240">
+  <conditionalFormatting sqref="F180:F181 F240:F241 E180:E242">
     <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
     </cfRule>
@@ -5941,26 +5981,26 @@
       <formula>NOT(ISERROR(SEARCH("Yes",F187)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F221">
+  <conditionalFormatting sqref="F223">
     <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="maybe">
-      <formula>NOT(ISERROR(SEARCH("maybe",F221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("maybe",F223)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",F221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",F223)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",F221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes",F223)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F213">
+  <conditionalFormatting sqref="F215">
     <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="maybe">
-      <formula>NOT(ISERROR(SEARCH("maybe",F213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("maybe",F215)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",F213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",F215)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Yes">
-      <formula>NOT(ISERROR(SEARCH("Yes",F213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Yes",F215)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F201">

</xml_diff>

<commit_message>
Update TODO items - not many left!
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="482">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1118" uniqueCount="483">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1486,6 +1486,9 @@
   </si>
   <si>
     <t>testing Vista fix for debug processing.</t>
+  </si>
+  <si>
+    <t>Checked in SAMnt rev 1722</t>
   </si>
 </sst>
 </file>
@@ -1682,7 +1685,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="34">
+  <dxfs count="37">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2354,8 +2378,8 @@
   <dimension ref="A1:I242"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E189" sqref="E189"/>
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A242" sqref="A242"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4942,7 +4966,7 @@
     </row>
     <row r="189" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A189" s="20" t="s">
-        <v>198</v>
+        <v>57</v>
       </c>
       <c r="B189" s="24" t="s">
         <v>362</v>
@@ -4952,6 +4976,9 @@
       </c>
       <c r="E189" t="s">
         <v>454</v>
+      </c>
+      <c r="F189" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="190" spans="1:6" x14ac:dyDescent="0.25">
@@ -5893,124 +5920,124 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A95 A98:A1048576">
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="35" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="34" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="33" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="32" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="29" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="28" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="27" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="26" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="25" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="24" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="23" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="22" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="21" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="20" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B179:F179">
-    <cfRule type="containsText" dxfId="16" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="19" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B179)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="18" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B179)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F180:F181 F240:F241 E180:E242">
-    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="maybe">
+  <conditionalFormatting sqref="F180:F181 F240:F241 E180:E242 F189">
+    <cfRule type="containsText" dxfId="17" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E180)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="15" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E180)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F187">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="14" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="13" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F187)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F187)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F223">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F223)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F223)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F215">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="8" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F215)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="6" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F215)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F201">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F201)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F201)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F201)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
TODO and PV / commercial default updates.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785"/>
   </bookViews>
@@ -15,12 +20,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="489">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1499,6 +1504,9 @@
   </si>
   <si>
     <t>Severin</t>
+  </si>
+  <si>
+    <t>Diffuse view factor from shade tool instead of irradiation processor</t>
   </si>
 </sst>
 </file>
@@ -2120,7 +2128,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2155,7 +2163,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2364,11 +2372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I243"/>
+  <dimension ref="A1:I244"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
+      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A245" sqref="A245"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5913,6 +5921,17 @@
       </c>
       <c r="C243" t="s">
         <v>484</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A244" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="B244" s="24" t="s">
+        <v>488</v>
+      </c>
+      <c r="C244" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TODO list with tower feature requests from support forum
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do" sheetId="1" r:id="rId1"/>
@@ -20,12 +15,12 @@
   <definedNames>
     <definedName name="Types">'SAM Variable Changes'!$U$1:$U$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="491">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1507,6 +1502,12 @@
   </si>
   <si>
     <t>Diffuse view factor from shade tool instead of irradiation processor</t>
+  </si>
+  <si>
+    <t>SolarPilot add maximum tower height to restrict optimization https://sam.nrel.gov/node/69394, Mike Wagner email 4/27/2015</t>
+  </si>
+  <si>
+    <t>Report tower flux map as output https://sam.nrel.gov/node/69393, Mike Wagner email 4/27/2015</t>
   </si>
 </sst>
 </file>
@@ -2128,7 +2129,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2163,7 +2164,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2374,8 +2375,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I244"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A218" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A224" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A245" sqref="A245"/>
     </sheetView>
   </sheetViews>
@@ -6067,10 +6068,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6259,6 +6260,16 @@
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>365</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>490</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Started updating the version upgrader script, updated to-do list accordingly.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do- FY15 Release" sheetId="5" r:id="rId1"/>
@@ -1676,7 +1676,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1760,6 +1760,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1783,7 +1795,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1858,6 +1870,8 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -2960,9 +2974,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F144"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B35" sqref="B35"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3760,8 +3774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3798,14 +3812,13 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>205</v>
       </c>
       <c r="B2" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="C2" s="27"/>
       <c r="D2" s="27" t="s">
         <v>208</v>
       </c>
@@ -3815,11 +3828,11 @@
       <c r="F2" s="27">
         <v>10</v>
       </c>
-      <c r="U2" t="s">
+      <c r="U2" s="27" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>206</v>
       </c>
@@ -3835,12 +3848,11 @@
       <c r="E3" s="27" t="s">
         <v>212</v>
       </c>
-      <c r="F3" s="27"/>
-      <c r="U3" t="s">
+      <c r="U3" s="27" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>207</v>
       </c>
@@ -3850,97 +3862,95 @@
       <c r="C4" s="27" t="s">
         <v>213</v>
       </c>
-      <c r="D4" s="27"/>
       <c r="E4" s="27" t="s">
         <v>214</v>
       </c>
-      <c r="F4" s="27"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+    </row>
+    <row r="5" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="50" t="s">
         <v>254</v>
       </c>
-      <c r="E5" s="25" t="s">
+      <c r="E5" s="50" t="s">
         <v>249</v>
       </c>
-      <c r="F5" s="25">
+      <c r="F5" s="50">
         <v>0</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="50" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+    <row r="6" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="50" t="s">
         <v>251</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="50" t="s">
         <v>256</v>
       </c>
-      <c r="E6" s="25" t="s">
+      <c r="E6" s="50" t="s">
         <v>249</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="50" t="s">
         <v>258</v>
       </c>
-      <c r="G6" s="25" t="s">
+      <c r="G6" s="50" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="C7" s="25" t="s">
+      <c r="C7" s="50" t="s">
         <v>259</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="50" t="s">
         <v>249</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="50" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+    <row r="8" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="50" t="s">
         <v>207</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="50" t="s">
         <v>260</v>
       </c>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="50" t="s">
         <v>249</v>
       </c>
-      <c r="F8" s="25" t="s">
+      <c r="F8" s="50" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:21" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="51" t="s">
         <v>206</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="51" t="s">
         <v>267</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="51" t="s">
         <v>267</v>
       </c>
-      <c r="E9" s="25" t="s">
+      <c r="E9" s="51" t="s">
         <v>266</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="51" t="s">
         <v>268</v>
       </c>
     </row>
@@ -4392,23 +4402,23 @@
         <v>303</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="25" t="s">
+    <row r="30" spans="1:7" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B30" s="25" t="s">
+      <c r="B30" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="D30" s="25" t="s">
+      <c r="D30" s="50" t="s">
         <v>476</v>
       </c>
-      <c r="E30" s="25" t="s">
+      <c r="E30" s="50" t="s">
         <v>477</v>
       </c>
-      <c r="F30" s="25">
+      <c r="F30" s="50">
         <v>0</v>
       </c>
-      <c r="G30" s="25" t="s">
+      <c r="G30" s="50" t="s">
         <v>478</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update todo list and battery feedback doc
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785" activeTab="1"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="To Do- FY15 Release" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1230" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="515">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1579,6 +1579,9 @@
   </si>
   <si>
     <t>Make an awesome to-do list for our June release</t>
+  </si>
+  <si>
+    <t>Full simulation for each year to model module degradation and clipping inverters (https://sam.nrel.gov/node/69400)</t>
   </si>
 </sst>
 </file>
@@ -2976,7 +2979,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3774,7 +3777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -4437,7 +4440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
@@ -4986,10 +4989,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5188,6 +5191,11 @@
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>481</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>514</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add documentation tasks to release list in todo
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785" activeTab="3"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785"/>
   </bookViews>
   <sheets>
     <sheet name="To Do- FY15 Release" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="529">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1582,6 +1582,48 @@
   </si>
   <si>
     <t>Full simulation for each year to model module degradation and clipping inverters (https://sam.nrel.gov/node/69400)</t>
+  </si>
+  <si>
+    <t>Add SolarAnywhere to weather file converter macro</t>
+  </si>
+  <si>
+    <t>Fix tech/market window help</t>
+  </si>
+  <si>
+    <t>New battery storage help topics</t>
+  </si>
+  <si>
+    <t>New third party financing help</t>
+  </si>
+  <si>
+    <t>New LCOE calculator help</t>
+  </si>
+  <si>
+    <t>Update financial spreadsheets on website for new SAM</t>
+  </si>
+  <si>
+    <t>Paul/Nick</t>
+  </si>
+  <si>
+    <t>Fix single owner end-to-excel to work with fixed debt fraction option</t>
+  </si>
+  <si>
+    <t>Update registration proxy instructions in help</t>
+  </si>
+  <si>
+    <t>Revise weather file format topic to only describe SAM CSV and SRW</t>
+  </si>
+  <si>
+    <t>Power tower help review and revision</t>
+  </si>
+  <si>
+    <t>Physical trough help review and revision</t>
+  </si>
+  <si>
+    <t>LCOE and financial metrics review and revision</t>
+  </si>
+  <si>
+    <t>Update electricity rates help for monthly/hourly reconciliation</t>
   </si>
 </sst>
 </file>
@@ -1798,7 +1840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1875,12 +1917,84 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="84">
+  <dxfs count="91">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF33CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2975,11 +3089,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F144"/>
+  <dimension ref="A1:F148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3195,50 +3309,45 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B14" s="48" t="s">
+        <v>522</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="48" t="s">
         <v>513</v>
       </c>
-      <c r="C14" s="48" t="s">
+      <c r="C15" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48" t="s">
+      <c r="D15" s="48"/>
+      <c r="E15" s="48" t="s">
         <v>510</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A15" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B15" s="40" t="s">
-        <v>231</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="42"/>
-      <c r="E15" s="41" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>487</v>
+      <c r="B16" s="40" t="s">
+        <v>231</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>488</v>
-      </c>
-      <c r="D16" s="41"/>
+        <v>74</v>
+      </c>
+      <c r="D16" s="42"/>
       <c r="E16" s="41" t="s">
         <v>511</v>
-      </c>
-      <c r="F16" s="32" t="s">
-        <v>491</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -3246,25 +3355,28 @@
         <v>192</v>
       </c>
       <c r="B17" s="41" t="s">
-        <v>496</v>
+        <v>487</v>
       </c>
       <c r="C17" s="41" t="s">
-        <v>46</v>
+        <v>488</v>
       </c>
       <c r="D17" s="41"/>
       <c r="E17" s="41" t="s">
         <v>511</v>
       </c>
+      <c r="F17" s="32" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
-        <v>499</v>
+        <v>192</v>
       </c>
       <c r="B18" s="41" t="s">
-        <v>504</v>
+        <v>496</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>478</v>
+        <v>46</v>
       </c>
       <c r="D18" s="41"/>
       <c r="E18" s="41" t="s">
@@ -3276,10 +3388,10 @@
         <v>499</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>501</v>
+        <v>478</v>
       </c>
       <c r="D19" s="41"/>
       <c r="E19" s="41" t="s">
@@ -3288,13 +3400,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>192</v>
+        <v>499</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>45</v>
+        <v>501</v>
       </c>
       <c r="D20" s="41"/>
       <c r="E20" s="41" t="s">
@@ -3306,7 +3418,7 @@
         <v>192</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="C21" s="41" t="s">
         <v>45</v>
@@ -3321,7 +3433,7 @@
         <v>192</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="C22" s="41" t="s">
         <v>45</v>
@@ -3335,33 +3447,30 @@
       <c r="A23" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B23" s="44" t="s">
-        <v>357</v>
-      </c>
-      <c r="C23" s="45" t="s">
-        <v>493</v>
-      </c>
-      <c r="D23" s="46"/>
-      <c r="E23" s="45" t="s">
-        <v>512</v>
+      <c r="B23" s="41" t="s">
+        <v>509</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="45" t="s">
-        <v>489</v>
+      <c r="B24" s="44" t="s">
+        <v>357</v>
       </c>
       <c r="C24" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24" s="45"/>
+        <v>493</v>
+      </c>
+      <c r="D24" s="46"/>
       <c r="E24" s="45" t="s">
         <v>512</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>490</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -3369,7 +3478,7 @@
         <v>192</v>
       </c>
       <c r="B25" s="45" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C25" s="45" t="s">
         <v>45</v>
@@ -3378,16 +3487,19 @@
       <c r="E25" s="45" t="s">
         <v>512</v>
       </c>
+      <c r="F25" s="32" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
         <v>192</v>
       </c>
       <c r="B26" s="45" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="C26" s="45" t="s">
-        <v>478</v>
+        <v>45</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="45" t="s">
@@ -3396,36 +3508,40 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="C27" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
+        <v>192</v>
+      </c>
+      <c r="B27" s="45" t="s">
+        <v>506</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>478</v>
+      </c>
+      <c r="D27" s="45"/>
+      <c r="E27" s="45" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B28" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C28" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
+        <v>55</v>
+      </c>
+      <c r="B28" s="45" t="s">
+        <v>515</v>
+      </c>
+      <c r="C28" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D28" s="45"/>
+      <c r="E28" s="45" t="s">
+        <v>512</v>
+      </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
         <v>135</v>
       </c>
       <c r="B29" s="43" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C29" s="43" t="s">
         <v>49</v>
@@ -3438,7 +3554,7 @@
         <v>135</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C30" s="43" t="s">
         <v>49</v>
@@ -3447,57 +3563,195 @@
       <c r="E30" s="43"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31" s="33"/>
+      <c r="A31" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C31" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32" s="33"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B32" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C32" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="33"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="33"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="33"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="33"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="33"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="33"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="33"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="33"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="33"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="33"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="33"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="33"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="33"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="53"/>
+      <c r="E34" s="53"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B35" s="52" t="s">
+        <v>516</v>
+      </c>
+      <c r="C35" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D35" s="52"/>
+      <c r="E35" s="52"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B36" s="52" t="s">
+        <v>517</v>
+      </c>
+      <c r="C36" s="52" t="s">
+        <v>521</v>
+      </c>
+      <c r="D36" s="52"/>
+      <c r="E36" s="52"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B37" s="52" t="s">
+        <v>518</v>
+      </c>
+      <c r="C37" s="52" t="s">
+        <v>233</v>
+      </c>
+      <c r="D37" s="52"/>
+      <c r="E37" s="52"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B38" s="52" t="s">
+        <v>519</v>
+      </c>
+      <c r="C38" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D38" s="52"/>
+      <c r="E38" s="52"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B39" s="52" t="s">
+        <v>520</v>
+      </c>
+      <c r="C39" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="52"/>
+      <c r="E39" s="52"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B40" s="52" t="s">
+        <v>523</v>
+      </c>
+      <c r="C40" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="52"/>
+      <c r="E40" s="52"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B41" s="52" t="s">
+        <v>524</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" s="52" t="s">
+        <v>525</v>
+      </c>
+      <c r="C42" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D42" s="52"/>
+      <c r="E42" s="52"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B43" s="52" t="s">
+        <v>526</v>
+      </c>
+      <c r="C43" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" s="52"/>
+      <c r="E43" s="52"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B44" s="52" t="s">
+        <v>527</v>
+      </c>
+      <c r="C44" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D44" s="52"/>
+      <c r="E44" s="52"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B45" s="52" t="s">
+        <v>528</v>
+      </c>
+      <c r="C45" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="52"/>
+      <c r="E45" s="52"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="33"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="33"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="33"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.2">
@@ -3657,7 +3911,7 @@
       <c r="A100" s="33"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A101" s="34"/>
+      <c r="A101" s="33"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="33"/>
@@ -3669,7 +3923,7 @@
       <c r="A104" s="33"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="33"/>
+      <c r="A105" s="34"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="33"/>
@@ -3683,89 +3937,101 @@
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="33"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A144" s="34"/>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A110" s="33"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A111" s="33"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A112" s="33"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="33"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A148" s="34"/>
     </row>
   </sheetData>
   <sortState ref="A2:F30">
     <sortCondition ref="E2:E30"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A95">
-    <cfRule type="containsText" dxfId="83" priority="53" operator="containsText" text="NGTD">
+  <conditionalFormatting sqref="A1:A99">
+    <cfRule type="containsText" dxfId="90" priority="53" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="54" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="89" priority="54" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="55" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="88" priority="55" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="56" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="87" priority="56" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="57" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="86" priority="57" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A206">
-    <cfRule type="containsText" dxfId="78" priority="46" operator="containsText" text="POUT">
+  <conditionalFormatting sqref="A1:A210">
+    <cfRule type="containsText" dxfId="85" priority="46" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="47" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="84" priority="47" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="76" priority="20" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="83" priority="20" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="82" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="22" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="81" priority="22" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
+  <conditionalFormatting sqref="A100:A101">
+    <cfRule type="containsText" dxfId="80" priority="3" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
+    <cfRule type="containsText" dxfId="79" priority="4" operator="containsText" text="Test">
+      <formula>NOT(ISERROR(SEARCH("Test",A100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
+    <cfRule type="containsText" dxfId="78" priority="5" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",A100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
+    <cfRule type="containsText" dxfId="77" priority="6" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
+    <cfRule type="containsText" dxfId="76" priority="7" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A100)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A209:A1048576">
-    <cfRule type="containsText" dxfId="68" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A209)))</formula>
+  <conditionalFormatting sqref="A213:A1048576">
+    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="POUT">
+      <formula>NOT(ISERROR(SEARCH("POUT",A213)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A209)))</formula>
+    <cfRule type="containsText" dxfId="74" priority="2" operator="containsText" text="Pre-release">
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A213)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A98:A206 A209:A1048576">
-    <cfRule type="containsText" dxfId="66" priority="8" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A98)))</formula>
+  <conditionalFormatting sqref="A102:A210 A213:A1048576">
+    <cfRule type="containsText" dxfId="73" priority="8" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="9" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A98)))</formula>
+    <cfRule type="containsText" dxfId="72" priority="9" operator="containsText" text="Test">
+      <formula>NOT(ISERROR(SEARCH("Test",A102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="10" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A98)))</formula>
+    <cfRule type="containsText" dxfId="71" priority="10" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",A102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="11" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A98)))</formula>
+    <cfRule type="containsText" dxfId="70" priority="11" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="12" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A98)))</formula>
+    <cfRule type="containsText" dxfId="69" priority="12" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A102)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4884,102 +5150,102 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1 A5:A34">
-    <cfRule type="containsText" dxfId="61" priority="38" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="68" priority="38" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="39" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="67" priority="39" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="66" priority="40" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="41" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="65" priority="41" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="42" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="64" priority="42" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A5:A34">
-    <cfRule type="containsText" dxfId="56" priority="36" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="63" priority="36" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="37" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="62" priority="37" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="54" priority="31" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="61" priority="31" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="32" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="60" priority="32" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="59" priority="33" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="34" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="58" priority="34" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="35" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="57" priority="35" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="49" priority="29" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="30" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="55" priority="30" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="containsText" dxfId="47" priority="24" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="54" priority="24" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="25" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="53" priority="25" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="52" priority="26" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="27" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="51" priority="27" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="28" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="50" priority="28" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="49" priority="22" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="48" priority="23" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="40" priority="17" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="47" priority="17" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="46" priority="18" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="19" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="45" priority="19" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="20" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="44" priority="20" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="42" priority="15" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="16" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="41" priority="16" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4991,7 +5257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -8280,124 +8546,124 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A92 A95:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:A94">
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="16" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F142:F143 F201:F202 F151 E142:E203">
-    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F149">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F149)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F184">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F184)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F176">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F162">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F162)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fixed bug in wind farm layout file import: rows with negative x values were being skipped. #bugfix #wind
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1924,77 +1924,7 @@
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="91">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF33CC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="84">
     <dxf>
       <fill>
         <patternFill>
@@ -3093,7 +3023,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3445,7 +3375,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B23" s="41" t="s">
         <v>509</v>
@@ -3957,80 +3887,80 @@
     <sortCondition ref="E2:E30"/>
   </sortState>
   <conditionalFormatting sqref="A1:A99">
-    <cfRule type="containsText" dxfId="90" priority="53" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="83" priority="53" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="54" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="82" priority="54" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="55" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="81" priority="55" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="56" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="80" priority="56" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="57" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="79" priority="57" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A210">
-    <cfRule type="containsText" dxfId="85" priority="46" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="78" priority="46" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="47" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="77" priority="47" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="containsText" dxfId="83" priority="20" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="76" priority="20" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="75" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="22" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="74" priority="22" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A100:A101">
-    <cfRule type="containsText" dxfId="80" priority="3" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="4" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="5" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="6" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A100)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A100)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A213:A1048576">
-    <cfRule type="containsText" dxfId="75" priority="1" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="68" priority="1" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A213)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="2" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A213)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A102:A210 A213:A1048576">
-    <cfRule type="containsText" dxfId="73" priority="8" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="66" priority="8" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="9" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="65" priority="9" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="10" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="64" priority="10" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="11" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="63" priority="11" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A102)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="12" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="62" priority="12" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A102)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5150,102 +5080,102 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1 A5:A34">
-    <cfRule type="containsText" dxfId="68" priority="38" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="61" priority="38" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="39" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="60" priority="39" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="40" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="59" priority="40" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="41" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="58" priority="41" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="42" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="57" priority="42" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A5:A34">
-    <cfRule type="containsText" dxfId="63" priority="36" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="56" priority="36" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="37" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="55" priority="37" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="61" priority="31" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="54" priority="31" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="32" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="53" priority="32" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="33" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="52" priority="33" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="34" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="51" priority="34" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="35" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="50" priority="35" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="56" priority="29" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="49" priority="29" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="30" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="48" priority="30" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="containsText" dxfId="54" priority="24" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="47" priority="24" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="25" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="46" priority="25" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="26" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="45" priority="26" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="27" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="44" priority="27" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="28" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="43" priority="28" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="containsText" dxfId="49" priority="22" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="42" priority="22" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="23" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="41" priority="23" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="47" priority="17" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="40" priority="17" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="18" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="39" priority="18" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="19" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="38" priority="19" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="20" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="37" priority="20" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="36" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="42" priority="15" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="35" priority="15" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="16" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="34" priority="16" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8546,124 +8476,124 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A92 A95:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="41" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="42" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="43" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:A94">
-    <cfRule type="containsText" dxfId="35" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="26" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="24" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="23" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="16" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F142:F143 F201:F202 F151 E142:E203">
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F149">
-    <cfRule type="containsText" dxfId="18" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F149)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F184">
-    <cfRule type="containsText" dxfId="15" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F184)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F176">
-    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F162">
-    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F162)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated the version upgrader for all PV variables.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="10785"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
   </bookViews>
   <sheets>
     <sheet name="To Do- FY15 Release" sheetId="5" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1279" uniqueCount="531">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1491,9 +1491,6 @@
     <t>stacked LCOE macro</t>
   </si>
   <si>
-    <t>Update SAM upgrade script for all variable changes</t>
-  </si>
-  <si>
     <t>Nate's parametric bug</t>
   </si>
   <si>
@@ -1624,6 +1621,15 @@
   </si>
   <si>
     <t>Update electricity rates help for monthly/hourly reconciliation</t>
+  </si>
+  <si>
+    <t>Update SAM upgrade script for CSP variable changes</t>
+  </si>
+  <si>
+    <t>Update SAM upgrade script for PV variable changes</t>
+  </si>
+  <si>
+    <t>Update SAM upgrade script for all battery/lifetime variables</t>
   </si>
 </sst>
 </file>
@@ -1721,7 +1727,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1811,12 +1817,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1840,7 +1840,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1916,7 +1916,6 @@
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
@@ -3019,11 +3018,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3069,7 +3068,7 @@
       </c>
       <c r="D2" s="49"/>
       <c r="E2" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -3084,7 +3083,7 @@
       </c>
       <c r="D3" s="49"/>
       <c r="E3" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3099,22 +3098,22 @@
       </c>
       <c r="D4" s="49"/>
       <c r="E4" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>484</v>
+        <v>529</v>
       </c>
       <c r="C5" s="48" t="s">
         <v>45</v>
       </c>
       <c r="D5" s="48"/>
       <c r="E5" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -3122,14 +3121,14 @@
         <v>192</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>485</v>
+        <v>528</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>47</v>
+        <v>303</v>
       </c>
       <c r="D6" s="48"/>
       <c r="E6" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -3137,14 +3136,14 @@
         <v>192</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>486</v>
+        <v>530</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>478</v>
+        <v>308</v>
       </c>
       <c r="D7" s="48"/>
       <c r="E7" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -3152,14 +3151,14 @@
         <v>192</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>225</v>
+        <v>47</v>
       </c>
       <c r="D8" s="48"/>
       <c r="E8" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -3167,14 +3166,14 @@
         <v>192</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>68</v>
+        <v>478</v>
       </c>
       <c r="D9" s="48"/>
       <c r="E9" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -3182,258 +3181,255 @@
         <v>192</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>308</v>
+        <v>225</v>
       </c>
       <c r="D10" s="48"/>
       <c r="E10" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="33" t="s">
-        <v>499</v>
+        <v>192</v>
       </c>
       <c r="B11" s="48" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>45</v>
+        <v>68</v>
       </c>
       <c r="D11" s="48"/>
       <c r="E11" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="33" t="s">
-        <v>499</v>
+        <v>192</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>501</v>
+        <v>308</v>
       </c>
       <c r="D12" s="48"/>
       <c r="E12" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="33" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>503</v>
+        <v>45</v>
       </c>
       <c r="D13" s="48"/>
       <c r="E13" s="48" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="33" t="s">
-        <v>192</v>
+        <v>498</v>
       </c>
       <c r="B14" s="48" t="s">
-        <v>522</v>
+        <v>499</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>68</v>
+        <v>500</v>
       </c>
       <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
+      <c r="E14" s="48" t="s">
+        <v>509</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="33" t="s">
-        <v>55</v>
+        <v>498</v>
       </c>
       <c r="B15" s="48" t="s">
-        <v>513</v>
+        <v>501</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>45</v>
+        <v>502</v>
       </c>
       <c r="D15" s="48"/>
       <c r="E15" s="48" t="s">
-        <v>510</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="40" t="s">
-        <v>231</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="42"/>
-      <c r="E16" s="41" t="s">
-        <v>511</v>
-      </c>
+      <c r="B16" s="48" t="s">
+        <v>521</v>
+      </c>
+      <c r="C16" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B17" s="41" t="s">
-        <v>487</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>488</v>
-      </c>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41" t="s">
-        <v>511</v>
-      </c>
-      <c r="F17" s="32" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+      <c r="B17" s="48" t="s">
+        <v>512</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B18" s="41" t="s">
-        <v>496</v>
+      <c r="B18" s="40" t="s">
+        <v>231</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D18" s="41"/>
+        <v>74</v>
+      </c>
+      <c r="D18" s="42"/>
       <c r="E18" s="41" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="33" t="s">
-        <v>499</v>
+        <v>192</v>
       </c>
       <c r="B19" s="41" t="s">
-        <v>504</v>
+        <v>486</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="D19" s="41"/>
       <c r="E19" s="41" t="s">
-        <v>511</v>
+        <v>510</v>
+      </c>
+      <c r="F19" s="32" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="33" t="s">
-        <v>499</v>
+        <v>192</v>
       </c>
       <c r="B20" s="41" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>501</v>
+        <v>46</v>
       </c>
       <c r="D20" s="41"/>
       <c r="E20" s="41" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="33" t="s">
-        <v>192</v>
+        <v>498</v>
       </c>
       <c r="B21" s="41" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>45</v>
+        <v>478</v>
       </c>
       <c r="D21" s="41"/>
       <c r="E21" s="41" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="33" t="s">
-        <v>192</v>
+        <v>498</v>
       </c>
       <c r="B22" s="41" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>45</v>
+        <v>500</v>
       </c>
       <c r="D22" s="41"/>
       <c r="E22" s="41" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="33" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="C23" s="41" t="s">
         <v>45</v>
       </c>
       <c r="D23" s="41"/>
       <c r="E23" s="41" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B24" s="44" t="s">
-        <v>357</v>
-      </c>
-      <c r="C24" s="45" t="s">
-        <v>493</v>
-      </c>
-      <c r="D24" s="46"/>
-      <c r="E24" s="45" t="s">
-        <v>512</v>
+      <c r="B24" s="41" t="s">
+        <v>507</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B25" s="45" t="s">
-        <v>489</v>
-      </c>
-      <c r="C25" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="B25" s="41" t="s">
+        <v>508</v>
+      </c>
+      <c r="C25" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="45"/>
-      <c r="E25" s="45" t="s">
-        <v>512</v>
-      </c>
-      <c r="F25" s="32" t="s">
-        <v>490</v>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="44" t="s">
+        <v>357</v>
+      </c>
+      <c r="C26" s="45" t="s">
         <v>492</v>
       </c>
-      <c r="C26" s="45" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="45"/>
+      <c r="D26" s="46"/>
       <c r="E26" s="45" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
@@ -3441,63 +3437,70 @@
         <v>192</v>
       </c>
       <c r="B27" s="45" t="s">
-        <v>506</v>
+        <v>488</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>478</v>
+        <v>45</v>
       </c>
       <c r="D27" s="45"/>
       <c r="E27" s="45" t="s">
-        <v>512</v>
+        <v>511</v>
+      </c>
+      <c r="F27" s="32" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="33" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B28" s="45" t="s">
-        <v>515</v>
+        <v>491</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>68</v>
+        <v>45</v>
       </c>
       <c r="D28" s="45"/>
       <c r="E28" s="45" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" s="43" t="s">
-        <v>118</v>
-      </c>
-      <c r="C29" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
+        <v>192</v>
+      </c>
+      <c r="B29" s="45" t="s">
+        <v>505</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>478</v>
+      </c>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="33" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="43" t="s">
-        <v>119</v>
-      </c>
-      <c r="C30" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="D30" s="43"/>
-      <c r="E30" s="43"/>
+        <v>55</v>
+      </c>
+      <c r="B30" s="45" t="s">
+        <v>514</v>
+      </c>
+      <c r="C30" s="45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45" t="s">
+        <v>511</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="33" t="s">
         <v>135</v>
       </c>
       <c r="B31" s="43" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="C31" s="43" t="s">
         <v>49</v>
@@ -3510,7 +3513,7 @@
         <v>135</v>
       </c>
       <c r="B32" s="43" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="C32" s="43" t="s">
         <v>49</v>
@@ -3519,42 +3522,42 @@
       <c r="E32" s="43"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="33"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
+      <c r="A33" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B33" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="C33" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="33"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="53"/>
-      <c r="E34" s="53"/>
+      <c r="A34" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>136</v>
+      </c>
+      <c r="C34" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="43"/>
+      <c r="E34" s="43"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B35" s="52" t="s">
-        <v>516</v>
-      </c>
-      <c r="C35" s="52" t="s">
-        <v>68</v>
-      </c>
+      <c r="A35" s="33"/>
+      <c r="B35" s="52"/>
+      <c r="C35" s="52"/>
       <c r="D35" s="52"/>
       <c r="E35" s="52"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="33" t="s">
-        <v>192</v>
-      </c>
-      <c r="B36" s="52" t="s">
-        <v>517</v>
-      </c>
-      <c r="C36" s="52" t="s">
-        <v>521</v>
-      </c>
+      <c r="A36" s="33"/>
+      <c r="B36" s="52"/>
+      <c r="C36" s="52"/>
       <c r="D36" s="52"/>
       <c r="E36" s="52"/>
     </row>
@@ -3562,124 +3565,144 @@
       <c r="A37" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B37" s="52" t="s">
-        <v>518</v>
-      </c>
-      <c r="C37" s="52" t="s">
-        <v>233</v>
-      </c>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
+      <c r="B37" s="51" t="s">
+        <v>515</v>
+      </c>
+      <c r="C37" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D37" s="51"/>
+      <c r="E37" s="51"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B38" s="52" t="s">
-        <v>519</v>
-      </c>
-      <c r="C38" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="52"/>
-      <c r="E38" s="52"/>
+      <c r="B38" s="51" t="s">
+        <v>516</v>
+      </c>
+      <c r="C38" s="51" t="s">
+        <v>520</v>
+      </c>
+      <c r="D38" s="51"/>
+      <c r="E38" s="51"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B39" s="52" t="s">
-        <v>520</v>
-      </c>
-      <c r="C39" s="52" t="s">
-        <v>68</v>
-      </c>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
+      <c r="B39" s="51" t="s">
+        <v>517</v>
+      </c>
+      <c r="C39" s="51" t="s">
+        <v>233</v>
+      </c>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B40" s="52" t="s">
-        <v>523</v>
-      </c>
-      <c r="C40" s="52" t="s">
+      <c r="B40" s="51" t="s">
+        <v>518</v>
+      </c>
+      <c r="C40" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="52"/>
-      <c r="E40" s="52"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B41" s="52" t="s">
-        <v>524</v>
-      </c>
-      <c r="C41" s="52" t="s">
+      <c r="B41" s="51" t="s">
+        <v>519</v>
+      </c>
+      <c r="C41" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B42" s="52" t="s">
-        <v>525</v>
-      </c>
-      <c r="C42" s="52" t="s">
+      <c r="B42" s="51" t="s">
+        <v>522</v>
+      </c>
+      <c r="C42" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D42" s="52"/>
-      <c r="E42" s="52"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B43" s="52" t="s">
-        <v>526</v>
-      </c>
-      <c r="C43" s="52" t="s">
+      <c r="B43" s="51" t="s">
+        <v>523</v>
+      </c>
+      <c r="C43" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="52"/>
-      <c r="E43" s="52"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="51"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B44" s="52" t="s">
-        <v>527</v>
-      </c>
-      <c r="C44" s="52" t="s">
+      <c r="B44" s="51" t="s">
+        <v>524</v>
+      </c>
+      <c r="C44" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="52"/>
-      <c r="E44" s="52"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="33" t="s">
         <v>192</v>
       </c>
-      <c r="B45" s="52" t="s">
-        <v>528</v>
-      </c>
-      <c r="C45" s="52" t="s">
+      <c r="B45" s="51" t="s">
+        <v>525</v>
+      </c>
+      <c r="C45" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="52"/>
-      <c r="E45" s="52"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46" s="33"/>
+      <c r="A46" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B46" s="51" t="s">
+        <v>526</v>
+      </c>
+      <c r="C46" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D46" s="51"/>
+      <c r="E46" s="51"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47" s="33"/>
+      <c r="A47" s="33" t="s">
+        <v>192</v>
+      </c>
+      <c r="B47" s="51" t="s">
+        <v>527</v>
+      </c>
+      <c r="C47" s="51" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="51"/>
+      <c r="E47" s="51"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="33"/>
@@ -3853,13 +3876,13 @@
       <c r="A104" s="33"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="34"/>
+      <c r="A105" s="33"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="33"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="33"/>
+      <c r="A107" s="34"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="33"/>
@@ -3879,14 +3902,20 @@
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="33"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148" s="34"/>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="33"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="33"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="34"/>
     </row>
   </sheetData>
   <sortState ref="A2:F30">
     <sortCondition ref="E2:E30"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A99">
+  <conditionalFormatting sqref="A1:A101">
     <cfRule type="containsText" dxfId="83" priority="53" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -3903,7 +3932,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A210">
+  <conditionalFormatting sqref="A1:A212">
     <cfRule type="containsText" dxfId="78" priority="46" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -3911,7 +3940,7 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E5">
+  <conditionalFormatting sqref="E5:E7">
     <cfRule type="containsText" dxfId="76" priority="20" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E5)))</formula>
     </cfRule>
@@ -3922,46 +3951,46 @@
       <formula>NOT(ISERROR(SEARCH("Yes",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A100:A101">
+  <conditionalFormatting sqref="A102:A103">
     <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A102)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A213:A1048576">
+  <conditionalFormatting sqref="A215:A1048576">
     <cfRule type="containsText" dxfId="68" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A215)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A215)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A102:A210 A213:A1048576">
+  <conditionalFormatting sqref="A104:A212 A215:A1048576">
     <cfRule type="containsText" dxfId="66" priority="8" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="65" priority="9" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="64" priority="10" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="63" priority="11" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="62" priority="12" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A104)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3974,7 +4003,7 @@
   <dimension ref="A1:U30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4133,471 +4162,471 @@
         <v>262</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="51" t="s">
+    <row r="9" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
         <v>206</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="50" t="s">
         <v>266</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="50" t="s">
         <v>267</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="50" t="s">
         <v>267</v>
       </c>
-      <c r="E9" s="51" t="s">
+      <c r="E9" s="50" t="s">
         <v>266</v>
       </c>
-      <c r="F9" s="51" t="s">
+      <c r="F9" s="50" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+    <row r="10" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="50" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="50" t="s">
         <v>270</v>
       </c>
-      <c r="F10" s="25">
+      <c r="F10" s="50">
         <v>-0.11</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="50" t="s">
         <v>205</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="50" t="s">
         <v>252</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="50" t="s">
         <v>271</v>
       </c>
-      <c r="E11" s="25" t="s">
+      <c r="E11" s="50" t="s">
         <v>270</v>
       </c>
-      <c r="F11" s="25">
+      <c r="F11" s="50">
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+    <row r="12" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="19" t="s">
         <v>312</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="19" t="s">
         <v>311</v>
       </c>
-      <c r="E12" s="25" t="s">
+      <c r="E12" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="G12" s="25" t="s">
+      <c r="G12" s="19" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="E13" s="25" t="s">
+      <c r="E13" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="F13" s="25" t="s">
+      <c r="F13" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="19" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+    <row r="14" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="C14" s="25" t="s">
+      <c r="C14" s="19" t="s">
         <v>318</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="E14" s="25" t="s">
+      <c r="E14" s="19" t="s">
         <v>319</v>
       </c>
-      <c r="F14" s="25" t="s">
+      <c r="F14" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="19" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+    <row r="15" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C15" s="25" t="s">
+      <c r="C15" s="19" t="s">
         <v>320</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="19" t="s">
         <v>324</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="F15" s="25" t="s">
+      <c r="F15" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G15" s="25" t="s">
+      <c r="G15" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="25" t="s">
+    <row r="16" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C16" s="25" t="s">
+      <c r="C16" s="19" t="s">
         <v>321</v>
       </c>
-      <c r="D16" s="25" t="s">
+      <c r="D16" s="19" t="s">
         <v>325</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="F16" s="25" t="s">
+      <c r="F16" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G16" s="25" t="s">
+      <c r="G16" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="25" t="s">
+    <row r="17" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C17" s="25" t="s">
+      <c r="C17" s="19" t="s">
         <v>323</v>
       </c>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="19" t="s">
         <v>326</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="F17" s="25" t="s">
+      <c r="F17" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
+    <row r="18" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B18" s="25" t="s">
+      <c r="B18" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C18" s="25" t="s">
+      <c r="C18" s="19" t="s">
         <v>322</v>
       </c>
-      <c r="D18" s="25" t="s">
+      <c r="D18" s="19" t="s">
         <v>340</v>
       </c>
-      <c r="E18" s="25" t="s">
+      <c r="E18" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="F18" s="25" t="s">
+      <c r="F18" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G18" s="25" t="s">
+      <c r="G18" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+    <row r="19" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B19" s="25" t="s">
+      <c r="B19" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C19" s="25" t="s">
+      <c r="C19" s="19" t="s">
         <v>338</v>
       </c>
-      <c r="D19" s="25" t="s">
+      <c r="D19" s="19" t="s">
         <v>341</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="F19" s="25" t="s">
+      <c r="F19" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G19" s="25" t="s">
+      <c r="G19" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
+    <row r="20" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="19" t="s">
         <v>339</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="19" t="s">
         <v>342</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="25" t="s">
+    <row r="21" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C21" s="25" t="s">
+      <c r="C21" s="19" t="s">
         <v>343</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="19" t="s">
         <v>346</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E21" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="F21" s="25" t="s">
+      <c r="F21" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G21" s="25" t="s">
+      <c r="G21" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="25" t="s">
+    <row r="22" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B22" s="25" t="s">
+      <c r="B22" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C22" s="25" t="s">
+      <c r="C22" s="19" t="s">
         <v>344</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="19" t="s">
         <v>347</v>
       </c>
-      <c r="E22" s="25" t="s">
+      <c r="E22" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="F22" s="25" t="s">
+      <c r="F22" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G22" s="25" t="s">
+      <c r="G22" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="25" t="s">
+    <row r="23" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C23" s="25" t="s">
+      <c r="C23" s="19" t="s">
         <v>345</v>
       </c>
-      <c r="D23" s="25" t="s">
+      <c r="D23" s="19" t="s">
         <v>348</v>
       </c>
-      <c r="E23" s="25" t="s">
+      <c r="E23" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="25" t="s">
+    <row r="24" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="19" t="s">
         <v>349</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="19" t="s">
         <v>352</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+    <row r="25" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="19" t="s">
         <v>350</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="19" t="s">
         <v>353</v>
       </c>
-      <c r="E25" s="25" t="s">
+      <c r="E25" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="F25" s="25" t="s">
+      <c r="F25" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G25" s="25" t="s">
+      <c r="G25" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+    <row r="26" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="C26" s="25" t="s">
+      <c r="C26" s="19" t="s">
         <v>351</v>
       </c>
-      <c r="D26" s="25" t="s">
+      <c r="D26" s="19" t="s">
         <v>354</v>
       </c>
-      <c r="E26" s="25" t="s">
+      <c r="E26" s="19" t="s">
         <v>355</v>
       </c>
-      <c r="F26" s="25" t="s">
+      <c r="F26" s="19" t="s">
         <v>330</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="19" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="25" t="s">
+    <row r="27" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B27" s="25" t="s">
+      <c r="B27" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C27" s="25" t="s">
+      <c r="C27" s="19" t="s">
         <v>332</v>
       </c>
-      <c r="D27" s="25" t="s">
+      <c r="D27" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="E27" s="25" t="s">
+      <c r="E27" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="F27" s="25" t="s">
+      <c r="F27" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="G27" s="25" t="s">
+      <c r="G27" s="19" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="25" t="s">
+    <row r="28" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="C28" s="19" t="s">
         <v>336</v>
       </c>
-      <c r="D28" s="25" t="s">
+      <c r="D28" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="E28" s="25" t="s">
+      <c r="E28" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="F28" s="25" t="s">
+      <c r="F28" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="G28" s="25" t="s">
+      <c r="G28" s="19" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+    <row r="29" spans="1:7" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="19" t="s">
         <v>206</v>
       </c>
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="19" t="s">
         <v>337</v>
       </c>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="19" t="s">
         <v>334</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="19" t="s">
         <v>333</v>
       </c>
-      <c r="F29" s="25" t="s">
+      <c r="F29" s="19" t="s">
         <v>335</v>
       </c>
-      <c r="G29" s="25" t="s">
+      <c r="G29" s="19" t="s">
         <v>303</v>
       </c>
     </row>
@@ -5391,7 +5420,7 @@
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated To-Do list for battery variables
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1727,7 +1727,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1817,6 +1817,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -1840,7 +1846,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1918,6 +1924,9 @@
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -3022,7 +3031,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3132,8 +3141,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="33" t="s">
-        <v>192</v>
+      <c r="A7" s="53" t="s">
+        <v>55</v>
       </c>
       <c r="B7" s="48" t="s">
         <v>530</v>

</xml_diff>

<commit_message>
to do list update.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="552">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -3139,8 +3139,8 @@
   <dimension ref="A1:F154"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D35" sqref="D35"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3661,9 +3661,7 @@
       <c r="B34" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="C34" s="42" t="s">
-        <v>46</v>
-      </c>
+      <c r="C34" s="42"/>
       <c r="D34" s="42"/>
       <c r="E34" s="42"/>
     </row>

</xml_diff>

<commit_message>
Updated wind power commercial default with buy=sell removed Updated TODO items Updated default configuration outputs
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
   </bookViews>
@@ -18,12 +23,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="554">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1694,6 +1699,12 @@
   </si>
   <si>
     <t>Test web update system for all platforms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">battery macro tests and dc connected battery loss diagram for inverter efficiency </t>
+  </si>
+  <si>
+    <t>Nick/Steve</t>
   </si>
 </sst>
 </file>
@@ -2887,7 +2898,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2922,7 +2933,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3131,11 +3142,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F154"/>
+  <dimension ref="A1:F155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3881,7 +3892,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
-        <v>192</v>
+        <v>460</v>
       </c>
       <c r="B52" s="50" t="s">
         <v>547</v>
@@ -3894,7 +3905,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
-        <v>192</v>
+        <v>460</v>
       </c>
       <c r="B53" s="50" t="s">
         <v>548</v>
@@ -3910,14 +3921,24 @@
         <v>192</v>
       </c>
       <c r="B54" s="50" t="s">
-        <v>549</v>
-      </c>
-      <c r="C54" s="50"/>
+        <v>552</v>
+      </c>
+      <c r="C54" s="50" t="s">
+        <v>553</v>
+      </c>
       <c r="D54" s="50"/>
       <c r="E54" s="50"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="32"/>
+      <c r="A55" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B55" s="50" t="s">
+        <v>549</v>
+      </c>
+      <c r="C55" s="50"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="50"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="32"/>
@@ -4085,10 +4106,10 @@
       <c r="A110" s="32"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A111" s="33"/>
+      <c r="A111" s="32"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A112" s="32"/>
+      <c r="A112" s="33"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="32"/>
@@ -4111,14 +4132,17 @@
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="32"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A154" s="33"/>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="32"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A155" s="33"/>
     </row>
   </sheetData>
   <sortState ref="A2:F30">
     <sortCondition ref="E2:E30"/>
   </sortState>
-  <conditionalFormatting sqref="A1:A105">
+  <conditionalFormatting sqref="A1:A106">
     <cfRule type="containsText" dxfId="83" priority="53" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4135,7 +4159,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A216">
+  <conditionalFormatting sqref="A1:A217">
     <cfRule type="containsText" dxfId="78" priority="46" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4154,46 +4178,46 @@
       <formula>NOT(ISERROR(SEARCH("Yes",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A106:A107">
+  <conditionalFormatting sqref="A107:A108">
     <cfRule type="containsText" dxfId="73" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="72" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="71" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="70" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="69" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A107)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A219:A1048576">
+  <conditionalFormatting sqref="A220:A1048576">
     <cfRule type="containsText" dxfId="68" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A219)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A220)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="67" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A219)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A220)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A108:A216 A219:A1048576">
+  <conditionalFormatting sqref="A109:A217 A220:A1048576">
     <cfRule type="containsText" dxfId="66" priority="8" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="65" priority="9" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="64" priority="10" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="63" priority="11" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="62" priority="12" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
deleted UI variables from MSPT to reflect TES is assumed direct in this model
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="To Do- FY15 Release" sheetId="5" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1354" uniqueCount="555">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="560">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1703,6 +1703,21 @@
   </si>
   <si>
     <t>Decouple the transposition model from the 3D shading model for diffuse</t>
+  </si>
+  <si>
+    <t>csp.pt.tes.storage_bypass</t>
+  </si>
+  <si>
+    <t>Bypass N/A for tower because storage HTF = rec/pc HTF (no storage HX)</t>
+  </si>
+  <si>
+    <t>tes_pump_coef</t>
+  </si>
+  <si>
+    <t>Molten Salt Tower Parasitics</t>
+  </si>
+  <si>
+    <t>storage HTF = rec/pc HTF (no storage HX), so no pumping losses</t>
   </si>
 </sst>
 </file>
@@ -3142,7 +3157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F155"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
@@ -4233,17 +4248,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:V35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="25" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="25" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="25" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51" style="25" customWidth="1"/>
@@ -5024,6 +5039,52 @@
         <v>540</v>
       </c>
       <c r="H33" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>555</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>556</v>
+      </c>
+      <c r="G34" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F35" s="25" t="s">
+        <v>559</v>
+      </c>
+      <c r="G35" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H35" s="19" t="s">
         <v>302</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#deleted unused variables in Molten Salt Tower Parasitics UI page
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1368" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="568">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1718,6 +1718,30 @@
   </si>
   <si>
     <t>storage HTF = rec/pc HTF (no storage HX), so no pumping losses</t>
+  </si>
+  <si>
+    <t>P_storage_pump</t>
+  </si>
+  <si>
+    <t>storage_bypass</t>
+  </si>
+  <si>
+    <t>recirc_source</t>
+  </si>
+  <si>
+    <t>not used</t>
+  </si>
+  <si>
+    <t>recirc_htf_eff</t>
+  </si>
+  <si>
+    <t>flow_from_storage</t>
+  </si>
+  <si>
+    <t>P_hot_tank</t>
+  </si>
+  <si>
+    <t>csp.pt.par.bop_c1</t>
   </si>
 </sst>
 </file>
@@ -4248,10 +4272,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V35"/>
+  <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5085,6 +5109,167 @@
         <v>541</v>
       </c>
       <c r="H35" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F36" s="25" t="s">
+        <v>559</v>
+      </c>
+      <c r="G36" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H36" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F37" s="25" t="s">
+        <v>559</v>
+      </c>
+      <c r="G37" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G38" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>564</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G39" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>565</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G40" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H40" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>566</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G41" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G42" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H42" s="19" t="s">
         <v>302</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#deleted unused variables and removed corresponding SSC INPUTS from dsg tower compute module.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="568">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="569">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1742,6 +1742,9 @@
   </si>
   <si>
     <t>csp.pt.par.bop_c1</t>
+  </si>
+  <si>
+    <t>Direct Steam Tower Parasitics</t>
   </si>
 </sst>
 </file>
@@ -4272,10 +4275,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V42"/>
+  <dimension ref="A1:V48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5040,7 +5043,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="19" t="s">
         <v>206</v>
       </c>
@@ -5066,7 +5069,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
         <v>207</v>
       </c>
@@ -5089,7 +5092,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>207</v>
       </c>
@@ -5112,7 +5115,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="25" t="s">
         <v>207</v>
       </c>
@@ -5135,7 +5138,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>207</v>
       </c>
@@ -5158,7 +5161,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="25" t="s">
         <v>207</v>
       </c>
@@ -5181,7 +5184,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="25" t="s">
         <v>207</v>
       </c>
@@ -5204,7 +5207,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="25" t="s">
         <v>207</v>
       </c>
@@ -5227,7 +5230,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="25" t="s">
         <v>207</v>
       </c>
@@ -5250,7 +5253,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="25" t="s">
         <v>207</v>
       </c>
@@ -5270,6 +5273,145 @@
         <v>541</v>
       </c>
       <c r="H42" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>560</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G43" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H43" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="I43" s="19"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>566</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G44" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>562</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G45" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>561</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G46" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>564</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G47" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>565</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>568</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G48" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H48" s="19" t="s">
         <v>302</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#deleted additional unused variables and removed corresponding SSC INPUTs
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1459" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="578">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1745,6 +1745,33 @@
   </si>
   <si>
     <t>Direct Steam Tower Parasitics</t>
+  </si>
+  <si>
+    <t>rec_htf_flow</t>
+  </si>
+  <si>
+    <t>Direct Steam Tower Receiver</t>
+  </si>
+  <si>
+    <t>ref_htf_flow</t>
+  </si>
+  <si>
+    <t>P_cold_tank</t>
+  </si>
+  <si>
+    <t>P_tower_conv</t>
+  </si>
+  <si>
+    <t>P_tower_rad</t>
+  </si>
+  <si>
+    <t>P_htf_pump</t>
+  </si>
+  <si>
+    <t>night_recirc</t>
+  </si>
+  <si>
+    <t>mode</t>
   </si>
 </sst>
 </file>
@@ -4275,10 +4302,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V48"/>
+  <dimension ref="A1:V56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5412,6 +5439,190 @@
         <v>541</v>
       </c>
       <c r="H48" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C49" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G49" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H49" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>571</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G50" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H50" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B51" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>572</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G51" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H51" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B52" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>573</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G52" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>574</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G53" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H53" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>575</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G54" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B55" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C55" s="19" t="s">
+        <v>576</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G55" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H55" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B56" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C56" s="19" t="s">
+        <v>577</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F56" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G56" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H56" s="19" t="s">
         <v>302</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed ui variables that were previously used in DSG tower model to describe material connecting receiver tubes. current model only allows design with tubes that are directly adjacent
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1515" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="583">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1772,6 +1772,21 @@
   </si>
   <si>
     <t>mode</t>
+  </si>
+  <si>
+    <t>th_fin</t>
+  </si>
+  <si>
+    <t>l_fin</t>
+  </si>
+  <si>
+    <t>emis_fin</t>
+  </si>
+  <si>
+    <t>abs_fin</t>
+  </si>
+  <si>
+    <t>mat_fin</t>
   </si>
 </sst>
 </file>
@@ -4302,10 +4317,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V56"/>
+  <dimension ref="A1:V61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5626,9 +5641,124 @@
         <v>302</v>
       </c>
     </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B57" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C57" s="19" t="s">
+        <v>578</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G57" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>579</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G58" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H58" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C59" s="19" t="s">
+        <v>580</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G59" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H59" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C60" s="19" t="s">
+        <v>581</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G60" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H60" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B61" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C61" s="19" t="s">
+        <v>582</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G61" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H61" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A58">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A65">
       <formula1>Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Deleted independent emis and abs values for boiler/sh/rh and using one set for all. (previously, sh and rh were hardcoded in the ui and the boiler values were exposed to the user)
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="589">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1787,6 +1787,24 @@
   </si>
   <si>
     <t>mat_fin</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>abs_boiler</t>
+  </si>
+  <si>
+    <t>emis_sh</t>
+  </si>
+  <si>
+    <t>abs_sh</t>
+  </si>
+  <si>
+    <t>emis_rh</t>
+  </si>
+  <si>
+    <t>abs_rh</t>
   </si>
 </sst>
 </file>
@@ -4317,10 +4335,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V61"/>
+  <dimension ref="A1:V67"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="C60" sqref="C60"/>
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5046,6 +5064,7 @@
       <c r="C31" s="19" t="s">
         <v>531</v>
       </c>
+      <c r="D31" s="19"/>
       <c r="E31" s="19" t="s">
         <v>532</v>
       </c>
@@ -5121,6 +5140,7 @@
       <c r="C34" s="19" t="s">
         <v>555</v>
       </c>
+      <c r="D34" s="19"/>
       <c r="E34" s="19" t="s">
         <v>532</v>
       </c>
@@ -5144,6 +5164,7 @@
       <c r="C35" s="19" t="s">
         <v>557</v>
       </c>
+      <c r="D35" s="19"/>
       <c r="E35" s="19" t="s">
         <v>558</v>
       </c>
@@ -5167,6 +5188,7 @@
       <c r="C36" s="19" t="s">
         <v>560</v>
       </c>
+      <c r="D36" s="19"/>
       <c r="E36" s="19" t="s">
         <v>558</v>
       </c>
@@ -5190,6 +5212,7 @@
       <c r="C37" s="19" t="s">
         <v>561</v>
       </c>
+      <c r="D37" s="19"/>
       <c r="E37" s="19" t="s">
         <v>558</v>
       </c>
@@ -5213,6 +5236,7 @@
       <c r="C38" s="19" t="s">
         <v>562</v>
       </c>
+      <c r="D38" s="19"/>
       <c r="E38" s="19" t="s">
         <v>558</v>
       </c>
@@ -5236,6 +5260,7 @@
       <c r="C39" s="19" t="s">
         <v>564</v>
       </c>
+      <c r="D39" s="19"/>
       <c r="E39" s="19" t="s">
         <v>558</v>
       </c>
@@ -5259,6 +5284,7 @@
       <c r="C40" s="19" t="s">
         <v>565</v>
       </c>
+      <c r="D40" s="19"/>
       <c r="E40" s="19" t="s">
         <v>558</v>
       </c>
@@ -5282,6 +5308,7 @@
       <c r="C41" s="19" t="s">
         <v>566</v>
       </c>
+      <c r="D41" s="19"/>
       <c r="E41" s="19" t="s">
         <v>558</v>
       </c>
@@ -5305,6 +5332,7 @@
       <c r="C42" s="19" t="s">
         <v>567</v>
       </c>
+      <c r="D42" s="19"/>
       <c r="E42" s="19" t="s">
         <v>558</v>
       </c>
@@ -5328,6 +5356,7 @@
       <c r="C43" s="19" t="s">
         <v>560</v>
       </c>
+      <c r="D43" s="19"/>
       <c r="E43" s="19" t="s">
         <v>568</v>
       </c>
@@ -5352,6 +5381,7 @@
       <c r="C44" s="19" t="s">
         <v>566</v>
       </c>
+      <c r="D44" s="19"/>
       <c r="E44" s="19" t="s">
         <v>568</v>
       </c>
@@ -5375,6 +5405,7 @@
       <c r="C45" s="19" t="s">
         <v>562</v>
       </c>
+      <c r="D45" s="19"/>
       <c r="E45" s="19" t="s">
         <v>568</v>
       </c>
@@ -5398,6 +5429,7 @@
       <c r="C46" s="19" t="s">
         <v>561</v>
       </c>
+      <c r="D46" s="19"/>
       <c r="E46" s="19" t="s">
         <v>568</v>
       </c>
@@ -5421,6 +5453,7 @@
       <c r="C47" s="19" t="s">
         <v>564</v>
       </c>
+      <c r="D47" s="19"/>
       <c r="E47" s="19" t="s">
         <v>568</v>
       </c>
@@ -5444,6 +5477,7 @@
       <c r="C48" s="19" t="s">
         <v>565</v>
       </c>
+      <c r="D48" s="19"/>
       <c r="E48" s="19" t="s">
         <v>568</v>
       </c>
@@ -5467,6 +5501,7 @@
       <c r="C49" s="19" t="s">
         <v>569</v>
       </c>
+      <c r="D49" s="19"/>
       <c r="E49" s="19" t="s">
         <v>570</v>
       </c>
@@ -5490,6 +5525,7 @@
       <c r="C50" s="19" t="s">
         <v>571</v>
       </c>
+      <c r="D50" s="19"/>
       <c r="E50" s="19" t="s">
         <v>570</v>
       </c>
@@ -5513,6 +5549,7 @@
       <c r="C51" s="19" t="s">
         <v>572</v>
       </c>
+      <c r="D51" s="19"/>
       <c r="E51" s="19" t="s">
         <v>570</v>
       </c>
@@ -5536,6 +5573,7 @@
       <c r="C52" s="19" t="s">
         <v>573</v>
       </c>
+      <c r="D52" s="19"/>
       <c r="E52" s="19" t="s">
         <v>570</v>
       </c>
@@ -5559,6 +5597,7 @@
       <c r="C53" s="19" t="s">
         <v>574</v>
       </c>
+      <c r="D53" s="19"/>
       <c r="E53" s="19" t="s">
         <v>570</v>
       </c>
@@ -5582,6 +5621,7 @@
       <c r="C54" s="19" t="s">
         <v>575</v>
       </c>
+      <c r="D54" s="19"/>
       <c r="E54" s="19" t="s">
         <v>570</v>
       </c>
@@ -5605,6 +5645,7 @@
       <c r="C55" s="19" t="s">
         <v>576</v>
       </c>
+      <c r="D55" s="19"/>
       <c r="E55" s="19" t="s">
         <v>570</v>
       </c>
@@ -5628,6 +5669,7 @@
       <c r="C56" s="19" t="s">
         <v>577</v>
       </c>
+      <c r="D56" s="19"/>
       <c r="E56" s="19" t="s">
         <v>570</v>
       </c>
@@ -5651,6 +5693,7 @@
       <c r="C57" s="19" t="s">
         <v>578</v>
       </c>
+      <c r="D57" s="19"/>
       <c r="E57" s="19" t="s">
         <v>570</v>
       </c>
@@ -5674,6 +5717,7 @@
       <c r="C58" s="19" t="s">
         <v>579</v>
       </c>
+      <c r="D58" s="19"/>
       <c r="E58" s="19" t="s">
         <v>570</v>
       </c>
@@ -5697,6 +5741,7 @@
       <c r="C59" s="19" t="s">
         <v>580</v>
       </c>
+      <c r="D59" s="19"/>
       <c r="E59" s="19" t="s">
         <v>570</v>
       </c>
@@ -5720,6 +5765,7 @@
       <c r="C60" s="19" t="s">
         <v>581</v>
       </c>
+      <c r="D60" s="19"/>
       <c r="E60" s="19" t="s">
         <v>570</v>
       </c>
@@ -5743,6 +5789,7 @@
       <c r="C61" s="19" t="s">
         <v>582</v>
       </c>
+      <c r="D61" s="19"/>
       <c r="E61" s="19" t="s">
         <v>570</v>
       </c>
@@ -5756,9 +5803,133 @@
         <v>302</v>
       </c>
     </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B62" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C62" s="19" t="s">
+        <v>584</v>
+      </c>
+      <c r="D62" s="19"/>
+      <c r="E62" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G62" s="56" t="s">
+        <v>583</v>
+      </c>
+      <c r="H62" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B63" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C63" s="19" t="s">
+        <v>585</v>
+      </c>
+      <c r="D63" s="19"/>
+      <c r="E63" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G63" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H63" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B64" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>586</v>
+      </c>
+      <c r="D64" s="19"/>
+      <c r="E64" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G64" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H64" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B65" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>587</v>
+      </c>
+      <c r="D65" s="19"/>
+      <c r="E65" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G65" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H65" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B66" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C66" s="19" t="s">
+        <v>588</v>
+      </c>
+      <c r="D66" s="19"/>
+      <c r="E66" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G66" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H66" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E67" s="19"/>
+      <c r="F67" s="19"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A65">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A66">
       <formula1>Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
removed aux_array and bop_array that were hardcoded to 0 and passed to Type251. Now hardcoding in the compute module
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1585" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="591">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1805,6 +1805,12 @@
   </si>
   <si>
     <t>abs_rh</t>
+  </si>
+  <si>
+    <t>aux_array</t>
+  </si>
+  <si>
+    <t>bop_array</t>
   </si>
 </sst>
 </file>
@@ -4335,10 +4341,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V67"/>
+  <dimension ref="A1:V68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C68" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5924,12 +5930,54 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E67" s="19"/>
-      <c r="F67" s="19"/>
+      <c r="A67" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B67" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>589</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G67" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H67" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B68" s="19" t="s">
+        <v>251</v>
+      </c>
+      <c r="C68" s="19" t="s">
+        <v>590</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>558</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G68" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H68" s="19" t="s">
+        <v>302</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A66">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A73">
       <formula1>Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
deleted variables that were either redundant, unused, or constant (and could be hardcoded in the computer module)
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1599" uniqueCount="591">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1725" uniqueCount="611">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1811,6 +1811,66 @@
   </si>
   <si>
     <t>bop_array</t>
+  </si>
+  <si>
+    <t>m_dot_htf_ref</t>
+  </si>
+  <si>
+    <t>Molten Salt Tower Power Block</t>
+  </si>
+  <si>
+    <t>T_pb_out</t>
+  </si>
+  <si>
+    <t>fthr_ok</t>
+  </si>
+  <si>
+    <t>pb_fixed_par_cntl</t>
+  </si>
+  <si>
+    <t>dt_cold</t>
+  </si>
+  <si>
+    <t>dt_hot</t>
+  </si>
+  <si>
+    <t>hx_config</t>
+  </si>
+  <si>
+    <t>is_hx</t>
+  </si>
+  <si>
+    <t>tech_type</t>
+  </si>
+  <si>
+    <t>deg_wind</t>
+  </si>
+  <si>
+    <t>Molten Salt Tower Receiver</t>
+  </si>
+  <si>
+    <t>P_htf</t>
+  </si>
+  <si>
+    <t>T_salt_cold</t>
+  </si>
+  <si>
+    <t>Molten Salt Power Block</t>
+  </si>
+  <si>
+    <t>HTF</t>
+  </si>
+  <si>
+    <t>Design_power</t>
+  </si>
+  <si>
+    <t>csp.pt.pwrb.min_restart_time</t>
+  </si>
+  <si>
+    <t>csp.pt.rec.max_rec_flux</t>
+  </si>
+  <si>
+    <t>store_fluid</t>
   </si>
 </sst>
 </file>
@@ -4341,17 +4401,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V68"/>
+  <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C68" sqref="C68"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.85546875" style="25" customWidth="1"/>
     <col min="2" max="2" width="21.140625" style="25" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" style="25" customWidth="1"/>
+    <col min="3" max="3" width="28" style="25" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" style="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33" style="25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="51" style="25" customWidth="1"/>
@@ -5975,9 +6035,423 @@
         <v>302</v>
       </c>
     </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B69" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C69" s="19" t="s">
+        <v>591</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G69" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H69" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B70" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C70" s="19" t="s">
+        <v>593</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G70" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H70" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B71" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C71" s="19" t="s">
+        <v>577</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G71" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H71" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B72" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C72" s="19" t="s">
+        <v>594</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G72" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H72" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B73" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C73" s="19" t="s">
+        <v>595</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G73" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H73" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B74" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C74" s="19" t="s">
+        <v>596</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G74" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H74" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B75" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C75" s="19" t="s">
+        <v>597</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G75" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H75" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B76" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C76" s="19" t="s">
+        <v>598</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G76" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H76" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B77" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C77" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G77" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H77" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B78" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C78" s="19" t="s">
+        <v>600</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>592</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G78" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H78" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B79" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>601</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G79" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H79" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B80" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C80" s="19" t="s">
+        <v>603</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G80" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H80" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B81" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C81" s="19" t="s">
+        <v>604</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G81" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H81" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B82" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C82" s="19" t="s">
+        <v>606</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="F82" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G82" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H82" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B83" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C83" s="19" t="s">
+        <v>607</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="F83" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G83" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H83" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B84" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>608</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="F84" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G84" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H84" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B85" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C85" s="19" t="s">
+        <v>609</v>
+      </c>
+      <c r="E85" s="19" t="s">
+        <v>605</v>
+      </c>
+      <c r="F85" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G85" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H85" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="B86" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C86" s="19" t="s">
+        <v>610</v>
+      </c>
+      <c r="E86" s="19" t="s">
+        <v>532</v>
+      </c>
+      <c r="F86" s="19" t="s">
+        <v>563</v>
+      </c>
+      <c r="G86" s="56" t="s">
+        <v>541</v>
+      </c>
+      <c r="H86" s="19" t="s">
+        <v>302</v>
+      </c>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A73">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A86">
       <formula1>Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
#variable_changes to DSG PT
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1739" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="619">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1880,6 +1880,21 @@
   </si>
   <si>
     <t>redundant - different variable used in compute module</t>
+  </si>
+  <si>
+    <t>csp.pt.par.piping_length_const</t>
+  </si>
+  <si>
+    <t>piping_length_mult</t>
+  </si>
+  <si>
+    <t>variables were incorrectly switched in old version - would only impact simulations that performed real-time tower height optimization</t>
+  </si>
+  <si>
+    <t>csp.pt.par.piping_length_mult</t>
+  </si>
+  <si>
+    <t>piping_length_add</t>
   </si>
 </sst>
 </file>
@@ -2096,7 +2111,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2189,6 +2204,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4410,10 +4437,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V88"/>
+  <dimension ref="A1:V90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6504,9 +6531,49 @@
         <v>302</v>
       </c>
     </row>
+    <row r="89" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A89" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="B89" s="58" t="s">
+        <v>252</v>
+      </c>
+      <c r="C89" s="58" t="s">
+        <v>614</v>
+      </c>
+      <c r="D89" s="57"/>
+      <c r="E89" s="58" t="s">
+        <v>615</v>
+      </c>
+      <c r="F89" s="59" t="s">
+        <v>616</v>
+      </c>
+      <c r="G89" s="57"/>
+      <c r="H89" s="60"/>
+    </row>
+    <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90" s="57" t="s">
+        <v>206</v>
+      </c>
+      <c r="B90" s="58" t="s">
+        <v>252</v>
+      </c>
+      <c r="C90" s="58" t="s">
+        <v>617</v>
+      </c>
+      <c r="D90" s="57"/>
+      <c r="E90" s="58" t="s">
+        <v>618</v>
+      </c>
+      <c r="F90" s="59" t="s">
+        <v>616</v>
+      </c>
+      <c r="G90" s="57"/>
+      <c r="H90" s="60"/>
+    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A88">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A2:A90">
       <formula1>Types</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
#changed emis_boiler to rec_emis
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1749" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1761" uniqueCount="622">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1789,9 +1789,6 @@
     <t>mat_fin</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>abs_boiler</t>
   </si>
   <si>
@@ -1895,6 +1892,18 @@
   </si>
   <si>
     <t>piping_length_add</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>emis_boiler</t>
+  </si>
+  <si>
+    <t>rec_emis</t>
+  </si>
+  <si>
+    <t>User-input emissivity used for boiler/sh/rh</t>
   </si>
 </sst>
 </file>
@@ -2111,7 +2120,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2214,8 +2223,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4437,10 +4449,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V90"/>
+  <dimension ref="A1:V91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D90" sqref="D90"/>
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5913,7 +5925,7 @@
         <v>252</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D62" s="19"/>
       <c r="E62" s="19" t="s">
@@ -5923,7 +5935,7 @@
         <v>563</v>
       </c>
       <c r="G62" s="56" t="s">
-        <v>583</v>
+        <v>541</v>
       </c>
       <c r="H62" s="19" t="s">
         <v>302</v>
@@ -5937,7 +5949,7 @@
         <v>252</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D63" s="19"/>
       <c r="E63" s="19" t="s">
@@ -5961,7 +5973,7 @@
         <v>252</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D64" s="19"/>
       <c r="E64" s="19" t="s">
@@ -5985,7 +5997,7 @@
         <v>252</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D65" s="19"/>
       <c r="E65" s="19" t="s">
@@ -6009,7 +6021,7 @@
         <v>252</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="D66" s="19"/>
       <c r="E66" s="19" t="s">
@@ -6033,7 +6045,7 @@
         <v>251</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E67" s="19" t="s">
         <v>558</v>
@@ -6056,7 +6068,7 @@
         <v>251</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="E68" s="19" t="s">
         <v>558</v>
@@ -6079,10 +6091,10 @@
         <v>252</v>
       </c>
       <c r="C69" s="19" t="s">
+        <v>590</v>
+      </c>
+      <c r="E69" s="19" t="s">
         <v>591</v>
-      </c>
-      <c r="E69" s="19" t="s">
-        <v>592</v>
       </c>
       <c r="F69" s="19" t="s">
         <v>563</v>
@@ -6102,10 +6114,10 @@
         <v>252</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F70" s="19" t="s">
         <v>563</v>
@@ -6128,7 +6140,7 @@
         <v>577</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F71" s="19" t="s">
         <v>563</v>
@@ -6148,10 +6160,10 @@
         <v>252</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F72" s="19" t="s">
         <v>563</v>
@@ -6171,10 +6183,10 @@
         <v>252</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F73" s="19" t="s">
         <v>563</v>
@@ -6194,10 +6206,10 @@
         <v>252</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F74" s="19" t="s">
         <v>563</v>
@@ -6217,10 +6229,10 @@
         <v>252</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F75" s="19" t="s">
         <v>563</v>
@@ -6240,10 +6252,10 @@
         <v>252</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F76" s="19" t="s">
         <v>563</v>
@@ -6263,10 +6275,10 @@
         <v>252</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F77" s="19" t="s">
         <v>563</v>
@@ -6286,10 +6298,10 @@
         <v>252</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F78" s="19" t="s">
         <v>563</v>
@@ -6309,10 +6321,10 @@
         <v>252</v>
       </c>
       <c r="C79" s="19" t="s">
+        <v>600</v>
+      </c>
+      <c r="E79" s="19" t="s">
         <v>601</v>
-      </c>
-      <c r="E79" s="19" t="s">
-        <v>602</v>
       </c>
       <c r="F79" s="19" t="s">
         <v>563</v>
@@ -6332,10 +6344,10 @@
         <v>252</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F80" s="19" t="s">
         <v>563</v>
@@ -6355,10 +6367,10 @@
         <v>252</v>
       </c>
       <c r="C81" s="19" t="s">
+        <v>603</v>
+      </c>
+      <c r="E81" s="19" t="s">
         <v>604</v>
-      </c>
-      <c r="E81" s="19" t="s">
-        <v>605</v>
       </c>
       <c r="F81" s="19" t="s">
         <v>563</v>
@@ -6378,10 +6390,10 @@
         <v>252</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E82" s="19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F82" s="19" t="s">
         <v>563</v>
@@ -6401,10 +6413,10 @@
         <v>252</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F83" s="19" t="s">
         <v>563</v>
@@ -6424,10 +6436,10 @@
         <v>252</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E84" s="19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F84" s="19" t="s">
         <v>563</v>
@@ -6447,10 +6459,10 @@
         <v>252</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F85" s="19" t="s">
         <v>563</v>
@@ -6470,7 +6482,7 @@
         <v>252</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E86" s="19" t="s">
         <v>532</v>
@@ -6493,13 +6505,13 @@
         <v>252</v>
       </c>
       <c r="C87" s="19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E87" s="19" t="s">
         <v>568</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G87" s="56" t="s">
         <v>541</v>
@@ -6516,13 +6528,13 @@
         <v>252</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="E88" s="19" t="s">
         <v>568</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="G88" s="56" t="s">
         <v>541</v>
@@ -6539,17 +6551,23 @@
         <v>252</v>
       </c>
       <c r="C89" s="58" t="s">
+        <v>613</v>
+      </c>
+      <c r="D89" s="58" t="s">
         <v>614</v>
       </c>
-      <c r="D89" s="57"/>
       <c r="E89" s="58" t="s">
+        <v>568</v>
+      </c>
+      <c r="F89" s="59" t="s">
         <v>615</v>
       </c>
-      <c r="F89" s="59" t="s">
-        <v>616</v>
-      </c>
-      <c r="G89" s="57"/>
-      <c r="H89" s="60"/>
+      <c r="G89" s="60" t="s">
+        <v>618</v>
+      </c>
+      <c r="H89" s="61" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="90" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="57" t="s">
@@ -6559,17 +6577,43 @@
         <v>252</v>
       </c>
       <c r="C90" s="58" t="s">
+        <v>616</v>
+      </c>
+      <c r="D90" s="58" t="s">
         <v>617</v>
       </c>
-      <c r="D90" s="57"/>
       <c r="E90" s="58" t="s">
+        <v>568</v>
+      </c>
+      <c r="F90" s="59" t="s">
+        <v>615</v>
+      </c>
+      <c r="G90" s="60" t="s">
         <v>618</v>
       </c>
-      <c r="F90" s="59" t="s">
-        <v>616</v>
-      </c>
-      <c r="G90" s="57"/>
-      <c r="H90" s="60"/>
+      <c r="H90" s="61" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="B91" s="19" t="s">
+        <v>252</v>
+      </c>
+      <c r="C91" s="19" t="s">
+        <v>619</v>
+      </c>
+      <c r="D91" s="25" t="s">
+        <v>620</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>570</v>
+      </c>
+      <c r="F91" s="19" t="s">
+        <v>621</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>

<commit_message>
#updated TODO list and rerun defaults and check merge from Nick - DSPT was only difference - from Ty. Nick's merges look good!
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
   </bookViews>
@@ -18,12 +23,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1766" uniqueCount="623">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1770" uniqueCount="624">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1624,9 +1629,6 @@
     <t>Update SAM upgrade script for all battery/lifetime variables</t>
   </si>
   <si>
-    <t>Nate</t>
-  </si>
-  <si>
     <t>monthly fixed tilt</t>
   </si>
   <si>
@@ -1907,6 +1909,12 @@
   </si>
   <si>
     <t>Add back non-net metering, unFIT things</t>
+  </si>
+  <si>
+    <t>Ty/Aron</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High DPI screens </t>
   </si>
 </sst>
 </file>
@@ -3115,7 +3123,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3150,7 +3158,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3362,8 +3370,8 @@
   <dimension ref="A1:F155"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3420,7 +3428,7 @@
         <v>285</v>
       </c>
       <c r="C3" s="47" t="s">
-        <v>528</v>
+        <v>68</v>
       </c>
       <c r="D3" s="48"/>
       <c r="E3" s="47" t="s">
@@ -3597,7 +3605,7 @@
         <v>55</v>
       </c>
       <c r="B15" s="47" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C15" s="47" t="s">
         <v>499</v>
@@ -3612,7 +3620,7 @@
         <v>55</v>
       </c>
       <c r="B16" s="47" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C16" s="47" t="s">
         <v>45</v>
@@ -3882,7 +3890,7 @@
         <v>135</v>
       </c>
       <c r="B34" s="42" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C34" s="42"/>
       <c r="D34" s="42"/>
@@ -3893,7 +3901,7 @@
         <v>135</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="C35" s="42" t="s">
         <v>46</v>
@@ -3919,7 +3927,7 @@
         <v>135</v>
       </c>
       <c r="B37" s="42" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="C37" s="42"/>
       <c r="D37" s="42"/>
@@ -3930,7 +3938,7 @@
         <v>135</v>
       </c>
       <c r="B38" s="42" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C38" s="42" t="s">
         <v>46</v>
@@ -3943,7 +3951,7 @@
         <v>135</v>
       </c>
       <c r="B39" s="42" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C39" s="42" t="s">
         <v>47</v>
@@ -3956,7 +3964,7 @@
         <v>135</v>
       </c>
       <c r="B40" s="42" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C40" s="42" t="s">
         <v>46</v>
@@ -4096,7 +4104,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B51" s="50" t="s">
         <v>524</v>
@@ -4112,7 +4120,7 @@
         <v>460</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C52" s="50" t="s">
         <v>47</v>
@@ -4125,7 +4133,7 @@
         <v>460</v>
       </c>
       <c r="B53" s="50" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="C53" s="50" t="s">
         <v>47</v>
@@ -4135,37 +4143,39 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B54" s="50" t="s">
+        <v>551</v>
+      </c>
+      <c r="C54" s="50" t="s">
         <v>552</v>
-      </c>
-      <c r="C54" s="50" t="s">
-        <v>553</v>
       </c>
       <c r="D54" s="50"/>
       <c r="E54" s="50"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B55" s="50" t="s">
-        <v>549</v>
-      </c>
-      <c r="C55" s="50"/>
+        <v>548</v>
+      </c>
+      <c r="C55" s="50" t="s">
+        <v>622</v>
+      </c>
       <c r="D55" s="50"/>
       <c r="E55" s="50"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -4173,14 +4183,22 @@
         <v>192</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="C57" s="31" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="32"/>
+      <c r="A58" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="31" t="s">
+        <v>623</v>
+      </c>
+      <c r="C58" s="31" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="32"/>
@@ -4498,7 +4516,7 @@
         <v>261</v>
       </c>
       <c r="G1" s="53" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="V1" s="24" t="s">
         <v>205</v>
@@ -4710,7 +4728,7 @@
         <v>313</v>
       </c>
       <c r="G12" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H12" s="19" t="s">
         <v>302</v>
@@ -4736,7 +4754,7 @@
         <v>313</v>
       </c>
       <c r="G13" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H13" s="19" t="s">
         <v>302</v>
@@ -4762,7 +4780,7 @@
         <v>313</v>
       </c>
       <c r="G14" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H14" s="19" t="s">
         <v>302</v>
@@ -4788,7 +4806,7 @@
         <v>329</v>
       </c>
       <c r="G15" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H15" s="19" t="s">
         <v>330</v>
@@ -4814,7 +4832,7 @@
         <v>329</v>
       </c>
       <c r="G16" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H16" s="19" t="s">
         <v>330</v>
@@ -4840,7 +4858,7 @@
         <v>329</v>
       </c>
       <c r="G17" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>330</v>
@@ -4866,7 +4884,7 @@
         <v>329</v>
       </c>
       <c r="G18" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H18" s="19" t="s">
         <v>330</v>
@@ -4892,7 +4910,7 @@
         <v>329</v>
       </c>
       <c r="G19" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H19" s="19" t="s">
         <v>330</v>
@@ -4918,7 +4936,7 @@
         <v>329</v>
       </c>
       <c r="G20" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H20" s="19" t="s">
         <v>330</v>
@@ -4944,7 +4962,7 @@
         <v>329</v>
       </c>
       <c r="G21" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H21" s="19" t="s">
         <v>330</v>
@@ -4970,7 +4988,7 @@
         <v>329</v>
       </c>
       <c r="G22" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H22" s="19" t="s">
         <v>330</v>
@@ -4996,7 +5014,7 @@
         <v>329</v>
       </c>
       <c r="G23" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H23" s="19" t="s">
         <v>330</v>
@@ -5022,7 +5040,7 @@
         <v>329</v>
       </c>
       <c r="G24" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>330</v>
@@ -5048,7 +5066,7 @@
         <v>329</v>
       </c>
       <c r="G25" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>330</v>
@@ -5074,7 +5092,7 @@
         <v>329</v>
       </c>
       <c r="G26" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>330</v>
@@ -5100,7 +5118,7 @@
         <v>334</v>
       </c>
       <c r="G27" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H27" s="19" t="s">
         <v>302</v>
@@ -5126,7 +5144,7 @@
         <v>334</v>
       </c>
       <c r="G28" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H28" s="19" t="s">
         <v>302</v>
@@ -5152,7 +5170,7 @@
         <v>334</v>
       </c>
       <c r="G29" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H29" s="19" t="s">
         <v>302</v>
@@ -5187,17 +5205,17 @@
         <v>252</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D31" s="19"/>
       <c r="E31" s="19" t="s">
+        <v>531</v>
+      </c>
+      <c r="F31" s="19" t="s">
         <v>532</v>
       </c>
-      <c r="F31" s="19" t="s">
-        <v>533</v>
-      </c>
       <c r="G31" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H31" s="19" t="s">
         <v>302</v>
@@ -5211,19 +5229,19 @@
         <v>252</v>
       </c>
       <c r="C32" s="19" t="s">
+        <v>533</v>
+      </c>
+      <c r="D32" s="19" t="s">
         <v>534</v>
       </c>
-      <c r="D32" s="19" t="s">
+      <c r="E32" s="19" t="s">
+        <v>531</v>
+      </c>
+      <c r="F32" s="19" t="s">
         <v>535</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>532</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>536</v>
-      </c>
       <c r="G32" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H32" s="19" t="s">
         <v>302</v>
@@ -5237,19 +5255,19 @@
         <v>252</v>
       </c>
       <c r="C33" s="19" t="s">
+        <v>536</v>
+      </c>
+      <c r="D33" s="19" t="s">
         <v>537</v>
       </c>
-      <c r="D33" s="19" t="s">
-        <v>538</v>
-      </c>
       <c r="E33" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F33" s="19" t="s">
         <v>313</v>
       </c>
       <c r="G33" s="56" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="H33" s="19" t="s">
         <v>302</v>
@@ -5263,17 +5281,17 @@
         <v>252</v>
       </c>
       <c r="C34" s="19" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D34" s="19"/>
       <c r="E34" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F34" s="19" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="G34" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H34" s="19" t="s">
         <v>302</v>
@@ -5287,17 +5305,17 @@
         <v>252</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D35" s="19"/>
       <c r="E35" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="F35" s="25" t="s">
         <v>558</v>
       </c>
-      <c r="F35" s="25" t="s">
-        <v>559</v>
-      </c>
       <c r="G35" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H35" s="19" t="s">
         <v>302</v>
@@ -5311,17 +5329,17 @@
         <v>252</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D36" s="19"/>
       <c r="E36" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="F36" s="25" t="s">
         <v>558</v>
       </c>
-      <c r="F36" s="25" t="s">
-        <v>559</v>
-      </c>
       <c r="G36" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H36" s="19" t="s">
         <v>302</v>
@@ -5335,17 +5353,17 @@
         <v>252</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D37" s="19"/>
       <c r="E37" s="19" t="s">
+        <v>557</v>
+      </c>
+      <c r="F37" s="25" t="s">
         <v>558</v>
       </c>
-      <c r="F37" s="25" t="s">
-        <v>559</v>
-      </c>
       <c r="G37" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H37" s="19" t="s">
         <v>302</v>
@@ -5359,17 +5377,17 @@
         <v>252</v>
       </c>
       <c r="C38" s="19" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D38" s="19"/>
       <c r="E38" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G38" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H38" s="19" t="s">
         <v>302</v>
@@ -5383,17 +5401,17 @@
         <v>252</v>
       </c>
       <c r="C39" s="19" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D39" s="19"/>
       <c r="E39" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G39" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H39" s="19" t="s">
         <v>302</v>
@@ -5407,17 +5425,17 @@
         <v>252</v>
       </c>
       <c r="C40" s="19" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D40" s="19"/>
       <c r="E40" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F40" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G40" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H40" s="19" t="s">
         <v>302</v>
@@ -5431,17 +5449,17 @@
         <v>252</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D41" s="19"/>
       <c r="E41" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G41" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H41" s="19" t="s">
         <v>302</v>
@@ -5455,17 +5473,17 @@
         <v>252</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="D42" s="19"/>
       <c r="E42" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G42" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H42" s="19" t="s">
         <v>302</v>
@@ -5479,17 +5497,17 @@
         <v>252</v>
       </c>
       <c r="C43" s="19" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="D43" s="19"/>
       <c r="E43" s="19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F43" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G43" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H43" s="19" t="s">
         <v>302</v>
@@ -5504,17 +5522,17 @@
         <v>252</v>
       </c>
       <c r="C44" s="19" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D44" s="19"/>
       <c r="E44" s="19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F44" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G44" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H44" s="19" t="s">
         <v>302</v>
@@ -5528,17 +5546,17 @@
         <v>252</v>
       </c>
       <c r="C45" s="19" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D45" s="19"/>
       <c r="E45" s="19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F45" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G45" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H45" s="19" t="s">
         <v>302</v>
@@ -5552,17 +5570,17 @@
         <v>252</v>
       </c>
       <c r="C46" s="19" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D46" s="19"/>
       <c r="E46" s="19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F46" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G46" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H46" s="19" t="s">
         <v>302</v>
@@ -5576,17 +5594,17 @@
         <v>252</v>
       </c>
       <c r="C47" s="19" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D47" s="19"/>
       <c r="E47" s="19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F47" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G47" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H47" s="19" t="s">
         <v>302</v>
@@ -5600,17 +5618,17 @@
         <v>252</v>
       </c>
       <c r="C48" s="19" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D48" s="19"/>
       <c r="E48" s="19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G48" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H48" s="19" t="s">
         <v>302</v>
@@ -5624,17 +5642,17 @@
         <v>252</v>
       </c>
       <c r="C49" s="19" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D49" s="19"/>
       <c r="E49" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F49" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G49" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H49" s="19" t="s">
         <v>302</v>
@@ -5648,17 +5666,17 @@
         <v>252</v>
       </c>
       <c r="C50" s="19" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="D50" s="19"/>
       <c r="E50" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F50" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G50" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H50" s="19" t="s">
         <v>302</v>
@@ -5672,17 +5690,17 @@
         <v>252</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="D51" s="19"/>
       <c r="E51" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G51" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H51" s="19" t="s">
         <v>302</v>
@@ -5696,17 +5714,17 @@
         <v>252</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="D52" s="19"/>
       <c r="E52" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G52" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H52" s="19" t="s">
         <v>302</v>
@@ -5720,17 +5738,17 @@
         <v>252</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="D53" s="19"/>
       <c r="E53" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G53" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H53" s="19" t="s">
         <v>302</v>
@@ -5744,17 +5762,17 @@
         <v>252</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D54" s="19"/>
       <c r="E54" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G54" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H54" s="19" t="s">
         <v>302</v>
@@ -5768,17 +5786,17 @@
         <v>252</v>
       </c>
       <c r="C55" s="19" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="D55" s="19"/>
       <c r="E55" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F55" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G55" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H55" s="19" t="s">
         <v>302</v>
@@ -5792,17 +5810,17 @@
         <v>252</v>
       </c>
       <c r="C56" s="19" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="D56" s="19"/>
       <c r="E56" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G56" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H56" s="19" t="s">
         <v>302</v>
@@ -5816,17 +5834,17 @@
         <v>252</v>
       </c>
       <c r="C57" s="19" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="D57" s="19"/>
       <c r="E57" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G57" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H57" s="19" t="s">
         <v>302</v>
@@ -5840,17 +5858,17 @@
         <v>252</v>
       </c>
       <c r="C58" s="19" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D58" s="19"/>
       <c r="E58" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G58" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H58" s="19" t="s">
         <v>302</v>
@@ -5864,17 +5882,17 @@
         <v>252</v>
       </c>
       <c r="C59" s="19" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D59" s="19"/>
       <c r="E59" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G59" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H59" s="19" t="s">
         <v>302</v>
@@ -5888,17 +5906,17 @@
         <v>252</v>
       </c>
       <c r="C60" s="19" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="D60" s="19"/>
       <c r="E60" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F60" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G60" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H60" s="19" t="s">
         <v>302</v>
@@ -5912,17 +5930,17 @@
         <v>252</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D61" s="19"/>
       <c r="E61" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G61" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H61" s="19" t="s">
         <v>302</v>
@@ -5936,17 +5954,17 @@
         <v>252</v>
       </c>
       <c r="C62" s="19" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="D62" s="19"/>
       <c r="E62" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F62" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G62" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H62" s="19" t="s">
         <v>302</v>
@@ -5960,17 +5978,17 @@
         <v>252</v>
       </c>
       <c r="C63" s="19" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D63" s="19"/>
       <c r="E63" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F63" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G63" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H63" s="19" t="s">
         <v>302</v>
@@ -5984,17 +6002,17 @@
         <v>252</v>
       </c>
       <c r="C64" s="19" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D64" s="19"/>
       <c r="E64" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G64" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H64" s="19" t="s">
         <v>302</v>
@@ -6008,17 +6026,17 @@
         <v>252</v>
       </c>
       <c r="C65" s="19" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="D65" s="19"/>
       <c r="E65" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F65" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G65" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H65" s="19" t="s">
         <v>302</v>
@@ -6032,17 +6050,17 @@
         <v>252</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="D66" s="19"/>
       <c r="E66" s="19" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G66" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H66" s="19" t="s">
         <v>302</v>
@@ -6056,16 +6074,16 @@
         <v>251</v>
       </c>
       <c r="C67" s="19" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="E67" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F67" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G67" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H67" s="19" t="s">
         <v>302</v>
@@ -6079,16 +6097,16 @@
         <v>251</v>
       </c>
       <c r="C68" s="19" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="E68" s="19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F68" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G68" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H68" s="19" t="s">
         <v>302</v>
@@ -6102,16 +6120,16 @@
         <v>252</v>
       </c>
       <c r="C69" s="19" t="s">
+        <v>589</v>
+      </c>
+      <c r="E69" s="19" t="s">
         <v>590</v>
       </c>
-      <c r="E69" s="19" t="s">
-        <v>591</v>
-      </c>
       <c r="F69" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G69" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H69" s="19" t="s">
         <v>302</v>
@@ -6125,16 +6143,16 @@
         <v>252</v>
       </c>
       <c r="C70" s="19" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="E70" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F70" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G70" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H70" s="19" t="s">
         <v>302</v>
@@ -6148,16 +6166,16 @@
         <v>252</v>
       </c>
       <c r="C71" s="19" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="E71" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F71" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G71" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H71" s="19" t="s">
         <v>302</v>
@@ -6171,16 +6189,16 @@
         <v>252</v>
       </c>
       <c r="C72" s="19" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="E72" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F72" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G72" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H72" s="19" t="s">
         <v>302</v>
@@ -6194,16 +6212,16 @@
         <v>252</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="E73" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G73" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H73" s="19" t="s">
         <v>302</v>
@@ -6217,16 +6235,16 @@
         <v>252</v>
       </c>
       <c r="C74" s="19" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="E74" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F74" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G74" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H74" s="19" t="s">
         <v>302</v>
@@ -6240,16 +6258,16 @@
         <v>252</v>
       </c>
       <c r="C75" s="19" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="E75" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F75" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G75" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H75" s="19" t="s">
         <v>302</v>
@@ -6263,16 +6281,16 @@
         <v>252</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="E76" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G76" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H76" s="19" t="s">
         <v>302</v>
@@ -6286,16 +6304,16 @@
         <v>252</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G77" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H77" s="19" t="s">
         <v>302</v>
@@ -6309,16 +6327,16 @@
         <v>252</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E78" s="19" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G78" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H78" s="19" t="s">
         <v>302</v>
@@ -6332,16 +6350,16 @@
         <v>252</v>
       </c>
       <c r="C79" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="E79" s="19" t="s">
         <v>600</v>
       </c>
-      <c r="E79" s="19" t="s">
-        <v>601</v>
-      </c>
       <c r="F79" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G79" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H79" s="19" t="s">
         <v>302</v>
@@ -6355,16 +6373,16 @@
         <v>252</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E80" s="19" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F80" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G80" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H80" s="19" t="s">
         <v>302</v>
@@ -6378,16 +6396,16 @@
         <v>252</v>
       </c>
       <c r="C81" s="19" t="s">
+        <v>602</v>
+      </c>
+      <c r="E81" s="19" t="s">
         <v>603</v>
       </c>
-      <c r="E81" s="19" t="s">
-        <v>604</v>
-      </c>
       <c r="F81" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G81" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H81" s="19" t="s">
         <v>302</v>
@@ -6401,16 +6419,16 @@
         <v>252</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="E82" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G82" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H82" s="19" t="s">
         <v>302</v>
@@ -6424,16 +6442,16 @@
         <v>252</v>
       </c>
       <c r="C83" s="19" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="E83" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G83" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H83" s="19" t="s">
         <v>302</v>
@@ -6447,16 +6465,16 @@
         <v>252</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="E84" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G84" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H84" s="19" t="s">
         <v>302</v>
@@ -6470,16 +6488,16 @@
         <v>252</v>
       </c>
       <c r="C85" s="19" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G85" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H85" s="19" t="s">
         <v>302</v>
@@ -6493,16 +6511,16 @@
         <v>252</v>
       </c>
       <c r="C86" s="19" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="G86" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H86" s="19" t="s">
         <v>302</v>
@@ -6516,16 +6534,16 @@
         <v>252</v>
       </c>
       <c r="C87" s="19" t="s">
+        <v>610</v>
+      </c>
+      <c r="E87" s="19" t="s">
+        <v>567</v>
+      </c>
+      <c r="F87" s="19" t="s">
         <v>611</v>
       </c>
-      <c r="E87" s="19" t="s">
-        <v>568</v>
-      </c>
-      <c r="F87" s="19" t="s">
-        <v>612</v>
-      </c>
       <c r="G87" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H87" s="19" t="s">
         <v>302</v>
@@ -6539,16 +6557,16 @@
         <v>252</v>
       </c>
       <c r="C88" s="19" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="G88" s="56" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="H88" s="19" t="s">
         <v>302</v>
@@ -6562,19 +6580,19 @@
         <v>252</v>
       </c>
       <c r="C89" s="58" t="s">
+        <v>612</v>
+      </c>
+      <c r="D89" s="58" t="s">
         <v>613</v>
       </c>
-      <c r="D89" s="58" t="s">
+      <c r="E89" s="58" t="s">
+        <v>567</v>
+      </c>
+      <c r="F89" s="59" t="s">
         <v>614</v>
       </c>
-      <c r="E89" s="58" t="s">
-        <v>568</v>
-      </c>
-      <c r="F89" s="59" t="s">
-        <v>615</v>
-      </c>
       <c r="G89" s="60" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H89" s="61" t="s">
         <v>302</v>
@@ -6588,19 +6606,19 @@
         <v>252</v>
       </c>
       <c r="C90" s="58" t="s">
+        <v>615</v>
+      </c>
+      <c r="D90" s="58" t="s">
         <v>616</v>
       </c>
-      <c r="D90" s="58" t="s">
+      <c r="E90" s="58" t="s">
+        <v>567</v>
+      </c>
+      <c r="F90" s="59" t="s">
+        <v>614</v>
+      </c>
+      <c r="G90" s="60" t="s">
         <v>617</v>
-      </c>
-      <c r="E90" s="58" t="s">
-        <v>568</v>
-      </c>
-      <c r="F90" s="59" t="s">
-        <v>615</v>
-      </c>
-      <c r="G90" s="60" t="s">
-        <v>618</v>
       </c>
       <c r="H90" s="61" t="s">
         <v>302</v>
@@ -6614,19 +6632,19 @@
         <v>252</v>
       </c>
       <c r="C91" s="19" t="s">
+        <v>618</v>
+      </c>
+      <c r="D91" s="19" t="s">
         <v>619</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="E91" s="19" t="s">
+        <v>569</v>
+      </c>
+      <c r="F91" s="19" t="s">
         <v>620</v>
       </c>
-      <c r="E91" s="19" t="s">
-        <v>570</v>
-      </c>
-      <c r="F91" s="19" t="s">
-        <v>621</v>
-      </c>
       <c r="G91" s="56" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="H91" s="19" t="s">
         <v>302</v>
@@ -7094,7 +7112,7 @@
         <v>108</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all the to-do list updates!
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -3623,7 +3623,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3828,7 +3828,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B15" s="63" t="s">
         <v>642</v>

</xml_diff>

<commit_message>
updated TODO list for Feb 2016 release
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adobos\Projects\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
   </bookViews>
@@ -20,12 +25,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1912" uniqueCount="672">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1992,13 +1997,70 @@
     <t>Show both resource and calculated irradiance outputs</t>
   </si>
   <si>
-    <t>Linear shading option (and upgrade project files!)</t>
-  </si>
-  <si>
     <t>Check file upgrades from previous versions</t>
   </si>
   <si>
     <t>Testing</t>
+  </si>
+  <si>
+    <t>Linear shading option for PV self-shading model (and upgrade project files!)</t>
+  </si>
+  <si>
+    <t>Battery automatic dispatch and testing, project file upgrader, etc</t>
+  </si>
+  <si>
+    <t>Finish testing of POA model, project upgrade, documentation</t>
+  </si>
+  <si>
+    <t>Updates to utility rate model metering options and input/output structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proxy autodetection on Windows </t>
+  </si>
+  <si>
+    <t>Validation and fixes to 3D shading database</t>
+  </si>
+  <si>
+    <t>Steve/Sara</t>
+  </si>
+  <si>
+    <t>Remove webkitgtk dependencies on Linux OS, rebuild on CentOS 6.4 as standard</t>
+  </si>
+  <si>
+    <t>Wind wizard</t>
+  </si>
+  <si>
+    <t>User defined power cycle input option</t>
+  </si>
+  <si>
+    <t>Molten salt power tower model with new controller framework</t>
+  </si>
+  <si>
+    <t>Dispatch optimization for power tower model</t>
+  </si>
+  <si>
+    <t>Merge updates from SolarPilot standalone version into SAM, update defaults</t>
+  </si>
+  <si>
+    <t>Check s3d file format reader: does it read old .s3d files OK with group property removed/renamed? Notice in project file upgrader</t>
+  </si>
+  <si>
+    <t>LK 'global' variable space keyword</t>
+  </si>
+  <si>
+    <t>Update LK documentation in line with language changes in VM</t>
+  </si>
+  <si>
+    <t>Checkbox on tower page to update inputs from results based on a script.  Add a post-simulation script framework</t>
+  </si>
+  <si>
+    <t>Aron/Ty</t>
+  </si>
+  <si>
+    <t>Remove HCPV model and augment simple efficiency model accordingly</t>
+  </si>
+  <si>
+    <t>Janine/Paul</t>
   </si>
 </sst>
 </file>
@@ -3402,7 +3464,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3437,7 +3499,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3646,11 +3708,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F127"/>
+  <dimension ref="A1:F143"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B17" sqref="B17"/>
+      <selection pane="bottomLeft" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3764,7 +3826,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B8" s="63" t="s">
         <v>631</v>
@@ -3829,7 +3891,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B13" s="63" t="s">
         <v>638</v>
@@ -3897,7 +3959,7 @@
         <v>192</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="C18" s="63" t="s">
         <v>45</v>
@@ -3925,7 +3987,9 @@
       <c r="B20" s="63" t="s">
         <v>648</v>
       </c>
-      <c r="C20" s="63"/>
+      <c r="C20" s="63" t="s">
+        <v>671</v>
+      </c>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
     </row>
@@ -3944,214 +4008,374 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" s="40" t="s">
-        <v>549</v>
-      </c>
-      <c r="C22" s="40"/>
-      <c r="D22" s="40"/>
-      <c r="E22" s="40"/>
+        <v>192</v>
+      </c>
+      <c r="B22" s="63" t="s">
+        <v>653</v>
+      </c>
+      <c r="C22" s="63" t="s">
+        <v>307</v>
+      </c>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B23" s="40" t="s">
-        <v>550</v>
-      </c>
-      <c r="C23" s="40"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
+        <v>651</v>
+      </c>
+      <c r="B23" s="63" t="s">
+        <v>654</v>
+      </c>
+      <c r="C23" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B24" s="40" t="s">
-        <v>651</v>
-      </c>
-      <c r="C24" s="40"/>
-      <c r="D24" s="40"/>
-      <c r="E24" s="40"/>
+        <v>192</v>
+      </c>
+      <c r="B24" s="63" t="s">
+        <v>655</v>
+      </c>
+      <c r="C24" s="63" t="s">
+        <v>225</v>
+      </c>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B25" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="40"/>
+        <v>192</v>
+      </c>
+      <c r="B25" s="63" t="s">
+        <v>656</v>
+      </c>
+      <c r="C25" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="63"/>
+      <c r="E25" s="63"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B26" s="40" t="s">
-        <v>545</v>
-      </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="40"/>
-      <c r="E26" s="40"/>
+        <v>651</v>
+      </c>
+      <c r="B26" s="63" t="s">
+        <v>657</v>
+      </c>
+      <c r="C26" s="63" t="s">
+        <v>658</v>
+      </c>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B27" s="40" t="s">
-        <v>542</v>
-      </c>
-      <c r="C27" s="40"/>
-      <c r="D27" s="40"/>
-      <c r="E27" s="40"/>
+        <v>192</v>
+      </c>
+      <c r="B27" s="63" t="s">
+        <v>659</v>
+      </c>
+      <c r="C27" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="63"/>
+      <c r="E27" s="63"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B28" s="40" t="s">
-        <v>543</v>
-      </c>
-      <c r="C28" s="40"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
+        <v>55</v>
+      </c>
+      <c r="B28" s="63" t="s">
+        <v>660</v>
+      </c>
+      <c r="C28" s="63" t="s">
+        <v>45</v>
+      </c>
+      <c r="D28" s="63"/>
+      <c r="E28" s="63"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B29" s="40" t="s">
-        <v>544</v>
-      </c>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
+        <v>651</v>
+      </c>
+      <c r="B29" s="63" t="s">
+        <v>661</v>
+      </c>
+      <c r="C29" s="63" t="s">
+        <v>302</v>
+      </c>
+      <c r="D29" s="63"/>
+      <c r="E29" s="63"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B30" s="40" t="s">
-        <v>646</v>
-      </c>
-      <c r="C30" s="40"/>
-      <c r="D30" s="40"/>
-      <c r="E30" s="40"/>
+        <v>651</v>
+      </c>
+      <c r="B30" s="63" t="s">
+        <v>662</v>
+      </c>
+      <c r="C30" s="63" t="s">
+        <v>302</v>
+      </c>
+      <c r="D30" s="63"/>
+      <c r="E30" s="63"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
+        <v>651</v>
+      </c>
+      <c r="B31" s="63" t="s">
+        <v>663</v>
+      </c>
+      <c r="C31" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B32" s="63" t="s">
+        <v>664</v>
+      </c>
+      <c r="C32" s="63" t="s">
+        <v>124</v>
+      </c>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="32" t="s">
+        <v>651</v>
+      </c>
+      <c r="B33" s="63" t="s">
+        <v>665</v>
+      </c>
+      <c r="C33" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" s="63"/>
+      <c r="E33" s="63"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B34" s="63" t="s">
+        <v>666</v>
+      </c>
+      <c r="C34" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B35" s="63" t="s">
+        <v>667</v>
+      </c>
+      <c r="C35" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="63"/>
+      <c r="E35" s="63"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="63" t="s">
+        <v>668</v>
+      </c>
+      <c r="C36" s="63" t="s">
+        <v>669</v>
+      </c>
+      <c r="D36" s="63"/>
+      <c r="E36" s="63"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B37" s="63" t="s">
+        <v>670</v>
+      </c>
+      <c r="C37" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="B31" s="40" t="s">
+      <c r="B38" s="40" t="s">
+        <v>549</v>
+      </c>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B39" s="40" t="s">
+        <v>550</v>
+      </c>
+      <c r="C39" s="40"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="40" t="s">
+        <v>650</v>
+      </c>
+      <c r="C40" s="40"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B41" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>545</v>
+      </c>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" s="40" t="s">
+        <v>542</v>
+      </c>
+      <c r="C43" s="40"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B44" s="40" t="s">
+        <v>543</v>
+      </c>
+      <c r="C44" s="40"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" s="40" t="s">
+        <v>544</v>
+      </c>
+      <c r="C45" s="40"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B46" s="40" t="s">
+        <v>646</v>
+      </c>
+      <c r="C46" s="40"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B47" s="40" t="s">
         <v>643</v>
       </c>
-      <c r="C31" s="40"/>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32" s="32"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="32"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="32"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="32"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="32"/>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="32"/>
-      <c r="B37" s="31" t="s">
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="32"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="32"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="32"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="32"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="32"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="32"/>
+      <c r="B53" s="31" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="32"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39" s="32"/>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40" s="32"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41" s="32"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42" s="32"/>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43" s="32"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44" s="32"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45" s="32"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46" s="32"/>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47" s="32"/>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48" s="32"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="32"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="32"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="32"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="32"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="32"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="32"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="32"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="32"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="32"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="32"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="32"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="32"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="32"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="32"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="32"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
@@ -4212,7 +4436,7 @@
       <c r="A83" s="32"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="33"/>
+      <c r="A84" s="32"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="32"/>
@@ -4238,11 +4462,59 @@
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="32"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A127" s="33"/>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A93" s="32"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A94" s="32"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A95" s="32"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A96" s="32"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A97" s="32"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A98" s="32"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A99" s="32"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A100" s="33"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A101" s="32"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A102" s="32"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A103" s="32"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A104" s="32"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A105" s="32"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A106" s="32"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A107" s="32"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A108" s="32"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A143" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A78">
+  <conditionalFormatting sqref="A1:A94">
     <cfRule type="containsText" dxfId="102" priority="18" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4259,7 +4531,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A189">
+  <conditionalFormatting sqref="A1:A205">
     <cfRule type="containsText" dxfId="97" priority="16" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4267,46 +4539,46 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A79:A80">
+  <conditionalFormatting sqref="A95:A96">
     <cfRule type="containsText" dxfId="95" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A79)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A95)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A79)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A95)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A79)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A95)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A79)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A95)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="91" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A79)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A95)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A192:A1048576">
+  <conditionalFormatting sqref="A208:A1048576">
     <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A192)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A208)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A192)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A208)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A81:A189 A192:A1048576">
+  <conditionalFormatting sqref="A97:A205 A208:A1048576">
     <cfRule type="containsText" dxfId="88" priority="8" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A81)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A97)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A81)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A97)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="86" priority="10" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A81)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A97)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A81)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A97)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A81)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A97)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated TODO list for wxWidgets patch
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1916" uniqueCount="674">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="675">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2062,6 +2062,9 @@
   </si>
   <si>
     <t>Next release: enable seasonally tilted PV systems (macro? Input?)</t>
+  </si>
+  <si>
+    <t>Patch in wxAuiNotebook change: http://trac.wxwidgets.org/ticket/16605#comment:5</t>
   </si>
 </sst>
 </file>
@@ -2397,7 +2400,147 @@
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="105">
+  <dxfs count="119">
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF33CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF33CC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3399,8 +3542,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="104"/>
-      <tableStyleElement type="headerRow" dxfId="103"/>
+      <tableStyleElement type="wholeTable" dxfId="118"/>
+      <tableStyleElement type="headerRow" dxfId="117"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -3713,7 +3856,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4338,58 +4481,66 @@
       <c r="D48" s="40"/>
       <c r="E48" s="40"/>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49" s="32"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="40" t="s">
+        <v>674</v>
+      </c>
+      <c r="C49" s="40"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="32"/>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="32"/>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="32"/>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="32"/>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="32"/>
       <c r="B54" s="31" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="32"/>
       <c r="B55" s="31" t="s">
         <v>673</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="32"/>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="32"/>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="32"/>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="32"/>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="32"/>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="32"/>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="32"/>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="32"/>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
@@ -4531,71 +4682,96 @@
       <c r="A144" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A95">
-    <cfRule type="containsText" dxfId="102" priority="18" operator="containsText" text="NGTD">
+  <conditionalFormatting sqref="A1:A48 A50:A95">
+    <cfRule type="containsText" dxfId="116" priority="25" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="19" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="115" priority="26" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="20" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="114" priority="27" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="21" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="113" priority="28" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="22" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="112" priority="29" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A206">
-    <cfRule type="containsText" dxfId="97" priority="16" operator="containsText" text="POUT">
+  <conditionalFormatting sqref="A1:A48 A50:A206">
+    <cfRule type="containsText" dxfId="111" priority="23" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="17" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="110" priority="24" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:A97">
-    <cfRule type="containsText" dxfId="95" priority="3" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="109" priority="10" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="4" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="108" priority="11" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="5" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="107" priority="12" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="6" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="106" priority="13" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A96)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="105" priority="14" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A1048576">
-    <cfRule type="containsText" dxfId="90" priority="1" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="104" priority="8" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A209)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="2" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="103" priority="9" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A209)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A98:A206 A209:A1048576">
-    <cfRule type="containsText" dxfId="88" priority="8" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="102" priority="15" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A98)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="9" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="101" priority="16" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A98)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="10" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="100" priority="17" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A98)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="99" priority="18" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A98)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="98" priority="19" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A98)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",A49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="4" operator="containsText" text="Test">
+      <formula>NOT(ISERROR(SEARCH("Test",A49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="5" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",A49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",A49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",A49)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A49">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="POUT">
+      <formula>NOT(ISERROR(SEARCH("POUT",A49)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Pre-release">
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A49)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7271,102 +7447,102 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1 A5:A38">
-    <cfRule type="containsText" dxfId="83" priority="38" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="97" priority="38" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="39" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="96" priority="39" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="40" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="95" priority="40" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="41" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="94" priority="41" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="42" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="93" priority="42" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1 A5:A38">
-    <cfRule type="containsText" dxfId="78" priority="36" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="92" priority="36" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="37" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="91" priority="37" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="76" priority="31" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="90" priority="31" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="32" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="89" priority="32" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="33" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="88" priority="33" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="34" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="87" priority="34" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="35" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="86" priority="35" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="71" priority="29" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="85" priority="29" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="30" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="84" priority="30" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="containsText" dxfId="69" priority="24" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="83" priority="24" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="25" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="82" priority="25" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="26" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="81" priority="26" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="27" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="80" priority="27" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="28" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="79" priority="28" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="containsText" dxfId="64" priority="22" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="78" priority="22" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="23" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="77" priority="23" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="62" priority="17" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="76" priority="17" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="18" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="75" priority="18" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="19" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="74" priority="19" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="20" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="73" priority="20" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="72" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="57" priority="15" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="71" priority="15" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="16" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="70" priority="16" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8639,80 +8815,80 @@
     <sortCondition ref="E2:E30"/>
   </sortState>
   <conditionalFormatting sqref="A1:A106">
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="69" priority="53" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="68" priority="54" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="67" priority="55" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="66" priority="56" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="57" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="65" priority="57" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A217">
-    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="64" priority="46" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="63" priority="47" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E7">
-    <cfRule type="containsText" dxfId="48" priority="20" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="62" priority="20" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="61" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="22" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="60" priority="22" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107:A108">
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="59" priority="3" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="58" priority="4" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="57" priority="5" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="56" priority="6" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="55" priority="7" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A220:A1048576">
-    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="54" priority="1" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A220)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="53" priority="2" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:A217 A220:A1048576">
-    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="52" priority="8" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="9" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="51" priority="9" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="10" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="50" priority="10" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="11" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="49" priority="11" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="12" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="48" priority="12" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A109)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11778,124 +11954,124 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A92 A95:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="47" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="46" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="45" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="44" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="43" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:A94">
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="42" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="41" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="40" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="37" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="36" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="35" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="34" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="33" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="16" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="30" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F142:F143 F201:F202 F151 E142:E203">
-    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="28" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="27" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="26" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F149">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="25" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="24" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="23" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F149)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F184">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="22" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="20" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F184)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F176">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="19" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="18" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="17" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F162">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="14" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F162)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
added todo list item
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1930" uniqueCount="679">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="680">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2082,6 +2082,9 @@
   </si>
   <si>
     <t>Tweak shading nonlinear loss database UI for public release</t>
+  </si>
+  <si>
+    <t>JSON read/write functions to write LK objects to disk and retrieve?</t>
   </si>
 </sst>
 </file>
@@ -3799,11 +3802,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F148"/>
+  <dimension ref="A1:F149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
+      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4362,31 +4365,33 @@
         <v>192</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>675</v>
+        <v>679</v>
       </c>
       <c r="C42" s="63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D42" s="63"/>
       <c r="E42" s="63"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B43" s="40" t="s">
-        <v>549</v>
-      </c>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
+        <v>192</v>
+      </c>
+      <c r="B43" s="63" t="s">
+        <v>675</v>
+      </c>
+      <c r="C43" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" s="63"/>
+      <c r="E43" s="63"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C44" s="40"/>
       <c r="D44" s="40"/>
@@ -4397,7 +4402,7 @@
         <v>135</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>650</v>
+        <v>550</v>
       </c>
       <c r="C45" s="40"/>
       <c r="D45" s="40"/>
@@ -4408,7 +4413,7 @@
         <v>135</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>136</v>
+        <v>650</v>
       </c>
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
@@ -4419,7 +4424,7 @@
         <v>135</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>545</v>
+        <v>136</v>
       </c>
       <c r="C47" s="40"/>
       <c r="D47" s="40"/>
@@ -4430,7 +4435,7 @@
         <v>135</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C48" s="40"/>
       <c r="D48" s="40"/>
@@ -4441,7 +4446,7 @@
         <v>135</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C49" s="40"/>
       <c r="D49" s="40"/>
@@ -4452,7 +4457,7 @@
         <v>135</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C50" s="40"/>
       <c r="D50" s="40"/>
@@ -4463,7 +4468,7 @@
         <v>135</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>646</v>
+        <v>544</v>
       </c>
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
@@ -4474,7 +4479,7 @@
         <v>135</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
@@ -4485,14 +4490,22 @@
         <v>135</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>674</v>
+        <v>643</v>
       </c>
       <c r="C53" s="40"/>
       <c r="D53" s="40"/>
       <c r="E53" s="40"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="32"/>
+      <c r="A54" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B54" s="40" t="s">
+        <v>674</v>
+      </c>
+      <c r="C54" s="40"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="32"/>
@@ -4505,18 +4518,18 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="32"/>
-      <c r="B58" s="31" t="s">
-        <v>639</v>
-      </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="32"/>
       <c r="B59" s="31" t="s">
-        <v>673</v>
+        <v>639</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="32"/>
+      <c r="B60" s="31" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="32"/>
@@ -4651,10 +4664,10 @@
       <c r="A104" s="32"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A105" s="33"/>
+      <c r="A105" s="32"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="32"/>
+      <c r="A106" s="33"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="32"/>
@@ -4677,11 +4690,14 @@
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="32"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A148" s="33"/>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A114" s="32"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A149" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A54:A99 A1:A52">
+  <conditionalFormatting sqref="A55:A100 A1:A53">
     <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4698,7 +4714,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A210 A1:A52">
+  <conditionalFormatting sqref="A55:A211 A1:A53">
     <cfRule type="containsText" dxfId="104" priority="23" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4706,71 +4722,71 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A100:A101">
+  <conditionalFormatting sqref="A101:A102">
     <cfRule type="containsText" dxfId="102" priority="10" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A101)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="11" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A101)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="12" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A101)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="13" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A101)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="98" priority="14" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A100)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A101)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A213:A1048576">
+  <conditionalFormatting sqref="A214:A1048576">
     <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A214)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A213)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A214)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A102:A210 A213:A1048576">
+  <conditionalFormatting sqref="A103:A211 A214:A1048576">
     <cfRule type="containsText" dxfId="95" priority="15" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A103)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="16" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A103)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="17" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A103)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="18" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A103)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="91" priority="19" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A102)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A103)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
+  <conditionalFormatting sqref="A54">
     <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
+  <conditionalFormatting sqref="A54">
     <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added bug to TODO list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adobos\Projects\SAMnt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arond\Documents\NREL_Projects\SAMnt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1936" uniqueCount="681">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2085,6 +2085,9 @@
   </si>
   <si>
     <t>JSON read/write functions to write LK objects to disk and retrieve?</t>
+  </si>
+  <si>
+    <t>environment scope bug in LK ++/-- operator</t>
   </si>
 </sst>
 </file>
@@ -3802,11 +3805,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F149"/>
+  <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4388,21 +4391,23 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B44" s="40" t="s">
-        <v>549</v>
-      </c>
-      <c r="C44" s="40"/>
-      <c r="D44" s="40"/>
-      <c r="E44" s="40"/>
+        <v>192</v>
+      </c>
+      <c r="B44" s="63" t="s">
+        <v>680</v>
+      </c>
+      <c r="C44" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D44" s="63"/>
+      <c r="E44" s="63"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C45" s="40"/>
       <c r="D45" s="40"/>
@@ -4413,7 +4418,7 @@
         <v>135</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>650</v>
+        <v>550</v>
       </c>
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
@@ -4424,7 +4429,7 @@
         <v>135</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>136</v>
+        <v>650</v>
       </c>
       <c r="C47" s="40"/>
       <c r="D47" s="40"/>
@@ -4435,7 +4440,7 @@
         <v>135</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>545</v>
+        <v>136</v>
       </c>
       <c r="C48" s="40"/>
       <c r="D48" s="40"/>
@@ -4446,7 +4451,7 @@
         <v>135</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C49" s="40"/>
       <c r="D49" s="40"/>
@@ -4457,7 +4462,7 @@
         <v>135</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C50" s="40"/>
       <c r="D50" s="40"/>
@@ -4468,7 +4473,7 @@
         <v>135</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
@@ -4479,7 +4484,7 @@
         <v>135</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>646</v>
+        <v>544</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
@@ -4490,7 +4495,7 @@
         <v>135</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="C53" s="40"/>
       <c r="D53" s="40"/>
@@ -4501,14 +4506,22 @@
         <v>135</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>674</v>
+        <v>643</v>
       </c>
       <c r="C54" s="40"/>
       <c r="D54" s="40"/>
       <c r="E54" s="40"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="32"/>
+      <c r="A55" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="40" t="s">
+        <v>674</v>
+      </c>
+      <c r="C55" s="40"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="32"/>
@@ -4521,18 +4534,18 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="32"/>
-      <c r="B59" s="31" t="s">
-        <v>639</v>
-      </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="32"/>
       <c r="B60" s="31" t="s">
-        <v>673</v>
+        <v>639</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="32"/>
+      <c r="B61" s="31" t="s">
+        <v>673</v>
+      </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="32"/>
@@ -4667,10 +4680,10 @@
       <c r="A105" s="32"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A106" s="33"/>
+      <c r="A106" s="32"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A107" s="32"/>
+      <c r="A107" s="33"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="32"/>
@@ -4693,11 +4706,14 @@
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="32"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A149" s="33"/>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A115" s="32"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A150" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A55:A100 A1:A53">
+  <conditionalFormatting sqref="A56:A101 A1:A54">
     <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4714,7 +4730,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A55:A211 A1:A53">
+  <conditionalFormatting sqref="A56:A212 A1:A54">
     <cfRule type="containsText" dxfId="104" priority="23" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4722,71 +4738,71 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A101:A102">
+  <conditionalFormatting sqref="A102:A103">
     <cfRule type="containsText" dxfId="102" priority="10" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A101)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="11" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A101)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="12" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A101)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="13" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A101)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A102)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="98" priority="14" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A101)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A102)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A214:A1048576">
+  <conditionalFormatting sqref="A215:A1048576">
     <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A215)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A214)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A215)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A103:A211 A214:A1048576">
+  <conditionalFormatting sqref="A104:A212 A215:A1048576">
     <cfRule type="containsText" dxfId="95" priority="15" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A103)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="16" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A103)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="17" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A103)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="18" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A103)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A104)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="91" priority="19" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A103)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A104)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
+  <conditionalFormatting sqref="A55">
     <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54">
+  <conditionalFormatting sqref="A55">
     <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A55)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A54)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A55)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added proxy auto detection on Windows - hard to test without a proxy server!
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arond\Documents\NREL_Projects\SAMnt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adobos\Projects\SAMnt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3808,8 +3808,8 @@
   <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>192</v>
+        <v>651</v>
       </c>
       <c r="B27" s="63" t="s">
         <v>656</v>
@@ -4391,7 +4391,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B44" s="63" t="s">
         <v>680</v>

</xml_diff>

<commit_message>
updated TODO with linux version updates
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -2024,9 +2024,6 @@
     <t>Steve/Sara</t>
   </si>
   <si>
-    <t>Remove webkitgtk dependencies on Linux OS, rebuild on CentOS 6.4 as standard</t>
-  </si>
-  <si>
     <t>Wind wizard</t>
   </si>
   <si>
@@ -2088,6 +2085,9 @@
   </si>
   <si>
     <t>environment scope bug in LK ++/-- operator</t>
+  </si>
+  <si>
+    <t>Remove webkitgtk dependencies on Linux OS, rebuild on CentOS 6.6 as standard</t>
   </si>
 </sst>
 </file>
@@ -3808,8 +3808,8 @@
   <dimension ref="A1:F150"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3887,7 +3887,7 @@
         <v>192</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C5" s="63" t="s">
         <v>47</v>
@@ -3900,7 +3900,7 @@
         <v>192</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C6" s="63" t="s">
         <v>47</v>
@@ -4111,7 +4111,7 @@
         <v>648</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
@@ -4170,7 +4170,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>651</v>
+        <v>55</v>
       </c>
       <c r="B27" s="63" t="s">
         <v>656</v>
@@ -4199,7 +4199,7 @@
         <v>192</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C29" s="63" t="s">
         <v>645</v>
@@ -4209,10 +4209,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B30" s="63" t="s">
-        <v>659</v>
+        <v>680</v>
       </c>
       <c r="C30" s="63" t="s">
         <v>46</v>
@@ -4225,7 +4225,7 @@
         <v>55</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C31" s="63" t="s">
         <v>45</v>
@@ -4238,7 +4238,7 @@
         <v>651</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C32" s="63" t="s">
         <v>302</v>
@@ -4251,7 +4251,7 @@
         <v>651</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C33" s="63" t="s">
         <v>302</v>
@@ -4264,7 +4264,7 @@
         <v>651</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C34" s="63" t="s">
         <v>124</v>
@@ -4277,7 +4277,7 @@
         <v>192</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C35" s="63" t="s">
         <v>124</v>
@@ -4290,7 +4290,7 @@
         <v>651</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C36" s="63" t="s">
         <v>47</v>
@@ -4300,10 +4300,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B37" s="63" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C37" s="63" t="s">
         <v>46</v>
@@ -4316,7 +4316,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="C38" s="63" t="s">
         <v>46</v>
@@ -4329,7 +4329,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C39" s="63" t="s">
         <v>46</v>
@@ -4342,10 +4342,10 @@
         <v>108</v>
       </c>
       <c r="B40" s="63" t="s">
+        <v>667</v>
+      </c>
+      <c r="C40" s="63" t="s">
         <v>668</v>
-      </c>
-      <c r="C40" s="63" t="s">
-        <v>669</v>
       </c>
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
@@ -4355,7 +4355,7 @@
         <v>108</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C41" s="63" t="s">
         <v>46</v>
@@ -4368,7 +4368,7 @@
         <v>192</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C42" s="63" t="s">
         <v>46</v>
@@ -4381,7 +4381,7 @@
         <v>192</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C43" s="63" t="s">
         <v>47</v>
@@ -4394,7 +4394,7 @@
         <v>55</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="C44" s="63" t="s">
         <v>46</v>
@@ -4517,7 +4517,7 @@
         <v>135</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="40"/>
@@ -4544,7 +4544,7 @@
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="32"/>
       <c r="B61" s="31" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update to todo list.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="690">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1967,9 +1967,6 @@
     <t>Next release: enable lifetime analysis for no financials (includes moving analysis period into performance models)</t>
   </si>
   <si>
-    <t>Hook to the new NSRDB</t>
-  </si>
-  <si>
     <t>Check output timestamp labels for 1-min data</t>
   </si>
   <si>
@@ -2024,9 +2021,6 @@
     <t>Steve/Sara</t>
   </si>
   <si>
-    <t>Wind wizard</t>
-  </si>
-  <si>
     <t>User defined power cycle input option</t>
   </si>
   <si>
@@ -2090,13 +2084,37 @@
     <t>Remove webkitgtk dependencies on Linux OS, rebuild on CentOS 6.6 as standard</t>
   </si>
   <si>
-    <t xml:space="preserve">remove solar prospector hook?  </t>
-  </si>
-  <si>
     <t>aron</t>
   </si>
   <si>
     <t>p50/p90 better outputs</t>
+  </si>
+  <si>
+    <t>Hamburger menu!</t>
+  </si>
+  <si>
+    <t>Hook to the new NSRDB. Fix issue with SAMAPIKEY exceeding rate limit. Put URL in webapi.conf</t>
+  </si>
+  <si>
+    <t>remove solar prospector code</t>
+  </si>
+  <si>
+    <t>review stack overflow issue when deleting nodes</t>
+  </si>
+  <si>
+    <t>ngtd</t>
+  </si>
+  <si>
+    <t>Aron/Steve/Nick</t>
+  </si>
+  <si>
+    <t>Year-by-year hourly results from P50/P90 runs</t>
+  </si>
+  <si>
+    <t>Wind wizard (test with latest version of LK that is checked in)</t>
+  </si>
+  <si>
+    <t>Fix todo list formatting issues or fix users.</t>
   </si>
 </sst>
 </file>
@@ -3814,11 +3832,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F152"/>
+  <dimension ref="A1:F156"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3854,7 +3872,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
-        <v>192</v>
+        <v>685</v>
       </c>
       <c r="B2" s="62" t="s">
         <v>281</v>
@@ -3867,15 +3885,15 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="63" t="s">
-        <v>516</v>
+        <v>192</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>689</v>
       </c>
       <c r="C3" s="63" t="s">
-        <v>68</v>
-      </c>
-      <c r="D3" s="63"/>
+        <v>45</v>
+      </c>
+      <c r="D3" s="64"/>
       <c r="E3" s="63"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -3883,23 +3901,23 @@
         <v>55</v>
       </c>
       <c r="B4" s="63" t="s">
-        <v>621</v>
+        <v>516</v>
       </c>
       <c r="C4" s="63" t="s">
-        <v>225</v>
+        <v>68</v>
       </c>
       <c r="D4" s="63"/>
       <c r="E4" s="63"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>676</v>
+        <v>621</v>
       </c>
       <c r="C5" s="63" t="s">
-        <v>47</v>
+        <v>225</v>
       </c>
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
@@ -3909,88 +3927,88 @@
         <v>192</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>675</v>
+        <v>684</v>
       </c>
       <c r="C6" s="63" t="s">
-        <v>47</v>
+        <v>686</v>
       </c>
       <c r="D6" s="63"/>
       <c r="E6" s="63"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
-        <v>108</v>
+        <v>192</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>628</v>
+        <v>674</v>
       </c>
       <c r="C7" s="63" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="D7" s="63"/>
       <c r="E7" s="63"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B8" s="63" t="s">
-        <v>630</v>
+        <v>673</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>237</v>
+        <v>47</v>
       </c>
       <c r="D8" s="63"/>
       <c r="E8" s="63"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>477</v>
+        <v>65</v>
       </c>
       <c r="D9" s="63"/>
       <c r="E9" s="63"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="B10" s="63" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C10" s="63" t="s">
-        <v>46</v>
+        <v>237</v>
       </c>
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="C11" s="63" t="s">
-        <v>45</v>
+        <v>477</v>
       </c>
       <c r="D11" s="63"/>
       <c r="E11" s="63"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>634</v>
+        <v>631</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D12" s="63"/>
       <c r="E12" s="63"/>
@@ -4000,7 +4018,7 @@
         <v>192</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>635</v>
+        <v>632</v>
       </c>
       <c r="C13" s="63" t="s">
         <v>45</v>
@@ -4013,7 +4031,7 @@
         <v>192</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="C14" s="63" t="s">
         <v>45</v>
@@ -4023,13 +4041,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>637</v>
+        <v>45</v>
       </c>
       <c r="D15" s="63"/>
       <c r="E15" s="63"/>
@@ -4039,7 +4057,7 @@
         <v>192</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="C16" s="63" t="s">
         <v>45</v>
@@ -4052,10 +4070,10 @@
         <v>55</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>642</v>
+        <v>637</v>
       </c>
       <c r="D17" s="63"/>
       <c r="E17" s="63"/>
@@ -4065,23 +4083,23 @@
         <v>192</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>644</v>
+        <v>633</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>645</v>
+        <v>45</v>
       </c>
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>649</v>
+        <v>640</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>45</v>
+        <v>641</v>
       </c>
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
@@ -4091,20 +4109,20 @@
         <v>192</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>45</v>
+        <v>644</v>
       </c>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>108</v>
+        <v>192</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="C21" s="63" t="s">
         <v>45</v>
@@ -4114,39 +4132,39 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>108</v>
+        <v>192</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>670</v>
+        <v>45</v>
       </c>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>651</v>
+        <v>108</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>640</v>
+        <v>646</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D23" s="63"/>
       <c r="E23" s="63"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>681</v>
+        <v>647</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>682</v>
+        <v>668</v>
       </c>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
@@ -4156,88 +4174,88 @@
         <v>192</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>682</v>
+        <v>46</v>
       </c>
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>651</v>
+        <v>192</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>653</v>
+        <v>683</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>307</v>
+        <v>679</v>
       </c>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>651</v>
+        <v>108</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>654</v>
+        <v>680</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>45</v>
+        <v>679</v>
       </c>
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>655</v>
+        <v>687</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>225</v>
+        <v>46</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>656</v>
+        <v>681</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>46</v>
+        <v>679</v>
       </c>
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B30" s="63" t="s">
-        <v>657</v>
+        <v>652</v>
       </c>
       <c r="C30" s="63" t="s">
-        <v>658</v>
+        <v>307</v>
       </c>
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>192</v>
+        <v>650</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>677</v>
+        <v>653</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>645</v>
+        <v>45</v>
       </c>
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
@@ -4247,10 +4265,10 @@
         <v>55</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>680</v>
+        <v>654</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>46</v>
+        <v>225</v>
       </c>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
@@ -4260,134 +4278,134 @@
         <v>55</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>302</v>
+        <v>657</v>
       </c>
       <c r="D34" s="63"/>
       <c r="E34" s="63"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
-        <v>651</v>
+        <v>192</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>661</v>
+        <v>675</v>
       </c>
       <c r="C35" s="63" t="s">
-        <v>302</v>
+        <v>68</v>
       </c>
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>662</v>
+        <v>678</v>
       </c>
       <c r="C36" s="63" t="s">
-        <v>124</v>
+        <v>46</v>
       </c>
       <c r="D36" s="63"/>
       <c r="E36" s="63"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
-        <v>192</v>
+        <v>650</v>
       </c>
       <c r="B37" s="63" t="s">
-        <v>663</v>
+        <v>688</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>124</v>
+        <v>45</v>
       </c>
       <c r="D37" s="63"/>
       <c r="E37" s="63"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>664</v>
+        <v>658</v>
       </c>
       <c r="C38" s="63" t="s">
-        <v>47</v>
+        <v>302</v>
       </c>
       <c r="D38" s="63"/>
       <c r="E38" s="63"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
-        <v>55</v>
+        <v>650</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>671</v>
+        <v>659</v>
       </c>
       <c r="C39" s="63" t="s">
-        <v>46</v>
+        <v>302</v>
       </c>
       <c r="D39" s="63"/>
       <c r="E39" s="63"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
-        <v>55</v>
+        <v>650</v>
       </c>
       <c r="B40" s="63" t="s">
-        <v>665</v>
+        <v>660</v>
       </c>
       <c r="C40" s="63" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>666</v>
+        <v>661</v>
       </c>
       <c r="C41" s="63" t="s">
-        <v>46</v>
+        <v>124</v>
       </c>
       <c r="D41" s="63"/>
       <c r="E41" s="63"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>108</v>
+        <v>650</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>667</v>
+        <v>662</v>
       </c>
       <c r="C42" s="63" t="s">
-        <v>668</v>
+        <v>47</v>
       </c>
       <c r="D42" s="63"/>
       <c r="E42" s="63"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
-        <v>108</v>
+        <v>650</v>
       </c>
       <c r="B43" s="63" t="s">
         <v>669</v>
@@ -4400,10 +4418,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>678</v>
+        <v>663</v>
       </c>
       <c r="C44" s="63" t="s">
         <v>46</v>
@@ -4413,80 +4431,88 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B45" s="63" t="s">
-        <v>674</v>
+        <v>664</v>
       </c>
       <c r="C45" s="63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D45" s="63"/>
       <c r="E45" s="63"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="B46" s="63" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="C46" s="63" t="s">
-        <v>46</v>
+        <v>666</v>
       </c>
       <c r="D46" s="63"/>
       <c r="E46" s="63"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B47" s="40" t="s">
-        <v>549</v>
-      </c>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
+        <v>108</v>
+      </c>
+      <c r="B47" s="63" t="s">
+        <v>667</v>
+      </c>
+      <c r="C47" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D47" s="63"/>
+      <c r="E47" s="63"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B48" s="40" t="s">
-        <v>550</v>
-      </c>
-      <c r="C48" s="40"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
+        <v>192</v>
+      </c>
+      <c r="B48" s="63" t="s">
+        <v>676</v>
+      </c>
+      <c r="C48" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D48" s="63"/>
+      <c r="E48" s="63"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B49" s="40" t="s">
-        <v>650</v>
-      </c>
-      <c r="C49" s="40"/>
-      <c r="D49" s="40"/>
-      <c r="E49" s="40"/>
+        <v>192</v>
+      </c>
+      <c r="B49" s="63" t="s">
+        <v>672</v>
+      </c>
+      <c r="C49" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="63"/>
+      <c r="E49" s="63"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B50" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" s="40"/>
-      <c r="D50" s="40"/>
-      <c r="E50" s="40"/>
+        <v>55</v>
+      </c>
+      <c r="B50" s="63" t="s">
+        <v>677</v>
+      </c>
+      <c r="C50" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>545</v>
+        <v>549</v>
       </c>
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
@@ -4497,7 +4523,7 @@
         <v>135</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>542</v>
+        <v>550</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
@@ -4508,7 +4534,7 @@
         <v>135</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>543</v>
+        <v>649</v>
       </c>
       <c r="C53" s="40"/>
       <c r="D53" s="40"/>
@@ -4519,7 +4545,7 @@
         <v>135</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>544</v>
+        <v>136</v>
       </c>
       <c r="C54" s="40"/>
       <c r="D54" s="40"/>
@@ -4530,7 +4556,7 @@
         <v>135</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>646</v>
+        <v>545</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="40"/>
@@ -4541,7 +4567,7 @@
         <v>135</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>643</v>
+        <v>542</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="40"/>
@@ -4552,85 +4578,117 @@
         <v>135</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>673</v>
+        <v>543</v>
       </c>
       <c r="C57" s="40"/>
       <c r="D57" s="40"/>
       <c r="E57" s="40"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="32"/>
+      <c r="A58" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B58" s="40" t="s">
+        <v>544</v>
+      </c>
+      <c r="C58" s="40"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="32"/>
+      <c r="A59" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B59" s="40" t="s">
+        <v>645</v>
+      </c>
+      <c r="C59" s="40"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60" s="32"/>
+      <c r="A60" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B60" s="40" t="s">
+        <v>642</v>
+      </c>
+      <c r="C60" s="40"/>
+      <c r="D60" s="40"/>
+      <c r="E60" s="40"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61" s="32"/>
+      <c r="A61" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="40" t="s">
+        <v>671</v>
+      </c>
+      <c r="C61" s="40"/>
+      <c r="D61" s="40"/>
+      <c r="E61" s="40"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="32"/>
-      <c r="B62" s="31" t="s">
-        <v>639</v>
-      </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="32"/>
-      <c r="B63" s="31" t="s">
-        <v>672</v>
-      </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="32"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="32"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="32"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B66" s="31" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="32"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B67" s="31" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="32"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="32"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="32"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="32"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="32"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="32"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="32"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="32"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="32"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="32"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="32"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="32"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="32"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
@@ -4718,7 +4776,7 @@
       <c r="A108" s="32"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A109" s="33"/>
+      <c r="A109" s="32"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="32"/>
@@ -4730,7 +4788,7 @@
       <c r="A112" s="32"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="32"/>
+      <c r="A113" s="33"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="32"/>
@@ -4744,11 +4802,23 @@
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="32"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A152" s="33"/>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A118" s="32"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A119" s="32"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A120" s="32"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A121" s="32"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A156" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A58:A103 A1:A56">
+  <conditionalFormatting sqref="A62:A107 A1:A60">
     <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4765,7 +4835,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A58:A214 A1:A56">
+  <conditionalFormatting sqref="A62:A218 A1:A60">
     <cfRule type="containsText" dxfId="104" priority="23" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4773,71 +4843,71 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A104:A105">
+  <conditionalFormatting sqref="A108:A109">
     <cfRule type="containsText" dxfId="102" priority="10" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A104)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A108)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="11" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A104)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A108)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="12" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A104)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A108)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="13" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A104)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A108)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="98" priority="14" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A104)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A108)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A217:A1048576">
+  <conditionalFormatting sqref="A221:A1048576">
     <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A217)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A221)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A217)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A221)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A106:A214 A217:A1048576">
+  <conditionalFormatting sqref="A110:A218 A221:A1048576">
     <cfRule type="containsText" dxfId="95" priority="15" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A110)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="16" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A110)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="17" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A110)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="18" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A110)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="91" priority="19" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A106)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A110)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
+  <conditionalFormatting sqref="A61">
     <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57">
+  <conditionalFormatting sqref="A61">
     <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A61)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A57)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A61)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added issue about copy to clipboard for wxExtGridCtrl
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adobos\Projects\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
   </bookViews>
@@ -20,12 +25,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1954" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1957" uniqueCount="691">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2110,6 +2115,9 @@
   </si>
   <si>
     <t>Made blade &amp; tower design advanced by default- put something in project file upgrader?</t>
+  </si>
+  <si>
+    <t>SDK tool Copy-to-clipboard issues due to changes in wxExtGridCtrl</t>
   </si>
 </sst>
 </file>
@@ -3583,7 +3591,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3618,7 +3626,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3827,11 +3835,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F156"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4052,62 +4060,62 @@
         <v>192</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D16" s="63"/>
       <c r="E16" s="63"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>637</v>
+        <v>689</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>636</v>
+        <v>45</v>
       </c>
       <c r="D17" s="63"/>
       <c r="E17" s="63"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>45</v>
+        <v>636</v>
       </c>
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>640</v>
+        <v>45</v>
       </c>
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
@@ -4117,10 +4125,10 @@
         <v>192</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>45</v>
+        <v>643</v>
       </c>
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
@@ -4130,7 +4138,7 @@
         <v>192</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C22" s="63" t="s">
         <v>45</v>
@@ -4140,10 +4148,10 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>108</v>
+        <v>192</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="C23" s="63" t="s">
         <v>45</v>
@@ -4156,23 +4164,23 @@
         <v>108</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>667</v>
+        <v>45</v>
       </c>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>681</v>
+        <v>646</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>46</v>
+        <v>667</v>
       </c>
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
@@ -4182,20 +4190,20 @@
         <v>192</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>678</v>
+        <v>46</v>
       </c>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>108</v>
+        <v>192</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="C27" s="63" t="s">
         <v>678</v>
@@ -4208,36 +4216,36 @@
         <v>108</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>46</v>
+        <v>678</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>678</v>
+        <v>46</v>
       </c>
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>649</v>
+        <v>192</v>
       </c>
       <c r="B30" s="63" t="s">
-        <v>651</v>
+        <v>680</v>
       </c>
       <c r="C30" s="63" t="s">
-        <v>307</v>
+        <v>678</v>
       </c>
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
@@ -4247,23 +4255,23 @@
         <v>649</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>45</v>
+        <v>307</v>
       </c>
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
-        <v>55</v>
+        <v>649</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
@@ -4273,49 +4281,49 @@
         <v>55</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>46</v>
+        <v>225</v>
       </c>
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
-        <v>649</v>
+        <v>55</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>656</v>
+        <v>46</v>
       </c>
       <c r="D34" s="63"/>
       <c r="E34" s="63"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
-        <v>192</v>
+        <v>649</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>674</v>
+        <v>655</v>
       </c>
       <c r="C35" s="63" t="s">
-        <v>68</v>
+        <v>656</v>
       </c>
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>649</v>
+        <v>192</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C36" s="63" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D36" s="63"/>
       <c r="E36" s="63"/>
@@ -4325,10 +4333,10 @@
         <v>649</v>
       </c>
       <c r="B37" s="63" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D37" s="63"/>
       <c r="E37" s="63"/>
@@ -4338,10 +4346,10 @@
         <v>649</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>657</v>
+        <v>687</v>
       </c>
       <c r="C38" s="63" t="s">
-        <v>302</v>
+        <v>45</v>
       </c>
       <c r="D38" s="63"/>
       <c r="E38" s="63"/>
@@ -4351,7 +4359,7 @@
         <v>649</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C39" s="63" t="s">
         <v>302</v>
@@ -4364,20 +4372,20 @@
         <v>649</v>
       </c>
       <c r="B40" s="63" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C40" s="63" t="s">
-        <v>124</v>
+        <v>302</v>
       </c>
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
-        <v>192</v>
+        <v>649</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C41" s="63" t="s">
         <v>124</v>
@@ -4387,13 +4395,13 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>649</v>
+        <v>192</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C42" s="63" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="D42" s="63"/>
       <c r="E42" s="63"/>
@@ -4403,20 +4411,20 @@
         <v>649</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="C43" s="63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D43" s="63"/>
       <c r="E43" s="63"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
-        <v>55</v>
+        <v>649</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
       <c r="C44" s="63" t="s">
         <v>46</v>
@@ -4429,7 +4437,7 @@
         <v>55</v>
       </c>
       <c r="B45" s="63" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C45" s="63" t="s">
         <v>46</v>
@@ -4439,13 +4447,13 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="B46" s="63" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C46" s="63" t="s">
-        <v>665</v>
+        <v>46</v>
       </c>
       <c r="D46" s="63"/>
       <c r="E46" s="63"/>
@@ -4455,20 +4463,20 @@
         <v>108</v>
       </c>
       <c r="B47" s="63" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C47" s="63" t="s">
-        <v>46</v>
+        <v>665</v>
       </c>
       <c r="D47" s="63"/>
       <c r="E47" s="63"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B48" s="63" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
       <c r="C48" s="63" t="s">
         <v>46</v>
@@ -4481,44 +4489,46 @@
         <v>192</v>
       </c>
       <c r="B49" s="63" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="C49" s="63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D49" s="63"/>
       <c r="E49" s="63"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B50" s="63" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="C50" s="63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D50" s="63"/>
       <c r="E50" s="63"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B51" s="40" t="s">
-        <v>549</v>
-      </c>
-      <c r="C51" s="40"/>
-      <c r="D51" s="40"/>
-      <c r="E51" s="40"/>
+        <v>55</v>
+      </c>
+      <c r="B51" s="63" t="s">
+        <v>676</v>
+      </c>
+      <c r="C51" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="63"/>
+      <c r="E51" s="63"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
@@ -4529,7 +4539,7 @@
         <v>135</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>648</v>
+        <v>550</v>
       </c>
       <c r="C53" s="40"/>
       <c r="D53" s="40"/>
@@ -4540,7 +4550,7 @@
         <v>135</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>136</v>
+        <v>648</v>
       </c>
       <c r="C54" s="40"/>
       <c r="D54" s="40"/>
@@ -4551,7 +4561,7 @@
         <v>135</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>545</v>
+        <v>136</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="40"/>
@@ -4562,7 +4572,7 @@
         <v>135</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="40"/>
@@ -4573,7 +4583,7 @@
         <v>135</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C57" s="40"/>
       <c r="D57" s="40"/>
@@ -4584,7 +4594,7 @@
         <v>135</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C58" s="40"/>
       <c r="D58" s="40"/>
@@ -4595,7 +4605,7 @@
         <v>135</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>644</v>
+        <v>544</v>
       </c>
       <c r="C59" s="40"/>
       <c r="D59" s="40"/>
@@ -4606,7 +4616,7 @@
         <v>135</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="C60" s="40"/>
       <c r="D60" s="40"/>
@@ -4617,14 +4627,22 @@
         <v>135</v>
       </c>
       <c r="B61" s="40" t="s">
-        <v>670</v>
+        <v>641</v>
       </c>
       <c r="C61" s="40"/>
       <c r="D61" s="40"/>
       <c r="E61" s="40"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A62" s="32"/>
+      <c r="A62" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B62" s="40" t="s">
+        <v>670</v>
+      </c>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="40"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="32"/>
@@ -4637,18 +4655,18 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="32"/>
-      <c r="B66" s="31" t="s">
-        <v>638</v>
-      </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="32"/>
       <c r="B67" s="31" t="s">
-        <v>669</v>
+        <v>638</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="32"/>
+      <c r="B68" s="31" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="32"/>
@@ -4783,10 +4801,10 @@
       <c r="A112" s="32"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="33"/>
+      <c r="A113" s="32"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="32"/>
+      <c r="A114" s="33"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="32"/>
@@ -4809,11 +4827,14 @@
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="32"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156" s="33"/>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="32"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A62:A107 A1:A60">
+  <conditionalFormatting sqref="A63:A108 A1:A61">
     <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4830,7 +4851,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A62:A218 A1:A60">
+  <conditionalFormatting sqref="A63:A219 A1:A61">
     <cfRule type="containsText" dxfId="104" priority="23" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4838,71 +4859,71 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A108:A109">
+  <conditionalFormatting sqref="A109:A110">
     <cfRule type="containsText" dxfId="102" priority="10" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="11" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="12" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="13" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="98" priority="14" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A109)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A221:A1048576">
+  <conditionalFormatting sqref="A222:A1048576">
     <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A222)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A222)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A110:A218 A221:A1048576">
+  <conditionalFormatting sqref="A111:A219 A222:A1048576">
     <cfRule type="containsText" dxfId="95" priority="15" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="16" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="17" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="18" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="91" priority="19" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A111)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
+  <conditionalFormatting sqref="A62">
     <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A61">
+  <conditionalFormatting sqref="A62">
     <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A62)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A61)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Removed solar prospector code.  Using new NSRDB APIs.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -3839,7 +3839,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4200,7 +4200,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B27" s="63" t="s">
         <v>682</v>

</xml_diff>

<commit_message>
Added case import feature.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1960" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="694">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2124,6 +2124,9 @@
   </si>
   <si>
     <t>Aron/Anthony</t>
+  </si>
+  <si>
+    <t>Add case import feature to bring in cases from other project files</t>
   </si>
 </sst>
 </file>
@@ -3841,11 +3844,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F158"/>
+  <dimension ref="A1:F159"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4024,13 +4027,13 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>632</v>
+        <v>693</v>
       </c>
       <c r="C13" s="63" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
@@ -4040,7 +4043,7 @@
         <v>192</v>
       </c>
       <c r="B14" s="63" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="C14" s="63" t="s">
         <v>45</v>
@@ -4053,7 +4056,7 @@
         <v>192</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="C15" s="63" t="s">
         <v>45</v>
@@ -4066,10 +4069,10 @@
         <v>192</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>690</v>
+        <v>635</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" s="63"/>
       <c r="E16" s="63"/>
@@ -4079,62 +4082,62 @@
         <v>192</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" s="63"/>
       <c r="E17" s="63"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>637</v>
+        <v>689</v>
       </c>
       <c r="C18" s="63" t="s">
-        <v>636</v>
+        <v>45</v>
       </c>
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>45</v>
+        <v>636</v>
       </c>
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>640</v>
+        <v>45</v>
       </c>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
@@ -4144,10 +4147,10 @@
         <v>192</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>45</v>
+        <v>643</v>
       </c>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
@@ -4157,7 +4160,7 @@
         <v>192</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="C23" s="63" t="s">
         <v>45</v>
@@ -4167,10 +4170,10 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
-        <v>108</v>
+        <v>192</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>645</v>
+        <v>650</v>
       </c>
       <c r="C24" s="63" t="s">
         <v>45</v>
@@ -4183,59 +4186,59 @@
         <v>108</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>667</v>
+        <v>45</v>
       </c>
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>691</v>
+        <v>646</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>692</v>
+        <v>667</v>
       </c>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>649</v>
+        <v>192</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>681</v>
+        <v>691</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>46</v>
+        <v>692</v>
       </c>
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>55</v>
+        <v>649</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>678</v>
+        <v>46</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="C29" s="63" t="s">
         <v>678</v>
@@ -4248,36 +4251,36 @@
         <v>108</v>
       </c>
       <c r="B30" s="63" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
       <c r="C30" s="63" t="s">
-        <v>46</v>
+        <v>678</v>
       </c>
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>680</v>
+        <v>686</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>678</v>
+        <v>46</v>
       </c>
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
-        <v>649</v>
+        <v>192</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>651</v>
+        <v>680</v>
       </c>
       <c r="C32" s="63" t="s">
-        <v>307</v>
+        <v>678</v>
       </c>
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
@@ -4287,23 +4290,23 @@
         <v>649</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>45</v>
+        <v>307</v>
       </c>
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
-        <v>55</v>
+        <v>649</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C34" s="63" t="s">
-        <v>225</v>
+        <v>45</v>
       </c>
       <c r="D34" s="63"/>
       <c r="E34" s="63"/>
@@ -4313,49 +4316,49 @@
         <v>55</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="C35" s="63" t="s">
-        <v>46</v>
+        <v>225</v>
       </c>
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
-        <v>649</v>
+        <v>55</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="C36" s="63" t="s">
-        <v>656</v>
+        <v>46</v>
       </c>
       <c r="D36" s="63"/>
       <c r="E36" s="63"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
-        <v>192</v>
+        <v>649</v>
       </c>
       <c r="B37" s="63" t="s">
-        <v>674</v>
+        <v>655</v>
       </c>
       <c r="C37" s="63" t="s">
-        <v>68</v>
+        <v>656</v>
       </c>
       <c r="D37" s="63"/>
       <c r="E37" s="63"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
-        <v>649</v>
+        <v>192</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="C38" s="63" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="D38" s="63"/>
       <c r="E38" s="63"/>
@@ -4365,10 +4368,10 @@
         <v>649</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>687</v>
+        <v>677</v>
       </c>
       <c r="C39" s="63" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D39" s="63"/>
       <c r="E39" s="63"/>
@@ -4378,10 +4381,10 @@
         <v>649</v>
       </c>
       <c r="B40" s="63" t="s">
-        <v>657</v>
+        <v>687</v>
       </c>
       <c r="C40" s="63" t="s">
-        <v>302</v>
+        <v>45</v>
       </c>
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
@@ -4391,7 +4394,7 @@
         <v>649</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C41" s="63" t="s">
         <v>302</v>
@@ -4404,20 +4407,20 @@
         <v>649</v>
       </c>
       <c r="B42" s="63" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C42" s="63" t="s">
-        <v>124</v>
+        <v>302</v>
       </c>
       <c r="D42" s="63"/>
       <c r="E42" s="63"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
-        <v>192</v>
+        <v>649</v>
       </c>
       <c r="B43" s="63" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C43" s="63" t="s">
         <v>124</v>
@@ -4427,13 +4430,13 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
-        <v>649</v>
+        <v>192</v>
       </c>
       <c r="B44" s="63" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C44" s="63" t="s">
-        <v>47</v>
+        <v>124</v>
       </c>
       <c r="D44" s="63"/>
       <c r="E44" s="63"/>
@@ -4443,20 +4446,20 @@
         <v>649</v>
       </c>
       <c r="B45" s="63" t="s">
-        <v>668</v>
+        <v>661</v>
       </c>
       <c r="C45" s="63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D45" s="63"/>
       <c r="E45" s="63"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
-        <v>55</v>
+        <v>649</v>
       </c>
       <c r="B46" s="63" t="s">
-        <v>662</v>
+        <v>668</v>
       </c>
       <c r="C46" s="63" t="s">
         <v>46</v>
@@ -4469,7 +4472,7 @@
         <v>55</v>
       </c>
       <c r="B47" s="63" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="C47" s="63" t="s">
         <v>46</v>
@@ -4479,13 +4482,13 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="B48" s="63" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="C48" s="63" t="s">
-        <v>665</v>
+        <v>46</v>
       </c>
       <c r="D48" s="63"/>
       <c r="E48" s="63"/>
@@ -4495,20 +4498,20 @@
         <v>108</v>
       </c>
       <c r="B49" s="63" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="C49" s="63" t="s">
-        <v>46</v>
+        <v>665</v>
       </c>
       <c r="D49" s="63"/>
       <c r="E49" s="63"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="B50" s="63" t="s">
-        <v>675</v>
+        <v>666</v>
       </c>
       <c r="C50" s="63" t="s">
         <v>46</v>
@@ -4521,44 +4524,46 @@
         <v>192</v>
       </c>
       <c r="B51" s="63" t="s">
-        <v>671</v>
+        <v>675</v>
       </c>
       <c r="C51" s="63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D51" s="63"/>
       <c r="E51" s="63"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B52" s="63" t="s">
-        <v>676</v>
+        <v>671</v>
       </c>
       <c r="C52" s="63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D52" s="63"/>
       <c r="E52" s="63"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" s="40" t="s">
-        <v>549</v>
-      </c>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
+        <v>55</v>
+      </c>
+      <c r="B53" s="63" t="s">
+        <v>676</v>
+      </c>
+      <c r="C53" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D53" s="63"/>
+      <c r="E53" s="63"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C54" s="40"/>
       <c r="D54" s="40"/>
@@ -4569,7 +4574,7 @@
         <v>135</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>648</v>
+        <v>550</v>
       </c>
       <c r="C55" s="40"/>
       <c r="D55" s="40"/>
@@ -4580,7 +4585,7 @@
         <v>135</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>136</v>
+        <v>648</v>
       </c>
       <c r="C56" s="40"/>
       <c r="D56" s="40"/>
@@ -4591,7 +4596,7 @@
         <v>135</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>545</v>
+        <v>136</v>
       </c>
       <c r="C57" s="40"/>
       <c r="D57" s="40"/>
@@ -4602,7 +4607,7 @@
         <v>135</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C58" s="40"/>
       <c r="D58" s="40"/>
@@ -4613,7 +4618,7 @@
         <v>135</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="C59" s="40"/>
       <c r="D59" s="40"/>
@@ -4624,7 +4629,7 @@
         <v>135</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C60" s="40"/>
       <c r="D60" s="40"/>
@@ -4635,7 +4640,7 @@
         <v>135</v>
       </c>
       <c r="B61" s="40" t="s">
-        <v>644</v>
+        <v>544</v>
       </c>
       <c r="C61" s="40"/>
       <c r="D61" s="40"/>
@@ -4646,7 +4651,7 @@
         <v>135</v>
       </c>
       <c r="B62" s="40" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="C62" s="40"/>
       <c r="D62" s="40"/>
@@ -4657,14 +4662,22 @@
         <v>135</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>670</v>
+        <v>641</v>
       </c>
       <c r="C63" s="40"/>
       <c r="D63" s="40"/>
       <c r="E63" s="40"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A64" s="32"/>
+      <c r="A64" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" s="40" t="s">
+        <v>670</v>
+      </c>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="32"/>
@@ -4677,18 +4690,18 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="32"/>
-      <c r="B68" s="31" t="s">
-        <v>638</v>
-      </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="32"/>
       <c r="B69" s="31" t="s">
-        <v>669</v>
+        <v>638</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="32"/>
+      <c r="B70" s="31" t="s">
+        <v>669</v>
+      </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="32"/>
@@ -4823,10 +4836,10 @@
       <c r="A114" s="32"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A115" s="33"/>
+      <c r="A115" s="32"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A116" s="32"/>
+      <c r="A116" s="33"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="32"/>
@@ -4849,11 +4862,14 @@
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="32"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A158" s="33"/>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A124" s="32"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A159" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A64:A109 A1:A62">
+  <conditionalFormatting sqref="A65:A110 A1:A63">
     <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4870,7 +4886,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A64:A220 A1:A62">
+  <conditionalFormatting sqref="A65:A221 A1:A63">
     <cfRule type="containsText" dxfId="104" priority="23" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4878,71 +4894,71 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A110:A111">
+  <conditionalFormatting sqref="A111:A112">
     <cfRule type="containsText" dxfId="102" priority="10" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="11" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="12" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="13" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="98" priority="14" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A111)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A223:A1048576">
+  <conditionalFormatting sqref="A224:A1048576">
     <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A223)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A224)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A223)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A224)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A112:A220 A223:A1048576">
+  <conditionalFormatting sqref="A113:A221 A224:A1048576">
     <cfRule type="containsText" dxfId="95" priority="15" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A112)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A113)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="16" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A112)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A113)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="17" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A112)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A113)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="18" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A112)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A113)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="91" priority="19" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A112)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A113)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
+  <conditionalFormatting sqref="A64">
     <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
+  <conditionalFormatting sqref="A64">
     <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated wind wizard intro message box and to-do list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1963" uniqueCount="693">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1965" uniqueCount="693">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2097,9 +2097,6 @@
     <t>Year-by-year hourly results from P50/P90 runs</t>
   </si>
   <si>
-    <t>Wind wizard (test with latest version of LK that is checked in)</t>
-  </si>
-  <si>
     <t>Fix todo list formatting issues or fix users.</t>
   </si>
   <si>
@@ -2119,6 +2116,9 @@
   </si>
   <si>
     <t>Add simulation warning if negative wind turbine power curve values are input</t>
+  </si>
+  <si>
+    <t>Wind wizard sensitivity labels are null- fix and also check tornado chart macro</t>
   </si>
 </sst>
 </file>
@@ -3836,11 +3836,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F153"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G63" sqref="G63"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3879,7 +3879,7 @@
         <v>55</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="C2" s="63" t="s">
         <v>45</v>
@@ -3970,7 +3970,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C9" s="63" t="s">
         <v>46</v>
@@ -4009,7 +4009,7 @@
         <v>192</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="C12" s="63" t="s">
         <v>46</v>
@@ -4019,10 +4019,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C13" s="63" t="s">
         <v>45</v>
@@ -4045,26 +4045,26 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B15" s="63" t="s">
-        <v>633</v>
+        <v>638</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>45</v>
+        <v>639</v>
       </c>
       <c r="D15" s="63"/>
       <c r="E15" s="63"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B16" s="63" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="C16" s="63" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="D16" s="63"/>
       <c r="E16" s="63"/>
@@ -4074,10 +4074,10 @@
         <v>192</v>
       </c>
       <c r="B17" s="63" t="s">
-        <v>641</v>
+        <v>646</v>
       </c>
       <c r="C17" s="63" t="s">
-        <v>642</v>
+        <v>45</v>
       </c>
       <c r="D17" s="63"/>
       <c r="E17" s="63"/>
@@ -4087,7 +4087,7 @@
         <v>192</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="C18" s="63" t="s">
         <v>45</v>
@@ -4100,46 +4100,46 @@
         <v>192</v>
       </c>
       <c r="B19" s="63" t="s">
-        <v>649</v>
+        <v>688</v>
       </c>
       <c r="C19" s="63" t="s">
-        <v>45</v>
+        <v>689</v>
       </c>
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>192</v>
+        <v>648</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>689</v>
+        <v>680</v>
       </c>
       <c r="C20" s="63" t="s">
-        <v>690</v>
+        <v>46</v>
       </c>
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
-        <v>648</v>
+        <v>55</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>46</v>
+        <v>677</v>
       </c>
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C22" s="63" t="s">
         <v>677</v>
@@ -4149,13 +4149,13 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>192</v>
+        <v>648</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>679</v>
+        <v>650</v>
       </c>
       <c r="C23" s="63" t="s">
-        <v>677</v>
+        <v>307</v>
       </c>
       <c r="D23" s="63"/>
       <c r="E23" s="63"/>
@@ -4165,23 +4165,23 @@
         <v>648</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="C24" s="63" t="s">
-        <v>307</v>
+        <v>45</v>
       </c>
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
-        <v>648</v>
+        <v>55</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C25" s="63" t="s">
-        <v>45</v>
+        <v>225</v>
       </c>
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
@@ -4191,62 +4191,62 @@
         <v>55</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C26" s="63" t="s">
-        <v>225</v>
+        <v>46</v>
       </c>
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
-        <v>55</v>
+        <v>648</v>
       </c>
       <c r="B27" s="63" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C27" s="63" t="s">
-        <v>46</v>
+        <v>655</v>
       </c>
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>648</v>
+        <v>192</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>654</v>
+        <v>673</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>655</v>
+        <v>68</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
-        <v>192</v>
+        <v>648</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="C29" s="63" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
-        <v>648</v>
+        <v>192</v>
       </c>
       <c r="B30" s="63" t="s">
-        <v>676</v>
+        <v>692</v>
       </c>
       <c r="C30" s="63" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
@@ -4256,10 +4256,10 @@
         <v>648</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>685</v>
+        <v>656</v>
       </c>
       <c r="C31" s="63" t="s">
-        <v>45</v>
+        <v>302</v>
       </c>
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
@@ -4269,7 +4269,7 @@
         <v>648</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="C32" s="63" t="s">
         <v>302</v>
@@ -4282,20 +4282,20 @@
         <v>648</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="C33" s="63" t="s">
-        <v>302</v>
+        <v>124</v>
       </c>
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
-        <v>648</v>
+        <v>192</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C34" s="63" t="s">
         <v>124</v>
@@ -4305,13 +4305,13 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
-        <v>192</v>
+        <v>648</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="C35" s="63" t="s">
-        <v>124</v>
+        <v>47</v>
       </c>
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
@@ -4321,20 +4321,20 @@
         <v>648</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>660</v>
+        <v>667</v>
       </c>
       <c r="C36" s="63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D36" s="63"/>
       <c r="E36" s="63"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
-        <v>648</v>
+        <v>55</v>
       </c>
       <c r="B37" s="63" t="s">
-        <v>667</v>
+        <v>661</v>
       </c>
       <c r="C37" s="63" t="s">
         <v>46</v>
@@ -4347,7 +4347,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C38" s="63" t="s">
         <v>46</v>
@@ -4357,10 +4357,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>662</v>
+        <v>674</v>
       </c>
       <c r="C39" s="63" t="s">
         <v>46</v>
@@ -4373,46 +4373,44 @@
         <v>192</v>
       </c>
       <c r="B40" s="63" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="C40" s="63" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>670</v>
+        <v>675</v>
       </c>
       <c r="C41" s="63" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D41" s="63"/>
       <c r="E41" s="63"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="63" t="s">
-        <v>675</v>
-      </c>
-      <c r="C42" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="63"/>
-      <c r="E42" s="63"/>
+        <v>135</v>
+      </c>
+      <c r="B42" s="40" t="s">
+        <v>549</v>
+      </c>
+      <c r="C42" s="40"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C43" s="40"/>
       <c r="D43" s="40"/>
@@ -4423,7 +4421,7 @@
         <v>135</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>550</v>
+        <v>647</v>
       </c>
       <c r="C44" s="40"/>
       <c r="D44" s="40"/>
@@ -4434,7 +4432,7 @@
         <v>135</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>647</v>
+        <v>136</v>
       </c>
       <c r="C45" s="40"/>
       <c r="D45" s="40"/>
@@ -4445,7 +4443,7 @@
         <v>135</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>136</v>
+        <v>545</v>
       </c>
       <c r="C46" s="40"/>
       <c r="D46" s="40"/>
@@ -4456,7 +4454,7 @@
         <v>135</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="C47" s="40"/>
       <c r="D47" s="40"/>
@@ -4467,7 +4465,7 @@
         <v>135</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C48" s="40"/>
       <c r="D48" s="40"/>
@@ -4478,7 +4476,7 @@
         <v>135</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C49" s="40"/>
       <c r="D49" s="40"/>
@@ -4489,7 +4487,7 @@
         <v>135</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>544</v>
+        <v>643</v>
       </c>
       <c r="C50" s="40"/>
       <c r="D50" s="40"/>
@@ -4500,7 +4498,7 @@
         <v>135</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="C51" s="40"/>
       <c r="D51" s="40"/>
@@ -4511,7 +4509,7 @@
         <v>135</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>640</v>
+        <v>669</v>
       </c>
       <c r="C52" s="40"/>
       <c r="D52" s="40"/>
@@ -4519,181 +4517,193 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B53" s="40" t="s">
-        <v>669</v>
-      </c>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="40"/>
+        <v>108</v>
+      </c>
+      <c r="B53" s="47" t="s">
+        <v>633</v>
+      </c>
+      <c r="C53" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D53" s="47"/>
+      <c r="E53" s="47"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54" s="32"/>
+      <c r="A54" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>637</v>
+      </c>
+      <c r="C54" s="47"/>
+      <c r="D54" s="47"/>
+      <c r="E54" s="47"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55" s="32"/>
+      <c r="A55" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="47" t="s">
+        <v>668</v>
+      </c>
+      <c r="C55" s="47"/>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56" s="32"/>
+      <c r="A56" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="47" t="s">
+        <v>628</v>
+      </c>
+      <c r="C56" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="47"/>
+      <c r="E56" s="47"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57" s="32"/>
+      <c r="A57" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>630</v>
+      </c>
+      <c r="C57" s="47" t="s">
+        <v>237</v>
+      </c>
+      <c r="D57" s="47"/>
+      <c r="E57" s="47"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58" s="32"/>
-      <c r="B58" s="31" t="s">
-        <v>637</v>
-      </c>
+      <c r="A58" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B58" s="47" t="s">
+        <v>631</v>
+      </c>
+      <c r="C58" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D58" s="47"/>
+      <c r="E58" s="47"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59" s="32"/>
-      <c r="B59" s="31" t="s">
-        <v>668</v>
-      </c>
+      <c r="A59" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B59" s="47" t="s">
+        <v>691</v>
+      </c>
+      <c r="C59" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D59" s="47"/>
+      <c r="E59" s="47"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="63" t="s">
-        <v>628</v>
-      </c>
-      <c r="C60" s="63" t="s">
-        <v>65</v>
-      </c>
-      <c r="D60" s="63"/>
-      <c r="E60" s="63"/>
+      <c r="B60" s="47" t="s">
+        <v>644</v>
+      </c>
+      <c r="C60" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B61" s="63" t="s">
-        <v>630</v>
-      </c>
-      <c r="C61" s="63" t="s">
-        <v>237</v>
-      </c>
-      <c r="D61" s="63"/>
-      <c r="E61" s="63"/>
+      <c r="B61" s="47" t="s">
+        <v>645</v>
+      </c>
+      <c r="C61" s="47" t="s">
+        <v>666</v>
+      </c>
+      <c r="D61" s="47"/>
+      <c r="E61" s="47"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B62" s="63" t="s">
-        <v>631</v>
-      </c>
-      <c r="C62" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="D62" s="63"/>
-      <c r="E62" s="63"/>
+      <c r="B62" s="47" t="s">
+        <v>678</v>
+      </c>
+      <c r="C62" s="47" t="s">
+        <v>677</v>
+      </c>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="63" t="s">
-        <v>692</v>
-      </c>
-      <c r="C63" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="D63" s="63"/>
-      <c r="E63" s="63"/>
+      <c r="B63" s="47" t="s">
+        <v>684</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B64" s="63" t="s">
-        <v>644</v>
-      </c>
-      <c r="C64" s="63" t="s">
-        <v>45</v>
-      </c>
-      <c r="D64" s="63"/>
-      <c r="E64" s="63"/>
+      <c r="B64" s="47" t="s">
+        <v>663</v>
+      </c>
+      <c r="C64" s="47" t="s">
+        <v>664</v>
+      </c>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B65" s="63" t="s">
-        <v>645</v>
-      </c>
-      <c r="C65" s="63" t="s">
-        <v>666</v>
-      </c>
-      <c r="D65" s="63"/>
-      <c r="E65" s="63"/>
+      <c r="B65" s="47" t="s">
+        <v>665</v>
+      </c>
+      <c r="C65" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B66" s="63" t="s">
-        <v>678</v>
-      </c>
-      <c r="C66" s="63" t="s">
-        <v>677</v>
-      </c>
-      <c r="D66" s="63"/>
-      <c r="E66" s="63"/>
+        <v>104</v>
+      </c>
+      <c r="B66" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="C66" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D66" s="48"/>
+      <c r="E66" s="47"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A67" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B67" s="63" t="s">
-        <v>684</v>
-      </c>
-      <c r="C67" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="D67" s="63"/>
-      <c r="E67" s="63"/>
+      <c r="A67" s="32"/>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A68" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B68" s="63" t="s">
-        <v>663</v>
-      </c>
-      <c r="C68" s="63" t="s">
-        <v>664</v>
-      </c>
-      <c r="D68" s="63"/>
-      <c r="E68" s="63"/>
+      <c r="A68" s="32"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A69" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B69" s="63" t="s">
-        <v>665</v>
-      </c>
-      <c r="C69" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="D69" s="63"/>
-      <c r="E69" s="63"/>
+      <c r="A69" s="32"/>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B70" s="62" t="s">
-        <v>281</v>
-      </c>
-      <c r="C70" s="63" t="s">
-        <v>74</v>
-      </c>
-      <c r="D70" s="64"/>
-      <c r="E70" s="63"/>
+      <c r="A70" s="32"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="32"/>
@@ -4813,7 +4823,7 @@
       <c r="A109" s="32"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A110" s="32"/>
+      <c r="A110" s="33"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="32"/>
@@ -4825,7 +4835,7 @@
       <c r="A113" s="32"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="33"/>
+      <c r="A114" s="32"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="32"/>
@@ -4839,23 +4849,11 @@
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="32"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A119" s="32"/>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A120" s="32"/>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A121" s="32"/>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A122" s="32"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A157" s="33"/>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A153" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A54:A108 A1:A52">
+  <conditionalFormatting sqref="A1:A51 A53:A104">
     <cfRule type="containsText" dxfId="109" priority="25" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4872,7 +4870,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A54:A219 A1:A52">
+  <conditionalFormatting sqref="A1:A51 A53:A215">
     <cfRule type="containsText" dxfId="104" priority="23" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4880,71 +4878,71 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A109:A110">
+  <conditionalFormatting sqref="A105:A106">
     <cfRule type="containsText" dxfId="102" priority="10" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A109)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A105)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="11" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A109)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A105)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="12" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A109)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A105)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="13" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A109)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A105)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="98" priority="14" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A109)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A105)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A222:A1048576">
+  <conditionalFormatting sqref="A218:A1048576">
     <cfRule type="containsText" dxfId="97" priority="8" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A222)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A218)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="96" priority="9" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A222)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A218)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A111:A219 A222:A1048576">
+  <conditionalFormatting sqref="A107:A215 A218:A1048576">
     <cfRule type="containsText" dxfId="95" priority="15" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A111)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="16" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A111)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="17" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A111)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="18" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A111)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A107)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="91" priority="19" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A111)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A107)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
+  <conditionalFormatting sqref="A52">
     <cfRule type="containsText" dxfId="90" priority="3" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A52)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="4" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A52)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="5" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A52)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="6" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A52)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="86" priority="7" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A52)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
+  <conditionalFormatting sqref="A52">
     <cfRule type="containsText" dxfId="85" priority="1" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A52)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="84" priority="2" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A52)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed some alignment issues of widgets in shading database input control. updated todo list.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adobos\Projects\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
   </bookViews>
@@ -20,12 +25,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="703">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2146,6 +2151,9 @@
   </si>
   <si>
     <t>0 is now none, 1 is non-linear, 2 is linear (new)</t>
+  </si>
+  <si>
+    <t>Paul/Aron</t>
   </si>
 </sst>
 </file>
@@ -3627,7 +3635,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3662,7 +3670,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3874,8 +3882,8 @@
   <dimension ref="A1:F156"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4255,7 +4263,7 @@
         <v>671</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>68</v>
+        <v>702</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
@@ -4418,7 +4426,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B41" s="63" t="s">
         <v>698</v>

</xml_diff>

<commit_message>
Updated TODO items based on 2/25/16 meeting
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adobos\Projects\SAMnt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,12 +25,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1991" uniqueCount="702">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="703">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -1991,9 +1991,6 @@
     <t>Check file upgrades from previous versions</t>
   </si>
   <si>
-    <t>Testing</t>
-  </si>
-  <si>
     <t>Linear shading option for PV self-shading model (and upgrade project files!)</t>
   </si>
   <si>
@@ -2151,12 +2148,18 @@
   </si>
   <si>
     <t>Paul/Aron</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>Rework Utility Rate pages and compute module per 2/25/16 meeting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3665,6 +3668,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3700,6 +3720,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3876,11 +3913,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F156"/>
+  <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A66" sqref="A66"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3919,7 +3956,7 @@
         <v>55</v>
       </c>
       <c r="B2" s="62" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="C2" s="63" t="s">
         <v>45</v>
@@ -3958,20 +3995,20 @@
         <v>55</v>
       </c>
       <c r="B5" s="63" t="s">
+        <v>678</v>
+      </c>
+      <c r="C5" s="63" t="s">
         <v>679</v>
-      </c>
-      <c r="C5" s="63" t="s">
-        <v>680</v>
       </c>
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
-        <v>648</v>
+        <v>55</v>
       </c>
       <c r="B6" s="63" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="C6" s="63" t="s">
         <v>47</v>
@@ -3984,7 +4021,7 @@
         <v>55</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="C7" s="63" t="s">
         <v>47</v>
@@ -4010,7 +4047,7 @@
         <v>55</v>
       </c>
       <c r="B9" s="63" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="C9" s="63" t="s">
         <v>46</v>
@@ -4049,7 +4086,7 @@
         <v>192</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="C12" s="63" t="s">
         <v>46</v>
@@ -4062,7 +4099,7 @@
         <v>55</v>
       </c>
       <c r="B13" s="63" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="C13" s="63" t="s">
         <v>45</v>
@@ -4127,7 +4164,7 @@
         <v>55</v>
       </c>
       <c r="B18" s="63" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="C18" s="63" t="s">
         <v>45</v>
@@ -4140,10 +4177,10 @@
         <v>55</v>
       </c>
       <c r="B19" s="63" t="s">
+        <v>684</v>
+      </c>
+      <c r="C19" s="63" t="s">
         <v>685</v>
-      </c>
-      <c r="C19" s="63" t="s">
-        <v>686</v>
       </c>
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
@@ -4153,7 +4190,7 @@
         <v>55</v>
       </c>
       <c r="B20" s="63" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="C20" s="63" t="s">
         <v>46</v>
@@ -4166,10 +4203,10 @@
         <v>55</v>
       </c>
       <c r="B21" s="63" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="C21" s="63" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
@@ -4179,20 +4216,20 @@
         <v>55</v>
       </c>
       <c r="B22" s="63" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="C22" s="63" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
-        <v>648</v>
+        <v>55</v>
       </c>
       <c r="B23" s="63" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="C23" s="63" t="s">
         <v>307</v>
@@ -4205,7 +4242,7 @@
         <v>55</v>
       </c>
       <c r="B24" s="63" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="C24" s="63" t="s">
         <v>45</v>
@@ -4218,7 +4255,7 @@
         <v>55</v>
       </c>
       <c r="B25" s="63" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="C25" s="63" t="s">
         <v>225</v>
@@ -4231,7 +4268,7 @@
         <v>55</v>
       </c>
       <c r="B26" s="63" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="C26" s="63" t="s">
         <v>46</v>
@@ -4244,23 +4281,23 @@
         <v>55</v>
       </c>
       <c r="B27" s="63" t="s">
+        <v>653</v>
+      </c>
+      <c r="C27" s="63" t="s">
         <v>654</v>
-      </c>
-      <c r="C27" s="63" t="s">
-        <v>655</v>
       </c>
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B28" s="63" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="C28" s="63" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
@@ -4270,7 +4307,7 @@
         <v>55</v>
       </c>
       <c r="B29" s="63" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="C29" s="63" t="s">
         <v>46</v>
@@ -4283,7 +4320,7 @@
         <v>55</v>
       </c>
       <c r="B30" s="63" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="C30" s="63" t="s">
         <v>70</v>
@@ -4296,7 +4333,7 @@
         <v>55</v>
       </c>
       <c r="B31" s="63" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C31" s="63" t="s">
         <v>302</v>
@@ -4309,7 +4346,7 @@
         <v>55</v>
       </c>
       <c r="B32" s="63" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="C32" s="63" t="s">
         <v>302</v>
@@ -4322,7 +4359,7 @@
         <v>55</v>
       </c>
       <c r="B33" s="63" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C33" s="63" t="s">
         <v>124</v>
@@ -4335,7 +4372,7 @@
         <v>55</v>
       </c>
       <c r="B34" s="63" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="C34" s="63" t="s">
         <v>124</v>
@@ -4348,7 +4385,7 @@
         <v>55</v>
       </c>
       <c r="B35" s="63" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="C35" s="63" t="s">
         <v>47</v>
@@ -4361,7 +4398,7 @@
         <v>55</v>
       </c>
       <c r="B36" s="63" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="C36" s="63" t="s">
         <v>46</v>
@@ -4374,7 +4411,7 @@
         <v>55</v>
       </c>
       <c r="B37" s="63" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="C37" s="63" t="s">
         <v>46</v>
@@ -4387,7 +4424,7 @@
         <v>55</v>
       </c>
       <c r="B38" s="63" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="C38" s="63" t="s">
         <v>46</v>
@@ -4400,7 +4437,7 @@
         <v>55</v>
       </c>
       <c r="B39" s="63" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="C39" s="63" t="s">
         <v>46</v>
@@ -4413,7 +4450,7 @@
         <v>55</v>
       </c>
       <c r="B40" s="63" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C40" s="63" t="s">
         <v>46</v>
@@ -4426,7 +4463,7 @@
         <v>55</v>
       </c>
       <c r="B41" s="63" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C41" s="63" t="s">
         <v>46</v>
@@ -4436,49 +4473,49 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" s="40" t="s">
-        <v>549</v>
-      </c>
-      <c r="C42" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="40"/>
-      <c r="E42" s="40"/>
+        <v>701</v>
+      </c>
+      <c r="B42" s="63" t="s">
+        <v>702</v>
+      </c>
+      <c r="C42" s="63" t="s">
+        <v>233</v>
+      </c>
+      <c r="D42" s="63"/>
+      <c r="E42" s="63"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B43" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D43" s="40"/>
       <c r="E43" s="40"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>647</v>
+        <v>550</v>
       </c>
       <c r="C44" s="40" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D44" s="40"/>
       <c r="E44" s="40"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B45" s="40" t="s">
-        <v>136</v>
+        <v>647</v>
       </c>
       <c r="C45" s="40" t="s">
         <v>45</v>
@@ -4491,10 +4528,10 @@
         <v>135</v>
       </c>
       <c r="B46" s="40" t="s">
-        <v>545</v>
+        <v>136</v>
       </c>
       <c r="C46" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D46" s="40"/>
       <c r="E46" s="40"/>
@@ -4504,10 +4541,10 @@
         <v>135</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C47" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D47" s="40"/>
       <c r="E47" s="40"/>
@@ -4517,36 +4554,36 @@
         <v>135</v>
       </c>
       <c r="B48" s="40" t="s">
-        <v>690</v>
+        <v>542</v>
       </c>
       <c r="C48" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D48" s="40"/>
       <c r="E48" s="40"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="B49" s="40" t="s">
-        <v>544</v>
+        <v>689</v>
       </c>
       <c r="C49" s="40" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D49" s="40"/>
       <c r="E49" s="40"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
-        <v>135</v>
+        <v>192</v>
       </c>
       <c r="B50" s="40" t="s">
-        <v>696</v>
+        <v>544</v>
       </c>
       <c r="C50" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D50" s="40"/>
       <c r="E50" s="40"/>
@@ -4556,10 +4593,10 @@
         <v>135</v>
       </c>
       <c r="B51" s="40" t="s">
-        <v>643</v>
+        <v>695</v>
       </c>
       <c r="C51" s="40" t="s">
-        <v>694</v>
+        <v>45</v>
       </c>
       <c r="D51" s="40"/>
       <c r="E51" s="40"/>
@@ -4569,10 +4606,10 @@
         <v>135</v>
       </c>
       <c r="B52" s="40" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="C52" s="40" t="s">
-        <v>46</v>
+        <v>693</v>
       </c>
       <c r="D52" s="40"/>
       <c r="E52" s="40"/>
@@ -4582,57 +4619,59 @@
         <v>135</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>669</v>
+        <v>640</v>
       </c>
       <c r="C53" s="40" t="s">
-        <v>307</v>
+        <v>46</v>
       </c>
       <c r="D53" s="40"/>
       <c r="E53" s="40"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="47" t="s">
-        <v>633</v>
-      </c>
-      <c r="C54" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D54" s="47"/>
-      <c r="E54" s="47"/>
+        <v>135</v>
+      </c>
+      <c r="B54" s="40" t="s">
+        <v>668</v>
+      </c>
+      <c r="C54" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B55" s="47" t="s">
-        <v>672</v>
-      </c>
-      <c r="C55" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="D55" s="63"/>
-      <c r="E55" s="63"/>
+        <v>633</v>
+      </c>
+      <c r="C55" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D55" s="47"/>
+      <c r="E55" s="47"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B56" s="47" t="s">
-        <v>637</v>
-      </c>
-      <c r="C56" s="47"/>
-      <c r="D56" s="47"/>
-      <c r="E56" s="47"/>
+        <v>671</v>
+      </c>
+      <c r="C56" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D56" s="63"/>
+      <c r="E56" s="63"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B57" s="47" t="s">
-        <v>691</v>
+        <v>637</v>
       </c>
       <c r="C57" s="47"/>
       <c r="D57" s="47"/>
@@ -4643,7 +4682,7 @@
         <v>108</v>
       </c>
       <c r="B58" s="47" t="s">
-        <v>668</v>
+        <v>690</v>
       </c>
       <c r="C58" s="47"/>
       <c r="D58" s="47"/>
@@ -4654,11 +4693,9 @@
         <v>108</v>
       </c>
       <c r="B59" s="47" t="s">
-        <v>628</v>
-      </c>
-      <c r="C59" s="47" t="s">
-        <v>65</v>
-      </c>
+        <v>667</v>
+      </c>
+      <c r="C59" s="47"/>
       <c r="D59" s="47"/>
       <c r="E59" s="47"/>
     </row>
@@ -4667,10 +4704,10 @@
         <v>108</v>
       </c>
       <c r="B60" s="47" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C60" s="47" t="s">
-        <v>237</v>
+        <v>65</v>
       </c>
       <c r="D60" s="47"/>
       <c r="E60" s="47"/>
@@ -4680,10 +4717,10 @@
         <v>108</v>
       </c>
       <c r="B61" s="47" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C61" s="47" t="s">
-        <v>46</v>
+        <v>237</v>
       </c>
       <c r="D61" s="47"/>
       <c r="E61" s="47"/>
@@ -4693,10 +4730,10 @@
         <v>108</v>
       </c>
       <c r="B62" s="47" t="s">
-        <v>688</v>
+        <v>631</v>
       </c>
       <c r="C62" s="47" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D62" s="47"/>
       <c r="E62" s="47"/>
@@ -4706,7 +4743,7 @@
         <v>108</v>
       </c>
       <c r="B63" s="47" t="s">
-        <v>644</v>
+        <v>687</v>
       </c>
       <c r="C63" s="47" t="s">
         <v>45</v>
@@ -4719,10 +4756,10 @@
         <v>108</v>
       </c>
       <c r="B64" s="47" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C64" s="47" t="s">
-        <v>666</v>
+        <v>45</v>
       </c>
       <c r="D64" s="47"/>
       <c r="E64" s="47"/>
@@ -4732,10 +4769,10 @@
         <v>108</v>
       </c>
       <c r="B65" s="47" t="s">
-        <v>675</v>
+        <v>645</v>
       </c>
       <c r="C65" s="47" t="s">
-        <v>674</v>
+        <v>665</v>
       </c>
       <c r="D65" s="47"/>
       <c r="E65" s="47"/>
@@ -4745,10 +4782,10 @@
         <v>108</v>
       </c>
       <c r="B66" s="47" t="s">
-        <v>681</v>
+        <v>674</v>
       </c>
       <c r="C66" s="47" t="s">
-        <v>46</v>
+        <v>673</v>
       </c>
       <c r="D66" s="47"/>
       <c r="E66" s="47"/>
@@ -4758,10 +4795,10 @@
         <v>108</v>
       </c>
       <c r="B67" s="47" t="s">
-        <v>663</v>
+        <v>680</v>
       </c>
       <c r="C67" s="47" t="s">
-        <v>664</v>
+        <v>46</v>
       </c>
       <c r="D67" s="47"/>
       <c r="E67" s="47"/>
@@ -4771,29 +4808,39 @@
         <v>108</v>
       </c>
       <c r="B68" s="47" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="C68" s="47" t="s">
-        <v>46</v>
+        <v>663</v>
       </c>
       <c r="D68" s="47"/>
       <c r="E68" s="47"/>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="B69" s="47" t="s">
+        <v>664</v>
+      </c>
+      <c r="C69" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="32" t="s">
         <v>104</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="B70" s="46" t="s">
         <v>281</v>
       </c>
-      <c r="C69" s="47" t="s">
+      <c r="C70" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="D69" s="48"/>
-      <c r="E69" s="47"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A70" s="32"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="47"/>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="32"/>
@@ -4922,10 +4969,10 @@
       <c r="A112" s="32"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="33"/>
+      <c r="A113" s="32"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A114" s="32"/>
+      <c r="A114" s="33"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="32"/>
@@ -4948,11 +4995,14 @@
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="32"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A156" s="33"/>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A122" s="32"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A157" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A52 A54:A107">
+  <conditionalFormatting sqref="A1:A53 A55:A108">
     <cfRule type="containsText" dxfId="110" priority="26" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -4969,7 +5019,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A52 A54:A218">
+  <conditionalFormatting sqref="A1:A53 A55:A219">
     <cfRule type="containsText" dxfId="105" priority="24" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -4977,71 +5027,71 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A108:A109">
+  <conditionalFormatting sqref="A109:A110">
     <cfRule type="containsText" dxfId="103" priority="11" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="13" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="14" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A109)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="15" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A108)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A109)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A221:A1048576">
+  <conditionalFormatting sqref="A222:A1048576">
     <cfRule type="containsText" dxfId="98" priority="9" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A222)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="97" priority="10" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A221)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A222)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A110:A218 A221:A1048576">
+  <conditionalFormatting sqref="A111:A219 A222:A1048576">
     <cfRule type="containsText" dxfId="96" priority="16" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="95" priority="17" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="18" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="19" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A111)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="20" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A110)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A111)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
+  <conditionalFormatting sqref="A54">
     <cfRule type="containsText" dxfId="91" priority="4" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="90" priority="5" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="6" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="7" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="8" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A53">
+  <conditionalFormatting sqref="A54">
     <cfRule type="containsText" dxfId="86" priority="2" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A54)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="85" priority="3" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A53)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A54)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7246,19 +7296,19 @@
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="25" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B92" s="19" t="s">
         <v>252</v>
       </c>
       <c r="C92" s="19" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>476</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G92" s="56" t="s">
         <v>617</v>

</xml_diff>

<commit_message>
revised treatment of start offset hours for plotting time series data - depends on value read in from simulation models
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adobos\Projects\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
   </bookViews>
@@ -20,12 +25,12 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="713">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="714">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2179,6 +2184,9 @@
   </si>
   <si>
     <t>Rework reports for res/com models to match new utility rates inputs and results</t>
+  </si>
+  <si>
+    <t>Update sscapi.py script in SDK to include data_set_table() functions</t>
   </si>
 </sst>
 </file>
@@ -3660,7 +3668,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3695,7 +3703,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3904,11 +3912,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F166"/>
+  <dimension ref="A1:F167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A44" sqref="A44"/>
+      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3922,7 +3930,7 @@
     <col min="7" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>54</v>
       </c>
@@ -3942,7 +3950,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>55</v>
       </c>
@@ -3955,7 +3963,7 @@
       <c r="D2" s="64"/>
       <c r="E2" s="63"/>
     </row>
-    <row r="3" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>55</v>
       </c>
@@ -3968,7 +3976,7 @@
       <c r="D3" s="63"/>
       <c r="E3" s="63"/>
     </row>
-    <row r="4" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>55</v>
       </c>
@@ -3981,7 +3989,7 @@
       <c r="D4" s="63"/>
       <c r="E4" s="63"/>
     </row>
-    <row r="5" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>55</v>
       </c>
@@ -3994,7 +4002,7 @@
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
     </row>
-    <row r="6" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>55</v>
       </c>
@@ -4007,7 +4015,7 @@
       <c r="D6" s="63"/>
       <c r="E6" s="63"/>
     </row>
-    <row r="7" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>55</v>
       </c>
@@ -4020,7 +4028,7 @@
       <c r="D7" s="63"/>
       <c r="E7" s="63"/>
     </row>
-    <row r="8" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>55</v>
       </c>
@@ -4033,7 +4041,7 @@
       <c r="D8" s="63"/>
       <c r="E8" s="63"/>
     </row>
-    <row r="9" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>55</v>
       </c>
@@ -4046,7 +4054,7 @@
       <c r="D9" s="63"/>
       <c r="E9" s="63"/>
     </row>
-    <row r="10" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>55</v>
       </c>
@@ -4059,7 +4067,7 @@
       <c r="D10" s="63"/>
       <c r="E10" s="63"/>
     </row>
-    <row r="11" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>55</v>
       </c>
@@ -4072,7 +4080,7 @@
       <c r="D11" s="63"/>
       <c r="E11" s="63"/>
     </row>
-    <row r="12" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>55</v>
       </c>
@@ -4085,7 +4093,7 @@
       <c r="D12" s="63"/>
       <c r="E12" s="63"/>
     </row>
-    <row r="13" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>55</v>
       </c>
@@ -4098,7 +4106,7 @@
       <c r="D13" s="63"/>
       <c r="E13" s="63"/>
     </row>
-    <row r="14" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>55</v>
       </c>
@@ -4111,7 +4119,7 @@
       <c r="D14" s="63"/>
       <c r="E14" s="63"/>
     </row>
-    <row r="15" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>55</v>
       </c>
@@ -4124,7 +4132,7 @@
       <c r="D15" s="63"/>
       <c r="E15" s="63"/>
     </row>
-    <row r="16" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>192</v>
       </c>
@@ -4137,7 +4145,7 @@
       <c r="D16" s="63"/>
       <c r="E16" s="63"/>
     </row>
-    <row r="17" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>55</v>
       </c>
@@ -4150,7 +4158,7 @@
       <c r="D17" s="63"/>
       <c r="E17" s="63"/>
     </row>
-    <row r="18" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>55</v>
       </c>
@@ -4163,7 +4171,7 @@
       <c r="D18" s="63"/>
       <c r="E18" s="63"/>
     </row>
-    <row r="19" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>55</v>
       </c>
@@ -4176,7 +4184,7 @@
       <c r="D19" s="63"/>
       <c r="E19" s="63"/>
     </row>
-    <row r="20" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>55</v>
       </c>
@@ -4189,7 +4197,7 @@
       <c r="D20" s="63"/>
       <c r="E20" s="63"/>
     </row>
-    <row r="21" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>55</v>
       </c>
@@ -4202,7 +4210,7 @@
       <c r="D21" s="63"/>
       <c r="E21" s="63"/>
     </row>
-    <row r="22" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>55</v>
       </c>
@@ -4215,7 +4223,7 @@
       <c r="D22" s="63"/>
       <c r="E22" s="63"/>
     </row>
-    <row r="23" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>55</v>
       </c>
@@ -4228,7 +4236,7 @@
       <c r="D23" s="63"/>
       <c r="E23" s="63"/>
     </row>
-    <row r="24" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>55</v>
       </c>
@@ -4241,7 +4249,7 @@
       <c r="D24" s="63"/>
       <c r="E24" s="63"/>
     </row>
-    <row r="25" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>55</v>
       </c>
@@ -4254,7 +4262,7 @@
       <c r="D25" s="63"/>
       <c r="E25" s="63"/>
     </row>
-    <row r="26" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>55</v>
       </c>
@@ -4267,7 +4275,7 @@
       <c r="D26" s="63"/>
       <c r="E26" s="63"/>
     </row>
-    <row r="27" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>55</v>
       </c>
@@ -4280,7 +4288,7 @@
       <c r="D27" s="63"/>
       <c r="E27" s="63"/>
     </row>
-    <row r="28" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>55</v>
       </c>
@@ -4293,7 +4301,7 @@
       <c r="D28" s="63"/>
       <c r="E28" s="63"/>
     </row>
-    <row r="29" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>55</v>
       </c>
@@ -4306,7 +4314,7 @@
       <c r="D29" s="63"/>
       <c r="E29" s="63"/>
     </row>
-    <row r="30" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>55</v>
       </c>
@@ -4319,7 +4327,7 @@
       <c r="D30" s="63"/>
       <c r="E30" s="63"/>
     </row>
-    <row r="31" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>55</v>
       </c>
@@ -4332,7 +4340,7 @@
       <c r="D31" s="63"/>
       <c r="E31" s="63"/>
     </row>
-    <row r="32" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>55</v>
       </c>
@@ -4345,7 +4353,7 @@
       <c r="D32" s="63"/>
       <c r="E32" s="63"/>
     </row>
-    <row r="33" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>55</v>
       </c>
@@ -4358,7 +4366,7 @@
       <c r="D33" s="63"/>
       <c r="E33" s="63"/>
     </row>
-    <row r="34" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>55</v>
       </c>
@@ -4371,7 +4379,7 @@
       <c r="D34" s="63"/>
       <c r="E34" s="63"/>
     </row>
-    <row r="35" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>55</v>
       </c>
@@ -4384,7 +4392,7 @@
       <c r="D35" s="63"/>
       <c r="E35" s="63"/>
     </row>
-    <row r="36" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>55</v>
       </c>
@@ -4397,7 +4405,7 @@
       <c r="D36" s="63"/>
       <c r="E36" s="63"/>
     </row>
-    <row r="37" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>55</v>
       </c>
@@ -4410,7 +4418,7 @@
       <c r="D37" s="63"/>
       <c r="E37" s="63"/>
     </row>
-    <row r="38" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
         <v>55</v>
       </c>
@@ -4423,7 +4431,7 @@
       <c r="D38" s="63"/>
       <c r="E38" s="63"/>
     </row>
-    <row r="39" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>55</v>
       </c>
@@ -4436,7 +4444,7 @@
       <c r="D39" s="63"/>
       <c r="E39" s="63"/>
     </row>
-    <row r="40" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
         <v>55</v>
       </c>
@@ -4449,7 +4457,7 @@
       <c r="D40" s="63"/>
       <c r="E40" s="63"/>
     </row>
-    <row r="41" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>55</v>
       </c>
@@ -4462,7 +4470,7 @@
       <c r="D41" s="63"/>
       <c r="E41" s="63"/>
     </row>
-    <row r="42" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
         <v>192</v>
       </c>
@@ -4475,7 +4483,7 @@
       <c r="D42" s="63"/>
       <c r="E42" s="63"/>
     </row>
-    <row r="43" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>192</v>
       </c>
@@ -4488,7 +4496,7 @@
       <c r="D43" s="63"/>
       <c r="E43" s="63"/>
     </row>
-    <row r="44" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
         <v>192</v>
       </c>
@@ -4501,7 +4509,7 @@
       <c r="D44" s="63"/>
       <c r="E44" s="63"/>
     </row>
-    <row r="45" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
         <v>192</v>
       </c>
@@ -4514,7 +4522,7 @@
       <c r="D45" s="63"/>
       <c r="E45" s="63"/>
     </row>
-    <row r="46" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
         <v>192</v>
       </c>
@@ -4527,7 +4535,7 @@
       <c r="D46" s="63"/>
       <c r="E46" s="63"/>
     </row>
-    <row r="47" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
         <v>192</v>
       </c>
@@ -4540,7 +4548,7 @@
       <c r="D47" s="63"/>
       <c r="E47" s="63"/>
     </row>
-    <row r="48" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
         <v>192</v>
       </c>
@@ -4553,7 +4561,7 @@
       <c r="D48" s="63"/>
       <c r="E48" s="63"/>
     </row>
-    <row r="49" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
         <v>55</v>
       </c>
@@ -4566,7 +4574,7 @@
       <c r="D49" s="63"/>
       <c r="E49" s="63"/>
     </row>
-    <row r="50" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
         <v>192</v>
       </c>
@@ -4579,7 +4587,7 @@
       <c r="D50" s="63"/>
       <c r="E50" s="63"/>
     </row>
-    <row r="51" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
         <v>192</v>
       </c>
@@ -4592,51 +4600,51 @@
       <c r="D51" s="63"/>
       <c r="E51" s="63"/>
     </row>
-    <row r="52" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
-        <v>135</v>
-      </c>
-      <c r="B52" s="40" t="s">
-        <v>549</v>
-      </c>
-      <c r="C52" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="D52" s="40"/>
-      <c r="E52" s="40"/>
-    </row>
-    <row r="53" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+      <c r="B52" s="63" t="s">
+        <v>713</v>
+      </c>
+      <c r="C52" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D52" s="63"/>
+      <c r="E52" s="63"/>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B53" s="40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C53" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D53" s="40"/>
       <c r="E53" s="40"/>
     </row>
-    <row r="54" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
-        <v>55</v>
+        <v>135</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>647</v>
+        <v>550</v>
       </c>
       <c r="C54" s="40" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D54" s="40"/>
       <c r="E54" s="40"/>
     </row>
-    <row r="55" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B55" s="40" t="s">
-        <v>136</v>
+        <v>647</v>
       </c>
       <c r="C55" s="40" t="s">
         <v>45</v>
@@ -4644,80 +4652,80 @@
       <c r="D55" s="40"/>
       <c r="E55" s="40"/>
     </row>
-    <row r="56" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B56" s="40" t="s">
-        <v>545</v>
+        <v>136</v>
       </c>
       <c r="C56" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D56" s="40"/>
       <c r="E56" s="40"/>
     </row>
-    <row r="57" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B57" s="40" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="C57" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D57" s="40"/>
       <c r="E57" s="40"/>
     </row>
-    <row r="58" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="32" t="s">
         <v>135</v>
       </c>
       <c r="B58" s="40" t="s">
-        <v>689</v>
+        <v>542</v>
       </c>
       <c r="C58" s="40" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D58" s="40"/>
       <c r="E58" s="40"/>
     </row>
-    <row r="59" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="32" t="s">
-        <v>192</v>
+        <v>135</v>
       </c>
       <c r="B59" s="40" t="s">
-        <v>544</v>
+        <v>689</v>
       </c>
       <c r="C59" s="40" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D59" s="40"/>
       <c r="E59" s="40"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="32" t="s">
-        <v>55</v>
+        <v>192</v>
       </c>
       <c r="B60" s="40" t="s">
-        <v>695</v>
+        <v>544</v>
       </c>
       <c r="C60" s="40" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D60" s="40"/>
       <c r="E60" s="40"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="32" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B61" s="40" t="s">
-        <v>643</v>
+        <v>695</v>
       </c>
       <c r="C61" s="40" t="s">
-        <v>693</v>
+        <v>45</v>
       </c>
       <c r="D61" s="40"/>
       <c r="E61" s="40"/>
@@ -4727,10 +4735,10 @@
         <v>135</v>
       </c>
       <c r="B62" s="40" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="C62" s="40" t="s">
-        <v>46</v>
+        <v>693</v>
       </c>
       <c r="D62" s="40"/>
       <c r="E62" s="40"/>
@@ -4740,57 +4748,59 @@
         <v>135</v>
       </c>
       <c r="B63" s="40" t="s">
-        <v>668</v>
+        <v>640</v>
       </c>
       <c r="C63" s="40" t="s">
-        <v>307</v>
+        <v>46</v>
       </c>
       <c r="D63" s="40"/>
       <c r="E63" s="40"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="B64" s="47" t="s">
-        <v>633</v>
-      </c>
-      <c r="C64" s="47" t="s">
-        <v>45</v>
-      </c>
-      <c r="D64" s="47"/>
-      <c r="E64" s="47"/>
+        <v>135</v>
+      </c>
+      <c r="B64" s="40" t="s">
+        <v>668</v>
+      </c>
+      <c r="C64" s="40" t="s">
+        <v>307</v>
+      </c>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B65" s="47" t="s">
-        <v>671</v>
-      </c>
-      <c r="C65" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="D65" s="63"/>
-      <c r="E65" s="63"/>
+        <v>633</v>
+      </c>
+      <c r="C65" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B66" s="47" t="s">
-        <v>637</v>
-      </c>
-      <c r="C66" s="47"/>
-      <c r="D66" s="47"/>
-      <c r="E66" s="47"/>
+        <v>671</v>
+      </c>
+      <c r="C66" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="D66" s="63"/>
+      <c r="E66" s="63"/>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="32" t="s">
         <v>108</v>
       </c>
       <c r="B67" s="47" t="s">
-        <v>690</v>
+        <v>637</v>
       </c>
       <c r="C67" s="47"/>
       <c r="D67" s="47"/>
@@ -4801,7 +4811,7 @@
         <v>108</v>
       </c>
       <c r="B68" s="47" t="s">
-        <v>667</v>
+        <v>690</v>
       </c>
       <c r="C68" s="47"/>
       <c r="D68" s="47"/>
@@ -4812,11 +4822,9 @@
         <v>108</v>
       </c>
       <c r="B69" s="47" t="s">
-        <v>628</v>
-      </c>
-      <c r="C69" s="47" t="s">
-        <v>65</v>
-      </c>
+        <v>667</v>
+      </c>
+      <c r="C69" s="47"/>
       <c r="D69" s="47"/>
       <c r="E69" s="47"/>
     </row>
@@ -4825,10 +4833,10 @@
         <v>108</v>
       </c>
       <c r="B70" s="47" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C70" s="47" t="s">
-        <v>237</v>
+        <v>65</v>
       </c>
       <c r="D70" s="47"/>
       <c r="E70" s="47"/>
@@ -4838,10 +4846,10 @@
         <v>108</v>
       </c>
       <c r="B71" s="47" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="C71" s="47" t="s">
-        <v>46</v>
+        <v>237</v>
       </c>
       <c r="D71" s="47"/>
       <c r="E71" s="47"/>
@@ -4851,10 +4859,10 @@
         <v>108</v>
       </c>
       <c r="B72" s="47" t="s">
-        <v>687</v>
+        <v>631</v>
       </c>
       <c r="C72" s="47" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D72" s="47"/>
       <c r="E72" s="47"/>
@@ -4864,7 +4872,7 @@
         <v>108</v>
       </c>
       <c r="B73" s="47" t="s">
-        <v>644</v>
+        <v>687</v>
       </c>
       <c r="C73" s="47" t="s">
         <v>45</v>
@@ -4877,10 +4885,10 @@
         <v>108</v>
       </c>
       <c r="B74" s="47" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="C74" s="47" t="s">
-        <v>665</v>
+        <v>45</v>
       </c>
       <c r="D74" s="47"/>
       <c r="E74" s="47"/>
@@ -4890,10 +4898,10 @@
         <v>108</v>
       </c>
       <c r="B75" s="47" t="s">
-        <v>674</v>
+        <v>645</v>
       </c>
       <c r="C75" s="47" t="s">
-        <v>673</v>
+        <v>665</v>
       </c>
       <c r="D75" s="47"/>
       <c r="E75" s="47"/>
@@ -4903,10 +4911,10 @@
         <v>108</v>
       </c>
       <c r="B76" s="47" t="s">
-        <v>680</v>
+        <v>674</v>
       </c>
       <c r="C76" s="47" t="s">
-        <v>46</v>
+        <v>673</v>
       </c>
       <c r="D76" s="47"/>
       <c r="E76" s="47"/>
@@ -4916,10 +4924,10 @@
         <v>108</v>
       </c>
       <c r="B77" s="47" t="s">
-        <v>662</v>
+        <v>680</v>
       </c>
       <c r="C77" s="47" t="s">
-        <v>663</v>
+        <v>46</v>
       </c>
       <c r="D77" s="47"/>
       <c r="E77" s="47"/>
@@ -4929,81 +4937,91 @@
         <v>108</v>
       </c>
       <c r="B78" s="47" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="C78" s="47" t="s">
-        <v>46</v>
+        <v>663</v>
       </c>
       <c r="D78" s="47"/>
       <c r="E78" s="47"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="B79" s="46" t="s">
-        <v>281</v>
+        <v>108</v>
+      </c>
+      <c r="B79" s="47" t="s">
+        <v>664</v>
       </c>
       <c r="C79" s="47" t="s">
-        <v>74</v>
-      </c>
-      <c r="D79" s="48"/>
+        <v>46</v>
+      </c>
+      <c r="D79" s="47"/>
       <c r="E79" s="47"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="B80" s="46" t="s">
+        <v>281</v>
+      </c>
+      <c r="C80" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D80" s="48"/>
+      <c r="E80" s="47"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="32" t="s">
         <v>108</v>
       </c>
-      <c r="B80" s="31" t="s">
+      <c r="B81" s="31" t="s">
         <v>702</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="32"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="32"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="32"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="32"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="32"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="32"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="32"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="32"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="32"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="32"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="32"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="32"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="32"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="32"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="32"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="32"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
@@ -5085,10 +5103,10 @@
       <c r="A122" s="32"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A123" s="33"/>
+      <c r="A123" s="32"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A124" s="32"/>
+      <c r="A124" s="33"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="32"/>
@@ -5108,14 +5126,17 @@
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="32"/>
     </row>
-    <row r="131" spans="1:1" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="32"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A166" s="33"/>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A132" s="32"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A167" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A62 A64:A117">
+  <conditionalFormatting sqref="A1:A63 A65:A118">
     <cfRule type="containsText" dxfId="110" priority="26" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
@@ -5132,7 +5153,7 @@
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A62 A64:A228">
+  <conditionalFormatting sqref="A1:A63 A65:A229">
     <cfRule type="containsText" dxfId="105" priority="24" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
@@ -5140,71 +5161,71 @@
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A118:A119">
+  <conditionalFormatting sqref="A119:A120">
     <cfRule type="containsText" dxfId="103" priority="11" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A118)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A119)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="102" priority="12" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A118)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A119)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="101" priority="13" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A118)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A119)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="100" priority="14" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A118)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A119)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="99" priority="15" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A118)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A119)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A231:A1048576">
+  <conditionalFormatting sqref="A232:A1048576">
     <cfRule type="containsText" dxfId="98" priority="9" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A231)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A232)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="97" priority="10" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A231)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A232)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A120:A228 A231:A1048576">
+  <conditionalFormatting sqref="A121:A229 A232:A1048576">
     <cfRule type="containsText" dxfId="96" priority="16" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A120)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A121)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="95" priority="17" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A120)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A121)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="94" priority="18" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A120)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A121)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="93" priority="19" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A120)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A121)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="92" priority="20" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A120)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A121)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
+  <conditionalFormatting sqref="A64">
     <cfRule type="containsText" dxfId="91" priority="4" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("NGTD",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="90" priority="5" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Test",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="89" priority="6" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Future",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="88" priority="7" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Not done",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="87" priority="8" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Done",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A63">
+  <conditionalFormatting sqref="A64">
     <cfRule type="containsText" dxfId="86" priority="2" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("POUT",A64)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="85" priority="3" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("Pre-release",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5253,7 +5274,7 @@
     <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="24" customFormat="1" ht="28.9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="24" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="52" t="s">
         <v>201</v>
       </c>
@@ -5279,7 +5300,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="26" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="26" t="s">
         <v>205</v>
       </c>
@@ -5300,7 +5321,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="3" spans="1:22" s="26" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="26" t="s">
         <v>206</v>
       </c>
@@ -5321,7 +5342,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="26" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="26" t="s">
         <v>207</v>
       </c>
@@ -5336,7 +5357,7 @@
       </c>
       <c r="G4" s="54"/>
     </row>
-    <row r="5" spans="1:22" s="49" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
         <v>205</v>
       </c>
@@ -5357,7 +5378,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="49" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="49" t="s">
         <v>205</v>
       </c>
@@ -5378,7 +5399,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="7" spans="1:22" s="49" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
         <v>207</v>
       </c>
@@ -5393,7 +5414,7 @@
       </c>
       <c r="G7" s="55"/>
     </row>
-    <row r="8" spans="1:22" s="49" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
         <v>207</v>
       </c>
@@ -5408,7 +5429,7 @@
       </c>
       <c r="G8" s="55"/>
     </row>
-    <row r="9" spans="1:22" s="49" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" s="49" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="49" t="s">
         <v>206</v>
       </c>
@@ -5465,7 +5486,7 @@
       </c>
       <c r="G11" s="55"/>
     </row>
-    <row r="12" spans="1:22" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>206</v>
       </c>
@@ -5491,7 +5512,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="13" spans="1:22" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>206</v>
       </c>
@@ -5517,7 +5538,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="14" spans="1:22" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>206</v>
       </c>
@@ -5543,7 +5564,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="15" spans="1:22" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>206</v>
       </c>
@@ -5569,7 +5590,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="16" spans="1:22" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>206</v>
       </c>
@@ -5595,7 +5616,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="17" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>206</v>
       </c>
@@ -5621,7 +5642,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>206</v>
       </c>
@@ -5647,7 +5668,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>206</v>
       </c>
@@ -5673,7 +5694,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="20" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="19" t="s">
         <v>206</v>
       </c>
@@ -5699,7 +5720,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="21" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
         <v>206</v>
       </c>
@@ -5725,7 +5746,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="22" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
         <v>206</v>
       </c>
@@ -5751,7 +5772,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="19" t="s">
         <v>206</v>
       </c>
@@ -5777,7 +5798,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="24" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>206</v>
       </c>
@@ -5803,7 +5824,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="25" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
         <v>206</v>
       </c>
@@ -5829,7 +5850,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="26" spans="1:8" s="19" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
         <v>206</v>
       </c>
@@ -7459,7 +7480,7 @@
     <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>54</v>
       </c>
@@ -7479,7 +7500,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>172</v>
       </c>
@@ -7495,7 +7516,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>172</v>
       </c>
@@ -7509,7 +7530,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>108</v>
       </c>
@@ -7523,7 +7544,7 @@
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
     </row>
-    <row r="5" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>172</v>
       </c>
@@ -7536,7 +7557,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>108</v>
       </c>
@@ -7549,7 +7570,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>108</v>
       </c>
@@ -7562,7 +7583,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>108</v>
       </c>
@@ -7575,7 +7596,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>108</v>
       </c>
@@ -7590,7 +7611,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>108</v>
       </c>
@@ -7601,7 +7622,7 @@
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>108</v>
       </c>
@@ -7612,7 +7633,7 @@
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>108</v>
       </c>
@@ -7623,7 +7644,7 @@
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
     </row>
-    <row r="13" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>108</v>
       </c>
@@ -7634,7 +7655,7 @@
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>108</v>
       </c>
@@ -7645,7 +7666,7 @@
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>108</v>
       </c>
@@ -7656,7 +7677,7 @@
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>108</v>
       </c>
@@ -7667,7 +7688,7 @@
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
     </row>
-    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>108</v>
       </c>
@@ -7678,7 +7699,7 @@
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
     </row>
-    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>108</v>
       </c>
@@ -7689,7 +7710,7 @@
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
     </row>
-    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>108</v>
       </c>
@@ -7704,7 +7725,7 @@
       </c>
       <c r="E19" s="19"/>
     </row>
-    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>108</v>
       </c>
@@ -7715,7 +7736,7 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>108</v>
       </c>
@@ -7726,7 +7747,7 @@
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
     </row>
-    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>108</v>
       </c>
@@ -7737,7 +7758,7 @@
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
     </row>
-    <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>108</v>
       </c>
@@ -7748,7 +7769,7 @@
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
     </row>
-    <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>108</v>
       </c>
@@ -7762,7 +7783,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>108</v>
       </c>
@@ -8040,92 +8061,92 @@
     <col min="1" max="1" width="113.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="13" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="14" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="15" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="16" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>215</v>
       </c>
@@ -8133,67 +8154,67 @@
         <v>263</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="33" spans="1:1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>287</v>
       </c>
@@ -8253,7 +8274,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>308</v>
       </c>
@@ -8283,7 +8304,7 @@
     <col min="7" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>54</v>
       </c>
@@ -8303,7 +8324,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>192</v>
       </c>
@@ -8318,7 +8339,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>55</v>
       </c>
@@ -8333,7 +8354,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>55</v>
       </c>
@@ -8348,7 +8369,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>55</v>
       </c>
@@ -8363,7 +8384,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>55</v>
       </c>
@@ -8378,7 +8399,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="51" t="s">
         <v>55</v>
       </c>
@@ -8393,7 +8414,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>55</v>
       </c>
@@ -8408,7 +8429,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>55</v>
       </c>
@@ -8423,7 +8444,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>55</v>
       </c>
@@ -8438,7 +8459,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>55</v>
       </c>
@@ -8453,7 +8474,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>55</v>
       </c>
@@ -8468,7 +8489,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>55</v>
       </c>
@@ -8483,7 +8504,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>55</v>
       </c>
@@ -8498,7 +8519,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>55</v>
       </c>
@@ -8513,7 +8534,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>55</v>
       </c>
@@ -8528,7 +8549,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>55</v>
       </c>
@@ -8541,7 +8562,7 @@
       <c r="D17" s="47"/>
       <c r="E17" s="47"/>
     </row>
-    <row r="18" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>55</v>
       </c>
@@ -8556,7 +8577,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="26.45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>104</v>
       </c>
@@ -8571,7 +8592,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>104</v>
       </c>
@@ -8589,7 +8610,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>55</v>
       </c>
@@ -8604,7 +8625,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>55</v>
       </c>
@@ -8619,7 +8640,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>55</v>
       </c>
@@ -8634,7 +8655,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>55</v>
       </c>
@@ -8649,7 +8670,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>55</v>
       </c>
@@ -8664,7 +8685,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>55</v>
       </c>
@@ -8679,7 +8700,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>108</v>
       </c>
@@ -8694,7 +8715,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>55</v>
       </c>
@@ -8712,7 +8733,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>55</v>
       </c>
@@ -8727,7 +8748,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>55</v>
       </c>
@@ -8742,7 +8763,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>55</v>
       </c>
@@ -8757,7 +8778,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>55</v>
       </c>
@@ -8770,7 +8791,7 @@
       <c r="D32" s="42"/>
       <c r="E32" s="42"/>
     </row>
-    <row r="33" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>55</v>
       </c>
@@ -8783,7 +8804,7 @@
       <c r="D33" s="42"/>
       <c r="E33" s="42"/>
     </row>
-    <row r="34" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>135</v>
       </c>
@@ -8794,7 +8815,7 @@
       <c r="D34" s="42"/>
       <c r="E34" s="42"/>
     </row>
-    <row r="35" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>135</v>
       </c>
@@ -8807,7 +8828,7 @@
       <c r="D35" s="42"/>
       <c r="E35" s="42"/>
     </row>
-    <row r="36" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="32" t="s">
         <v>135</v>
       </c>
@@ -8820,7 +8841,7 @@
       <c r="D36" s="42"/>
       <c r="E36" s="42"/>
     </row>
-    <row r="37" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="32" t="s">
         <v>135</v>
       </c>
@@ -8831,7 +8852,7 @@
       <c r="D37" s="42"/>
       <c r="E37" s="42"/>
     </row>
-    <row r="38" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="32" t="s">
         <v>135</v>
       </c>
@@ -8844,7 +8865,7 @@
       <c r="D38" s="42"/>
       <c r="E38" s="42"/>
     </row>
-    <row r="39" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="32" t="s">
         <v>135</v>
       </c>
@@ -8857,7 +8878,7 @@
       <c r="D39" s="42"/>
       <c r="E39" s="42"/>
     </row>
-    <row r="40" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="32" t="s">
         <v>135</v>
       </c>
@@ -8870,7 +8891,7 @@
       <c r="D40" s="42"/>
       <c r="E40" s="42"/>
     </row>
-    <row r="41" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="32" t="s">
         <v>55</v>
       </c>
@@ -8883,7 +8904,7 @@
       <c r="D41" s="50"/>
       <c r="E41" s="50"/>
     </row>
-    <row r="42" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
         <v>55</v>
       </c>
@@ -8896,7 +8917,7 @@
       <c r="D42" s="50"/>
       <c r="E42" s="50"/>
     </row>
-    <row r="43" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="32" t="s">
         <v>55</v>
       </c>
@@ -8909,7 +8930,7 @@
       <c r="D43" s="50"/>
       <c r="E43" s="50"/>
     </row>
-    <row r="44" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="32" t="s">
         <v>55</v>
       </c>
@@ -8922,7 +8943,7 @@
       <c r="D44" s="50"/>
       <c r="E44" s="50"/>
     </row>
-    <row r="45" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="32" t="s">
         <v>108</v>
       </c>
@@ -8935,7 +8956,7 @@
       <c r="D45" s="50"/>
       <c r="E45" s="50"/>
     </row>
-    <row r="46" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="32" t="s">
         <v>55</v>
       </c>
@@ -8948,7 +8969,7 @@
       <c r="D46" s="50"/>
       <c r="E46" s="50"/>
     </row>
-    <row r="47" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
         <v>55</v>
       </c>
@@ -8961,7 +8982,7 @@
       <c r="D47" s="50"/>
       <c r="E47" s="50"/>
     </row>
-    <row r="48" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="32" t="s">
         <v>55</v>
       </c>
@@ -8974,7 +8995,7 @@
       <c r="D48" s="50"/>
       <c r="E48" s="50"/>
     </row>
-    <row r="49" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="32" t="s">
         <v>55</v>
       </c>
@@ -8987,7 +9008,7 @@
       <c r="D49" s="50"/>
       <c r="E49" s="50"/>
     </row>
-    <row r="50" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="32" t="s">
         <v>55</v>
       </c>
@@ -9000,7 +9021,7 @@
       <c r="D50" s="50"/>
       <c r="E50" s="50"/>
     </row>
-    <row r="51" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="32" t="s">
         <v>55</v>
       </c>
@@ -9013,7 +9034,7 @@
       <c r="D51" s="50"/>
       <c r="E51" s="50"/>
     </row>
-    <row r="52" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
         <v>460</v>
       </c>
@@ -9026,7 +9047,7 @@
       <c r="D52" s="50"/>
       <c r="E52" s="50"/>
     </row>
-    <row r="53" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
         <v>460</v>
       </c>
@@ -9039,7 +9060,7 @@
       <c r="D53" s="50"/>
       <c r="E53" s="50"/>
     </row>
-    <row r="54" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
         <v>55</v>
       </c>
@@ -9052,7 +9073,7 @@
       <c r="D54" s="50"/>
       <c r="E54" s="50"/>
     </row>
-    <row r="55" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="32" t="s">
         <v>55</v>
       </c>
@@ -9065,7 +9086,7 @@
       <c r="D55" s="50"/>
       <c r="E55" s="50"/>
     </row>
-    <row r="56" spans="1:5" ht="13.15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="32" t="s">
         <v>55</v>
       </c>
@@ -9393,7 +9414,7 @@
     <col min="6" max="6" width="47.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>54</v>
       </c>
@@ -9413,7 +9434,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="6" customFormat="1" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>55</v>
       </c>
@@ -9431,7 +9452,7 @@
       </c>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>55</v>
       </c>
@@ -9455,7 +9476,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>55</v>
       </c>
@@ -9472,7 +9493,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
         <v>55</v>
       </c>
@@ -9489,7 +9510,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>55</v>
       </c>
@@ -9506,7 +9527,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
         <v>55</v>
       </c>
@@ -9523,7 +9544,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
         <v>55</v>
       </c>
@@ -9540,7 +9561,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
         <v>55</v>
       </c>
@@ -9557,7 +9578,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
         <v>55</v>
       </c>
@@ -9574,7 +9595,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
         <v>55</v>
       </c>
@@ -9591,7 +9612,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
         <v>55</v>
       </c>
@@ -9608,7 +9629,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
         <v>55</v>
       </c>
@@ -9625,7 +9646,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
         <v>55</v>
       </c>
@@ -9642,7 +9663,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
         <v>55</v>
       </c>
@@ -9657,7 +9678,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>55</v>
       </c>
@@ -9674,7 +9695,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="17" t="s">
         <v>55</v>
       </c>
@@ -9691,7 +9712,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
         <v>55</v>
       </c>
@@ -9708,7 +9729,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="17" t="s">
         <v>55</v>
       </c>
@@ -9728,7 +9749,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
         <v>55</v>
       </c>
@@ -9745,7 +9766,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="17" t="s">
         <v>55</v>
       </c>
@@ -9762,7 +9783,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="17" t="s">
         <v>55</v>
       </c>
@@ -9779,7 +9800,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
         <v>55</v>
       </c>
@@ -9796,7 +9817,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="17" t="s">
         <v>55</v>
       </c>
@@ -9813,7 +9834,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="17" t="s">
         <v>55</v>
       </c>
@@ -9830,7 +9851,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
         <v>55</v>
       </c>
@@ -9847,7 +9868,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="17" t="s">
         <v>55</v>
       </c>
@@ -9862,7 +9883,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="17" t="s">
         <v>55</v>
       </c>
@@ -9879,7 +9900,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="17" t="s">
         <v>55</v>
       </c>
@@ -9896,7 +9917,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
         <v>55</v>
       </c>
@@ -9911,7 +9932,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
updated release notes with PVWatts and SWH update for 3D shading. moved some files to documentation. updated version numbers to Pi-day 3.14. Updated LK manual.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adobos\Projects\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
   </bookViews>
@@ -20,7 +25,7 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -3675,7 +3680,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3710,7 +3715,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3923,7 +3928,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4609,7 +4614,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="32" t="s">
-        <v>192</v>
+        <v>55</v>
       </c>
       <c r="B52" s="63" t="s">
         <v>713</v>

</xml_diff>

<commit_message>
updated todo list - pi release.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="717">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2193,9 +2193,6 @@
   </si>
   <si>
     <t>Check all output reports</t>
-  </si>
-  <si>
-    <t>testing</t>
   </si>
   <si>
     <t>Test web update system for all platforms (Test all the things)</t>
@@ -3927,8 +3924,8 @@
   <dimension ref="A1:F168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A68" sqref="A68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4484,7 +4481,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="32" t="s">
-        <v>716</v>
+        <v>55</v>
       </c>
       <c r="B42" s="63" t="s">
         <v>701</v>
@@ -4549,7 +4546,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="32" t="s">
-        <v>716</v>
+        <v>55</v>
       </c>
       <c r="B47" s="63" t="s">
         <v>708</v>
@@ -4627,7 +4624,7 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="32" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B53" s="40" t="s">
         <v>549</v>
@@ -4640,10 +4637,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="32" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B54" s="40" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="C54" s="40" t="s">
         <v>46</v>
@@ -4679,7 +4676,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="32" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B57" s="40" t="s">
         <v>136</v>
@@ -4692,7 +4689,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="32" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B58" s="40" t="s">
         <v>545</v>
@@ -4705,7 +4702,7 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="32" t="s">
-        <v>135</v>
+        <v>55</v>
       </c>
       <c r="B59" s="40" t="s">
         <v>542</v>
@@ -4718,7 +4715,7 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="32" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="B60" s="40" t="s">
         <v>689</v>
@@ -4731,7 +4728,7 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="32" t="s">
-        <v>714</v>
+        <v>55</v>
       </c>
       <c r="B61" s="40" t="s">
         <v>544</v>
@@ -4833,7 +4830,7 @@
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="32" t="s">
-        <v>108</v>
+        <v>55</v>
       </c>
       <c r="B69" s="47" t="s">
         <v>690</v>

</xml_diff>

<commit_message>
Add Crash Reports sheet to SAM TODO.xlsx and document user reported crashes - symptoms, bug and fixes and what revisions checked into what repositories.
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -1,32 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="16729"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\SAM\trunk\SAMnt\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="To Do- Next Release TBD" sheetId="8" r:id="rId1"/>
     <sheet name="SAM Variable Changes" sheetId="3" r:id="rId2"/>
     <sheet name="Future Project Ideas" sheetId="6" r:id="rId3"/>
-    <sheet name="Unsolved mysteries" sheetId="4" r:id="rId4"/>
-    <sheet name="To Do- FY16 Release (old)" sheetId="7" r:id="rId5"/>
-    <sheet name="To Do- FY15 Release (old)" sheetId="5" r:id="rId6"/>
-    <sheet name="To Do- FY14 Release (old)" sheetId="1" r:id="rId7"/>
+    <sheet name="Crash Reports" sheetId="9" r:id="rId4"/>
+    <sheet name="Unsolved mysteries" sheetId="4" r:id="rId5"/>
+    <sheet name="To Do- FY16 Release (old)" sheetId="7" r:id="rId6"/>
+    <sheet name="To Do- FY15 Release (old)" sheetId="5" r:id="rId7"/>
+    <sheet name="To Do- FY14 Release (old)" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2065" uniqueCount="712">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="733">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2178,12 +2184,75 @@
   <si>
     <t>Export time stamps with time series data (SWH request) (email John Sherwin FSEC, also Dean Laslett via support emao)</t>
   </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Fix</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>Troy Wahr</t>
+  </si>
+  <si>
+    <t>CDF/PDF generates crash when checking ignore zeros on CDF/PDF output page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bug </t>
+  </si>
+  <si>
+    <t>line 464 in dvpncdfctrl.cpp in wex</t>
+  </si>
+  <si>
+    <t>Add check on m_selectedDataSetIndex in wxDVPnCdfCtrl::OnShowZerosClick</t>
+  </si>
+  <si>
+    <t>Check in</t>
+  </si>
+  <si>
+    <t>wex trunk rev 509 and 2016.3.14 branch 510</t>
+  </si>
+  <si>
+    <t>Jennifer Crawford</t>
+  </si>
+  <si>
+    <t>Shading dialog generates a crash during simulation when the shading database is selected for 3 or fewer subarrays</t>
+  </si>
+  <si>
+    <t>two bugs - one on pvsamv1 for criteria to determine when to instatntiate, second on PV Shading.ui callback not setting string option values to zero for each subarray with shading database selected</t>
+  </si>
+  <si>
+    <t>Symptom</t>
+  </si>
+  <si>
+    <t>crash report generated in ShadeDB8_mpp::get_vector at line 126 called from the shading_factor_calculator class during simulation</t>
+  </si>
+  <si>
+    <t>ssc trunk 3888 and 2016.3.14 branch 3891 and SAMnt trunk 2983 and 2016.3.14 branch 2993</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dean Laslett </t>
+  </si>
+  <si>
+    <t>Power Tower Data tab on results page causing crash when Save to CSV file clicked with no data selected.</t>
+  </si>
+  <si>
+    <t>crash report generated in TabularBrowser::GetTextData at line 2883 in results.cpp in SAMnt</t>
+  </si>
+  <si>
+    <t>Add initialization of m_gridTable to NULL in TabularBrowser constructor and check for selected dataset (m_gridTableMap.size &gt; 0) when saving or copying or sending to Excel on Data tab</t>
+  </si>
+  <si>
+    <t>SAMnt trunk rev 2992 and 2016.3.14 branch rev 2993</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2279,6 +2348,13 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="18">
@@ -2406,7 +2482,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2526,6 +2602,11 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -3951,7 +4032,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3984,9 +4065,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -4019,6 +4117,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -6999,7 +7114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
@@ -7774,6 +7889,107 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="72" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>712</v>
+      </c>
+      <c r="B1" t="s">
+        <v>714</v>
+      </c>
+      <c r="C1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D1" t="s">
+        <v>717</v>
+      </c>
+      <c r="E1" t="s">
+        <v>713</v>
+      </c>
+      <c r="F1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="69">
+        <v>42471</v>
+      </c>
+      <c r="B2" t="s">
+        <v>715</v>
+      </c>
+      <c r="C2" t="s">
+        <v>716</v>
+      </c>
+      <c r="D2" t="s">
+        <v>718</v>
+      </c>
+      <c r="E2" t="s">
+        <v>719</v>
+      </c>
+      <c r="F2" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="69">
+        <v>42479</v>
+      </c>
+      <c r="B3" t="s">
+        <v>722</v>
+      </c>
+      <c r="C3" t="s">
+        <v>723</v>
+      </c>
+      <c r="D3" t="s">
+        <v>726</v>
+      </c>
+      <c r="E3" t="s">
+        <v>724</v>
+      </c>
+      <c r="F3" s="70" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="69">
+        <v>42474</v>
+      </c>
+      <c r="B4" s="71" t="s">
+        <v>728</v>
+      </c>
+      <c r="C4" t="s">
+        <v>729</v>
+      </c>
+      <c r="D4" t="s">
+        <v>730</v>
+      </c>
+      <c r="E4" t="s">
+        <v>731</v>
+      </c>
+      <c r="F4" t="s">
+        <v>732</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7792,7 +8008,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F151"/>
   <sheetViews>
@@ -8957,7 +9173,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F155"/>
   <sheetViews>
@@ -10068,7 +10284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I203"/>
   <sheetViews>

</xml_diff>

<commit_message>
Update todo and registration list
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2098" uniqueCount="738">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="741">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2256,6 +2256,15 @@
   </si>
   <si>
     <t>Aron/Janine/Steve</t>
+  </si>
+  <si>
+    <t>Wind hub height vs wind speed data height message on Turbine page reads library data, so incorrect with user file stored on computer</t>
+  </si>
+  <si>
+    <t>Option for "mid-year" discounting convention from former NRELian Cory Welch now at Navigant. See support email 2/25/2016</t>
+  </si>
+  <si>
+    <t>Fix linux installer script, see Ben Elliston email 8/10/2015 and Wiebke Toussaint 4/20/2016</t>
   </si>
 </sst>
 </file>
@@ -4290,7 +4299,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4660,10 +4669,30 @@
       <c r="E28" s="65"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="32"/>
+      <c r="A29" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" s="65" t="s">
+        <v>738</v>
+      </c>
+      <c r="C29" s="65" t="s">
+        <v>226</v>
+      </c>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="32"/>
+      <c r="A30" s="32" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="65" t="s">
+        <v>740</v>
+      </c>
+      <c r="C30" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="65"/>
+      <c r="E30" s="65"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="32"/>
@@ -7140,10 +7169,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F64"/>
+  <dimension ref="A1:F65"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7808,6 +7837,11 @@
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
         <v>711</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>739</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to do list to add a column for us to keep track of what things have been ported to Trac so far
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100"/>
+    <workbookView xWindow="-15" yWindow="45" windowWidth="12135" windowHeight="8100" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="To Do- Current" sheetId="8" r:id="rId1"/>
@@ -20,16 +20,16 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="0" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
-    <definedName name="Status">'To Do- Current'!$K$2:$K$5</definedName>
+    <definedName name="Status">'To Do- Current'!$L$2:$L$5</definedName>
     <definedName name="Types">'SAM Variable Changes'!$V$1:$V$3</definedName>
-    <definedName name="When">'To Do- Current'!$L$2:$L$4</definedName>
+    <definedName name="When">'To Do- Current'!$M$2:$M$4</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2193" uniqueCount="762">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2277" uniqueCount="763">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2330,6 +2330,9 @@
   </si>
   <si>
     <t>see file from scott stephens "POA from reference cell"</t>
+  </si>
+  <si>
+    <t>Entered into Trac?</t>
   </si>
 </sst>
 </file>
@@ -2708,7 +2711,112 @@
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="122">
+  <dxfs count="142">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3765,6 +3873,41 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FF33CCCC"/>
         </patternFill>
       </fill>
@@ -3856,8 +3999,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="121"/>
-      <tableStyleElement type="headerRow" dxfId="120"/>
+      <tableStyleElement type="wholeTable" dxfId="141"/>
+      <tableStyleElement type="headerRow" dxfId="140"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -4168,1216 +4311,1515 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L197"/>
+  <dimension ref="A1:M197"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="73" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" style="72" customWidth="1"/>
-    <col min="3" max="3" width="90.140625" style="31" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="31" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="31" customWidth="1"/>
-    <col min="7" max="10" width="9.140625" style="31"/>
-    <col min="11" max="11" width="10.7109375" style="31" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="31"/>
+    <col min="1" max="1" width="22.42578125" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" style="73" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" style="72" customWidth="1"/>
+    <col min="4" max="4" width="90.140625" style="31" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="31" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="31" customWidth="1"/>
+    <col min="7" max="7" width="30.140625" style="31" customWidth="1"/>
+    <col min="8" max="11" width="9.140625" style="31"/>
+    <col min="12" max="12" width="10.7109375" style="31" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="31"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="38" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
+        <v>762</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="C1" s="36" t="s">
         <v>738</v>
       </c>
-      <c r="C1" s="36" t="s">
+      <c r="D1" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="36" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>467</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="G1" s="36" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="72" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="B2" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C2" s="65" t="s">
+      <c r="D2" s="65" t="s">
         <v>730</v>
       </c>
-      <c r="D2" s="65" t="s">
+      <c r="E2" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="65"/>
-      <c r="K2" s="31" t="s">
+      <c r="F2" s="65"/>
+      <c r="L2" s="31" t="s">
         <v>181</v>
       </c>
-      <c r="L2" s="31" t="s">
+      <c r="M2" s="31" t="s">
         <v>748</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="72" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="B3" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="D3" s="65" t="s">
         <v>731</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="E3" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="65"/>
-      <c r="K3" s="31" t="s">
+      <c r="F3" s="65"/>
+      <c r="L3" s="31" t="s">
         <v>747</v>
       </c>
-      <c r="L3" s="31" t="s">
+      <c r="M3" s="31" t="s">
         <v>749</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="72" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B4" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="D4" s="65" t="s">
         <v>741</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="E4" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="65"/>
-      <c r="K4" s="31" t="s">
-        <v>55</v>
-      </c>
+      <c r="F4" s="65"/>
       <c r="L4" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="M4" s="31" t="s">
         <v>752</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="72" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B5" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C5" s="65" t="s">
+      <c r="D5" s="65" t="s">
         <v>742</v>
       </c>
-      <c r="D5" s="65" t="s">
+      <c r="E5" s="65" t="s">
         <v>289</v>
       </c>
-      <c r="E5" s="65"/>
-      <c r="K5" s="31" t="s">
+      <c r="F5" s="65"/>
+      <c r="L5" s="31" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="72" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B6" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C6" s="65" t="s">
+      <c r="D6" s="65" t="s">
         <v>743</v>
       </c>
-      <c r="D6" s="65" t="s">
+      <c r="E6" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="65"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F6" s="65"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="72" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B7" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C7" s="65" t="s">
+      <c r="D7" s="65" t="s">
         <v>744</v>
       </c>
-      <c r="D7" s="65" t="s">
+      <c r="E7" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="E7" s="65"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F7" s="65"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="72" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B8" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="D8" s="65" t="s">
         <v>745</v>
       </c>
-      <c r="D8" s="65" t="s">
+      <c r="E8" s="65" t="s">
         <v>222</v>
       </c>
-      <c r="E8" s="65"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F8" s="65"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="72" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B9" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C9" s="65" t="s">
+      <c r="D9" s="65" t="s">
         <v>746</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="E9" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="65"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F9" s="65"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="72" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="B10" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="72" t="s">
         <v>748</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="D10" s="65" t="s">
         <v>751</v>
       </c>
-      <c r="D10" s="65" t="s">
+      <c r="E10" s="65" t="s">
         <v>294</v>
       </c>
-      <c r="E10" s="65"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F10" s="65"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="72" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="B11" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C11" s="65" t="s">
+      <c r="D11" s="65" t="s">
         <v>691</v>
       </c>
-      <c r="D11" s="65" t="s">
+      <c r="E11" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="65"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F11" s="65"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B12" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C12" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="D12" s="65" t="s">
         <v>671</v>
       </c>
-      <c r="D12" s="65" t="s">
+      <c r="E12" s="65" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="65"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F12" s="65"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B13" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="D13" s="65" t="s">
         <v>617</v>
       </c>
-      <c r="D13" s="65" t="s">
+      <c r="E13" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="65"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F13" s="65"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B14" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C14" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C14" s="65" t="s">
+      <c r="D14" s="65" t="s">
         <v>669</v>
       </c>
-      <c r="D14" s="65" t="s">
+      <c r="E14" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="65"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F14" s="65"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B15" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C15" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C15" s="65" t="s">
+      <c r="D15" s="65" t="s">
         <v>627</v>
       </c>
-      <c r="D15" s="65" t="s">
+      <c r="E15" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E15" s="65"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F15" s="65"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B16" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C16" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C16" s="65" t="s">
+      <c r="D16" s="65" t="s">
         <v>732</v>
       </c>
-      <c r="D16" s="65" t="s">
+      <c r="E16" s="65" t="s">
         <v>733</v>
       </c>
-      <c r="E16" s="65"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F16" s="65"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B17" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C17" s="65" t="s">
+      <c r="D17" s="65" t="s">
         <v>735</v>
       </c>
-      <c r="D17" s="65" t="s">
+      <c r="E17" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E17" s="65"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F17" s="65"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B18" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C18" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C18" s="65" t="s">
+      <c r="D18" s="65" t="s">
         <v>753</v>
       </c>
-      <c r="D18" s="65" t="s">
+      <c r="E18" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="65"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F18" s="65"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="B19" s="72" t="s">
+      <c r="C19" s="72" t="s">
         <v>749</v>
       </c>
-      <c r="C19" s="65" t="s">
+      <c r="D19" s="65" t="s">
         <v>756</v>
       </c>
-      <c r="D19" s="65" t="s">
+      <c r="E19" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="65"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F19" s="65"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="72" t="s">
+        <v>104</v>
+      </c>
+      <c r="B20" s="72" t="s">
         <v>740</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="C20" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="65" t="s">
+      <c r="D20" s="65" t="s">
         <v>739</v>
       </c>
-      <c r="D20" s="65" t="s">
+      <c r="E20" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="65"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F20" s="65"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="72" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B21" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C21" s="65" t="s">
+      <c r="D21" s="65" t="s">
         <v>702</v>
       </c>
-      <c r="D21" s="65" t="s">
+      <c r="E21" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E21" s="65"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F21" s="65"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B22" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C22" s="65" t="s">
+      <c r="D22" s="65" t="s">
         <v>614</v>
       </c>
-      <c r="D22" s="65" t="s">
+      <c r="E22" s="65" t="s">
         <v>226</v>
       </c>
-      <c r="E22" s="65"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F22" s="65"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B23" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C23" s="65" t="s">
+      <c r="D23" s="65" t="s">
         <v>653</v>
       </c>
-      <c r="D23" s="65" t="s">
+      <c r="E23" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="65"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F23" s="65"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B24" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C24" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="D24" s="65" t="s">
         <v>701</v>
       </c>
-      <c r="D24" s="65"/>
       <c r="E24" s="65"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F24" s="65"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B25" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="65" t="s">
+      <c r="D25" s="65" t="s">
         <v>612</v>
       </c>
-      <c r="D25" s="65" t="s">
+      <c r="E25" s="65" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="65"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F25" s="65"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B26" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C26" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="65" t="s">
+      <c r="D26" s="65" t="s">
         <v>615</v>
       </c>
-      <c r="D26" s="65" t="s">
+      <c r="E26" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="65"/>
-    </row>
-    <row r="27" spans="1:6" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="F26" s="65"/>
+    </row>
+    <row r="27" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A27" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B27" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C27" s="65" t="s">
+      <c r="D27" s="65" t="s">
         <v>628</v>
       </c>
-      <c r="D27" s="65" t="s">
+      <c r="E27" s="65" t="s">
         <v>648</v>
       </c>
-      <c r="E27" s="65"/>
-      <c r="F27" s="31"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F27" s="65"/>
+      <c r="G27" s="31"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B28" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C28" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="65" t="s">
+      <c r="D28" s="65" t="s">
         <v>656</v>
       </c>
-      <c r="D28" s="65" t="s">
+      <c r="E28" s="65" t="s">
         <v>655</v>
       </c>
-      <c r="E28" s="65"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F28" s="65"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B29" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="65" t="s">
+      <c r="D29" s="65" t="s">
         <v>662</v>
       </c>
-      <c r="D29" s="65" t="s">
+      <c r="E29" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="65"/>
-    </row>
-    <row r="30" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+      <c r="F29" s="65"/>
+    </row>
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.25">
       <c r="A30" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B30" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C30" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="65" t="s">
+      <c r="D30" s="65" t="s">
         <v>645</v>
       </c>
-      <c r="D30" s="65" t="s">
+      <c r="E30" s="65" t="s">
         <v>646</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F30" s="65"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B31" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C31" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C31" s="65" t="s">
+      <c r="D31" s="65" t="s">
         <v>647</v>
       </c>
-      <c r="D31" s="65" t="s">
+      <c r="E31" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="65"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F31" s="65"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B32" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C32" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C32" s="66" t="s">
+      <c r="D32" s="66" t="s">
         <v>270</v>
       </c>
-      <c r="D32" s="65" t="s">
+      <c r="E32" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="E32" s="67"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="67"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B33" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C33" s="65" t="s">
+      <c r="D33" s="65" t="s">
         <v>684</v>
       </c>
-      <c r="D33" s="65"/>
       <c r="E33" s="65"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="65"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B34" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C34" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="65" t="s">
+      <c r="D34" s="65" t="s">
         <v>699</v>
       </c>
-      <c r="D34" s="65"/>
       <c r="E34" s="65"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="65"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B35" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C35" s="65" t="s">
+      <c r="D35" s="65" t="s">
         <v>700</v>
       </c>
-      <c r="D35" s="65"/>
       <c r="E35" s="65"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="65"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B36" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C36" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="65" t="s">
+      <c r="D36" s="65" t="s">
         <v>703</v>
       </c>
-      <c r="D36" s="65" t="s">
+      <c r="E36" s="65" t="s">
         <v>262</v>
       </c>
-      <c r="E36" s="65"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="65"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B37" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C37" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C37" s="65" t="s">
+      <c r="D37" s="65" t="s">
         <v>163</v>
       </c>
-      <c r="D37" s="65"/>
       <c r="E37" s="65"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F37" s="65"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B38" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C38" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="65" t="s">
+      <c r="D38" s="65" t="s">
         <v>754</v>
       </c>
-      <c r="D38" s="65" t="s">
+      <c r="E38" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E38" s="65"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F38" s="65"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="72" t="s">
-        <v>181</v>
+        <v>104</v>
       </c>
       <c r="B39" s="72" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="65" t="s">
+      <c r="D39" s="65" t="s">
         <v>755</v>
       </c>
-      <c r="D39" s="65" t="s">
+      <c r="E39" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E39" s="65"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F39" s="65"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B40" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C40" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="65" t="s">
+      <c r="D40" s="65" t="s">
         <v>758</v>
       </c>
-      <c r="D40" s="65"/>
       <c r="E40" s="65"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F40" s="65"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="72" t="s">
         <v>181</v>
       </c>
-      <c r="C41" s="65" t="s">
+      <c r="B41" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="65" t="s">
         <v>759</v>
       </c>
-      <c r="D41" s="65"/>
       <c r="E41" s="65"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F41" s="65"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="72" t="s">
         <v>181</v>
       </c>
       <c r="B42" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="C42" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="C42" s="65" t="s">
+      <c r="D42" s="65" t="s">
         <v>760</v>
       </c>
-      <c r="D42" s="65" t="s">
+      <c r="E42" s="65" t="s">
         <v>45</v>
       </c>
-      <c r="E42" s="65" t="s">
+      <c r="F42" s="65" t="s">
         <v>761</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="72"/>
-      <c r="C43" s="65"/>
+      <c r="B43" s="72"/>
       <c r="D43" s="65"/>
       <c r="E43" s="65"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F43" s="65"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="72"/>
-      <c r="C44" s="65"/>
+      <c r="B44" s="72"/>
       <c r="D44" s="65"/>
       <c r="E44" s="65"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F44" s="65"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="72"/>
-      <c r="C45" s="65"/>
+      <c r="B45" s="72"/>
       <c r="D45" s="65"/>
       <c r="E45" s="65"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F45" s="65"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="72"/>
-      <c r="C46" s="65"/>
+      <c r="B46" s="72"/>
       <c r="D46" s="65"/>
       <c r="E46" s="65"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F46" s="65"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="72"/>
-      <c r="C47" s="65"/>
+      <c r="B47" s="72"/>
       <c r="D47" s="65"/>
       <c r="E47" s="65"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F47" s="65"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="72"/>
-      <c r="C48" s="65"/>
+      <c r="B48" s="72"/>
       <c r="D48" s="65"/>
       <c r="E48" s="65"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F48" s="65"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="72"/>
-      <c r="C49" s="65"/>
+      <c r="B49" s="72"/>
       <c r="D49" s="65"/>
       <c r="E49" s="65"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F49" s="65"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" s="72"/>
-      <c r="C50" s="65"/>
+      <c r="B50" s="72"/>
       <c r="D50" s="65"/>
       <c r="E50" s="65"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F50" s="65"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="72"/>
-      <c r="C51" s="65"/>
+      <c r="B51" s="72"/>
       <c r="D51" s="65"/>
       <c r="E51" s="65"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F51" s="65"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="72"/>
-      <c r="C52" s="65"/>
+      <c r="B52" s="72"/>
       <c r="D52" s="65"/>
       <c r="E52" s="65"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F52" s="65"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="72"/>
-      <c r="C53" s="65"/>
+      <c r="B53" s="72"/>
       <c r="D53" s="65"/>
       <c r="E53" s="65"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F53" s="65"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="72"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B54" s="72"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="72"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B55" s="72"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="72"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B56" s="72"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="72"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B57" s="72"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="72"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B58" s="72"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="72"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B59" s="72"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" s="72"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B60" s="72"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="72"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B61" s="72"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="72"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B62" s="72"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="72"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B63" s="72"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="72"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64" s="72"/>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="72"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65" s="72"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="72"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B66" s="72"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="72"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B67" s="72"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="72"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B68" s="72"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="72"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B69" s="72"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="72"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B70" s="72"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="72"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B71" s="72"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="72"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B72" s="72"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="72"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B73" s="72"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="72"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B74" s="72"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="72"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B75" s="72"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="72"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B76" s="72"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="72"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B77" s="72"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="72"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B78" s="72"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="72"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B79" s="72"/>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="72"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B80" s="72"/>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="72"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B81" s="72"/>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="72"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B82" s="72"/>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="72"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B83" s="72"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="72"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B84" s="72"/>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="72"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B85" s="72"/>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="72"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B86" s="72"/>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="72"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B87" s="72"/>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="72"/>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B88" s="72"/>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="72"/>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B89" s="72"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="72"/>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B90" s="72"/>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="72"/>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B91" s="72"/>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="72"/>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B92" s="72"/>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="72"/>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B93" s="72"/>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="72"/>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B94" s="72"/>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="72"/>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B95" s="72"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="72"/>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B96" s="72"/>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="72"/>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B97" s="72"/>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="72"/>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B98" s="72"/>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="72"/>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B99" s="72"/>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="72"/>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B100" s="72"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="72"/>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B101" s="72"/>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="72"/>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B102" s="72"/>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="72"/>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B103" s="72"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="72"/>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B104" s="72"/>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="72"/>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B105" s="72"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="72"/>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B106" s="72"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="72"/>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B107" s="72"/>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="72"/>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B108" s="72"/>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="72"/>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B109" s="72"/>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="72"/>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B110" s="72"/>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="72"/>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B111" s="72"/>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="72"/>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B112" s="72"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="72"/>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B113" s="72"/>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="72"/>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B114" s="72"/>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="72"/>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B115" s="72"/>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="72"/>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B116" s="72"/>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="72"/>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B117" s="72"/>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="72"/>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B118" s="72"/>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="72"/>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B119" s="72"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="72"/>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B120" s="72"/>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="72"/>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B121" s="72"/>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="72"/>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B122" s="72"/>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="72"/>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B123" s="72"/>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="72"/>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B124" s="72"/>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="72"/>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B125" s="72"/>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="72"/>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B126" s="72"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="72"/>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B127" s="72"/>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="72"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B128" s="72"/>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="72"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B129" s="72"/>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="72"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B130" s="72"/>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="72"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B131" s="72"/>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="72"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B132" s="72"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="72"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B133" s="72"/>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="72"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B134" s="72"/>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="72"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B135" s="72"/>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="72"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B136" s="72"/>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="72"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B137" s="72"/>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="72"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B138" s="72"/>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="72"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B139" s="72"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="72"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B140" s="72"/>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="72"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B141" s="72"/>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="72"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B142" s="72"/>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="72"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B143" s="72"/>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="72"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B144" s="72"/>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="72"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B145" s="72"/>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="72"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B146" s="72"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="72"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B147" s="72"/>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="72"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B148" s="72"/>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="72"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B149" s="72"/>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="72"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B150" s="72"/>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="72"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B151" s="72"/>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="72"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B152" s="72"/>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="72"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B153" s="72"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="72"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B154" s="72"/>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="72"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B155" s="72"/>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="72"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B156" s="72"/>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="72"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B157" s="72"/>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="72"/>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B158" s="72"/>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="72"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B159" s="72"/>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="72"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B160" s="72"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="72"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B161" s="72"/>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="72"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B162" s="72"/>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="72"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B163" s="72"/>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="72"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B164" s="72"/>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="72"/>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B165" s="72"/>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="72"/>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B166" s="72"/>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="72"/>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B167" s="72"/>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="72"/>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B168" s="72"/>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="72"/>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B169" s="72"/>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="72"/>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B170" s="72"/>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="72"/>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B171" s="72"/>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="72"/>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B172" s="72"/>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="72"/>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B173" s="72"/>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="72"/>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B174" s="72"/>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="72"/>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B175" s="72"/>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="72"/>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176" s="72"/>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="72"/>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177" s="72"/>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="72"/>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B178" s="72"/>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="72"/>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B179" s="72"/>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="72"/>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B180" s="72"/>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="72"/>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B181" s="72"/>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="72"/>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B182" s="72"/>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="72"/>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B183" s="72"/>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="72"/>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B184" s="72"/>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="72"/>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B185" s="72"/>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="72"/>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B186" s="72"/>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="72"/>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B187" s="72"/>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="72"/>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B188" s="72"/>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="72"/>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B189" s="72"/>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="72"/>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B190" s="72"/>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="72"/>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B191" s="72"/>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="72"/>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B192" s="72"/>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="72"/>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B193" s="72"/>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="72"/>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B194" s="72"/>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="72"/>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B195" s="72"/>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="72"/>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B196" s="72"/>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="72"/>
+      <c r="B197" s="72"/>
     </row>
   </sheetData>
-  <sortState ref="A2:F41">
-    <sortCondition ref="B2:B41" customList="Patch,Release,Pre-Release,Future"/>
+  <sortState ref="B2:G41">
+    <sortCondition ref="C2:C41" customList="Patch,Release,Pre-Release,Future"/>
   </sortState>
-  <conditionalFormatting sqref="B2:B198">
-    <cfRule type="containsText" dxfId="119" priority="85" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",B2)))</formula>
+  <conditionalFormatting sqref="C2:C198">
+    <cfRule type="containsText" dxfId="139" priority="90" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="containsText" dxfId="118" priority="27" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",B27)))</formula>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="containsText" dxfId="138" priority="32" operator="containsText" text="Pre-release">
+      <formula>NOT(ISERROR(SEARCH("Pre-release",C27)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B1048576">
-    <cfRule type="containsText" dxfId="117" priority="24" operator="containsText" text="patch">
-      <formula>NOT(ISERROR(SEARCH("patch",B2)))</formula>
+  <conditionalFormatting sqref="C2:C1048576">
+    <cfRule type="containsText" dxfId="137" priority="29" operator="containsText" text="patch">
+      <formula>NOT(ISERROR(SEARCH("patch",C2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="containsText" dxfId="136" priority="24" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",B1)))</formula>
+    </cfRule>
+    <cfRule type="beginsWith" dxfId="135" priority="25" operator="beginsWith" text="Done">
+      <formula>LEFT(B1,LEN("Done"))="Done"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="134" priority="26" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="133" priority="27" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="132" priority="28" operator="containsText" text="Not Done">
+      <formula>NOT(ISERROR(SEARCH("Not Done",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="containsText" dxfId="131" priority="6" operator="containsText" text="Release">
+      <formula>NOT(ISERROR(SEARCH("Release",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="116" priority="19" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="130" priority="1" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="115" priority="20" operator="beginsWith" text="Done">
+    <cfRule type="beginsWith" dxfId="129" priority="2" operator="beginsWith" text="Done">
       <formula>LEFT(A1,LEN("Done"))="Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="21" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="128" priority="3" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="22" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="127" priority="4" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="23" operator="containsText" text="Not Done">
+    <cfRule type="containsText" dxfId="126" priority="5" operator="containsText" text="Not Done">
       <formula>NOT(ISERROR(SEARCH("Not Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="111" priority="1" operator="containsText" text="Release">
-      <formula>NOT(ISERROR(SEARCH("Release",B1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="A2">
+    <dataValidation type="list" allowBlank="1" sqref="A2:B2">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" sqref="A3:A197">
+    <dataValidation type="list" sqref="A3:B197">
       <formula1>Status</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B2:B198">
+    <dataValidation type="list" allowBlank="1" sqref="C2:C198">
       <formula1>When</formula1>
     </dataValidation>
   </dataValidations>
@@ -7699,796 +8141,1421 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:G197"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="101.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.42578125" style="73" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="36" t="s">
+        <v>762</v>
+      </c>
+      <c r="B1" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="C2" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="D2" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="19"/>
       <c r="E2" s="19"/>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="19"/>
+      <c r="G2" s="19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="C3" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="C3" s="19"/>
       <c r="D3" s="19"/>
       <c r="E3" s="19"/>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="19"/>
+      <c r="G3" s="19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="19" t="s">
         <v>172</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="D4" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="19"/>
       <c r="E4" s="19"/>
       <c r="F4" s="19"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="17" t="s">
+      <c r="G4" s="19"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>161</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="14" t="s">
+      <c r="D5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="C6" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="19"/>
       <c r="D6" s="19"/>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="19"/>
+      <c r="F6" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="C7" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="19"/>
       <c r="D7" s="19"/>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="19"/>
+      <c r="F7" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="C8" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="19"/>
       <c r="D8" s="19"/>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="19"/>
+      <c r="F8" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B9" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="C9" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="D9" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="19"/>
+      <c r="F9" s="19" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B10" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="C10" s="19"/>
       <c r="D10" s="19"/>
       <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="F10" s="19"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B11" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="C11" s="19"/>
       <c r="D11" s="19"/>
       <c r="E11" s="19"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="F11" s="19"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B12" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="C12" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="C12" s="19"/>
       <c r="D12" s="19"/>
       <c r="E12" s="19"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="F12" s="19"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B13" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="C13" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="C13" s="19"/>
       <c r="D13" s="19"/>
       <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="F13" s="19"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B14" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="C14" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="C14" s="19"/>
       <c r="D14" s="19"/>
       <c r="E14" s="19"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="F14" s="19"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="C15" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="19"/>
       <c r="D15" s="19"/>
       <c r="E15" s="19"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="F15" s="19"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B16" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="C16" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="19"/>
       <c r="D16" s="19"/>
       <c r="E16" s="19"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="F16" s="19"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="C17" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C17" s="19"/>
       <c r="D17" s="19"/>
       <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="17" t="s">
+      <c r="F17" s="19"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B18" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="C18" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="C18" s="19"/>
       <c r="D18" s="19"/>
       <c r="E18" s="19"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="F18" s="19"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B19" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="C19" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="D19" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="D19" s="19">
+      <c r="E19" s="19">
         <v>2</v>
       </c>
-      <c r="E19" s="19"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="17" t="s">
+      <c r="F19" s="19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B20" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="C20" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="19"/>
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="F20" s="19"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B21" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="C21" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="C21" s="19"/>
       <c r="D21" s="19"/>
       <c r="E21" s="19"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B22" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="C22" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="C22" s="19"/>
       <c r="D22" s="19"/>
       <c r="E22" s="19"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="F22" s="19"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="C23" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="C23" s="19"/>
       <c r="D23" s="19"/>
       <c r="E23" s="19"/>
-      <c r="F23" s="19" t="s">
+      <c r="F23" s="19"/>
+      <c r="G23" s="19" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="C24" s="19" t="s">
         <v>132</v>
       </c>
-      <c r="C24" s="19" t="s">
+      <c r="D24" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="19"/>
       <c r="E24" s="19"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="F24" s="19"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B25" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="C25" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="D25" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="15"/>
+      <c r="F25" s="15" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B26" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="C26" s="14" t="s">
         <v>125</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="D26" s="14" t="s">
         <v>126</v>
       </c>
-      <c r="D26" s="14"/>
       <c r="E26" s="14"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="F26" s="14"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="C27" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="D27" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="D27" s="14"/>
       <c r="E27" s="14"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="F27" s="14"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B28" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="C28" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="14" t="s">
+      <c r="D28" s="14" t="s">
         <v>123</v>
       </c>
-      <c r="D28" s="14"/>
       <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="F28" s="14"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B29" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="C29" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="C29" s="14" t="s">
+      <c r="D29" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D29" s="14"/>
       <c r="E29" s="14"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+      <c r="F29" s="14"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B30" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="C30" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="C30" s="14"/>
       <c r="D30" s="14"/>
       <c r="E30" s="14"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="F30" s="14"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B31" s="17" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="19" t="s">
+      <c r="C31" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="D31" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="D31" s="19">
+      <c r="E31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="19"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="F31" s="19"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B32" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="C32" s="14" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B33" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="C33" s="14" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B34" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="C34" s="14" t="s">
         <v>610</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B35" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B36" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="17" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="17" t="s">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B38" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B41" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B42" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>204</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="72"/>
+      <c r="B43" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="72"/>
+      <c r="B44" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="72"/>
+      <c r="B45" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="72"/>
+      <c r="B46" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="72"/>
+      <c r="B47" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="72"/>
+      <c r="B48" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="72"/>
+      <c r="B49" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
         <v>757</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="27" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="72"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="72"/>
+      <c r="C51" s="27" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="72"/>
+      <c r="B52" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="72"/>
+      <c r="B53" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="72"/>
+      <c r="B54" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="17" t="s">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="72"/>
+      <c r="B55" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="17" t="s">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="72"/>
+      <c r="B56" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="17" t="s">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="72"/>
+      <c r="B57" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="17" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="72"/>
+      <c r="B58" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>750</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="72"/>
+      <c r="B59" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="72"/>
+      <c r="B60" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="17" t="s">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="72"/>
+      <c r="B61" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>736</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="17" t="s">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="72"/>
+      <c r="B62" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>465</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="72"/>
+      <c r="B63" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A64" s="17" t="s">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="72"/>
+      <c r="B64" s="17" t="s">
         <v>108</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>496</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="72"/>
+      <c r="C65" t="s">
         <v>708</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="72"/>
+      <c r="C66" t="s">
         <v>734</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="72"/>
+      <c r="C67" t="s">
         <v>737</v>
       </c>
     </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="72"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="72"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="72"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="72"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="72"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="72"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="72"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="72"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="72"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="72"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="72"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="72"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="72"/>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="72"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="72"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="72"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="72"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="72"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="72"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="72"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="72"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="72"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="72"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="72"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="72"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="72"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="72"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="72"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="72"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="72"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="72"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="72"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="72"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="72"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="72"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="72"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="72"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="72"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="72"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="72"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="72"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="72"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="72"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="72"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="72"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="72"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="72"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="72"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="72"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="72"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="72"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="72"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="72"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="72"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="72"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="72"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="72"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="72"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="72"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="72"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="72"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="72"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="72"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="72"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="72"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="72"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="72"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="72"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="72"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="72"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="72"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="72"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="72"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="72"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="72"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="72"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="72"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="72"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="72"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="72"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="72"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="72"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="72"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="72"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="72"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="72"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="72"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="72"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="72"/>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A157" s="72"/>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A158" s="72"/>
+    </row>
+    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A159" s="72"/>
+    </row>
+    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A160" s="72"/>
+    </row>
+    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A161" s="72"/>
+    </row>
+    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A162" s="72"/>
+    </row>
+    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A163" s="72"/>
+    </row>
+    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A164" s="72"/>
+    </row>
+    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A165" s="72"/>
+    </row>
+    <row r="166" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A166" s="72"/>
+    </row>
+    <row r="167" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A167" s="72"/>
+    </row>
+    <row r="168" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A168" s="72"/>
+    </row>
+    <row r="169" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A169" s="72"/>
+    </row>
+    <row r="170" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A170" s="72"/>
+    </row>
+    <row r="171" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A171" s="72"/>
+    </row>
+    <row r="172" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A172" s="72"/>
+    </row>
+    <row r="173" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A173" s="72"/>
+    </row>
+    <row r="174" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A174" s="72"/>
+    </row>
+    <row r="175" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A175" s="72"/>
+    </row>
+    <row r="176" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A176" s="72"/>
+    </row>
+    <row r="177" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A177" s="72"/>
+    </row>
+    <row r="178" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A178" s="72"/>
+    </row>
+    <row r="179" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A179" s="72"/>
+    </row>
+    <row r="180" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A180" s="72"/>
+    </row>
+    <row r="181" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A181" s="72"/>
+    </row>
+    <row r="182" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A182" s="72"/>
+    </row>
+    <row r="183" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A183" s="72"/>
+    </row>
+    <row r="184" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A184" s="72"/>
+    </row>
+    <row r="185" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A185" s="72"/>
+    </row>
+    <row r="186" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A186" s="72"/>
+    </row>
+    <row r="187" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A187" s="72"/>
+    </row>
+    <row r="188" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A188" s="72"/>
+    </row>
+    <row r="189" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A189" s="72"/>
+    </row>
+    <row r="190" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A190" s="72"/>
+    </row>
+    <row r="191" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A191" s="72"/>
+    </row>
+    <row r="192" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A192" s="72"/>
+    </row>
+    <row r="193" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A193" s="72"/>
+    </row>
+    <row r="194" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A194" s="72"/>
+    </row>
+    <row r="195" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A195" s="72"/>
+    </row>
+    <row r="196" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A196" s="72"/>
+    </row>
+    <row r="197" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A197" s="72"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1 A52:A64 A5:A49">
-    <cfRule type="containsText" dxfId="110" priority="38" operator="containsText" text="NGTD">
+  <conditionalFormatting sqref="B1 B52:B64 B5:B49">
+    <cfRule type="containsText" dxfId="125" priority="48" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="124" priority="49" operator="containsText" text="Test">
+      <formula>NOT(ISERROR(SEARCH("Test",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="123" priority="50" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="122" priority="51" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="121" priority="52" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1 B52:B64 B5:B49">
+    <cfRule type="containsText" dxfId="120" priority="46" operator="containsText" text="POUT">
+      <formula>NOT(ISERROR(SEARCH("POUT",B1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="119" priority="47" operator="containsText" text="Pre-release">
+      <formula>NOT(ISERROR(SEARCH("Pre-release",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="containsText" dxfId="118" priority="41" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="117" priority="42" operator="containsText" text="Test">
+      <formula>NOT(ISERROR(SEARCH("Test",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="116" priority="43" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="115" priority="44" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="114" priority="45" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2">
+    <cfRule type="containsText" dxfId="113" priority="39" operator="containsText" text="POUT">
+      <formula>NOT(ISERROR(SEARCH("POUT",B2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="112" priority="40" operator="containsText" text="Pre-release">
+      <formula>NOT(ISERROR(SEARCH("Pre-release",B2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="containsText" dxfId="111" priority="34" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="110" priority="35" operator="containsText" text="Test">
+      <formula>NOT(ISERROR(SEARCH("Test",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="109" priority="36" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="108" priority="37" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="107" priority="38" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3">
+    <cfRule type="containsText" dxfId="106" priority="32" operator="containsText" text="POUT">
+      <formula>NOT(ISERROR(SEARCH("POUT",B3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="105" priority="33" operator="containsText" text="Pre-release">
+      <formula>NOT(ISERROR(SEARCH("Pre-release",B3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="containsText" dxfId="104" priority="27" operator="containsText" text="NGTD">
+      <formula>NOT(ISERROR(SEARCH("NGTD",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="103" priority="28" operator="containsText" text="Test">
+      <formula>NOT(ISERROR(SEARCH("Test",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="102" priority="29" operator="containsText" text="Future">
+      <formula>NOT(ISERROR(SEARCH("Future",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="101" priority="30" operator="containsText" text="Not done">
+      <formula>NOT(ISERROR(SEARCH("Not done",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="100" priority="31" operator="containsText" text="Done">
+      <formula>NOT(ISERROR(SEARCH("Done",B4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4">
+    <cfRule type="containsText" dxfId="99" priority="25" operator="containsText" text="POUT">
+      <formula>NOT(ISERROR(SEARCH("POUT",B4)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="98" priority="26" operator="containsText" text="Pre-release">
+      <formula>NOT(ISERROR(SEARCH("Pre-release",B4)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="39" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
+    <cfRule type="beginsWith" dxfId="3" priority="2" operator="beginsWith" text="Done">
+      <formula>LEFT(A1,LEN("Done"))="Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="40" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Testing">
+      <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="41" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="In Progress">
+      <formula>NOT(ISERROR(SEARCH("In Progress",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="42" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Not Done">
+      <formula>NOT(ISERROR(SEARCH("Not Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1 A52:A64 A5:A49">
-    <cfRule type="containsText" dxfId="105" priority="36" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="37" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="103" priority="31" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="32" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="33" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="34" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="35" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A2">
-    <cfRule type="containsText" dxfId="98" priority="29" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="30" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A2)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="containsText" dxfId="96" priority="24" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="25" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="26" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="27" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="28" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A3">
-    <cfRule type="containsText" dxfId="91" priority="22" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="23" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A3)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="89" priority="17" operator="containsText" text="NGTD">
-      <formula>NOT(ISERROR(SEARCH("NGTD",A4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="18" operator="containsText" text="Test">
-      <formula>NOT(ISERROR(SEARCH("Test",A4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="19" operator="containsText" text="Future">
-      <formula>NOT(ISERROR(SEARCH("Future",A4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="20" operator="containsText" text="Not done">
-      <formula>NOT(ISERROR(SEARCH("Not done",A4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="21" operator="containsText" text="Done">
-      <formula>NOT(ISERROR(SEARCH("Done",A4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4">
-    <cfRule type="containsText" dxfId="84" priority="15" operator="containsText" text="POUT">
-      <formula>NOT(ISERROR(SEARCH("POUT",A4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="16" operator="containsText" text="Pre-release">
-      <formula>NOT(ISERROR(SEARCH("Pre-release",A4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="A2:A197">
+      <formula1>Status</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" text="NGTD" id="{9A92CD36-DE60-4B6E-9C4B-54DE9365E923}">
+            <xm:f>NOT(ISERROR(SEARCH("NGTD",'To Do- Current'!A1)))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.24994659260841701"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="beginsWith" priority="7" operator="beginsWith" text="Done" id="{27B2B313-A545-4C87-A62B-8E0225E2AEA4}">
+            <xm:f>LEFT('To Do- Current'!A1,LEN("Done"))="Done"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="8" operator="containsText" text="Testing" id="{6834EF77-DF35-4393-BD67-E31BDE2B6E6E}">
+            <xm:f>NOT(ISERROR(SEARCH("Testing",'To Do- Current'!A1)))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="9" operator="containsText" text="In Progress" id="{AEA61A27-EC71-40AF-B6C1-66F9D1DAD78A}">
+            <xm:f>NOT(ISERROR(SEARCH("In Progress",'To Do- Current'!A1)))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="5" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="10" operator="containsText" text="Not Done" id="{ECB0E109-DEF7-4FE0-BF4B-7A11AF9CF929}">
+            <xm:f>NOT(ISERROR(SEARCH("Not Done",'To Do- Current'!A1)))</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC00000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -9561,94 +10628,94 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A65:A102 A1:A63">
-    <cfRule type="containsText" dxfId="82" priority="26" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="97" priority="26" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="27" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="96" priority="27" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="28" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="95" priority="28" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="29" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="94" priority="29" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="30" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="93" priority="30" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:A213 A1:A63">
-    <cfRule type="containsText" dxfId="77" priority="24" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="92" priority="24" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="25" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="91" priority="25" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103:A104">
-    <cfRule type="containsText" dxfId="75" priority="11" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="90" priority="11" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="12" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="89" priority="12" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="13" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="88" priority="13" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="14" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="87" priority="14" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="15" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="86" priority="15" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A216:A1048576">
-    <cfRule type="containsText" dxfId="70" priority="9" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="85" priority="9" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="10" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="84" priority="10" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:A213 A216:A1048576">
-    <cfRule type="containsText" dxfId="68" priority="16" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="83" priority="16" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="17" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="82" priority="17" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="18" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="81" priority="18" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="19" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="80" priority="19" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="20" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="79" priority="20" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="63" priority="4" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="78" priority="4" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="5" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="6" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="7" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="75" priority="7" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="74" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="58" priority="2" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="73" priority="2" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="3" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="72" priority="3" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10706,80 +11773,80 @@
     <sortCondition ref="E2:E30"/>
   </sortState>
   <conditionalFormatting sqref="A1:A106">
-    <cfRule type="containsText" dxfId="55" priority="53" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="70" priority="53" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="54" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="69" priority="54" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="55" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="68" priority="55" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="56" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="67" priority="56" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="57" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="66" priority="57" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A217">
-    <cfRule type="containsText" dxfId="50" priority="46" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="65" priority="46" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="47" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="64" priority="47" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E7">
-    <cfRule type="containsText" dxfId="48" priority="20" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="63" priority="20" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="62" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="22" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="61" priority="22" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107:A108">
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="60" priority="3" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="59" priority="4" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="58" priority="5" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A220:A1048576">
-    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="55" priority="1" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A220)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:A217 A220:A1048576">
-    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="53" priority="8" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="9" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="52" priority="9" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="10" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="51" priority="10" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="11" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="12" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A109)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13845,124 +14912,124 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A92 A95:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="33" priority="39" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="48" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="40" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="47" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="41" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="46" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="42" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="45" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="43" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:A94">
-    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="43" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="42" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="41" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="40" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="23" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="38" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="37" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="21" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="36" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="35" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="33" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="16" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F142:F143 F201:F202 F151 E142:E203">
-    <cfRule type="containsText" dxfId="14" priority="22" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="29" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F149">
-    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F149)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F184">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F184)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F176">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F162">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F162)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated to do list with more information on what has been moved to trac
</commit_message>
<xml_diff>
--- a/SAM TODO.xlsx
+++ b/SAM TODO.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2277" uniqueCount="763">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2305" uniqueCount="764">
   <si>
     <t>HCPV user interface</t>
   </si>
@@ -2333,6 +2333,9 @@
   </si>
   <si>
     <t>Entered into Trac?</t>
+  </si>
+  <si>
+    <t>testing</t>
   </si>
 </sst>
 </file>
@@ -2711,42 +2714,7 @@
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="142">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="147">
     <dxf>
       <fill>
         <patternFill>
@@ -3591,6 +3559,76 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color theme="0"/>
       </font>
@@ -3999,8 +4037,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="141"/>
-      <tableStyleElement type="headerRow" dxfId="140"/>
+      <tableStyleElement type="wholeTable" dxfId="146"/>
+      <tableStyleElement type="headerRow" dxfId="145"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -5759,56 +5797,56 @@
     <sortCondition ref="C2:C41" customList="Patch,Release,Pre-Release,Future"/>
   </sortState>
   <conditionalFormatting sqref="C2:C198">
-    <cfRule type="containsText" dxfId="139" priority="90" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="144" priority="90" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="containsText" dxfId="138" priority="32" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="143" priority="32" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",C27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C1048576">
-    <cfRule type="containsText" dxfId="137" priority="29" operator="containsText" text="patch">
+    <cfRule type="containsText" dxfId="142" priority="29" operator="containsText" text="patch">
       <formula>NOT(ISERROR(SEARCH("patch",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="136" priority="24" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="141" priority="24" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="135" priority="25" operator="beginsWith" text="Done">
+    <cfRule type="beginsWith" dxfId="140" priority="25" operator="beginsWith" text="Done">
       <formula>LEFT(B1,LEN("Done"))="Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="134" priority="26" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="139" priority="26" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="27" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="138" priority="27" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="28" operator="containsText" text="Not Done">
+    <cfRule type="containsText" dxfId="137" priority="28" operator="containsText" text="Not Done">
       <formula>NOT(ISERROR(SEARCH("Not Done",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C1:C1048576">
-    <cfRule type="containsText" dxfId="131" priority="6" operator="containsText" text="Release">
+    <cfRule type="containsText" dxfId="136" priority="6" operator="containsText" text="Release">
       <formula>NOT(ISERROR(SEARCH("Release",C1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="130" priority="1" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="135" priority="1" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="129" priority="2" operator="beginsWith" text="Done">
+    <cfRule type="beginsWith" dxfId="134" priority="2" operator="beginsWith" text="Done">
       <formula>LEFT(A1,LEN("Done"))="Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="3" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="133" priority="3" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="4" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="132" priority="4" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="5" operator="containsText" text="Not Done">
+    <cfRule type="containsText" dxfId="131" priority="5" operator="containsText" text="Not Done">
       <formula>NOT(ISERROR(SEARCH("Not Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8144,7 +8182,7 @@
   <dimension ref="A1:G197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8255,7 +8293,7 @@
         <v>181</v>
       </c>
       <c r="B6" s="17" t="s">
-        <v>108</v>
+        <v>446</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>82</v>
@@ -8303,7 +8341,7 @@
         <v>181</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>108</v>
+        <v>763</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>52</v>
@@ -8756,7 +8794,7 @@
         <v>181</v>
       </c>
       <c r="B41" s="17" t="s">
-        <v>108</v>
+        <v>446</v>
       </c>
       <c r="C41" t="s">
         <v>187</v>
@@ -8777,16 +8815,20 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="72"/>
+      <c r="A43" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B43" s="17" t="s">
-        <v>108</v>
+        <v>763</v>
       </c>
       <c r="C43" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="72"/>
+      <c r="A44" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B44" s="17" t="s">
         <v>108</v>
       </c>
@@ -8795,7 +8837,9 @@
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="72"/>
+      <c r="A45" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B45" s="17" t="s">
         <v>108</v>
       </c>
@@ -8804,7 +8848,9 @@
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="72"/>
+      <c r="A46" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B46" s="17" t="s">
         <v>108</v>
       </c>
@@ -8813,7 +8859,9 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="72"/>
+      <c r="A47" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B47" s="17" t="s">
         <v>108</v>
       </c>
@@ -8822,7 +8870,9 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="72"/>
+      <c r="A48" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B48" s="17" t="s">
         <v>108</v>
       </c>
@@ -8831,7 +8881,9 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="72"/>
+      <c r="A49" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B49" s="17" t="s">
         <v>108</v>
       </c>
@@ -8840,16 +8892,22 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="72"/>
+      <c r="A50" s="72" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="72"/>
+      <c r="A51" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="C51" s="27" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="72"/>
+      <c r="A52" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B52" s="17" t="s">
         <v>108</v>
       </c>
@@ -8858,16 +8916,20 @@
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="72"/>
+      <c r="A53" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B53" s="17" t="s">
-        <v>108</v>
+        <v>763</v>
       </c>
       <c r="C53" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="72"/>
+      <c r="A54" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B54" s="17" t="s">
         <v>108</v>
       </c>
@@ -8876,7 +8938,9 @@
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="72"/>
+      <c r="A55" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B55" s="17" t="s">
         <v>108</v>
       </c>
@@ -8885,7 +8949,9 @@
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="72"/>
+      <c r="A56" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B56" s="17" t="s">
         <v>108</v>
       </c>
@@ -8894,7 +8960,9 @@
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="72"/>
+      <c r="A57" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B57" s="17" t="s">
         <v>108</v>
       </c>
@@ -8903,7 +8971,9 @@
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="72"/>
+      <c r="A58" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B58" s="17" t="s">
         <v>108</v>
       </c>
@@ -8912,7 +8982,9 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="72"/>
+      <c r="A59" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B59" s="17" t="s">
         <v>108</v>
       </c>
@@ -8921,16 +8993,20 @@
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="72"/>
+      <c r="A60" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B60" s="17" t="s">
-        <v>108</v>
+        <v>446</v>
       </c>
       <c r="C60" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="72"/>
+      <c r="A61" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B61" s="17" t="s">
         <v>108</v>
       </c>
@@ -8939,7 +9015,9 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="72"/>
+      <c r="A62" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B62" s="17" t="s">
         <v>108</v>
       </c>
@@ -8948,7 +9026,9 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="72"/>
+      <c r="A63" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B63" s="17" t="s">
         <v>108</v>
       </c>
@@ -8957,28 +9037,45 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="72"/>
+      <c r="A64" s="72" t="s">
+        <v>181</v>
+      </c>
       <c r="B64" s="17" t="s">
-        <v>108</v>
+        <v>446</v>
       </c>
       <c r="C64" t="s">
         <v>496</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="72"/>
+      <c r="A65" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B65" s="17" t="s">
+        <v>446</v>
+      </c>
       <c r="C65" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="72"/>
+      <c r="A66" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B66" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="C66" t="s">
         <v>734</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="72"/>
+      <c r="A67" s="72" t="s">
+        <v>181</v>
+      </c>
+      <c r="B67" s="17" t="s">
+        <v>108</v>
+      </c>
       <c r="C67" t="s">
         <v>737</v>
       </c>
@@ -9374,120 +9471,120 @@
       <c r="A197" s="72"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B1 B52:B64 B5:B49">
-    <cfRule type="containsText" dxfId="125" priority="48" operator="containsText" text="NGTD">
+  <conditionalFormatting sqref="B1 B5:B49 B52:B67">
+    <cfRule type="containsText" dxfId="130" priority="48" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="124" priority="49" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="129" priority="49" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="50" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="128" priority="50" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="51" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="127" priority="51" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="52" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="126" priority="52" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1 B52:B64 B5:B49">
-    <cfRule type="containsText" dxfId="120" priority="46" operator="containsText" text="POUT">
+  <conditionalFormatting sqref="B1 B5:B49 B52:B67">
+    <cfRule type="containsText" dxfId="125" priority="46" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="47" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="124" priority="47" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="118" priority="41" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="123" priority="41" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="42" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="122" priority="42" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="43" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="121" priority="43" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="44" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="120" priority="44" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="45" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="119" priority="45" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2">
-    <cfRule type="containsText" dxfId="113" priority="39" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="118" priority="39" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="40" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="117" priority="40" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="containsText" dxfId="111" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="116" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="115" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="114" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="113" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="112" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3">
-    <cfRule type="containsText" dxfId="106" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="111" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="110" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="containsText" dxfId="104" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="109" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="108" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="107" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="106" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="105" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="containsText" dxfId="99" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="104" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="103" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="102" priority="1" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="3" priority="2" operator="beginsWith" text="Done">
+    <cfRule type="beginsWith" dxfId="101" priority="2" operator="beginsWith" text="Done">
       <formula>LEFT(A1,LEN("Done"))="Done"</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="100" priority="3" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="In Progress">
+    <cfRule type="containsText" dxfId="99" priority="4" operator="containsText" text="In Progress">
       <formula>NOT(ISERROR(SEARCH("In Progress",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Not Done">
+    <cfRule type="containsText" dxfId="98" priority="5" operator="containsText" text="Not Done">
       <formula>NOT(ISERROR(SEARCH("Not Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10628,94 +10725,94 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A65:A102 A1:A63">
-    <cfRule type="containsText" dxfId="97" priority="26" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="92" priority="26" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="27" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="91" priority="27" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="28" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="90" priority="28" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="29" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="89" priority="29" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="30" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="88" priority="30" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A65:A213 A1:A63">
-    <cfRule type="containsText" dxfId="92" priority="24" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="87" priority="24" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="25" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="86" priority="25" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A103:A104">
-    <cfRule type="containsText" dxfId="90" priority="11" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="85" priority="11" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="12" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="84" priority="12" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="13" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="83" priority="13" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="14" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="82" priority="14" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A103)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="15" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="81" priority="15" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A103)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A216:A1048576">
-    <cfRule type="containsText" dxfId="85" priority="9" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="80" priority="9" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A216)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="84" priority="10" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="79" priority="10" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A216)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:A213 A216:A1048576">
-    <cfRule type="containsText" dxfId="83" priority="16" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="78" priority="16" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="17" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="77" priority="17" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="18" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="76" priority="18" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="19" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="75" priority="19" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A105)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="20" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="74" priority="20" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A105)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="78" priority="4" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="73" priority="4" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="5" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="72" priority="5" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="6" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="71" priority="6" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="7" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="70" priority="7" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="69" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A64">
-    <cfRule type="containsText" dxfId="73" priority="2" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="68" priority="2" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A64)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="3" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="67" priority="3" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A64)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11773,80 +11870,80 @@
     <sortCondition ref="E2:E30"/>
   </sortState>
   <conditionalFormatting sqref="A1:A106">
-    <cfRule type="containsText" dxfId="70" priority="53" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="65" priority="53" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="69" priority="54" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="64" priority="54" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="55" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="63" priority="55" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="56" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="62" priority="56" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="57" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="61" priority="57" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A217">
-    <cfRule type="containsText" dxfId="65" priority="46" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="60" priority="46" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="64" priority="47" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="59" priority="47" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5:E7">
-    <cfRule type="containsText" dxfId="63" priority="20" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="58" priority="20" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="21" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="57" priority="21" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E5)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="22" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="56" priority="22" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A107:A108">
-    <cfRule type="containsText" dxfId="60" priority="3" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="55" priority="3" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="4" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="54" priority="4" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="5" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="53" priority="5" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="6" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="52" priority="6" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A107)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="7" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="51" priority="7" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A107)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A220:A1048576">
-    <cfRule type="containsText" dxfId="55" priority="1" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="50" priority="1" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A220)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="2" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="49" priority="2" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A220)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A109:A217 A220:A1048576">
-    <cfRule type="containsText" dxfId="53" priority="8" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="48" priority="8" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="9" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="47" priority="9" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="10" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="11" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="45" priority="11" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A109)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="44" priority="12" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A109)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14912,124 +15009,124 @@
     <sortCondition ref="E2:E52"/>
   </sortState>
   <conditionalFormatting sqref="A1:A92 A95:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="48" priority="39" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="43" priority="39" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="40" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="42" priority="40" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="41" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="41" priority="41" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="42" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="40" priority="42" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="39" priority="43" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A93:A94">
-    <cfRule type="containsText" dxfId="43" priority="34" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="38" priority="34" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="35" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="37" priority="35" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="36" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="36" priority="36" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="37" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="35" priority="37" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",A93)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="38" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="34" priority="38" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",A93)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:A203 A206:A1048576">
-    <cfRule type="containsText" dxfId="38" priority="32" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="33" priority="32" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",A1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="33" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="36" priority="27" operator="containsText" text="NGTD">
+    <cfRule type="containsText" dxfId="31" priority="27" operator="containsText" text="NGTD">
       <formula>NOT(ISERROR(SEARCH("NGTD",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="28" operator="containsText" text="Test">
+    <cfRule type="containsText" dxfId="30" priority="28" operator="containsText" text="Test">
       <formula>NOT(ISERROR(SEARCH("Test",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="34" priority="29" operator="containsText" text="Future">
+    <cfRule type="containsText" dxfId="29" priority="29" operator="containsText" text="Future">
       <formula>NOT(ISERROR(SEARCH("Future",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="30" operator="containsText" text="Not done">
+    <cfRule type="containsText" dxfId="28" priority="30" operator="containsText" text="Not done">
       <formula>NOT(ISERROR(SEARCH("Not done",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="31" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="27" priority="31" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141:F141">
-    <cfRule type="containsText" dxfId="31" priority="25" operator="containsText" text="POUT">
+    <cfRule type="containsText" dxfId="26" priority="25" operator="containsText" text="POUT">
       <formula>NOT(ISERROR(SEARCH("POUT",B141)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="Pre-release">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="Pre-release">
       <formula>NOT(ISERROR(SEARCH("Pre-release",B141)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F142:F143 F201:F202 F151 E142:E203">
-    <cfRule type="containsText" dxfId="29" priority="22" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="24" priority="22" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="23" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",E142)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="22" priority="24" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",E142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F149">
-    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F149)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="19" priority="12" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F149)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F184">
-    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="18" priority="7" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="8" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="17" priority="8" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F184)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="9" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="16" priority="9" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F184)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F176">
-    <cfRule type="containsText" dxfId="20" priority="4" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="5" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="14" priority="5" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F176)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="13" priority="6" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F176)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F162">
-    <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="maybe">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="maybe">
       <formula>NOT(ISERROR(SEARCH("maybe",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="Done">
+    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="Done">
       <formula>NOT(ISERROR(SEARCH("Done",F162)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="Yes">
+    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Yes">
       <formula>NOT(ISERROR(SEARCH("Yes",F162)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>